<commit_message>
updated plotting to show triangle on piezo line and base at max depth.
</commit_message>
<xml_diff>
--- a/slices.xlsx
+++ b/slices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W21"/>
+  <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,10 +541,15 @@
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
+          <t>mat</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
           <t>phi</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>c</t>
         </is>
@@ -615,9 +620,12 @@
         <v>507.3291799932767</v>
       </c>
       <c r="V2" t="n">
+        <v>1</v>
+      </c>
+      <c r="W2" t="n">
         <v>28</v>
       </c>
-      <c r="W2" t="n">
+      <c r="X2" t="n">
         <v>200</v>
       </c>
     </row>
@@ -686,9 +694,12 @@
         <v>1609.919957329554</v>
       </c>
       <c r="V3" t="n">
+        <v>1</v>
+      </c>
+      <c r="W3" t="n">
         <v>28</v>
       </c>
-      <c r="W3" t="n">
+      <c r="X3" t="n">
         <v>200</v>
       </c>
     </row>
@@ -757,9 +768,12 @@
         <v>2356.808682944481</v>
       </c>
       <c r="V4" t="n">
+        <v>1</v>
+      </c>
+      <c r="W4" t="n">
         <v>28</v>
       </c>
-      <c r="W4" t="n">
+      <c r="X4" t="n">
         <v>200</v>
       </c>
     </row>
@@ -828,9 +842,12 @@
         <v>2924.979360427155</v>
       </c>
       <c r="V5" t="n">
+        <v>1</v>
+      </c>
+      <c r="W5" t="n">
         <v>28</v>
       </c>
-      <c r="W5" t="n">
+      <c r="X5" t="n">
         <v>200</v>
       </c>
     </row>
@@ -899,9 +916,12 @@
         <v>3371.815887377009</v>
       </c>
       <c r="V6" t="n">
+        <v>1</v>
+      </c>
+      <c r="W6" t="n">
         <v>28</v>
       </c>
-      <c r="W6" t="n">
+      <c r="X6" t="n">
         <v>200</v>
       </c>
     </row>
@@ -970,9 +990,12 @@
         <v>3699.083937823591</v>
       </c>
       <c r="V7" t="n">
+        <v>1</v>
+      </c>
+      <c r="W7" t="n">
         <v>28</v>
       </c>
-      <c r="W7" t="n">
+      <c r="X7" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1041,9 +1064,12 @@
         <v>3887.607788104114</v>
       </c>
       <c r="V8" t="n">
+        <v>1</v>
+      </c>
+      <c r="W8" t="n">
         <v>28</v>
       </c>
-      <c r="W8" t="n">
+      <c r="X8" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1112,9 +1138,12 @@
         <v>4006.611246223633</v>
       </c>
       <c r="V9" t="n">
+        <v>1</v>
+      </c>
+      <c r="W9" t="n">
         <v>28</v>
       </c>
-      <c r="W9" t="n">
+      <c r="X9" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1183,9 +1212,12 @@
         <v>4036.624824100284</v>
       </c>
       <c r="V10" t="n">
+        <v>1</v>
+      </c>
+      <c r="W10" t="n">
         <v>28</v>
       </c>
-      <c r="W10" t="n">
+      <c r="X10" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1254,9 +1286,12 @@
         <v>3972.491073373149</v>
       </c>
       <c r="V11" t="n">
+        <v>1</v>
+      </c>
+      <c r="W11" t="n">
         <v>28</v>
       </c>
-      <c r="W11" t="n">
+      <c r="X11" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1325,9 +1360,12 @@
         <v>3823.103391604091</v>
       </c>
       <c r="V12" t="n">
+        <v>1</v>
+      </c>
+      <c r="W12" t="n">
         <v>28</v>
       </c>
-      <c r="W12" t="n">
+      <c r="X12" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1396,9 +1434,12 @@
         <v>3523.376295930079</v>
       </c>
       <c r="V13" t="n">
+        <v>2</v>
+      </c>
+      <c r="W13" t="n">
         <v>32</v>
       </c>
-      <c r="W13" t="n">
+      <c r="X13" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1467,9 +1508,12 @@
         <v>3189.933993141789</v>
       </c>
       <c r="V14" t="n">
+        <v>2</v>
+      </c>
+      <c r="W14" t="n">
         <v>32</v>
       </c>
-      <c r="W14" t="n">
+      <c r="X14" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1538,9 +1582,12 @@
         <v>2589.604130495291</v>
       </c>
       <c r="V15" t="n">
+        <v>2</v>
+      </c>
+      <c r="W15" t="n">
         <v>32</v>
       </c>
-      <c r="W15" t="n">
+      <c r="X15" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1609,9 +1656,12 @@
         <v>2183.374395426713</v>
       </c>
       <c r="V16" t="n">
+        <v>3</v>
+      </c>
+      <c r="W16" t="n">
         <v>27</v>
       </c>
-      <c r="W16" t="n">
+      <c r="X16" t="n">
         <v>400</v>
       </c>
     </row>
@@ -1680,9 +1730,12 @@
         <v>1966.1871212571</v>
       </c>
       <c r="V17" t="n">
+        <v>3</v>
+      </c>
+      <c r="W17" t="n">
         <v>27</v>
       </c>
-      <c r="W17" t="n">
+      <c r="X17" t="n">
         <v>400</v>
       </c>
     </row>
@@ -1751,9 +1804,12 @@
         <v>1683.648139491839</v>
       </c>
       <c r="V18" t="n">
+        <v>3</v>
+      </c>
+      <c r="W18" t="n">
         <v>27</v>
       </c>
-      <c r="W18" t="n">
+      <c r="X18" t="n">
         <v>400</v>
       </c>
     </row>
@@ -1822,9 +1878,12 @@
         <v>1326.997382351359</v>
       </c>
       <c r="V19" t="n">
+        <v>3</v>
+      </c>
+      <c r="W19" t="n">
         <v>27</v>
       </c>
-      <c r="W19" t="n">
+      <c r="X19" t="n">
         <v>400</v>
       </c>
     </row>
@@ -1893,9 +1952,12 @@
         <v>882.7525498539574</v>
       </c>
       <c r="V20" t="n">
+        <v>3</v>
+      </c>
+      <c r="W20" t="n">
         <v>27</v>
       </c>
-      <c r="W20" t="n">
+      <c r="X20" t="n">
         <v>400</v>
       </c>
     </row>
@@ -1964,9 +2026,12 @@
         <v>329.0193472545882</v>
       </c>
       <c r="V21" t="n">
+        <v>3</v>
+      </c>
+      <c r="W21" t="n">
         <v>27</v>
       </c>
-      <c r="W21" t="n">
+      <c r="X21" t="n">
         <v>400</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tried to fix spencer advanced method
</commit_message>
<xml_diff>
--- a/slices.xlsx
+++ b/slices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X21"/>
+  <dimension ref="A1:Z21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,30 +526,40 @@
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
+          <t>shear_reinf</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>normal_reinf</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
           <t>piezo_y</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>hw</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>u</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>mat</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>phi</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>c</t>
         </is>
@@ -611,21 +621,27 @@
         <v>8320.000000000007</v>
       </c>
       <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
         <v>79.26666666666667</v>
       </c>
-      <c r="T2" t="n">
+      <c r="V2" t="n">
         <v>1.666666666666671</v>
       </c>
-      <c r="U2" t="n">
+      <c r="W2" t="n">
         <v>104.0000000000003</v>
       </c>
-      <c r="V2" t="n">
+      <c r="X2" t="n">
         <v>1</v>
       </c>
-      <c r="W2" t="n">
+      <c r="Y2" t="n">
         <v>28</v>
       </c>
-      <c r="X2" t="n">
+      <c r="Z2" t="n">
         <v>200</v>
       </c>
     </row>
@@ -685,21 +701,27 @@
         <v>24960</v>
       </c>
       <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
         <v>79.13333333333334</v>
       </c>
-      <c r="T3" t="n">
+      <c r="V3" t="n">
         <v>14.33333333333334</v>
       </c>
-      <c r="U3" t="n">
+      <c r="W3" t="n">
         <v>894.4000000000005</v>
       </c>
-      <c r="V3" t="n">
+      <c r="X3" t="n">
         <v>1</v>
       </c>
-      <c r="W3" t="n">
+      <c r="Y3" t="n">
         <v>28</v>
       </c>
-      <c r="X3" t="n">
+      <c r="Z3" t="n">
         <v>200</v>
       </c>
     </row>
@@ -759,21 +781,27 @@
         <v>40400</v>
       </c>
       <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
         <v>79</v>
       </c>
-      <c r="T4" t="n">
+      <c r="V4" t="n">
         <v>27</v>
       </c>
-      <c r="U4" t="n">
+      <c r="W4" t="n">
         <v>1684.8</v>
       </c>
-      <c r="V4" t="n">
+      <c r="X4" t="n">
         <v>1</v>
       </c>
-      <c r="W4" t="n">
+      <c r="Y4" t="n">
         <v>28</v>
       </c>
-      <c r="X4" t="n">
+      <c r="Z4" t="n">
         <v>200</v>
       </c>
     </row>
@@ -833,21 +861,27 @@
         <v>55856</v>
       </c>
       <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
         <v>78.18918918918919</v>
       </c>
-      <c r="T5" t="n">
+      <c r="V5" t="n">
         <v>38.98918918918919</v>
       </c>
-      <c r="U5" t="n">
+      <c r="W5" t="n">
         <v>2432.925405405405</v>
       </c>
-      <c r="V5" t="n">
+      <c r="X5" t="n">
         <v>1</v>
       </c>
-      <c r="W5" t="n">
+      <c r="Y5" t="n">
         <v>28</v>
       </c>
-      <c r="X5" t="n">
+      <c r="Z5" t="n">
         <v>200</v>
       </c>
     </row>
@@ -907,21 +941,27 @@
         <v>72752</v>
       </c>
       <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
         <v>77.37837837837837</v>
       </c>
-      <c r="T6" t="n">
+      <c r="V6" t="n">
         <v>50.97837837837837</v>
       </c>
-      <c r="U6" t="n">
+      <c r="W6" t="n">
         <v>3181.050810810811</v>
       </c>
-      <c r="V6" t="n">
+      <c r="X6" t="n">
         <v>1</v>
       </c>
-      <c r="W6" t="n">
+      <c r="Y6" t="n">
         <v>28</v>
       </c>
-      <c r="X6" t="n">
+      <c r="Z6" t="n">
         <v>200</v>
       </c>
     </row>
@@ -981,21 +1021,27 @@
         <v>106200</v>
       </c>
       <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="n">
         <v>76.56756756756756</v>
       </c>
-      <c r="T7" t="n">
+      <c r="V7" t="n">
         <v>56.56756756756756</v>
       </c>
-      <c r="U7" t="n">
+      <c r="W7" t="n">
         <v>3529.816216216216</v>
       </c>
-      <c r="V7" t="n">
+      <c r="X7" t="n">
         <v>1</v>
       </c>
-      <c r="W7" t="n">
+      <c r="Y7" t="n">
         <v>28</v>
       </c>
-      <c r="X7" t="n">
+      <c r="Z7" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1055,21 +1101,27 @@
         <v>106200</v>
       </c>
       <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
         <v>75.35714285714286</v>
       </c>
-      <c r="T8" t="n">
+      <c r="V8" t="n">
         <v>55.35714285714286</v>
       </c>
-      <c r="U8" t="n">
+      <c r="W8" t="n">
         <v>3454.285714285715</v>
       </c>
-      <c r="V8" t="n">
+      <c r="X8" t="n">
         <v>1</v>
       </c>
-      <c r="W8" t="n">
+      <c r="Y8" t="n">
         <v>28</v>
       </c>
-      <c r="X8" t="n">
+      <c r="Z8" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1129,21 +1181,27 @@
         <v>106200</v>
       </c>
       <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
         <v>73.21428571428571</v>
       </c>
-      <c r="T9" t="n">
+      <c r="V9" t="n">
         <v>53.21428571428571</v>
       </c>
-      <c r="U9" t="n">
+      <c r="W9" t="n">
         <v>3320.571428571428</v>
       </c>
-      <c r="V9" t="n">
+      <c r="X9" t="n">
         <v>1</v>
       </c>
-      <c r="W9" t="n">
+      <c r="Y9" t="n">
         <v>28</v>
       </c>
-      <c r="X9" t="n">
+      <c r="Z9" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1203,21 +1261,27 @@
         <v>106200</v>
       </c>
       <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" t="n">
         <v>71.07142857142857</v>
       </c>
-      <c r="T10" t="n">
+      <c r="V10" t="n">
         <v>51.07142857142857</v>
       </c>
-      <c r="U10" t="n">
+      <c r="W10" t="n">
         <v>3186.857142857143</v>
       </c>
-      <c r="V10" t="n">
+      <c r="X10" t="n">
         <v>1</v>
       </c>
-      <c r="W10" t="n">
+      <c r="Y10" t="n">
         <v>28</v>
       </c>
-      <c r="X10" t="n">
+      <c r="Z10" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1277,21 +1341,27 @@
         <v>106200</v>
       </c>
       <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" t="n">
         <v>68.5</v>
       </c>
-      <c r="T11" t="n">
+      <c r="V11" t="n">
         <v>48.5</v>
       </c>
-      <c r="U11" t="n">
+      <c r="W11" t="n">
         <v>3026.4</v>
       </c>
-      <c r="V11" t="n">
+      <c r="X11" t="n">
         <v>1</v>
       </c>
-      <c r="W11" t="n">
+      <c r="Y11" t="n">
         <v>28</v>
       </c>
-      <c r="X11" t="n">
+      <c r="Z11" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1351,21 +1421,27 @@
         <v>92254.49999999994</v>
       </c>
       <c r="S12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" t="n">
         <v>65.14749999999999</v>
       </c>
-      <c r="T12" t="n">
+      <c r="V12" t="n">
         <v>45.14749999999999</v>
       </c>
-      <c r="U12" t="n">
+      <c r="W12" t="n">
         <v>2817.204</v>
       </c>
-      <c r="V12" t="n">
+      <c r="X12" t="n">
         <v>1</v>
       </c>
-      <c r="W12" t="n">
+      <c r="Y12" t="n">
         <v>28</v>
       </c>
-      <c r="X12" t="n">
+      <c r="Z12" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1425,21 +1501,27 @@
         <v>76199.5</v>
       </c>
       <c r="S13" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0</v>
+      </c>
+      <c r="U13" t="n">
         <v>61.44250000000001</v>
       </c>
-      <c r="T13" t="n">
+      <c r="V13" t="n">
         <v>41.44250000000001</v>
       </c>
-      <c r="U13" t="n">
+      <c r="W13" t="n">
         <v>2586.012000000001</v>
       </c>
-      <c r="V13" t="n">
+      <c r="X13" t="n">
         <v>1</v>
       </c>
-      <c r="W13" t="n">
+      <c r="Y13" t="n">
         <v>28</v>
       </c>
-      <c r="X13" t="n">
+      <c r="Z13" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1499,21 +1581,27 @@
         <v>49728.00000000004</v>
       </c>
       <c r="S14" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" t="n">
         <v>56.55384615384616</v>
       </c>
-      <c r="T14" t="n">
+      <c r="V14" t="n">
         <v>36.55384615384616</v>
       </c>
-      <c r="U14" t="n">
+      <c r="W14" t="n">
         <v>2280.96</v>
       </c>
-      <c r="V14" t="n">
+      <c r="X14" t="n">
         <v>2</v>
       </c>
-      <c r="W14" t="n">
+      <c r="Y14" t="n">
         <v>32</v>
       </c>
-      <c r="X14" t="n">
+      <c r="Z14" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1573,21 +1661,27 @@
         <v>40256.00000000003</v>
       </c>
       <c r="S15" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" t="n">
         <v>52</v>
       </c>
-      <c r="T15" t="n">
+      <c r="V15" t="n">
         <v>32</v>
       </c>
-      <c r="U15" t="n">
+      <c r="W15" t="n">
         <v>1996.8</v>
       </c>
-      <c r="V15" t="n">
+      <c r="X15" t="n">
         <v>2</v>
       </c>
-      <c r="W15" t="n">
+      <c r="Y15" t="n">
         <v>32</v>
       </c>
-      <c r="X15" t="n">
+      <c r="Z15" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1647,21 +1741,27 @@
         <v>30784.00000000003</v>
       </c>
       <c r="S16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" t="n">
         <v>44</v>
       </c>
-      <c r="T16" t="n">
+      <c r="V16" t="n">
         <v>24</v>
       </c>
-      <c r="U16" t="n">
+      <c r="W16" t="n">
         <v>1497.6</v>
       </c>
-      <c r="V16" t="n">
+      <c r="X16" t="n">
         <v>2</v>
       </c>
-      <c r="W16" t="n">
+      <c r="Y16" t="n">
         <v>32</v>
       </c>
-      <c r="X16" t="n">
+      <c r="Z16" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1721,21 +1821,27 @@
         <v>20723.99999999999</v>
       </c>
       <c r="S17" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0</v>
+      </c>
+      <c r="U17" t="n">
         <v>40</v>
       </c>
-      <c r="T17" t="n">
-        <v>20</v>
-      </c>
-      <c r="U17" t="n">
+      <c r="V17" t="n">
+        <v>20</v>
+      </c>
+      <c r="W17" t="n">
         <v>1248</v>
       </c>
-      <c r="V17" t="n">
+      <c r="X17" t="n">
         <v>3</v>
       </c>
-      <c r="W17" t="n">
+      <c r="Y17" t="n">
         <v>27</v>
       </c>
-      <c r="X17" t="n">
+      <c r="Z17" t="n">
         <v>400</v>
       </c>
     </row>
@@ -1795,21 +1901,27 @@
         <v>20723.99999999999</v>
       </c>
       <c r="S18" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0</v>
+      </c>
+      <c r="U18" t="n">
         <v>40</v>
       </c>
-      <c r="T18" t="n">
-        <v>20</v>
-      </c>
-      <c r="U18" t="n">
+      <c r="V18" t="n">
+        <v>20</v>
+      </c>
+      <c r="W18" t="n">
         <v>1248</v>
       </c>
-      <c r="V18" t="n">
+      <c r="X18" t="n">
         <v>3</v>
       </c>
-      <c r="W18" t="n">
+      <c r="Y18" t="n">
         <v>27</v>
       </c>
-      <c r="X18" t="n">
+      <c r="Z18" t="n">
         <v>400</v>
       </c>
     </row>
@@ -1869,21 +1981,27 @@
         <v>22000</v>
       </c>
       <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0</v>
+      </c>
+      <c r="U19" t="n">
         <v>40</v>
       </c>
-      <c r="T19" t="n">
+      <c r="V19" t="n">
         <v>16.66666666666667</v>
       </c>
-      <c r="U19" t="n">
+      <c r="W19" t="n">
         <v>1040</v>
       </c>
-      <c r="V19" t="n">
+      <c r="X19" t="n">
         <v>3</v>
       </c>
-      <c r="W19" t="n">
+      <c r="Y19" t="n">
         <v>27</v>
       </c>
-      <c r="X19" t="n">
+      <c r="Z19" t="n">
         <v>400</v>
       </c>
     </row>
@@ -1943,21 +2061,27 @@
         <v>13200</v>
       </c>
       <c r="S20" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" t="n">
         <v>40</v>
       </c>
-      <c r="T20" t="n">
+      <c r="V20" t="n">
         <v>10</v>
       </c>
-      <c r="U20" t="n">
+      <c r="W20" t="n">
         <v>624</v>
       </c>
-      <c r="V20" t="n">
+      <c r="X20" t="n">
         <v>3</v>
       </c>
-      <c r="W20" t="n">
+      <c r="Y20" t="n">
         <v>27</v>
       </c>
-      <c r="X20" t="n">
+      <c r="Z20" t="n">
         <v>400</v>
       </c>
     </row>
@@ -2017,21 +2141,27 @@
         <v>4400.000000000004</v>
       </c>
       <c r="S21" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0</v>
+      </c>
+      <c r="U21" t="n">
         <v>40</v>
       </c>
-      <c r="T21" t="n">
+      <c r="V21" t="n">
         <v>3.333333333333336</v>
       </c>
-      <c r="U21" t="n">
+      <c r="W21" t="n">
         <v>208.0000000000001</v>
       </c>
-      <c r="V21" t="n">
+      <c r="X21" t="n">
         <v>3</v>
       </c>
-      <c r="W21" t="n">
+      <c r="Y21" t="n">
         <v>27</v>
       </c>
-      <c r="X21" t="n">
+      <c r="Z21" t="n">
         <v>400</v>
       </c>
     </row>

</xml_diff>

<commit_message>
generalized the solve functions.
</commit_message>
<xml_diff>
--- a/slices.xlsx
+++ b/slices.xlsx
@@ -570,43 +570,43 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>50</v>
+        <v>60.52735684831512</v>
       </c>
       <c r="C2" t="n">
-        <v>84</v>
+        <v>83.99980597459211</v>
       </c>
       <c r="D2" t="n">
         <v>84</v>
       </c>
       <c r="E2" t="n">
-        <v>60</v>
+        <v>70.39551763623633</v>
       </c>
       <c r="F2" t="n">
-        <v>71.2</v>
+        <v>61.19606926906113</v>
       </c>
       <c r="G2" t="n">
         <v>84</v>
       </c>
       <c r="H2" t="n">
-        <v>55</v>
+        <v>65.46143724227572</v>
       </c>
       <c r="I2" t="n">
-        <v>77.59999999999999</v>
+        <v>70.99690551636458</v>
       </c>
       <c r="J2" t="n">
         <v>84</v>
       </c>
       <c r="K2" t="n">
-        <v>10</v>
+        <v>9.868160787921219</v>
       </c>
       <c r="L2" t="n">
-        <v>52.00126755748238</v>
+        <v>65.89820373474561</v>
       </c>
       <c r="M2" t="n">
-        <v>16.24315240339286</v>
+        <v>24.1654007820007</v>
       </c>
       <c r="N2" t="n">
-        <v>6.400000000000006</v>
+        <v>13.00309448363542</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
@@ -618,7 +618,7 @@
         <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>8320.000000000007</v>
+        <v>16681.16152365595</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
@@ -627,13 +627,13 @@
         <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>79.26666666666667</v>
+        <v>79.12718083676965</v>
       </c>
       <c r="V2" t="n">
-        <v>1.666666666666671</v>
+        <v>8.130275320405076</v>
       </c>
       <c r="W2" t="n">
-        <v>104.0000000000003</v>
+        <v>507.3291799932767</v>
       </c>
       <c r="X2" t="n">
         <v>1</v>
@@ -650,46 +650,46 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>60</v>
+        <v>70.39551763623633</v>
       </c>
       <c r="C3" t="n">
-        <v>71.2</v>
+        <v>61.19606926906113</v>
       </c>
       <c r="D3" t="n">
         <v>84</v>
       </c>
       <c r="E3" t="n">
-        <v>70</v>
+        <v>80.26367842415756</v>
       </c>
       <c r="F3" t="n">
-        <v>58.4</v>
+        <v>46.34520128139259</v>
       </c>
       <c r="G3" t="n">
         <v>84</v>
       </c>
       <c r="H3" t="n">
-        <v>65</v>
+        <v>75.32959803019695</v>
       </c>
       <c r="I3" t="n">
-        <v>64.8</v>
+        <v>53.17327651921067</v>
       </c>
       <c r="J3" t="n">
         <v>84</v>
       </c>
       <c r="K3" t="n">
-        <v>10</v>
+        <v>9.868160787921227</v>
       </c>
       <c r="L3" t="n">
-        <v>52.00126755749349</v>
+        <v>56.15905274156578</v>
       </c>
       <c r="M3" t="n">
-        <v>16.24315240339689</v>
+        <v>17.72014640795434</v>
       </c>
       <c r="N3" t="n">
-        <v>19.2</v>
+        <v>20</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>10.82672348078933</v>
       </c>
       <c r="P3" t="n">
         <v>0</v>
@@ -698,7 +698,7 @@
         <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>24960</v>
+        <v>38477.99982237014</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
@@ -707,13 +707,13 @@
         <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>79.13333333333334</v>
+        <v>78.97327583538943</v>
       </c>
       <c r="V3" t="n">
-        <v>14.33333333333334</v>
+        <v>25.79999931617876</v>
       </c>
       <c r="W3" t="n">
-        <v>894.4000000000005</v>
+        <v>1609.919957329554</v>
       </c>
       <c r="X3" t="n">
         <v>1</v>
@@ -730,46 +730,46 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>70</v>
+        <v>80.26367842415756</v>
       </c>
       <c r="C4" t="n">
-        <v>58.4</v>
+        <v>46.34520128139259</v>
       </c>
       <c r="D4" t="n">
         <v>84</v>
       </c>
       <c r="E4" t="n">
-        <v>80</v>
+        <v>90.13183921207877</v>
       </c>
       <c r="F4" t="n">
-        <v>45.6</v>
+        <v>35.16253607942096</v>
       </c>
       <c r="G4" t="n">
         <v>84</v>
       </c>
       <c r="H4" t="n">
-        <v>75</v>
+        <v>85.19775881811816</v>
       </c>
       <c r="I4" t="n">
-        <v>52</v>
+        <v>40.40378477144077</v>
       </c>
       <c r="J4" t="n">
         <v>84</v>
       </c>
       <c r="K4" t="n">
-        <v>10</v>
+        <v>9.868160787921212</v>
       </c>
       <c r="L4" t="n">
-        <v>52.00126755749349</v>
+        <v>48.44782535860768</v>
       </c>
       <c r="M4" t="n">
-        <v>16.24315240339689</v>
+        <v>14.87733183099115</v>
       </c>
       <c r="N4" t="n">
         <v>20</v>
       </c>
       <c r="O4" t="n">
-        <v>12</v>
+        <v>23.59621522855923</v>
       </c>
       <c r="P4" t="n">
         <v>0</v>
@@ -778,7 +778,7 @@
         <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>40400</v>
+        <v>53599.36755201326</v>
       </c>
       <c r="S4" t="n">
         <v>0</v>
@@ -787,13 +787,13 @@
         <v>0</v>
       </c>
       <c r="U4" t="n">
-        <v>79</v>
+        <v>78.17315469042285</v>
       </c>
       <c r="V4" t="n">
-        <v>27</v>
+        <v>37.76936991898208</v>
       </c>
       <c r="W4" t="n">
-        <v>1684.8</v>
+        <v>2356.808682944481</v>
       </c>
       <c r="X4" t="n">
         <v>1</v>
@@ -810,40 +810,40 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>80</v>
+        <v>90.13183921207877</v>
       </c>
       <c r="C5" t="n">
-        <v>45.6</v>
+        <v>35.16253607942096</v>
       </c>
       <c r="D5" t="n">
         <v>84</v>
       </c>
       <c r="E5" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="F5" t="n">
-        <v>32.8</v>
+        <v>26.32503002402403</v>
       </c>
       <c r="G5" t="n">
         <v>84</v>
       </c>
       <c r="H5" t="n">
-        <v>85</v>
+        <v>95.06591960603939</v>
       </c>
       <c r="I5" t="n">
-        <v>39.2</v>
+        <v>30.4983643078416</v>
       </c>
       <c r="J5" t="n">
         <v>84</v>
       </c>
       <c r="K5" t="n">
-        <v>10</v>
+        <v>9.868160787921227</v>
       </c>
       <c r="L5" t="n">
-        <v>52.00126755750121</v>
+        <v>41.768101924379</v>
       </c>
       <c r="M5" t="n">
-        <v>16.24315240339969</v>
+        <v>13.23081183140688</v>
       </c>
       <c r="N5" t="n">
         <v>20</v>
@@ -852,13 +852,13 @@
         <v>24</v>
       </c>
       <c r="P5" t="n">
-        <v>0.7999999999999972</v>
+        <v>9.501635692158402</v>
       </c>
       <c r="Q5" t="n">
         <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>55856</v>
+        <v>66454.32539392641</v>
       </c>
       <c r="S5" t="n">
         <v>0</v>
@@ -867,13 +867,13 @@
         <v>0</v>
       </c>
       <c r="U5" t="n">
-        <v>78.18918918918919</v>
+        <v>77.37303354545627</v>
       </c>
       <c r="V5" t="n">
-        <v>38.98918918918919</v>
+        <v>46.87466923761467</v>
       </c>
       <c r="W5" t="n">
-        <v>2432.925405405405</v>
+        <v>2924.979360427155</v>
       </c>
       <c r="X5" t="n">
         <v>1</v>
@@ -890,28 +890,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C6" t="n">
-        <v>32.8</v>
+        <v>26.32503002402403</v>
       </c>
       <c r="D6" t="n">
         <v>84</v>
       </c>
       <c r="E6" t="n">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="F6" t="n">
-        <v>20</v>
+        <v>19.12879499083992</v>
       </c>
       <c r="G6" t="n">
         <v>84</v>
       </c>
       <c r="H6" t="n">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="I6" t="n">
-        <v>26.4</v>
+        <v>22.53205655191036</v>
       </c>
       <c r="J6" t="n">
         <v>84</v>
@@ -920,10 +920,10 @@
         <v>10</v>
       </c>
       <c r="L6" t="n">
-        <v>52.00126755748963</v>
+        <v>35.68533492922602</v>
       </c>
       <c r="M6" t="n">
-        <v>16.24315240339549</v>
+        <v>12.31174025844438</v>
       </c>
       <c r="N6" t="n">
         <v>20</v>
@@ -932,13 +932,13 @@
         <v>24</v>
       </c>
       <c r="P6" t="n">
-        <v>13.6</v>
+        <v>17.46794344808964</v>
       </c>
       <c r="Q6" t="n">
-        <v>0</v>
+        <v>25000</v>
       </c>
       <c r="R6" t="n">
-        <v>72752</v>
+        <v>102857.6853514783</v>
       </c>
       <c r="S6" t="n">
         <v>0</v>
@@ -947,13 +947,13 @@
         <v>0</v>
       </c>
       <c r="U6" t="n">
-        <v>77.37837837837837</v>
+        <v>76.56756756756756</v>
       </c>
       <c r="V6" t="n">
-        <v>50.97837837837837</v>
+        <v>54.03551101565721</v>
       </c>
       <c r="W6" t="n">
-        <v>3181.050810810811</v>
+        <v>3371.815887377009</v>
       </c>
       <c r="X6" t="n">
         <v>1</v>
@@ -970,28 +970,28 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C7" t="n">
-        <v>20</v>
+        <v>19.12879499083992</v>
       </c>
       <c r="D7" t="n">
         <v>84</v>
       </c>
       <c r="E7" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="F7" t="n">
-        <v>20</v>
+        <v>13.3463549614923</v>
       </c>
       <c r="G7" t="n">
         <v>84</v>
       </c>
       <c r="H7" t="n">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="I7" t="n">
-        <v>20</v>
+        <v>16.07695154586736</v>
       </c>
       <c r="J7" t="n">
         <v>84</v>
@@ -1000,10 +1000,10 @@
         <v>10</v>
       </c>
       <c r="L7" t="n">
-        <v>-0</v>
+        <v>30.00000015313622</v>
       </c>
       <c r="M7" t="n">
-        <v>10</v>
+        <v>11.54700540161072</v>
       </c>
       <c r="N7" t="n">
         <v>20</v>
@@ -1012,13 +1012,13 @@
         <v>24</v>
       </c>
       <c r="P7" t="n">
-        <v>20</v>
+        <v>23.92304845413264</v>
       </c>
       <c r="Q7" t="n">
         <v>25000</v>
       </c>
       <c r="R7" t="n">
-        <v>106200</v>
+        <v>111378.4239594551</v>
       </c>
       <c r="S7" t="n">
         <v>0</v>
@@ -1027,13 +1027,13 @@
         <v>0</v>
       </c>
       <c r="U7" t="n">
-        <v>76.56756756756756</v>
+        <v>75.35714285714286</v>
       </c>
       <c r="V7" t="n">
-        <v>56.56756756756756</v>
+        <v>59.2801913112755</v>
       </c>
       <c r="W7" t="n">
-        <v>3529.816216216216</v>
+        <v>3699.083937823591</v>
       </c>
       <c r="X7" t="n">
         <v>1</v>
@@ -1050,28 +1050,28 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="C8" t="n">
-        <v>20</v>
+        <v>13.3463549614923</v>
       </c>
       <c r="D8" t="n">
         <v>84</v>
       </c>
       <c r="E8" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="F8" t="n">
-        <v>20</v>
+        <v>8.757022693565062</v>
       </c>
       <c r="G8" t="n">
         <v>84</v>
       </c>
       <c r="H8" t="n">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="I8" t="n">
-        <v>20</v>
+        <v>10.91287885364285</v>
       </c>
       <c r="J8" t="n">
         <v>84</v>
@@ -1080,10 +1080,10 @@
         <v>10</v>
       </c>
       <c r="L8" t="n">
-        <v>-0</v>
+        <v>24.62431846252714</v>
       </c>
       <c r="M8" t="n">
-        <v>10</v>
+        <v>11.00038197405046</v>
       </c>
       <c r="N8" t="n">
         <v>20</v>
@@ -1092,13 +1092,13 @@
         <v>24</v>
       </c>
       <c r="P8" t="n">
-        <v>20</v>
+        <v>29.08712114635715</v>
       </c>
       <c r="Q8" t="n">
         <v>25000</v>
       </c>
       <c r="R8" t="n">
-        <v>106200</v>
+        <v>118194.9999131914</v>
       </c>
       <c r="S8" t="n">
         <v>0</v>
@@ -1107,13 +1107,13 @@
         <v>0</v>
       </c>
       <c r="U8" t="n">
-        <v>75.35714285714286</v>
+        <v>73.21428571428571</v>
       </c>
       <c r="V8" t="n">
-        <v>55.35714285714286</v>
+        <v>62.30140686064286</v>
       </c>
       <c r="W8" t="n">
-        <v>3454.285714285715</v>
+        <v>3887.607788104114</v>
       </c>
       <c r="X8" t="n">
         <v>1</v>
@@ -1130,28 +1130,28 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C9" t="n">
-        <v>20</v>
+        <v>8.757022693565062</v>
       </c>
       <c r="D9" t="n">
         <v>84</v>
       </c>
       <c r="E9" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="F9" t="n">
-        <v>20</v>
+        <v>5.217597167510036</v>
       </c>
       <c r="G9" t="n">
         <v>84</v>
       </c>
       <c r="H9" t="n">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="I9" t="n">
-        <v>20</v>
+        <v>6.862915010152392</v>
       </c>
       <c r="J9" t="n">
         <v>84</v>
@@ -1160,10 +1160,10 @@
         <v>10</v>
       </c>
       <c r="L9" t="n">
-        <v>-0</v>
+        <v>19.47122071361051</v>
       </c>
       <c r="M9" t="n">
-        <v>10</v>
+        <v>10.60660172297659</v>
       </c>
       <c r="N9" t="n">
         <v>20</v>
@@ -1172,13 +1172,13 @@
         <v>24</v>
       </c>
       <c r="P9" t="n">
-        <v>20</v>
+        <v>33.13708498984761</v>
       </c>
       <c r="Q9" t="n">
         <v>25000</v>
       </c>
       <c r="R9" t="n">
-        <v>106200</v>
+        <v>123540.9521865988</v>
       </c>
       <c r="S9" t="n">
         <v>0</v>
@@ -1187,13 +1187,13 @@
         <v>0</v>
       </c>
       <c r="U9" t="n">
-        <v>73.21428571428571</v>
+        <v>71.07142857142857</v>
       </c>
       <c r="V9" t="n">
-        <v>53.21428571428571</v>
+        <v>64.20851356127618</v>
       </c>
       <c r="W9" t="n">
-        <v>3320.571428571428</v>
+        <v>4006.611246223633</v>
       </c>
       <c r="X9" t="n">
         <v>1</v>
@@ -1210,28 +1210,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C10" t="n">
-        <v>20</v>
+        <v>5.217597167510036</v>
       </c>
       <c r="D10" t="n">
         <v>84</v>
       </c>
       <c r="E10" t="n">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="F10" t="n">
-        <v>20</v>
+        <v>2.633054056944971</v>
       </c>
       <c r="G10" t="n">
         <v>84</v>
       </c>
       <c r="H10" t="n">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="I10" t="n">
-        <v>20</v>
+        <v>3.810499613777495</v>
       </c>
       <c r="J10" t="n">
         <v>84</v>
@@ -1240,10 +1240,10 @@
         <v>10</v>
       </c>
       <c r="L10" t="n">
-        <v>-0</v>
+        <v>14.47751224073088</v>
       </c>
       <c r="M10" t="n">
-        <v>10</v>
+        <v>10.327955592437</v>
       </c>
       <c r="N10" t="n">
         <v>20</v>
@@ -1252,13 +1252,13 @@
         <v>24</v>
       </c>
       <c r="P10" t="n">
-        <v>20</v>
+        <v>36.18950038622251</v>
       </c>
       <c r="Q10" t="n">
         <v>25000</v>
       </c>
       <c r="R10" t="n">
-        <v>106200</v>
+        <v>127570.1405098137</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
@@ -1267,13 +1267,13 @@
         <v>0</v>
       </c>
       <c r="U10" t="n">
-        <v>71.07142857142857</v>
+        <v>68.5</v>
       </c>
       <c r="V10" t="n">
-        <v>51.07142857142857</v>
+        <v>64.68950038622251</v>
       </c>
       <c r="W10" t="n">
-        <v>3186.857142857143</v>
+        <v>4036.624824100284</v>
       </c>
       <c r="X10" t="n">
         <v>1</v>
@@ -1290,55 +1290,55 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="C11" t="n">
-        <v>20</v>
+        <v>2.633054056944971</v>
       </c>
       <c r="D11" t="n">
         <v>84</v>
       </c>
       <c r="E11" t="n">
-        <v>150</v>
+        <v>162.35</v>
       </c>
       <c r="F11" t="n">
-        <v>20</v>
+        <v>0.6686231538410539</v>
       </c>
       <c r="G11" t="n">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="H11" t="n">
-        <v>145</v>
+        <v>156.175</v>
       </c>
       <c r="I11" t="n">
-        <v>20</v>
+        <v>1.485784080558503</v>
       </c>
       <c r="J11" t="n">
-        <v>84</v>
+        <v>78.99999999999999</v>
       </c>
       <c r="K11" t="n">
-        <v>10</v>
+        <v>12.34999999999999</v>
       </c>
       <c r="L11" t="n">
-        <v>-0</v>
+        <v>9.025556359556186</v>
       </c>
       <c r="M11" t="n">
-        <v>10</v>
+        <v>12.50482896617596</v>
       </c>
       <c r="N11" t="n">
-        <v>20</v>
+        <v>14.99999999999999</v>
       </c>
       <c r="O11" t="n">
         <v>24</v>
       </c>
       <c r="P11" t="n">
-        <v>20</v>
+        <v>38.5142159194415</v>
       </c>
       <c r="Q11" t="n">
-        <v>25000</v>
+        <v>0</v>
       </c>
       <c r="R11" t="n">
-        <v>106200</v>
+        <v>122436.3747918735</v>
       </c>
       <c r="S11" t="n">
         <v>0</v>
@@ -1347,13 +1347,13 @@
         <v>0</v>
       </c>
       <c r="U11" t="n">
-        <v>68.5</v>
+        <v>65.14749999999999</v>
       </c>
       <c r="V11" t="n">
-        <v>48.5</v>
+        <v>63.66171591944149</v>
       </c>
       <c r="W11" t="n">
-        <v>3026.4</v>
+        <v>3972.491073373149</v>
       </c>
       <c r="X11" t="n">
         <v>1</v>
@@ -1370,55 +1370,55 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>150</v>
+        <v>162.35</v>
       </c>
       <c r="C12" t="n">
-        <v>20</v>
+        <v>0.6686231538410539</v>
       </c>
       <c r="D12" t="n">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="E12" t="n">
-        <v>158.2333333333333</v>
+        <v>174.7</v>
       </c>
       <c r="F12" t="n">
-        <v>20</v>
+        <v>0.000375000585933094</v>
       </c>
       <c r="G12" t="n">
-        <v>77.33333333333334</v>
+        <v>64</v>
       </c>
       <c r="H12" t="n">
-        <v>154.1166666666667</v>
+        <v>168.525</v>
       </c>
       <c r="I12" t="n">
-        <v>20</v>
+        <v>0.17481744224213</v>
       </c>
       <c r="J12" t="n">
-        <v>80.66666666666666</v>
+        <v>69.00000000000001</v>
       </c>
       <c r="K12" t="n">
-        <v>8.23333333333332</v>
+        <v>12.34999999999999</v>
       </c>
       <c r="L12" t="n">
-        <v>-0</v>
+        <v>3.093086941691099</v>
       </c>
       <c r="M12" t="n">
-        <v>8.23333333333332</v>
+        <v>12.3680178772166</v>
       </c>
       <c r="N12" t="n">
-        <v>16.66666666666666</v>
+        <v>5.000000000000014</v>
       </c>
       <c r="O12" t="n">
         <v>24</v>
       </c>
       <c r="P12" t="n">
-        <v>20</v>
+        <v>39.82518255775787</v>
       </c>
       <c r="Q12" t="n">
         <v>0</v>
       </c>
       <c r="R12" t="n">
-        <v>63286.88888888878</v>
+        <v>108518.5126056569</v>
       </c>
       <c r="S12" t="n">
         <v>0</v>
@@ -1427,13 +1427,13 @@
         <v>0</v>
       </c>
       <c r="U12" t="n">
-        <v>65.765</v>
+        <v>61.44250000000001</v>
       </c>
       <c r="V12" t="n">
-        <v>45.765</v>
+        <v>61.26768255775788</v>
       </c>
       <c r="W12" t="n">
-        <v>2855.736</v>
+        <v>3823.103391604091</v>
       </c>
       <c r="X12" t="n">
         <v>1</v>
@@ -1450,55 +1450,55 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>158.2333333333333</v>
+        <v>174.7</v>
       </c>
       <c r="C13" t="n">
+        <v>0.000375000585933094</v>
+      </c>
+      <c r="D13" t="n">
+        <v>64</v>
+      </c>
+      <c r="E13" t="n">
+        <v>184.5666666666667</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.3819458071278916</v>
+      </c>
+      <c r="G13" t="n">
+        <v>56</v>
+      </c>
+      <c r="H13" t="n">
+        <v>179.6333333333333</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.08948243701796343</v>
+      </c>
+      <c r="J13" t="n">
+        <v>60</v>
+      </c>
+      <c r="K13" t="n">
+        <v>9.866666666666674</v>
+      </c>
+      <c r="L13" t="n">
+        <v>-2.212803763689251</v>
+      </c>
+      <c r="M13" t="n">
+        <v>9.874029601984471</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
         <v>20</v>
       </c>
-      <c r="D13" t="n">
-        <v>77.33333333333334</v>
-      </c>
-      <c r="E13" t="n">
-        <v>166.4666666666667</v>
-      </c>
-      <c r="F13" t="n">
-        <v>20</v>
-      </c>
-      <c r="G13" t="n">
-        <v>70.66666666666666</v>
-      </c>
-      <c r="H13" t="n">
-        <v>162.35</v>
-      </c>
-      <c r="I13" t="n">
-        <v>20</v>
-      </c>
-      <c r="J13" t="n">
-        <v>74</v>
-      </c>
-      <c r="K13" t="n">
-        <v>8.233333333333348</v>
-      </c>
-      <c r="L13" t="n">
-        <v>-0</v>
-      </c>
-      <c r="M13" t="n">
-        <v>8.233333333333348</v>
-      </c>
-      <c r="N13" t="n">
-        <v>10</v>
-      </c>
-      <c r="O13" t="n">
-        <v>24</v>
-      </c>
       <c r="P13" t="n">
-        <v>20</v>
+        <v>39.91051756298204</v>
       </c>
       <c r="Q13" t="n">
         <v>0</v>
       </c>
       <c r="R13" t="n">
-        <v>56151.33333333344</v>
+        <v>75659.45807402786</v>
       </c>
       <c r="S13" t="n">
         <v>0</v>
@@ -1507,22 +1507,22 @@
         <v>0</v>
       </c>
       <c r="U13" t="n">
-        <v>63.295</v>
+        <v>56.55384615384616</v>
       </c>
       <c r="V13" t="n">
-        <v>43.295</v>
+        <v>56.4643637168282</v>
       </c>
       <c r="W13" t="n">
-        <v>2701.608</v>
+        <v>3523.376295930079</v>
       </c>
       <c r="X13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y13" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="Z13" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14">
@@ -1530,55 +1530,55 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>166.4666666666667</v>
+        <v>184.5666666666667</v>
       </c>
       <c r="C14" t="n">
-        <v>20</v>
+        <v>0.3819458071278916</v>
       </c>
       <c r="D14" t="n">
-        <v>70.66666666666666</v>
+        <v>56</v>
       </c>
       <c r="E14" t="n">
-        <v>174.7</v>
+        <v>194.4333333333333</v>
       </c>
       <c r="F14" t="n">
-        <v>20</v>
+        <v>1.58401478028587</v>
       </c>
       <c r="G14" t="n">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="H14" t="n">
-        <v>170.5833333333333</v>
+        <v>189.5</v>
       </c>
       <c r="I14" t="n">
-        <v>20</v>
+        <v>0.8792629304200403</v>
       </c>
       <c r="J14" t="n">
-        <v>67.33333333333334</v>
+        <v>52</v>
       </c>
       <c r="K14" t="n">
-        <v>8.23333333333332</v>
+        <v>9.866666666666674</v>
       </c>
       <c r="L14" t="n">
-        <v>-0</v>
+        <v>-6.940199065150054</v>
       </c>
       <c r="M14" t="n">
-        <v>8.23333333333332</v>
+        <v>9.939495248171937</v>
       </c>
       <c r="N14" t="n">
-        <v>3.333333333333343</v>
+        <v>0</v>
       </c>
       <c r="O14" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="P14" t="n">
-        <v>20</v>
+        <v>39.12073706957996</v>
       </c>
       <c r="Q14" t="n">
         <v>0</v>
       </c>
       <c r="R14" t="n">
-        <v>49015.77777777771</v>
+        <v>65158.84795942099</v>
       </c>
       <c r="S14" t="n">
         <v>0</v>
@@ -1587,22 +1587,22 @@
         <v>0</v>
       </c>
       <c r="U14" t="n">
-        <v>60.73076923076924</v>
+        <v>52</v>
       </c>
       <c r="V14" t="n">
-        <v>40.73076923076924</v>
+        <v>51.12073706957996</v>
       </c>
       <c r="W14" t="n">
-        <v>2541.6</v>
+        <v>3189.933993141789</v>
       </c>
       <c r="X14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y14" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="Z14" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15">
@@ -1610,55 +1610,55 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>174.7</v>
+        <v>194.4333333333333</v>
       </c>
       <c r="C15" t="n">
-        <v>20</v>
+        <v>1.58401478028587</v>
       </c>
       <c r="D15" t="n">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="E15" t="n">
-        <v>184.5666666666667</v>
+        <v>204.3</v>
       </c>
       <c r="F15" t="n">
-        <v>20</v>
+        <v>3.632006118520721</v>
       </c>
       <c r="G15" t="n">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="H15" t="n">
-        <v>179.6333333333333</v>
+        <v>199.3666666666667</v>
       </c>
       <c r="I15" t="n">
-        <v>20</v>
+        <v>2.499933806165217</v>
       </c>
       <c r="J15" t="n">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="K15" t="n">
         <v>9.866666666666674</v>
       </c>
       <c r="L15" t="n">
-        <v>-0</v>
+        <v>-11.71569679077994</v>
       </c>
       <c r="M15" t="n">
-        <v>9.866666666666674</v>
+        <v>10.07659006958593</v>
       </c>
       <c r="N15" t="n">
         <v>0</v>
       </c>
       <c r="O15" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="P15" t="n">
-        <v>20</v>
+        <v>37.50006619383478</v>
       </c>
       <c r="Q15" t="n">
         <v>0</v>
       </c>
       <c r="R15" t="n">
-        <v>49728.00000000004</v>
+        <v>53576.08621085047</v>
       </c>
       <c r="S15" t="n">
         <v>0</v>
@@ -1667,13 +1667,13 @@
         <v>0</v>
       </c>
       <c r="U15" t="n">
-        <v>56.55384615384616</v>
+        <v>44</v>
       </c>
       <c r="V15" t="n">
-        <v>36.55384615384616</v>
+        <v>41.50006619383478</v>
       </c>
       <c r="W15" t="n">
-        <v>2280.96</v>
+        <v>2589.604130495291</v>
       </c>
       <c r="X15" t="n">
         <v>2</v>
@@ -1690,55 +1690,55 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>184.5666666666667</v>
+        <v>204.3</v>
       </c>
       <c r="C16" t="n">
-        <v>20</v>
+        <v>3.632006118520721</v>
       </c>
       <c r="D16" t="n">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="E16" t="n">
-        <v>194.4333333333333</v>
+        <v>214.323780536418</v>
       </c>
       <c r="F16" t="n">
-        <v>20</v>
+        <v>6.626104043639586</v>
       </c>
       <c r="G16" t="n">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H16" t="n">
-        <v>189.5</v>
+        <v>209.311890268209</v>
       </c>
       <c r="I16" t="n">
-        <v>20</v>
+        <v>5.010025714315489</v>
       </c>
       <c r="J16" t="n">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="K16" t="n">
-        <v>9.866666666666674</v>
+        <v>10.02378053641795</v>
       </c>
       <c r="L16" t="n">
-        <v>-0</v>
+        <v>-16.61459186508567</v>
       </c>
       <c r="M16" t="n">
-        <v>9.866666666666674</v>
+        <v>10.46050903348247</v>
       </c>
       <c r="N16" t="n">
         <v>0</v>
       </c>
       <c r="O16" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>20</v>
+        <v>34.98997428568451</v>
       </c>
       <c r="Q16" t="n">
         <v>0</v>
       </c>
       <c r="R16" t="n">
-        <v>40256.00000000003</v>
+        <v>46296.60066432835</v>
       </c>
       <c r="S16" t="n">
         <v>0</v>
@@ -1747,22 +1747,22 @@
         <v>0</v>
       </c>
       <c r="U16" t="n">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="V16" t="n">
-        <v>32</v>
+        <v>34.98997428568451</v>
       </c>
       <c r="W16" t="n">
-        <v>1996.8</v>
+        <v>2183.374395426713</v>
       </c>
       <c r="X16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y16" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="Z16" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
     </row>
     <row r="17">
@@ -1770,55 +1770,55 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>194.4333333333333</v>
+        <v>214.323780536418</v>
       </c>
       <c r="C17" t="n">
-        <v>20</v>
+        <v>6.626104043639586</v>
       </c>
       <c r="D17" t="n">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E17" t="n">
-        <v>204.3</v>
+        <v>224.3475610728359</v>
       </c>
       <c r="F17" t="n">
-        <v>20</v>
+        <v>10.61618850962118</v>
       </c>
       <c r="G17" t="n">
         <v>40</v>
       </c>
       <c r="H17" t="n">
-        <v>199.3666666666667</v>
+        <v>219.3356708046269</v>
       </c>
       <c r="I17" t="n">
-        <v>20</v>
+        <v>8.49059100549519</v>
       </c>
       <c r="J17" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="K17" t="n">
-        <v>9.866666666666674</v>
+        <v>10.02378053641797</v>
       </c>
       <c r="L17" t="n">
-        <v>-0</v>
+        <v>-21.68255994558514</v>
       </c>
       <c r="M17" t="n">
-        <v>9.866666666666674</v>
+        <v>10.7870149791044</v>
       </c>
       <c r="N17" t="n">
         <v>0</v>
       </c>
       <c r="O17" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P17" t="n">
-        <v>20</v>
+        <v>31.50940899450481</v>
       </c>
       <c r="Q17" t="n">
         <v>0</v>
       </c>
       <c r="R17" t="n">
-        <v>30784.00000000003</v>
+        <v>41691.3288782959</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
@@ -1827,22 +1827,22 @@
         <v>0</v>
       </c>
       <c r="U17" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="V17" t="n">
-        <v>24</v>
+        <v>31.50940899450481</v>
       </c>
       <c r="W17" t="n">
-        <v>1497.6</v>
+        <v>1966.1871212571</v>
       </c>
       <c r="X17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y17" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="Z17" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
     </row>
     <row r="18">
@@ -1850,40 +1850,40 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>204.3</v>
+        <v>224.3475610728359</v>
       </c>
       <c r="C18" t="n">
-        <v>20</v>
+        <v>10.61618850962118</v>
       </c>
       <c r="D18" t="n">
         <v>40</v>
       </c>
       <c r="E18" t="n">
-        <v>212.15</v>
+        <v>234.3713416092539</v>
       </c>
       <c r="F18" t="n">
-        <v>20</v>
+        <v>15.71652194370731</v>
       </c>
       <c r="G18" t="n">
         <v>40</v>
       </c>
       <c r="H18" t="n">
-        <v>208.225</v>
+        <v>229.3594513410449</v>
       </c>
       <c r="I18" t="n">
-        <v>20</v>
+        <v>13.0184593030154</v>
       </c>
       <c r="J18" t="n">
         <v>40</v>
       </c>
       <c r="K18" t="n">
-        <v>7.849999999999994</v>
+        <v>10.02378053641795</v>
       </c>
       <c r="L18" t="n">
-        <v>-0</v>
+        <v>-26.93603065199318</v>
       </c>
       <c r="M18" t="n">
-        <v>7.849999999999994</v>
+        <v>11.24356274821377</v>
       </c>
       <c r="N18" t="n">
         <v>0</v>
@@ -1892,13 +1892,13 @@
         <v>0</v>
       </c>
       <c r="P18" t="n">
-        <v>20</v>
+        <v>26.9815406969846</v>
       </c>
       <c r="Q18" t="n">
         <v>0</v>
       </c>
       <c r="R18" t="n">
-        <v>20723.99999999999</v>
+        <v>35700.32960749238</v>
       </c>
       <c r="S18" t="n">
         <v>0</v>
@@ -1910,10 +1910,10 @@
         <v>40</v>
       </c>
       <c r="V18" t="n">
-        <v>20</v>
+        <v>26.9815406969846</v>
       </c>
       <c r="W18" t="n">
-        <v>1248</v>
+        <v>1683.648139491839</v>
       </c>
       <c r="X18" t="n">
         <v>3</v>
@@ -1930,40 +1930,40 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>212.15</v>
+        <v>234.3713416092539</v>
       </c>
       <c r="C19" t="n">
-        <v>20</v>
+        <v>15.71652194370731</v>
       </c>
       <c r="D19" t="n">
         <v>40</v>
       </c>
       <c r="E19" t="n">
-        <v>220</v>
+        <v>244.3951221456718</v>
       </c>
       <c r="F19" t="n">
-        <v>20</v>
+        <v>22.10047486127786</v>
       </c>
       <c r="G19" t="n">
         <v>40</v>
       </c>
       <c r="H19" t="n">
-        <v>216.075</v>
+        <v>239.3832318774628</v>
       </c>
       <c r="I19" t="n">
-        <v>20</v>
+        <v>18.73401630847181</v>
       </c>
       <c r="J19" t="n">
         <v>40</v>
       </c>
       <c r="K19" t="n">
-        <v>7.849999999999994</v>
+        <v>10.02378053641795</v>
       </c>
       <c r="L19" t="n">
-        <v>-0</v>
+        <v>-32.44752375024643</v>
       </c>
       <c r="M19" t="n">
-        <v>7.849999999999994</v>
+        <v>11.87816108521438</v>
       </c>
       <c r="N19" t="n">
         <v>0</v>
@@ -1972,13 +1972,13 @@
         <v>0</v>
       </c>
       <c r="P19" t="n">
-        <v>20</v>
+        <v>21.26598369152819</v>
       </c>
       <c r="Q19" t="n">
         <v>0</v>
       </c>
       <c r="R19" t="n">
-        <v>20723.99999999999</v>
+        <v>28137.85305076967</v>
       </c>
       <c r="S19" t="n">
         <v>0</v>
@@ -1990,10 +1990,10 @@
         <v>40</v>
       </c>
       <c r="V19" t="n">
-        <v>20</v>
+        <v>21.26598369152819</v>
       </c>
       <c r="W19" t="n">
-        <v>1248</v>
+        <v>1326.997382351359</v>
       </c>
       <c r="X19" t="n">
         <v>3</v>
@@ -2010,40 +2010,40 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>220</v>
+        <v>244.3951221456718</v>
       </c>
       <c r="C20" t="n">
-        <v>20</v>
+        <v>22.10047486127786</v>
       </c>
       <c r="D20" t="n">
         <v>40</v>
       </c>
       <c r="E20" t="n">
-        <v>230</v>
+        <v>254.4189026820898</v>
       </c>
       <c r="F20" t="n">
-        <v>30</v>
+        <v>30.04090987136011</v>
       </c>
       <c r="G20" t="n">
         <v>40</v>
       </c>
       <c r="H20" t="n">
-        <v>225</v>
+        <v>249.4070124138808</v>
       </c>
       <c r="I20" t="n">
-        <v>25</v>
+        <v>25.8533245215712</v>
       </c>
       <c r="J20" t="n">
         <v>40</v>
       </c>
       <c r="K20" t="n">
-        <v>10</v>
+        <v>10.02378053641795</v>
       </c>
       <c r="L20" t="n">
-        <v>-45</v>
+        <v>-38.32040221804986</v>
       </c>
       <c r="M20" t="n">
-        <v>14.14213562373095</v>
+        <v>12.77637964905471</v>
       </c>
       <c r="N20" t="n">
         <v>0</v>
@@ -2052,13 +2052,13 @@
         <v>0</v>
       </c>
       <c r="P20" t="n">
-        <v>15</v>
+        <v>14.1466754784288</v>
       </c>
       <c r="Q20" t="n">
         <v>0</v>
       </c>
       <c r="R20" t="n">
-        <v>19800</v>
+        <v>18718.01848167183</v>
       </c>
       <c r="S20" t="n">
         <v>0</v>
@@ -2070,10 +2070,10 @@
         <v>40</v>
       </c>
       <c r="V20" t="n">
-        <v>15</v>
+        <v>14.1466754784288</v>
       </c>
       <c r="W20" t="n">
-        <v>936</v>
+        <v>882.7525498539574</v>
       </c>
       <c r="X20" t="n">
         <v>3</v>
@@ -2090,40 +2090,40 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>230</v>
+        <v>254.4189026820898</v>
       </c>
       <c r="C21" t="n">
-        <v>30</v>
+        <v>30.04090987136011</v>
       </c>
       <c r="D21" t="n">
         <v>40</v>
       </c>
       <c r="E21" t="n">
-        <v>240</v>
+        <v>264.4426832185077</v>
       </c>
       <c r="F21" t="n">
-        <v>40</v>
+        <v>39.9999598832996</v>
       </c>
       <c r="G21" t="n">
         <v>40</v>
       </c>
       <c r="H21" t="n">
-        <v>235</v>
+        <v>259.4307929502987</v>
       </c>
       <c r="I21" t="n">
-        <v>35</v>
+        <v>34.72725405040724</v>
       </c>
       <c r="J21" t="n">
         <v>40</v>
       </c>
       <c r="K21" t="n">
-        <v>10</v>
+        <v>10.02378053641797</v>
       </c>
       <c r="L21" t="n">
-        <v>-45</v>
+        <v>-44.71574021543523</v>
       </c>
       <c r="M21" t="n">
-        <v>14.14213562373095</v>
+        <v>14.1059568222393</v>
       </c>
       <c r="N21" t="n">
         <v>0</v>
@@ -2132,13 +2132,13 @@
         <v>0</v>
       </c>
       <c r="P21" t="n">
-        <v>5</v>
+        <v>5.27274594959276</v>
       </c>
       <c r="Q21" t="n">
         <v>0</v>
       </c>
       <c r="R21" t="n">
-        <v>6600</v>
+        <v>6976.57596543661</v>
       </c>
       <c r="S21" t="n">
         <v>0</v>
@@ -2150,10 +2150,10 @@
         <v>40</v>
       </c>
       <c r="V21" t="n">
-        <v>5</v>
+        <v>5.27274594959276</v>
       </c>
       <c r="W21" t="n">
-        <v>312</v>
+        <v>329.0193472545882</v>
       </c>
       <c r="X21" t="n">
         <v>3</v>

</xml_diff>

<commit_message>
tried to get line of thrust to work. No luck.
</commit_message>
<xml_diff>
--- a/slices.xlsx
+++ b/slices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z21"/>
+  <dimension ref="A1:AB41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,80 +486,90 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>y_cg</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>dx</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>alpha</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>dl</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>h1</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>h2</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>h3</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>w_s</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>dload</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>w</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>shear_reinf</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>normal_reinf</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>piezo_y</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>hw</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>u</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>mat</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>phi</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>c</t>
         </is>
@@ -570,46 +580,46 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>60.52735684831512</v>
+        <v>62.98476960304922</v>
       </c>
       <c r="C2" t="n">
-        <v>83.99980597459211</v>
+        <v>76.95829744168995</v>
       </c>
       <c r="D2" t="n">
         <v>84</v>
       </c>
       <c r="E2" t="n">
-        <v>70.39551763623633</v>
+        <v>68.27265965975647</v>
       </c>
       <c r="F2" t="n">
-        <v>61.19606926906113</v>
+        <v>65.1431424168516</v>
       </c>
       <c r="G2" t="n">
         <v>84</v>
       </c>
       <c r="H2" t="n">
-        <v>65.46143724227572</v>
+        <v>65.62871463140284</v>
       </c>
       <c r="I2" t="n">
-        <v>70.99690551636458</v>
+        <v>70.62468291928764</v>
       </c>
       <c r="J2" t="n">
         <v>84</v>
       </c>
       <c r="K2" t="n">
-        <v>9.868160787921219</v>
+        <v>77.31234145964382</v>
       </c>
       <c r="L2" t="n">
-        <v>65.89820373474561</v>
+        <v>5.287890056707255</v>
       </c>
       <c r="M2" t="n">
-        <v>24.1654007820007</v>
+        <v>65.70335850078717</v>
       </c>
       <c r="N2" t="n">
-        <v>13.00309448363542</v>
+        <v>12.85149965970419</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>13.37531708071236</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
@@ -618,30 +628,36 @@
         <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>16681.16152365595</v>
+        <v>9194.536805532731</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>0</v>
+        <v>9194.536805532731</v>
       </c>
       <c r="U2" t="n">
-        <v>79.12718083676965</v>
+        <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>8.130275320405076</v>
+        <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>507.3291799932767</v>
+        <v>79.1249504715813</v>
       </c>
       <c r="X2" t="n">
+        <v>8.500267552293664</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>530.4166952631247</v>
+      </c>
+      <c r="Z2" t="n">
         <v>1</v>
       </c>
-      <c r="Y2" t="n">
+      <c r="AA2" t="n">
         <v>28</v>
       </c>
-      <c r="Z2" t="n">
+      <c r="AB2" t="n">
         <v>200</v>
       </c>
     </row>
@@ -650,78 +666,84 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>70.39551763623633</v>
+        <v>68.27265965975647</v>
       </c>
       <c r="C3" t="n">
-        <v>61.19606926906113</v>
+        <v>65.1431424168516</v>
       </c>
       <c r="D3" t="n">
         <v>84</v>
       </c>
       <c r="E3" t="n">
-        <v>80.26367842415756</v>
+        <v>73.56054971646373</v>
       </c>
       <c r="F3" t="n">
-        <v>46.34520128139259</v>
+        <v>55.89042250822446</v>
       </c>
       <c r="G3" t="n">
         <v>84</v>
       </c>
       <c r="H3" t="n">
-        <v>75.32959803019695</v>
+        <v>70.9166046881101</v>
       </c>
       <c r="I3" t="n">
-        <v>53.17327651921067</v>
+        <v>60.27858993335091</v>
       </c>
       <c r="J3" t="n">
         <v>84</v>
       </c>
       <c r="K3" t="n">
-        <v>9.868160787921227</v>
+        <v>72.26144581284299</v>
       </c>
       <c r="L3" t="n">
-        <v>56.15905274156578</v>
+        <v>5.287890056707255</v>
       </c>
       <c r="M3" t="n">
-        <v>17.72014640795434</v>
+        <v>60.15347758610228</v>
       </c>
       <c r="N3" t="n">
+        <v>10.62511473048265</v>
+      </c>
+      <c r="O3" t="n">
         <v>20</v>
       </c>
-      <c r="O3" t="n">
-        <v>10.82672348078933</v>
-      </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>3.721410066649085</v>
       </c>
       <c r="Q3" t="n">
         <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>38477.99982237014</v>
+        <v>16109.92302204254</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>0</v>
+        <v>16109.92302204254</v>
       </c>
       <c r="U3" t="n">
-        <v>78.97327583538943</v>
+        <v>0</v>
       </c>
       <c r="V3" t="n">
-        <v>25.79999931617876</v>
+        <v>0</v>
       </c>
       <c r="W3" t="n">
-        <v>1609.919957329554</v>
+        <v>79.0544452708252</v>
       </c>
       <c r="X3" t="n">
+        <v>18.77585533747428</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>1171.613373058395</v>
+      </c>
+      <c r="Z3" t="n">
         <v>1</v>
       </c>
-      <c r="Y3" t="n">
+      <c r="AA3" t="n">
         <v>28</v>
       </c>
-      <c r="Z3" t="n">
+      <c r="AB3" t="n">
         <v>200</v>
       </c>
     </row>
@@ -730,78 +752,84 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>80.26367842415756</v>
+        <v>73.56054971646373</v>
       </c>
       <c r="C4" t="n">
-        <v>46.34520128139259</v>
+        <v>55.89042250822446</v>
       </c>
       <c r="D4" t="n">
         <v>84</v>
       </c>
       <c r="E4" t="n">
-        <v>90.13183921207877</v>
+        <v>78.84843977317098</v>
       </c>
       <c r="F4" t="n">
-        <v>35.16253607942096</v>
+        <v>48.20252465478697</v>
       </c>
       <c r="G4" t="n">
         <v>84</v>
       </c>
       <c r="H4" t="n">
-        <v>85.19775881811816</v>
+        <v>76.20449474481735</v>
       </c>
       <c r="I4" t="n">
-        <v>40.40378477144077</v>
+        <v>51.88650543854634</v>
       </c>
       <c r="J4" t="n">
         <v>84</v>
       </c>
       <c r="K4" t="n">
-        <v>9.868160787921212</v>
+        <v>68.2420842947959</v>
       </c>
       <c r="L4" t="n">
-        <v>48.44782535860768</v>
+        <v>5.287890056707255</v>
       </c>
       <c r="M4" t="n">
-        <v>14.87733183099115</v>
+        <v>55.41609868797846</v>
       </c>
       <c r="N4" t="n">
+        <v>9.31602210806374</v>
+      </c>
+      <c r="O4" t="n">
         <v>20</v>
       </c>
-      <c r="O4" t="n">
-        <v>23.59621522855923</v>
-      </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>12.11349456145366</v>
       </c>
       <c r="Q4" t="n">
         <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>53599.36755201326</v>
+        <v>21435.09344065745</v>
       </c>
       <c r="S4" t="n">
         <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>0</v>
+        <v>21435.09344065745</v>
       </c>
       <c r="U4" t="n">
-        <v>78.17315469042285</v>
+        <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>37.76936991898208</v>
+        <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>2356.808682944481</v>
+        <v>78.90233826393373</v>
       </c>
       <c r="X4" t="n">
+        <v>27.01583282538739</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>1685.787968304173</v>
+      </c>
+      <c r="Z4" t="n">
         <v>1</v>
       </c>
-      <c r="Y4" t="n">
+      <c r="AA4" t="n">
         <v>28</v>
       </c>
-      <c r="Z4" t="n">
+      <c r="AB4" t="n">
         <v>200</v>
       </c>
     </row>
@@ -810,78 +838,84 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>90.13183921207877</v>
+        <v>78.84843977317098</v>
       </c>
       <c r="C5" t="n">
-        <v>35.16253607942096</v>
+        <v>48.20252465478697</v>
       </c>
       <c r="D5" t="n">
         <v>84</v>
       </c>
       <c r="E5" t="n">
-        <v>100</v>
+        <v>84.13632982987824</v>
       </c>
       <c r="F5" t="n">
-        <v>26.32503002402403</v>
+        <v>41.61764584286</v>
       </c>
       <c r="G5" t="n">
         <v>84</v>
       </c>
       <c r="H5" t="n">
-        <v>95.06591960603939</v>
+        <v>81.49238480152461</v>
       </c>
       <c r="I5" t="n">
-        <v>30.4983643078416</v>
+        <v>44.79145061966788</v>
       </c>
       <c r="J5" t="n">
         <v>84</v>
       </c>
       <c r="K5" t="n">
-        <v>9.868160787921227</v>
+        <v>64.78733484812248</v>
       </c>
       <c r="L5" t="n">
-        <v>41.768101924379</v>
+        <v>5.287890056707255</v>
       </c>
       <c r="M5" t="n">
-        <v>13.23081183140688</v>
+        <v>51.19014110290316</v>
       </c>
       <c r="N5" t="n">
+        <v>8.437163337199403</v>
+      </c>
+      <c r="O5" t="n">
         <v>20</v>
       </c>
-      <c r="O5" t="n">
-        <v>24</v>
-      </c>
       <c r="P5" t="n">
-        <v>9.501635692158402</v>
+        <v>19.20854938033212</v>
       </c>
       <c r="Q5" t="n">
         <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>66454.32539392641</v>
+        <v>25937.23782008228</v>
       </c>
       <c r="S5" t="n">
         <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>0</v>
+        <v>25937.23782008228</v>
       </c>
       <c r="U5" t="n">
-        <v>77.37303354545627</v>
+        <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>46.87466923761467</v>
+        <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>2924.979360427155</v>
+        <v>78.473590421498</v>
       </c>
       <c r="X5" t="n">
+        <v>33.68213980183012</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>2101.765523634199</v>
+      </c>
+      <c r="Z5" t="n">
         <v>1</v>
       </c>
-      <c r="Y5" t="n">
+      <c r="AA5" t="n">
         <v>28</v>
       </c>
-      <c r="Z5" t="n">
+      <c r="AB5" t="n">
         <v>200</v>
       </c>
     </row>
@@ -890,78 +924,84 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>100</v>
+        <v>84.13632982987824</v>
       </c>
       <c r="C6" t="n">
-        <v>26.32503002402403</v>
+        <v>41.61764584286</v>
       </c>
       <c r="D6" t="n">
         <v>84</v>
       </c>
       <c r="E6" t="n">
-        <v>110</v>
+        <v>89.42421988658549</v>
       </c>
       <c r="F6" t="n">
-        <v>19.12879499083992</v>
+        <v>35.87636563972923</v>
       </c>
       <c r="G6" t="n">
         <v>84</v>
       </c>
       <c r="H6" t="n">
-        <v>105</v>
+        <v>86.78027485823186</v>
       </c>
       <c r="I6" t="n">
-        <v>22.53205655191036</v>
+        <v>38.65333383653093</v>
       </c>
       <c r="J6" t="n">
         <v>84</v>
       </c>
       <c r="K6" t="n">
-        <v>10</v>
+        <v>61.7118276134477</v>
       </c>
       <c r="L6" t="n">
-        <v>35.68533492922602</v>
+        <v>5.287890056707255</v>
       </c>
       <c r="M6" t="n">
-        <v>12.31174025844438</v>
+        <v>47.32110797143554</v>
       </c>
       <c r="N6" t="n">
+        <v>7.800526344482068</v>
+      </c>
+      <c r="O6" t="n">
         <v>20</v>
       </c>
-      <c r="O6" t="n">
+      <c r="P6" t="n">
         <v>24</v>
       </c>
-      <c r="P6" t="n">
-        <v>17.46794344808964</v>
-      </c>
       <c r="Q6" t="n">
-        <v>25000</v>
+        <v>1.346666163469067</v>
       </c>
       <c r="R6" t="n">
-        <v>102857.6853514783</v>
+        <v>29917.61249600336</v>
       </c>
       <c r="S6" t="n">
         <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>0</v>
+        <v>29917.61249600336</v>
       </c>
       <c r="U6" t="n">
-        <v>76.56756756756756</v>
+        <v>0</v>
       </c>
       <c r="V6" t="n">
-        <v>54.03551101565721</v>
+        <v>0</v>
       </c>
       <c r="W6" t="n">
-        <v>3371.815887377009</v>
+        <v>78.04484257906228</v>
       </c>
       <c r="X6" t="n">
+        <v>39.39150874253134</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>2458.030145533956</v>
+      </c>
+      <c r="Z6" t="n">
         <v>1</v>
       </c>
-      <c r="Y6" t="n">
+      <c r="AA6" t="n">
         <v>28</v>
       </c>
-      <c r="Z6" t="n">
+      <c r="AB6" t="n">
         <v>200</v>
       </c>
     </row>
@@ -970,78 +1010,84 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>110</v>
+        <v>89.42421988658549</v>
       </c>
       <c r="C7" t="n">
-        <v>19.12879499083992</v>
+        <v>35.87636563972923</v>
       </c>
       <c r="D7" t="n">
         <v>84</v>
       </c>
       <c r="E7" t="n">
-        <v>120</v>
+        <v>94.71210994329275</v>
       </c>
       <c r="F7" t="n">
-        <v>13.3463549614923</v>
+        <v>30.81561397732175</v>
       </c>
       <c r="G7" t="n">
         <v>84</v>
       </c>
       <c r="H7" t="n">
-        <v>115</v>
+        <v>92.06816491493912</v>
       </c>
       <c r="I7" t="n">
-        <v>16.07695154586736</v>
+        <v>33.26874421856752</v>
       </c>
       <c r="J7" t="n">
         <v>84</v>
       </c>
       <c r="K7" t="n">
-        <v>10</v>
+        <v>58.83788452330973</v>
       </c>
       <c r="L7" t="n">
-        <v>30.00000015313622</v>
+        <v>5.287890056707255</v>
       </c>
       <c r="M7" t="n">
-        <v>11.54700540161072</v>
+        <v>43.71713801262754</v>
       </c>
       <c r="N7" t="n">
+        <v>7.316241474241941</v>
+      </c>
+      <c r="O7" t="n">
         <v>20</v>
       </c>
-      <c r="O7" t="n">
+      <c r="P7" t="n">
         <v>24</v>
       </c>
-      <c r="P7" t="n">
-        <v>23.92304845413264</v>
-      </c>
       <c r="Q7" t="n">
-        <v>25000</v>
+        <v>6.73125578143248</v>
       </c>
       <c r="R7" t="n">
-        <v>111378.4239594551</v>
+        <v>33676.06405884004</v>
       </c>
       <c r="S7" t="n">
         <v>0</v>
       </c>
       <c r="T7" t="n">
-        <v>0</v>
+        <v>33676.06405884004</v>
       </c>
       <c r="U7" t="n">
-        <v>75.35714285714286</v>
+        <v>0</v>
       </c>
       <c r="V7" t="n">
-        <v>59.2801913112755</v>
+        <v>0</v>
       </c>
       <c r="W7" t="n">
-        <v>3699.083937823591</v>
+        <v>77.61609473662656</v>
       </c>
       <c r="X7" t="n">
+        <v>44.34735051805905</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>2767.274672326884</v>
+      </c>
+      <c r="Z7" t="n">
         <v>1</v>
       </c>
-      <c r="Y7" t="n">
+      <c r="AA7" t="n">
         <v>28</v>
       </c>
-      <c r="Z7" t="n">
+      <c r="AB7" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1050,78 +1096,84 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>120</v>
+        <v>94.71210994329275</v>
       </c>
       <c r="C8" t="n">
-        <v>13.3463549614923</v>
+        <v>30.81561397732175</v>
       </c>
       <c r="D8" t="n">
         <v>84</v>
       </c>
       <c r="E8" t="n">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="F8" t="n">
-        <v>8.757022693565062</v>
+        <v>26.32503002402403</v>
       </c>
       <c r="G8" t="n">
         <v>84</v>
       </c>
       <c r="H8" t="n">
-        <v>125</v>
+        <v>97.35605497164637</v>
       </c>
       <c r="I8" t="n">
-        <v>10.91287885364285</v>
+        <v>28.5045476516237</v>
       </c>
       <c r="J8" t="n">
         <v>84</v>
       </c>
       <c r="K8" t="n">
-        <v>10</v>
+        <v>56.32583626846203</v>
       </c>
       <c r="L8" t="n">
-        <v>24.62431846252714</v>
+        <v>5.287890056707255</v>
       </c>
       <c r="M8" t="n">
-        <v>11.00038197405046</v>
+        <v>40.31826542849554</v>
       </c>
       <c r="N8" t="n">
+        <v>6.935282500358218</v>
+      </c>
+      <c r="O8" t="n">
         <v>20</v>
       </c>
-      <c r="O8" t="n">
+      <c r="P8" t="n">
         <v>24</v>
       </c>
-      <c r="P8" t="n">
-        <v>29.08712114635715</v>
-      </c>
       <c r="Q8" t="n">
-        <v>25000</v>
+        <v>11.4954523483763</v>
       </c>
       <c r="R8" t="n">
-        <v>118194.9999131914</v>
+        <v>37001.48034923946</v>
       </c>
       <c r="S8" t="n">
         <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>0</v>
+        <v>37001.48034923946</v>
       </c>
       <c r="U8" t="n">
-        <v>73.21428571428571</v>
+        <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>62.30140686064286</v>
+        <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>3887.607788104114</v>
+        <v>77.18734689419084</v>
       </c>
       <c r="X8" t="n">
+        <v>48.68279924256714</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>3037.80667273619</v>
+      </c>
+      <c r="Z8" t="n">
         <v>1</v>
       </c>
-      <c r="Y8" t="n">
+      <c r="AA8" t="n">
         <v>28</v>
       </c>
-      <c r="Z8" t="n">
+      <c r="AB8" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1130,78 +1182,84 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="C9" t="n">
-        <v>8.757022693565062</v>
+        <v>26.32503002402403</v>
       </c>
       <c r="D9" t="n">
         <v>84</v>
       </c>
       <c r="E9" t="n">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="F9" t="n">
-        <v>5.217597167510036</v>
+        <v>22.53205655191036</v>
       </c>
       <c r="G9" t="n">
         <v>84</v>
       </c>
       <c r="H9" t="n">
-        <v>135</v>
+        <v>102.5</v>
       </c>
       <c r="I9" t="n">
-        <v>6.862915010152392</v>
+        <v>24.37704250547361</v>
       </c>
       <c r="J9" t="n">
         <v>84</v>
       </c>
       <c r="K9" t="n">
-        <v>10</v>
+        <v>54.16702031458821</v>
       </c>
       <c r="L9" t="n">
-        <v>19.47122071361051</v>
+        <v>5</v>
       </c>
       <c r="M9" t="n">
-        <v>10.60660172297659</v>
+        <v>37.16889989353835</v>
       </c>
       <c r="N9" t="n">
+        <v>6.274643847115209</v>
+      </c>
+      <c r="O9" t="n">
         <v>20</v>
       </c>
-      <c r="O9" t="n">
+      <c r="P9" t="n">
         <v>24</v>
       </c>
-      <c r="P9" t="n">
-        <v>33.13708498984761</v>
-      </c>
       <c r="Q9" t="n">
-        <v>25000</v>
+        <v>15.62295749452639</v>
       </c>
       <c r="R9" t="n">
-        <v>123540.9521865988</v>
+        <v>37711.15194638741</v>
       </c>
       <c r="S9" t="n">
-        <v>0</v>
+        <v>12500</v>
       </c>
       <c r="T9" t="n">
-        <v>0</v>
+        <v>50211.15194638741</v>
       </c>
       <c r="U9" t="n">
-        <v>71.07142857142857</v>
+        <v>0</v>
       </c>
       <c r="V9" t="n">
-        <v>64.20851356127618</v>
+        <v>0</v>
       </c>
       <c r="W9" t="n">
-        <v>4006.611246223633</v>
+        <v>76.77027027027027</v>
       </c>
       <c r="X9" t="n">
+        <v>52.39322776479666</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>3269.337412523312</v>
+      </c>
+      <c r="Z9" t="n">
         <v>1</v>
       </c>
-      <c r="Y9" t="n">
+      <c r="AA9" t="n">
         <v>28</v>
       </c>
-      <c r="Z9" t="n">
+      <c r="AB9" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1210,78 +1268,84 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="C10" t="n">
-        <v>5.217597167510036</v>
+        <v>22.53205655191036</v>
       </c>
       <c r="D10" t="n">
         <v>84</v>
       </c>
       <c r="E10" t="n">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="F10" t="n">
-        <v>2.633054056944971</v>
+        <v>19.12879499083992</v>
       </c>
       <c r="G10" t="n">
         <v>84</v>
       </c>
       <c r="H10" t="n">
-        <v>145</v>
+        <v>107.5</v>
       </c>
       <c r="I10" t="n">
-        <v>3.810499613777495</v>
+        <v>20.78432583507785</v>
       </c>
       <c r="J10" t="n">
         <v>84</v>
       </c>
       <c r="K10" t="n">
-        <v>10</v>
+        <v>52.29843454860167</v>
       </c>
       <c r="L10" t="n">
-        <v>14.47751224073088</v>
+        <v>5</v>
       </c>
       <c r="M10" t="n">
-        <v>10.327955592437</v>
+        <v>34.22886652579309</v>
       </c>
       <c r="N10" t="n">
+        <v>6.047431582364187</v>
+      </c>
+      <c r="O10" t="n">
         <v>20</v>
       </c>
-      <c r="O10" t="n">
+      <c r="P10" t="n">
         <v>24</v>
       </c>
-      <c r="P10" t="n">
-        <v>36.18950038622251</v>
-      </c>
       <c r="Q10" t="n">
-        <v>25000</v>
+        <v>19.21567416492215</v>
       </c>
       <c r="R10" t="n">
-        <v>127570.1405098137</v>
+        <v>40082.34494884862</v>
       </c>
       <c r="S10" t="n">
-        <v>0</v>
+        <v>12500</v>
       </c>
       <c r="T10" t="n">
-        <v>0</v>
+        <v>52582.34494884862</v>
       </c>
       <c r="U10" t="n">
-        <v>68.5</v>
+        <v>0</v>
       </c>
       <c r="V10" t="n">
-        <v>64.68950038622251</v>
+        <v>0</v>
       </c>
       <c r="W10" t="n">
-        <v>4036.624824100284</v>
+        <v>76.36486486486487</v>
       </c>
       <c r="X10" t="n">
+        <v>55.58053902978702</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>3468.22563545871</v>
+      </c>
+      <c r="Z10" t="n">
         <v>1</v>
       </c>
-      <c r="Y10" t="n">
+      <c r="AA10" t="n">
         <v>28</v>
       </c>
-      <c r="Z10" t="n">
+      <c r="AB10" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1290,78 +1354,84 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="C11" t="n">
-        <v>2.633054056944971</v>
+        <v>19.12879499083992</v>
       </c>
       <c r="D11" t="n">
         <v>84</v>
       </c>
       <c r="E11" t="n">
-        <v>162.35</v>
+        <v>115</v>
       </c>
       <c r="F11" t="n">
-        <v>0.6686231538410539</v>
+        <v>16.07695154586736</v>
       </c>
       <c r="G11" t="n">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="H11" t="n">
-        <v>156.175</v>
+        <v>112.5</v>
       </c>
       <c r="I11" t="n">
-        <v>1.485784080558503</v>
+        <v>17.5609937572606</v>
       </c>
       <c r="J11" t="n">
-        <v>78.99999999999999</v>
+        <v>84</v>
       </c>
       <c r="K11" t="n">
-        <v>12.34999999999999</v>
+        <v>50.62887347383496</v>
       </c>
       <c r="L11" t="n">
-        <v>9.025556359556186</v>
+        <v>5</v>
       </c>
       <c r="M11" t="n">
-        <v>12.50482896617596</v>
+        <v>31.38816663089308</v>
       </c>
       <c r="N11" t="n">
-        <v>14.99999999999999</v>
+        <v>5.857143905147995</v>
       </c>
       <c r="O11" t="n">
+        <v>20</v>
+      </c>
+      <c r="P11" t="n">
         <v>24</v>
       </c>
-      <c r="P11" t="n">
-        <v>38.5142159194415</v>
-      </c>
       <c r="Q11" t="n">
-        <v>0</v>
+        <v>22.4390062427394</v>
       </c>
       <c r="R11" t="n">
-        <v>122436.3747918735</v>
+        <v>42209.744120208</v>
       </c>
       <c r="S11" t="n">
-        <v>0</v>
+        <v>12500</v>
       </c>
       <c r="T11" t="n">
-        <v>0</v>
+        <v>54709.744120208</v>
       </c>
       <c r="U11" t="n">
-        <v>65.14749999999999</v>
+        <v>0</v>
       </c>
       <c r="V11" t="n">
-        <v>63.66171591944149</v>
+        <v>0</v>
       </c>
       <c r="W11" t="n">
-        <v>3972.491073373149</v>
+        <v>75.89285714285714</v>
       </c>
       <c r="X11" t="n">
+        <v>58.33186338559653</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>3639.908275261223</v>
+      </c>
+      <c r="Z11" t="n">
         <v>1</v>
       </c>
-      <c r="Y11" t="n">
+      <c r="AA11" t="n">
         <v>28</v>
       </c>
-      <c r="Z11" t="n">
+      <c r="AB11" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1370,78 +1440,84 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>162.35</v>
+        <v>115</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6686231538410539</v>
+        <v>16.07695154586736</v>
       </c>
       <c r="D12" t="n">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="E12" t="n">
-        <v>174.7</v>
+        <v>120</v>
       </c>
       <c r="F12" t="n">
-        <v>0.000375000585933094</v>
+        <v>13.3463549614923</v>
       </c>
       <c r="G12" t="n">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="H12" t="n">
-        <v>168.525</v>
+        <v>117.5</v>
       </c>
       <c r="I12" t="n">
-        <v>0.17481744224213</v>
+        <v>14.67312783529552</v>
       </c>
       <c r="J12" t="n">
-        <v>69.00000000000001</v>
+        <v>84</v>
       </c>
       <c r="K12" t="n">
-        <v>12.34999999999999</v>
+        <v>49.1378131759883</v>
       </c>
       <c r="L12" t="n">
-        <v>3.093086941691099</v>
+        <v>5</v>
       </c>
       <c r="M12" t="n">
-        <v>12.3680178772166</v>
+        <v>28.63098997790105</v>
       </c>
       <c r="N12" t="n">
-        <v>5.000000000000014</v>
+        <v>5.696551966982327</v>
       </c>
       <c r="O12" t="n">
+        <v>20</v>
+      </c>
+      <c r="P12" t="n">
         <v>24</v>
       </c>
-      <c r="P12" t="n">
-        <v>39.82518255775787</v>
-      </c>
       <c r="Q12" t="n">
-        <v>0</v>
+        <v>25.32687216470448</v>
       </c>
       <c r="R12" t="n">
-        <v>108518.5126056569</v>
+        <v>44115.73562870496</v>
       </c>
       <c r="S12" t="n">
-        <v>0</v>
+        <v>12500</v>
       </c>
       <c r="T12" t="n">
-        <v>0</v>
+        <v>56615.73562870496</v>
       </c>
       <c r="U12" t="n">
-        <v>61.44250000000001</v>
+        <v>0</v>
       </c>
       <c r="V12" t="n">
-        <v>61.26768255775788</v>
+        <v>0</v>
       </c>
       <c r="W12" t="n">
-        <v>3823.103391604091</v>
+        <v>74.82142857142857</v>
       </c>
       <c r="X12" t="n">
+        <v>60.14830073613305</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>3753.253965934703</v>
+      </c>
+      <c r="Z12" t="n">
         <v>1</v>
       </c>
-      <c r="Y12" t="n">
+      <c r="AA12" t="n">
         <v>28</v>
       </c>
-      <c r="Z12" t="n">
+      <c r="AB12" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1450,79 +1526,85 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>174.7</v>
+        <v>120</v>
       </c>
       <c r="C13" t="n">
-        <v>0.000375000585933094</v>
+        <v>13.3463549614923</v>
       </c>
       <c r="D13" t="n">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="E13" t="n">
-        <v>184.5666666666667</v>
+        <v>125</v>
       </c>
       <c r="F13" t="n">
-        <v>0.3819458071278916</v>
+        <v>10.91287885364285</v>
       </c>
       <c r="G13" t="n">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="H13" t="n">
-        <v>179.6333333333333</v>
+        <v>122.5</v>
       </c>
       <c r="I13" t="n">
-        <v>0.08948243701796343</v>
+        <v>12.0937907254638</v>
       </c>
       <c r="J13" t="n">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="K13" t="n">
-        <v>9.866666666666674</v>
+        <v>47.80936713586546</v>
       </c>
       <c r="L13" t="n">
-        <v>-2.212803763689251</v>
+        <v>5</v>
       </c>
       <c r="M13" t="n">
-        <v>9.874029601984471</v>
+        <v>25.94447989206976</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>5.560384380507148</v>
       </c>
       <c r="O13" t="n">
         <v>20</v>
       </c>
       <c r="P13" t="n">
-        <v>39.91051756298204</v>
+        <v>24</v>
       </c>
       <c r="Q13" t="n">
-        <v>0</v>
+        <v>27.9062092745362</v>
       </c>
       <c r="R13" t="n">
-        <v>75659.45807402786</v>
+        <v>45818.09812119389</v>
       </c>
       <c r="S13" t="n">
-        <v>0</v>
+        <v>12500</v>
       </c>
       <c r="T13" t="n">
-        <v>0</v>
+        <v>58318.09812119389</v>
       </c>
       <c r="U13" t="n">
-        <v>56.55384615384616</v>
+        <v>0</v>
       </c>
       <c r="V13" t="n">
-        <v>56.4643637168282</v>
+        <v>0</v>
       </c>
       <c r="W13" t="n">
-        <v>3523.376295930079</v>
+        <v>73.75</v>
       </c>
       <c r="X13" t="n">
-        <v>2</v>
+        <v>61.6562092745362</v>
       </c>
       <c r="Y13" t="n">
-        <v>32</v>
+        <v>3847.347458731058</v>
       </c>
       <c r="Z13" t="n">
-        <v>100</v>
+        <v>1</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="14">
@@ -1530,79 +1612,85 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>184.5666666666667</v>
+        <v>125</v>
       </c>
       <c r="C14" t="n">
-        <v>0.3819458071278916</v>
+        <v>10.91287885364285</v>
       </c>
       <c r="D14" t="n">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="E14" t="n">
-        <v>194.4333333333333</v>
+        <v>130</v>
       </c>
       <c r="F14" t="n">
-        <v>1.58401478028587</v>
+        <v>8.757022693565062</v>
       </c>
       <c r="G14" t="n">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="H14" t="n">
-        <v>189.5</v>
+        <v>127.5</v>
       </c>
       <c r="I14" t="n">
-        <v>0.8792629304200403</v>
+        <v>9.801315797329053</v>
       </c>
       <c r="J14" t="n">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="K14" t="n">
-        <v>9.866666666666674</v>
+        <v>46.63100617850018</v>
       </c>
       <c r="L14" t="n">
-        <v>-6.940199065150054</v>
+        <v>5</v>
       </c>
       <c r="M14" t="n">
-        <v>9.939495248171937</v>
+        <v>23.31795716700442</v>
       </c>
       <c r="N14" t="n">
-        <v>0</v>
+        <v>5.444711112479689</v>
       </c>
       <c r="O14" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="P14" t="n">
-        <v>39.12073706957996</v>
+        <v>24</v>
       </c>
       <c r="Q14" t="n">
-        <v>0</v>
+        <v>30.19868420267095</v>
       </c>
       <c r="R14" t="n">
-        <v>65158.84795942099</v>
+        <v>47331.13157376282</v>
       </c>
       <c r="S14" t="n">
-        <v>0</v>
+        <v>12500</v>
       </c>
       <c r="T14" t="n">
-        <v>0</v>
+        <v>59831.13157376282</v>
       </c>
       <c r="U14" t="n">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="V14" t="n">
-        <v>51.12073706957996</v>
+        <v>0</v>
       </c>
       <c r="W14" t="n">
-        <v>3189.933993141789</v>
+        <v>72.67857142857143</v>
       </c>
       <c r="X14" t="n">
-        <v>2</v>
+        <v>62.87725563124238</v>
       </c>
       <c r="Y14" t="n">
-        <v>32</v>
+        <v>3923.540751389524</v>
       </c>
       <c r="Z14" t="n">
-        <v>100</v>
+        <v>1</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="15">
@@ -1610,79 +1698,85 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>194.4333333333333</v>
+        <v>130</v>
       </c>
       <c r="C15" t="n">
-        <v>1.58401478028587</v>
+        <v>8.757022693565062</v>
       </c>
       <c r="D15" t="n">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="E15" t="n">
-        <v>204.3</v>
+        <v>135</v>
       </c>
       <c r="F15" t="n">
-        <v>3.632006118520721</v>
+        <v>6.862915010152392</v>
       </c>
       <c r="G15" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="H15" t="n">
-        <v>199.3666666666667</v>
+        <v>132.5</v>
       </c>
       <c r="I15" t="n">
-        <v>2.499933806165217</v>
+        <v>7.778121562682799</v>
       </c>
       <c r="J15" t="n">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="K15" t="n">
-        <v>9.866666666666674</v>
+        <v>45.59271816028333</v>
       </c>
       <c r="L15" t="n">
-        <v>-11.71569679077994</v>
+        <v>5</v>
       </c>
       <c r="M15" t="n">
-        <v>10.07659006958593</v>
+        <v>20.74238004065533</v>
       </c>
       <c r="N15" t="n">
-        <v>0</v>
+        <v>5.346551035294511</v>
       </c>
       <c r="O15" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="P15" t="n">
-        <v>37.50006619383478</v>
+        <v>24</v>
       </c>
       <c r="Q15" t="n">
-        <v>0</v>
+        <v>32.2218784373172</v>
       </c>
       <c r="R15" t="n">
-        <v>53576.08621085047</v>
+        <v>48666.43976862935</v>
       </c>
       <c r="S15" t="n">
-        <v>0</v>
+        <v>12500</v>
       </c>
       <c r="T15" t="n">
-        <v>0</v>
+        <v>61166.43976862935</v>
       </c>
       <c r="U15" t="n">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="V15" t="n">
-        <v>41.50006619383478</v>
+        <v>0</v>
       </c>
       <c r="W15" t="n">
-        <v>2589.604130495291</v>
+        <v>71.60714285714286</v>
       </c>
       <c r="X15" t="n">
-        <v>2</v>
+        <v>63.82902129446006</v>
       </c>
       <c r="Y15" t="n">
-        <v>32</v>
+        <v>3982.930928774308</v>
       </c>
       <c r="Z15" t="n">
-        <v>100</v>
+        <v>1</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="16">
@@ -1690,79 +1784,85 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>204.3</v>
+        <v>135</v>
       </c>
       <c r="C16" t="n">
-        <v>3.632006118520721</v>
+        <v>6.862915010152392</v>
       </c>
       <c r="D16" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="E16" t="n">
-        <v>214.323780536418</v>
+        <v>140</v>
       </c>
       <c r="F16" t="n">
-        <v>6.626104043639586</v>
+        <v>5.217597167510036</v>
       </c>
       <c r="G16" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="H16" t="n">
-        <v>209.311890268209</v>
+        <v>137.5</v>
       </c>
       <c r="I16" t="n">
-        <v>5.010025714315489</v>
+        <v>6.009868848220023</v>
       </c>
       <c r="J16" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="K16" t="n">
-        <v>10.02378053641795</v>
+        <v>44.68643558648014</v>
       </c>
       <c r="L16" t="n">
-        <v>-16.61459186508567</v>
+        <v>5</v>
       </c>
       <c r="M16" t="n">
-        <v>10.46050903348247</v>
+        <v>18.2099569368199</v>
       </c>
       <c r="N16" t="n">
-        <v>0</v>
+        <v>5.263613561870373</v>
       </c>
       <c r="O16" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="P16" t="n">
-        <v>34.98997428568451</v>
+        <v>24</v>
       </c>
       <c r="Q16" t="n">
-        <v>0</v>
+        <v>33.99013115177998</v>
       </c>
       <c r="R16" t="n">
-        <v>46296.60066432835</v>
+        <v>49833.48656017479</v>
       </c>
       <c r="S16" t="n">
-        <v>0</v>
+        <v>12500</v>
       </c>
       <c r="T16" t="n">
-        <v>0</v>
+        <v>62333.48656017479</v>
       </c>
       <c r="U16" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="V16" t="n">
-        <v>34.98997428568451</v>
+        <v>0</v>
       </c>
       <c r="W16" t="n">
-        <v>2183.374395426713</v>
+        <v>70.53571428571429</v>
       </c>
       <c r="X16" t="n">
-        <v>3</v>
+        <v>64.52584543749427</v>
       </c>
       <c r="Y16" t="n">
-        <v>27</v>
+        <v>4026.412755299642</v>
       </c>
       <c r="Z16" t="n">
-        <v>400</v>
+        <v>1</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="17">
@@ -1770,79 +1870,85 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>214.323780536418</v>
+        <v>140</v>
       </c>
       <c r="C17" t="n">
-        <v>6.626104043639586</v>
+        <v>5.217597167510036</v>
       </c>
       <c r="D17" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="E17" t="n">
-        <v>224.3475610728359</v>
+        <v>145</v>
       </c>
       <c r="F17" t="n">
-        <v>10.61618850962118</v>
+        <v>3.810499613777495</v>
       </c>
       <c r="G17" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="H17" t="n">
-        <v>219.3356708046269</v>
+        <v>142.5</v>
       </c>
       <c r="I17" t="n">
-        <v>8.49059100549519</v>
+        <v>4.484849478520786</v>
       </c>
       <c r="J17" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="K17" t="n">
-        <v>10.02378053641797</v>
+        <v>43.90563434491562</v>
       </c>
       <c r="L17" t="n">
-        <v>-21.68255994558514</v>
+        <v>5</v>
       </c>
       <c r="M17" t="n">
-        <v>10.7870149791044</v>
+        <v>15.71386110841711</v>
       </c>
       <c r="N17" t="n">
-        <v>0</v>
+        <v>5.194123865738421</v>
       </c>
       <c r="O17" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="P17" t="n">
-        <v>31.50940899450481</v>
+        <v>24</v>
       </c>
       <c r="Q17" t="n">
-        <v>0</v>
+        <v>35.51515052147921</v>
       </c>
       <c r="R17" t="n">
-        <v>41691.3288782959</v>
+        <v>50839.99934417628</v>
       </c>
       <c r="S17" t="n">
-        <v>0</v>
+        <v>12500</v>
       </c>
       <c r="T17" t="n">
-        <v>0</v>
+        <v>63339.99934417628</v>
       </c>
       <c r="U17" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="V17" t="n">
-        <v>31.50940899450481</v>
+        <v>0</v>
       </c>
       <c r="W17" t="n">
-        <v>1966.1871212571</v>
+        <v>69.25</v>
       </c>
       <c r="X17" t="n">
-        <v>3</v>
+        <v>64.76515052147921</v>
       </c>
       <c r="Y17" t="n">
-        <v>27</v>
+        <v>4041.345392540303</v>
       </c>
       <c r="Z17" t="n">
-        <v>400</v>
+        <v>1</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="18">
@@ -1850,79 +1956,85 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>224.3475610728359</v>
+        <v>145</v>
       </c>
       <c r="C18" t="n">
-        <v>10.61618850962118</v>
+        <v>3.810499613777495</v>
       </c>
       <c r="D18" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="E18" t="n">
-        <v>234.3713416092539</v>
+        <v>150</v>
       </c>
       <c r="F18" t="n">
-        <v>15.71652194370731</v>
+        <v>2.633054056944971</v>
       </c>
       <c r="G18" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="H18" t="n">
-        <v>229.3594513410449</v>
+        <v>147.5</v>
       </c>
       <c r="I18" t="n">
-        <v>13.0184593030154</v>
+        <v>3.193536137763331</v>
       </c>
       <c r="J18" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="K18" t="n">
-        <v>10.02378053641795</v>
+        <v>43.24504620173425</v>
       </c>
       <c r="L18" t="n">
-        <v>-26.93603065199318</v>
+        <v>5</v>
       </c>
       <c r="M18" t="n">
-        <v>11.24356274821377</v>
+        <v>13.24801495512669</v>
       </c>
       <c r="N18" t="n">
-        <v>0</v>
+        <v>5.136702030716079</v>
       </c>
       <c r="O18" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="P18" t="n">
-        <v>26.9815406969846</v>
+        <v>24</v>
       </c>
       <c r="Q18" t="n">
-        <v>0</v>
+        <v>36.80646386223667</v>
       </c>
       <c r="R18" t="n">
-        <v>35700.32960749238</v>
+        <v>51692.2661490762</v>
       </c>
       <c r="S18" t="n">
-        <v>0</v>
+        <v>12500</v>
       </c>
       <c r="T18" t="n">
-        <v>0</v>
+        <v>64192.2661490762</v>
       </c>
       <c r="U18" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="V18" t="n">
-        <v>26.9815406969846</v>
+        <v>0</v>
       </c>
       <c r="W18" t="n">
-        <v>1683.648139491839</v>
+        <v>67.75</v>
       </c>
       <c r="X18" t="n">
-        <v>3</v>
+        <v>64.55646386223667</v>
       </c>
       <c r="Y18" t="n">
-        <v>27</v>
+        <v>4028.323345003568</v>
       </c>
       <c r="Z18" t="n">
-        <v>400</v>
+        <v>1</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="19">
@@ -1930,79 +2042,85 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>234.3713416092539</v>
+        <v>150</v>
       </c>
       <c r="C19" t="n">
-        <v>15.71652194370731</v>
+        <v>2.633054056944971</v>
       </c>
       <c r="D19" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="E19" t="n">
-        <v>244.3951221456718</v>
+        <v>154.94</v>
       </c>
       <c r="F19" t="n">
-        <v>22.10047486127786</v>
+        <v>1.688561837834129</v>
       </c>
       <c r="G19" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="H19" t="n">
-        <v>239.3832318774628</v>
+        <v>152.47</v>
       </c>
       <c r="I19" t="n">
-        <v>18.73401630847181</v>
+        <v>2.133978178611628</v>
       </c>
       <c r="J19" t="n">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="K19" t="n">
-        <v>10.02378053641795</v>
+        <v>41.67805064088522</v>
       </c>
       <c r="L19" t="n">
-        <v>-32.44752375024643</v>
+        <v>4.939999999999998</v>
       </c>
       <c r="M19" t="n">
-        <v>11.87816108521438</v>
+        <v>10.82150584127103</v>
       </c>
       <c r="N19" t="n">
-        <v>0</v>
+        <v>5.029439281290534</v>
       </c>
       <c r="O19" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="P19" t="n">
-        <v>21.26598369152819</v>
+        <v>24</v>
       </c>
       <c r="Q19" t="n">
-        <v>0</v>
+        <v>37.86602182138837</v>
       </c>
       <c r="R19" t="n">
-        <v>28137.85305076967</v>
+        <v>50478.4755092909</v>
       </c>
       <c r="S19" t="n">
         <v>0</v>
       </c>
       <c r="T19" t="n">
-        <v>0</v>
+        <v>50478.4755092909</v>
       </c>
       <c r="U19" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="V19" t="n">
-        <v>21.26598369152819</v>
+        <v>0</v>
       </c>
       <c r="W19" t="n">
-        <v>1326.997382351359</v>
+        <v>66.259</v>
       </c>
       <c r="X19" t="n">
-        <v>3</v>
+        <v>64.12502182138837</v>
       </c>
       <c r="Y19" t="n">
-        <v>27</v>
+        <v>4001.401361654634</v>
       </c>
       <c r="Z19" t="n">
-        <v>400</v>
+        <v>1</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="20">
@@ -2010,79 +2128,85 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>244.3951221456718</v>
+        <v>154.94</v>
       </c>
       <c r="C20" t="n">
-        <v>22.10047486127786</v>
+        <v>1.688561837834129</v>
       </c>
       <c r="D20" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E20" t="n">
-        <v>254.4189026820898</v>
+        <v>159.88</v>
       </c>
       <c r="F20" t="n">
-        <v>30.04090987136011</v>
+        <v>0.9563710230572724</v>
       </c>
       <c r="G20" t="n">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="H20" t="n">
-        <v>249.4070124138808</v>
+        <v>157.41</v>
       </c>
       <c r="I20" t="n">
-        <v>25.8533245215712</v>
+        <v>1.296200987499986</v>
       </c>
       <c r="J20" t="n">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="K20" t="n">
-        <v>10.02378053641795</v>
+        <v>39.19593974387418</v>
       </c>
       <c r="L20" t="n">
-        <v>-38.32040221804986</v>
+        <v>4.939999999999998</v>
       </c>
       <c r="M20" t="n">
-        <v>12.77637964905471</v>
+        <v>8.428977312275139</v>
       </c>
       <c r="N20" t="n">
-        <v>0</v>
+        <v>4.993942948563728</v>
       </c>
       <c r="O20" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="P20" t="n">
-        <v>14.1466754784288</v>
+        <v>24</v>
       </c>
       <c r="Q20" t="n">
-        <v>0</v>
+        <v>38.70379901250001</v>
       </c>
       <c r="R20" t="n">
-        <v>18718.01848167183</v>
+        <v>48455.97326007098</v>
       </c>
       <c r="S20" t="n">
         <v>0</v>
       </c>
       <c r="T20" t="n">
-        <v>0</v>
+        <v>48455.97326007098</v>
       </c>
       <c r="U20" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="V20" t="n">
-        <v>14.1466754784288</v>
+        <v>0</v>
       </c>
       <c r="W20" t="n">
-        <v>882.7525498539574</v>
+        <v>64.777</v>
       </c>
       <c r="X20" t="n">
-        <v>3</v>
+        <v>63.48079901250001</v>
       </c>
       <c r="Y20" t="n">
-        <v>27</v>
+        <v>3961.201858380001</v>
       </c>
       <c r="Z20" t="n">
-        <v>400</v>
+        <v>1</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="21">
@@ -2090,78 +2214,1804 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>254.4189026820898</v>
+        <v>159.88</v>
       </c>
       <c r="C21" t="n">
-        <v>30.04090987136011</v>
+        <v>0.9563710230572724</v>
       </c>
       <c r="D21" t="n">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="E21" t="n">
-        <v>264.4426832185077</v>
+        <v>164.82</v>
       </c>
       <c r="F21" t="n">
-        <v>39.9999598832996</v>
+        <v>0.4325813609744245</v>
       </c>
       <c r="G21" t="n">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="H21" t="n">
-        <v>259.4307929502987</v>
+        <v>162.35</v>
       </c>
       <c r="I21" t="n">
-        <v>34.72725405040724</v>
+        <v>0.6686231538410539</v>
       </c>
       <c r="J21" t="n">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="K21" t="n">
-        <v>10.02378053641797</v>
+        <v>36.81604803881384</v>
       </c>
       <c r="L21" t="n">
-        <v>-44.71574021543523</v>
+        <v>4.939999999999998</v>
       </c>
       <c r="M21" t="n">
-        <v>14.1059568222393</v>
+        <v>6.051173054154476</v>
       </c>
       <c r="N21" t="n">
-        <v>0</v>
+        <v>4.967679211374814</v>
       </c>
       <c r="O21" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P21" t="n">
-        <v>5.27274594959276</v>
+        <v>24</v>
       </c>
       <c r="Q21" t="n">
-        <v>0</v>
+        <v>39.33137684615895</v>
       </c>
       <c r="R21" t="n">
-        <v>6976.57596543661</v>
+        <v>46296.4042138433</v>
       </c>
       <c r="S21" t="n">
         <v>0</v>
       </c>
       <c r="T21" t="n">
-        <v>0</v>
+        <v>46296.4042138433</v>
       </c>
       <c r="U21" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="V21" t="n">
-        <v>5.27274594959276</v>
+        <v>0</v>
       </c>
       <c r="W21" t="n">
-        <v>329.0193472545882</v>
+        <v>63.295</v>
       </c>
       <c r="X21" t="n">
+        <v>62.62637684615895</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>3907.885915200318</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>164.82</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.4325813609744245</v>
+      </c>
+      <c r="D22" t="n">
+        <v>72</v>
+      </c>
+      <c r="E22" t="n">
+        <v>169.76</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.1144612557461073</v>
+      </c>
+      <c r="G22" t="n">
+        <v>68</v>
+      </c>
+      <c r="H22" t="n">
+        <v>167.29</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.2479398924594705</v>
+      </c>
+      <c r="J22" t="n">
+        <v>70</v>
+      </c>
+      <c r="K22" t="n">
+        <v>34.53537120860686</v>
+      </c>
+      <c r="L22" t="n">
+        <v>4.939999999999998</v>
+      </c>
+      <c r="M22" t="n">
+        <v>3.683791304041865</v>
+      </c>
+      <c r="N22" t="n">
+        <v>4.950227991703982</v>
+      </c>
+      <c r="O22" t="n">
+        <v>6</v>
+      </c>
+      <c r="P22" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>39.75206010754053</v>
+      </c>
+      <c r="R22" t="n">
+        <v>44001.92335492501</v>
+      </c>
+      <c r="S22" t="n">
+        <v>0</v>
+      </c>
+      <c r="T22" t="n">
+        <v>44001.92335492501</v>
+      </c>
+      <c r="U22" t="n">
+        <v>0</v>
+      </c>
+      <c r="V22" t="n">
+        <v>0</v>
+      </c>
+      <c r="W22" t="n">
+        <v>61.813</v>
+      </c>
+      <c r="X22" t="n">
+        <v>61.56506010754053</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>3841.659750710529</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>169.76</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.1144612557461073</v>
+      </c>
+      <c r="D23" t="n">
+        <v>68</v>
+      </c>
+      <c r="E23" t="n">
+        <v>174.7</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.000375000585933094</v>
+      </c>
+      <c r="G23" t="n">
+        <v>64</v>
+      </c>
+      <c r="H23" t="n">
+        <v>172.23</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.03197467658308994</v>
+      </c>
+      <c r="J23" t="n">
+        <v>66</v>
+      </c>
+      <c r="K23" t="n">
+        <v>32.35112536064496</v>
+      </c>
+      <c r="L23" t="n">
+        <v>4.939999999999998</v>
+      </c>
+      <c r="M23" t="n">
+        <v>1.322695063640637</v>
+      </c>
+      <c r="N23" t="n">
+        <v>4.941316641688443</v>
+      </c>
+      <c r="O23" t="n">
+        <v>2</v>
+      </c>
+      <c r="P23" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>39.96802532341691</v>
+      </c>
+      <c r="R23" t="n">
+        <v>41573.94995289368</v>
+      </c>
+      <c r="S23" t="n">
+        <v>0</v>
+      </c>
+      <c r="T23" t="n">
+        <v>41573.94995289368</v>
+      </c>
+      <c r="U23" t="n">
+        <v>0</v>
+      </c>
+      <c r="V23" t="n">
+        <v>0</v>
+      </c>
+      <c r="W23" t="n">
+        <v>59.97076923076924</v>
+      </c>
+      <c r="X23" t="n">
+        <v>59.93879455418615</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>3740.180780181216</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB23" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
+        <v>174.7</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.000375000585933094</v>
+      </c>
+      <c r="D24" t="n">
+        <v>64</v>
+      </c>
+      <c r="E24" t="n">
+        <v>179.6333333333333</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.08948243701796343</v>
+      </c>
+      <c r="G24" t="n">
+        <v>60</v>
+      </c>
+      <c r="H24" t="n">
+        <v>177.1666666666667</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.01956177961527317</v>
+      </c>
+      <c r="J24" t="n">
+        <v>62</v>
+      </c>
+      <c r="K24" t="n">
+        <v>30.34322293513772</v>
+      </c>
+      <c r="L24" t="n">
+        <v>4.933333333333337</v>
+      </c>
+      <c r="M24" t="n">
+        <v>-1.03456335067261</v>
+      </c>
+      <c r="N24" t="n">
+        <v>4.934137670953151</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>39.98043822038473</v>
+      </c>
+      <c r="R24" t="n">
+        <v>39059.26136911457</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T24" t="n">
+        <v>39059.26136911457</v>
+      </c>
+      <c r="U24" t="n">
+        <v>0</v>
+      </c>
+      <c r="V24" t="n">
+        <v>0</v>
+      </c>
+      <c r="W24" t="n">
+        <v>57.69230769230769</v>
+      </c>
+      <c r="X24" t="n">
+        <v>57.67274591269242</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>3598.779344952007</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>179.6333333333333</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.08948243701796343</v>
+      </c>
+      <c r="D25" t="n">
+        <v>60</v>
+      </c>
+      <c r="E25" t="n">
+        <v>184.5666666666667</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.3819458071278916</v>
+      </c>
+      <c r="G25" t="n">
+        <v>56</v>
+      </c>
+      <c r="H25" t="n">
+        <v>182.1</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.2102258120502114</v>
+      </c>
+      <c r="J25" t="n">
+        <v>58</v>
+      </c>
+      <c r="K25" t="n">
+        <v>28.52535702886011</v>
+      </c>
+      <c r="L25" t="n">
+        <v>4.933333333333337</v>
+      </c>
+      <c r="M25" t="n">
+        <v>-3.391981314539589</v>
+      </c>
+      <c r="N25" t="n">
+        <v>4.941991117525683</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" t="n">
+        <v>18</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>39.78977418794979</v>
+      </c>
+      <c r="R25" t="n">
+        <v>36567.10095119293</v>
+      </c>
+      <c r="S25" t="n">
+        <v>0</v>
+      </c>
+      <c r="T25" t="n">
+        <v>36567.10095119293</v>
+      </c>
+      <c r="U25" t="n">
+        <v>0</v>
+      </c>
+      <c r="V25" t="n">
+        <v>0</v>
+      </c>
+      <c r="W25" t="n">
+        <v>55.41538461538462</v>
+      </c>
+      <c r="X25" t="n">
+        <v>55.20515880333441</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>3444.801909328067</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>184.5666666666667</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.3819458071278916</v>
+      </c>
+      <c r="D26" t="n">
+        <v>56</v>
+      </c>
+      <c r="E26" t="n">
+        <v>189.5</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.8792629304200403</v>
+      </c>
+      <c r="G26" t="n">
+        <v>52</v>
+      </c>
+      <c r="H26" t="n">
+        <v>187.0333333333333</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.6048623733408078</v>
+      </c>
+      <c r="J26" t="n">
+        <v>54</v>
+      </c>
+      <c r="K26" t="n">
+        <v>26.82145509855564</v>
+      </c>
+      <c r="L26" t="n">
+        <v>4.933333333333337</v>
+      </c>
+      <c r="M26" t="n">
+        <v>-5.755166395760019</v>
+      </c>
+      <c r="N26" t="n">
+        <v>4.958325873137537</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0</v>
+      </c>
+      <c r="P26" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>39.39513762665919</v>
+      </c>
+      <c r="R26" t="n">
+        <v>33942.11362248049</v>
+      </c>
+      <c r="S26" t="n">
+        <v>0</v>
+      </c>
+      <c r="T26" t="n">
+        <v>33942.11362248049</v>
+      </c>
+      <c r="U26" t="n">
+        <v>0</v>
+      </c>
+      <c r="V26" t="n">
+        <v>0</v>
+      </c>
+      <c r="W26" t="n">
+        <v>53.13846153846154</v>
+      </c>
+      <c r="X26" t="n">
+        <v>52.53359916512073</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>3278.096587903534</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
+        <v>189.5</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.8792629304200403</v>
+      </c>
+      <c r="D27" t="n">
+        <v>52</v>
+      </c>
+      <c r="E27" t="n">
+        <v>194.4333333333333</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1.58401478028587</v>
+      </c>
+      <c r="G27" t="n">
+        <v>48</v>
+      </c>
+      <c r="H27" t="n">
+        <v>191.9666666666667</v>
+      </c>
+      <c r="I27" t="n">
+        <v>1.205504242737646</v>
+      </c>
+      <c r="J27" t="n">
+        <v>50</v>
+      </c>
+      <c r="K27" t="n">
+        <v>25.2345008397151</v>
+      </c>
+      <c r="L27" t="n">
+        <v>4.933333333333337</v>
+      </c>
+      <c r="M27" t="n">
+        <v>-8.128223259329671</v>
+      </c>
+      <c r="N27" t="n">
+        <v>4.983395874270569</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>38.79449575726235</v>
+      </c>
+      <c r="R27" t="n">
+        <v>31182.97563712927</v>
+      </c>
+      <c r="S27" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" t="n">
+        <v>31182.97563712927</v>
+      </c>
+      <c r="U27" t="n">
+        <v>0</v>
+      </c>
+      <c r="V27" t="n">
+        <v>0</v>
+      </c>
+      <c r="W27" t="n">
+        <v>50</v>
+      </c>
+      <c r="X27" t="n">
+        <v>48.79449575726235</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>3044.776535253171</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>194.4333333333333</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1.58401478028587</v>
+      </c>
+      <c r="D28" t="n">
+        <v>48</v>
+      </c>
+      <c r="E28" t="n">
+        <v>199.3666666666667</v>
+      </c>
+      <c r="F28" t="n">
+        <v>2.499933806165217</v>
+      </c>
+      <c r="G28" t="n">
+        <v>44</v>
+      </c>
+      <c r="H28" t="n">
+        <v>196.9</v>
+      </c>
+      <c r="I28" t="n">
+        <v>2.01529760176534</v>
+      </c>
+      <c r="J28" t="n">
+        <v>46</v>
+      </c>
+      <c r="K28" t="n">
+        <v>23.76916713274843</v>
+      </c>
+      <c r="L28" t="n">
+        <v>4.933333333333337</v>
+      </c>
+      <c r="M28" t="n">
+        <v>-10.51541175991534</v>
+      </c>
+      <c r="N28" t="n">
+        <v>5.017599638257309</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0</v>
+      </c>
+      <c r="P28" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>37.98470239823466</v>
+      </c>
+      <c r="R28" t="n">
+        <v>28287.63820173043</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0</v>
+      </c>
+      <c r="T28" t="n">
+        <v>28287.63820173043</v>
+      </c>
+      <c r="U28" t="n">
+        <v>0</v>
+      </c>
+      <c r="V28" t="n">
+        <v>0</v>
+      </c>
+      <c r="W28" t="n">
+        <v>46</v>
+      </c>
+      <c r="X28" t="n">
+        <v>43.98470239823466</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>2744.645429649843</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>199.3666666666667</v>
+      </c>
+      <c r="C29" t="n">
+        <v>2.499933806165217</v>
+      </c>
+      <c r="D29" t="n">
+        <v>44</v>
+      </c>
+      <c r="E29" t="n">
+        <v>204.3</v>
+      </c>
+      <c r="F29" t="n">
+        <v>3.632006118520721</v>
+      </c>
+      <c r="G29" t="n">
+        <v>40</v>
+      </c>
+      <c r="H29" t="n">
+        <v>201.8333333333333</v>
+      </c>
+      <c r="I29" t="n">
+        <v>3.038586609847172</v>
+      </c>
+      <c r="J29" t="n">
+        <v>42</v>
+      </c>
+      <c r="K29" t="n">
+        <v>22.43264648790648</v>
+      </c>
+      <c r="L29" t="n">
+        <v>4.933333333333337</v>
+      </c>
+      <c r="M29" t="n">
+        <v>-12.92121998739083</v>
+      </c>
+      <c r="N29" t="n">
+        <v>5.061498343382579</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>36.96141339015283</v>
+      </c>
+      <c r="R29" t="n">
+        <v>25253.27239966754</v>
+      </c>
+      <c r="S29" t="n">
+        <v>0</v>
+      </c>
+      <c r="T29" t="n">
+        <v>25253.27239966754</v>
+      </c>
+      <c r="U29" t="n">
+        <v>0</v>
+      </c>
+      <c r="V29" t="n">
+        <v>0</v>
+      </c>
+      <c r="W29" t="n">
+        <v>42</v>
+      </c>
+      <c r="X29" t="n">
+        <v>38.96141339015283</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>2431.192195545536</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>204.3</v>
+      </c>
+      <c r="C30" t="n">
+        <v>3.632006118520721</v>
+      </c>
+      <c r="D30" t="n">
+        <v>40</v>
+      </c>
+      <c r="E30" t="n">
+        <v>209.3118645579456</v>
+      </c>
+      <c r="F30" t="n">
+        <v>5.010018042625987</v>
+      </c>
+      <c r="G30" t="n">
+        <v>40</v>
+      </c>
+      <c r="H30" t="n">
+        <v>206.8059322789728</v>
+      </c>
+      <c r="I30" t="n">
+        <v>4.291821067543381</v>
+      </c>
+      <c r="J30" t="n">
+        <v>40</v>
+      </c>
+      <c r="K30" t="n">
+        <v>22.14591053377169</v>
+      </c>
+      <c r="L30" t="n">
+        <v>5.011864557945557</v>
+      </c>
+      <c r="M30" t="n">
+        <v>-15.36989035124163</v>
+      </c>
+      <c r="N30" t="n">
+        <v>5.197763482859122</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>35.70817893245662</v>
+      </c>
+      <c r="R30" t="n">
+        <v>23623.3214474872</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0</v>
+      </c>
+      <c r="T30" t="n">
+        <v>23623.3214474872</v>
+      </c>
+      <c r="U30" t="n">
+        <v>0</v>
+      </c>
+      <c r="V30" t="n">
+        <v>0</v>
+      </c>
+      <c r="W30" t="n">
+        <v>40</v>
+      </c>
+      <c r="X30" t="n">
+        <v>35.70817893245662</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>2228.190365385293</v>
+      </c>
+      <c r="Z30" t="n">
         <v>3</v>
       </c>
-      <c r="Y21" t="n">
+      <c r="AA30" t="n">
         <v>27</v>
       </c>
-      <c r="Z21" t="n">
+      <c r="AB30" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>209.3118645579456</v>
+      </c>
+      <c r="C31" t="n">
+        <v>5.010018042625987</v>
+      </c>
+      <c r="D31" t="n">
+        <v>40</v>
+      </c>
+      <c r="E31" t="n">
+        <v>214.3237291158911</v>
+      </c>
+      <c r="F31" t="n">
+        <v>6.62608620842262</v>
+      </c>
+      <c r="G31" t="n">
+        <v>40</v>
+      </c>
+      <c r="H31" t="n">
+        <v>211.8177968369183</v>
+      </c>
+      <c r="I31" t="n">
+        <v>5.787698403038007</v>
+      </c>
+      <c r="J31" t="n">
+        <v>40</v>
+      </c>
+      <c r="K31" t="n">
+        <v>22.893849201519</v>
+      </c>
+      <c r="L31" t="n">
+        <v>5.011864557945529</v>
+      </c>
+      <c r="M31" t="n">
+        <v>-17.8673905118829</v>
+      </c>
+      <c r="N31" t="n">
+        <v>5.265840358557494</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>34.21230159696199</v>
+      </c>
+      <c r="R31" t="n">
+        <v>22633.69968018153</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0</v>
+      </c>
+      <c r="T31" t="n">
+        <v>22633.69968018153</v>
+      </c>
+      <c r="U31" t="n">
+        <v>0</v>
+      </c>
+      <c r="V31" t="n">
+        <v>0</v>
+      </c>
+      <c r="W31" t="n">
+        <v>40</v>
+      </c>
+      <c r="X31" t="n">
+        <v>34.21230159696199</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>2134.847619650428</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>27</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="n">
+        <v>214.3237291158911</v>
+      </c>
+      <c r="C32" t="n">
+        <v>6.62608620842262</v>
+      </c>
+      <c r="D32" t="n">
+        <v>40</v>
+      </c>
+      <c r="E32" t="n">
+        <v>219.3355936738366</v>
+      </c>
+      <c r="F32" t="n">
+        <v>8.49056033864909</v>
+      </c>
+      <c r="G32" t="n">
+        <v>40</v>
+      </c>
+      <c r="H32" t="n">
+        <v>216.8296613948639</v>
+      </c>
+      <c r="I32" t="n">
+        <v>7.526539007679531</v>
+      </c>
+      <c r="J32" t="n">
+        <v>40</v>
+      </c>
+      <c r="K32" t="n">
+        <v>23.76326950383977</v>
+      </c>
+      <c r="L32" t="n">
+        <v>5.011864557945529</v>
+      </c>
+      <c r="M32" t="n">
+        <v>-20.4005175054688</v>
+      </c>
+      <c r="N32" t="n">
+        <v>5.347250293323763</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>32.47346099232047</v>
+      </c>
+      <c r="R32" t="n">
+        <v>21483.34164520336</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" t="n">
+        <v>21483.34164520336</v>
+      </c>
+      <c r="U32" t="n">
+        <v>0</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0</v>
+      </c>
+      <c r="W32" t="n">
+        <v>40</v>
+      </c>
+      <c r="X32" t="n">
+        <v>32.47346099232047</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>2026.343965920797</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>27</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="n">
+        <v>219.3355936738366</v>
+      </c>
+      <c r="C33" t="n">
+        <v>8.49056033864909</v>
+      </c>
+      <c r="D33" t="n">
+        <v>40</v>
+      </c>
+      <c r="E33" t="n">
+        <v>224.3474582317822</v>
+      </c>
+      <c r="F33" t="n">
+        <v>10.6161421138269</v>
+      </c>
+      <c r="G33" t="n">
+        <v>40</v>
+      </c>
+      <c r="H33" t="n">
+        <v>221.8415259528094</v>
+      </c>
+      <c r="I33" t="n">
+        <v>9.519814236161409</v>
+      </c>
+      <c r="J33" t="n">
+        <v>40</v>
+      </c>
+      <c r="K33" t="n">
+        <v>24.7599071180807</v>
+      </c>
+      <c r="L33" t="n">
+        <v>5.011864557945557</v>
+      </c>
+      <c r="M33" t="n">
+        <v>-22.97603342869171</v>
+      </c>
+      <c r="N33" t="n">
+        <v>5.443724983246797</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>30.48018576383859</v>
+      </c>
+      <c r="R33" t="n">
+        <v>20164.65828291808</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0</v>
+      </c>
+      <c r="T33" t="n">
+        <v>20164.65828291808</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0</v>
+      </c>
+      <c r="V33" t="n">
+        <v>0</v>
+      </c>
+      <c r="W33" t="n">
+        <v>40</v>
+      </c>
+      <c r="X33" t="n">
+        <v>30.48018576383859</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>1901.963591663528</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>27</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="n">
+        <v>224.3474582317822</v>
+      </c>
+      <c r="C34" t="n">
+        <v>10.6161421138269</v>
+      </c>
+      <c r="D34" t="n">
+        <v>40</v>
+      </c>
+      <c r="E34" t="n">
+        <v>229.3593227897277</v>
+      </c>
+      <c r="F34" t="n">
+        <v>13.01839398362826</v>
+      </c>
+      <c r="G34" t="n">
+        <v>40</v>
+      </c>
+      <c r="H34" t="n">
+        <v>226.853390510755</v>
+      </c>
+      <c r="I34" t="n">
+        <v>11.78158247073122</v>
+      </c>
+      <c r="J34" t="n">
+        <v>40</v>
+      </c>
+      <c r="K34" t="n">
+        <v>25.89079123536561</v>
+      </c>
+      <c r="L34" t="n">
+        <v>5.011864557945557</v>
+      </c>
+      <c r="M34" t="n">
+        <v>-25.60164173425728</v>
+      </c>
+      <c r="N34" t="n">
+        <v>5.557499003165231</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>28.21841752926878</v>
+      </c>
+      <c r="R34" t="n">
+        <v>18668.34904390524</v>
+      </c>
+      <c r="S34" t="n">
+        <v>0</v>
+      </c>
+      <c r="T34" t="n">
+        <v>18668.34904390524</v>
+      </c>
+      <c r="U34" t="n">
+        <v>0</v>
+      </c>
+      <c r="V34" t="n">
+        <v>0</v>
+      </c>
+      <c r="W34" t="n">
+        <v>40</v>
+      </c>
+      <c r="X34" t="n">
+        <v>28.21841752926878</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>1760.829253826372</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>27</v>
+      </c>
+      <c r="AB34" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="n">
+        <v>229.3593227897277</v>
+      </c>
+      <c r="C35" t="n">
+        <v>13.01839398362826</v>
+      </c>
+      <c r="D35" t="n">
+        <v>40</v>
+      </c>
+      <c r="E35" t="n">
+        <v>234.3711873476733</v>
+      </c>
+      <c r="F35" t="n">
+        <v>15.71643411866144</v>
+      </c>
+      <c r="G35" t="n">
+        <v>40</v>
+      </c>
+      <c r="H35" t="n">
+        <v>231.8652550687005</v>
+      </c>
+      <c r="I35" t="n">
+        <v>14.32908268605011</v>
+      </c>
+      <c r="J35" t="n">
+        <v>40</v>
+      </c>
+      <c r="K35" t="n">
+        <v>27.16454134302506</v>
+      </c>
+      <c r="L35" t="n">
+        <v>5.011864557945529</v>
+      </c>
+      <c r="M35" t="n">
+        <v>-28.28626507516133</v>
+      </c>
+      <c r="N35" t="n">
+        <v>5.691478441003543</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>25.67091731394989</v>
+      </c>
+      <c r="R35" t="n">
+        <v>16983.00920655711</v>
+      </c>
+      <c r="S35" t="n">
+        <v>0</v>
+      </c>
+      <c r="T35" t="n">
+        <v>16983.00920655711</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0</v>
+      </c>
+      <c r="V35" t="n">
+        <v>0</v>
+      </c>
+      <c r="W35" t="n">
+        <v>40</v>
+      </c>
+      <c r="X35" t="n">
+        <v>25.67091731394989</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>1601.865240390473</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>27</v>
+      </c>
+      <c r="AB35" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="n">
+        <v>234.3711873476733</v>
+      </c>
+      <c r="C36" t="n">
+        <v>15.71643411866144</v>
+      </c>
+      <c r="D36" t="n">
+        <v>40</v>
+      </c>
+      <c r="E36" t="n">
+        <v>239.3830519056188</v>
+      </c>
+      <c r="F36" t="n">
+        <v>18.73390188558466</v>
+      </c>
+      <c r="G36" t="n">
+        <v>40</v>
+      </c>
+      <c r="H36" t="n">
+        <v>236.877119626646</v>
+      </c>
+      <c r="I36" t="n">
+        <v>17.18355157510187</v>
+      </c>
+      <c r="J36" t="n">
+        <v>40</v>
+      </c>
+      <c r="K36" t="n">
+        <v>28.59177578755094</v>
+      </c>
+      <c r="L36" t="n">
+        <v>5.011864557945529</v>
+      </c>
+      <c r="M36" t="n">
+        <v>-31.04042135518254</v>
+      </c>
+      <c r="N36" t="n">
+        <v>5.849489621526809</v>
+      </c>
+      <c r="O36" t="n">
+        <v>0</v>
+      </c>
+      <c r="P36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>22.81644842489813</v>
+      </c>
+      <c r="R36" t="n">
+        <v>15094.58929425995</v>
+      </c>
+      <c r="S36" t="n">
+        <v>0</v>
+      </c>
+      <c r="T36" t="n">
+        <v>15094.58929425995</v>
+      </c>
+      <c r="U36" t="n">
+        <v>0</v>
+      </c>
+      <c r="V36" t="n">
+        <v>0</v>
+      </c>
+      <c r="W36" t="n">
+        <v>40</v>
+      </c>
+      <c r="X36" t="n">
+        <v>22.81644842489813</v>
+      </c>
+      <c r="Y36" t="n">
+        <v>1423.746381713643</v>
+      </c>
+      <c r="Z36" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA36" t="n">
+        <v>27</v>
+      </c>
+      <c r="AB36" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="n">
+        <v>239.3830519056188</v>
+      </c>
+      <c r="C37" t="n">
+        <v>18.73390188558466</v>
+      </c>
+      <c r="D37" t="n">
+        <v>40</v>
+      </c>
+      <c r="E37" t="n">
+        <v>244.3949164635644</v>
+      </c>
+      <c r="F37" t="n">
+        <v>22.10032906584965</v>
+      </c>
+      <c r="G37" t="n">
+        <v>40</v>
+      </c>
+      <c r="H37" t="n">
+        <v>241.8889841845916</v>
+      </c>
+      <c r="I37" t="n">
+        <v>20.37137060687094</v>
+      </c>
+      <c r="J37" t="n">
+        <v>40</v>
+      </c>
+      <c r="K37" t="n">
+        <v>30.18568530343547</v>
+      </c>
+      <c r="L37" t="n">
+        <v>5.011864557945557</v>
+      </c>
+      <c r="M37" t="n">
+        <v>-33.87674663054345</v>
+      </c>
+      <c r="N37" t="n">
+        <v>6.036655848650556</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0</v>
+      </c>
+      <c r="P37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>19.62862939312906</v>
+      </c>
+      <c r="R37" t="n">
+        <v>12985.6362208943</v>
+      </c>
+      <c r="S37" t="n">
+        <v>0</v>
+      </c>
+      <c r="T37" t="n">
+        <v>12985.6362208943</v>
+      </c>
+      <c r="U37" t="n">
+        <v>0</v>
+      </c>
+      <c r="V37" t="n">
+        <v>0</v>
+      </c>
+      <c r="W37" t="n">
+        <v>40</v>
+      </c>
+      <c r="X37" t="n">
+        <v>19.62862939312906</v>
+      </c>
+      <c r="Y37" t="n">
+        <v>1224.826474131253</v>
+      </c>
+      <c r="Z37" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA37" t="n">
+        <v>27</v>
+      </c>
+      <c r="AB37" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="n">
+        <v>244.3949164635644</v>
+      </c>
+      <c r="C38" t="n">
+        <v>22.10032906584965</v>
+      </c>
+      <c r="D38" t="n">
+        <v>40</v>
+      </c>
+      <c r="E38" t="n">
+        <v>249.4067810215099</v>
+      </c>
+      <c r="F38" t="n">
+        <v>25.8531416455277</v>
+      </c>
+      <c r="G38" t="n">
+        <v>40</v>
+      </c>
+      <c r="H38" t="n">
+        <v>246.9008487425371</v>
+      </c>
+      <c r="I38" t="n">
+        <v>23.92571649966472</v>
+      </c>
+      <c r="J38" t="n">
+        <v>40</v>
+      </c>
+      <c r="K38" t="n">
+        <v>31.96285824983236</v>
+      </c>
+      <c r="L38" t="n">
+        <v>5.011864557945557</v>
+      </c>
+      <c r="M38" t="n">
+        <v>-36.81074422175501</v>
+      </c>
+      <c r="N38" t="n">
+        <v>6.259986823384043</v>
+      </c>
+      <c r="O38" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>16.07428350033528</v>
+      </c>
+      <c r="R38" t="n">
+        <v>10634.20139360033</v>
+      </c>
+      <c r="S38" t="n">
+        <v>0</v>
+      </c>
+      <c r="T38" t="n">
+        <v>10634.20139360033</v>
+      </c>
+      <c r="U38" t="n">
+        <v>0</v>
+      </c>
+      <c r="V38" t="n">
+        <v>0</v>
+      </c>
+      <c r="W38" t="n">
+        <v>40</v>
+      </c>
+      <c r="X38" t="n">
+        <v>16.07428350033528</v>
+      </c>
+      <c r="Y38" t="n">
+        <v>1003.035290420922</v>
+      </c>
+      <c r="Z38" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA38" t="n">
+        <v>27</v>
+      </c>
+      <c r="AB38" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="n">
+        <v>249.4067810215099</v>
+      </c>
+      <c r="C39" t="n">
+        <v>25.8531416455277</v>
+      </c>
+      <c r="D39" t="n">
+        <v>40</v>
+      </c>
+      <c r="E39" t="n">
+        <v>254.4186455794554</v>
+      </c>
+      <c r="F39" t="n">
+        <v>30.04068289318309</v>
+      </c>
+      <c r="G39" t="n">
+        <v>40</v>
+      </c>
+      <c r="H39" t="n">
+        <v>251.9127133004827</v>
+      </c>
+      <c r="I39" t="n">
+        <v>27.88900970699665</v>
+      </c>
+      <c r="J39" t="n">
+        <v>40</v>
+      </c>
+      <c r="K39" t="n">
+        <v>33.94450485349832</v>
+      </c>
+      <c r="L39" t="n">
+        <v>5.011864557945529</v>
+      </c>
+      <c r="M39" t="n">
+        <v>-39.86189504715914</v>
+      </c>
+      <c r="N39" t="n">
+        <v>6.529337568856269</v>
+      </c>
+      <c r="O39" t="n">
+        <v>0</v>
+      </c>
+      <c r="P39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>12.11099029300335</v>
+      </c>
+      <c r="R39" t="n">
+        <v>8012.220877468611</v>
+      </c>
+      <c r="S39" t="n">
+        <v>0</v>
+      </c>
+      <c r="T39" t="n">
+        <v>8012.220877468611</v>
+      </c>
+      <c r="U39" t="n">
+        <v>0</v>
+      </c>
+      <c r="V39" t="n">
+        <v>0</v>
+      </c>
+      <c r="W39" t="n">
+        <v>40</v>
+      </c>
+      <c r="X39" t="n">
+        <v>12.11099029300335</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>755.7257942834093</v>
+      </c>
+      <c r="Z39" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA39" t="n">
+        <v>27</v>
+      </c>
+      <c r="AB39" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="n">
+        <v>254.4186455794554</v>
+      </c>
+      <c r="C40" t="n">
+        <v>30.04068289318309</v>
+      </c>
+      <c r="D40" t="n">
+        <v>40</v>
+      </c>
+      <c r="E40" t="n">
+        <v>259.430510137401</v>
+      </c>
+      <c r="F40" t="n">
+        <v>34.72697403083299</v>
+      </c>
+      <c r="G40" t="n">
+        <v>40</v>
+      </c>
+      <c r="H40" t="n">
+        <v>256.9245778584282</v>
+      </c>
+      <c r="I40" t="n">
+        <v>32.31668606446074</v>
+      </c>
+      <c r="J40" t="n">
+        <v>40</v>
+      </c>
+      <c r="K40" t="n">
+        <v>36.15834303223037</v>
+      </c>
+      <c r="L40" t="n">
+        <v>5.011864557945529</v>
+      </c>
+      <c r="M40" t="n">
+        <v>-43.0553705022208</v>
+      </c>
+      <c r="N40" t="n">
+        <v>6.859044479203896</v>
+      </c>
+      <c r="O40" t="n">
+        <v>0</v>
+      </c>
+      <c r="P40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>7.68331393553926</v>
+      </c>
+      <c r="R40" t="n">
+        <v>5083.020201744962</v>
+      </c>
+      <c r="S40" t="n">
+        <v>0</v>
+      </c>
+      <c r="T40" t="n">
+        <v>5083.020201744962</v>
+      </c>
+      <c r="U40" t="n">
+        <v>0</v>
+      </c>
+      <c r="V40" t="n">
+        <v>0</v>
+      </c>
+      <c r="W40" t="n">
+        <v>40</v>
+      </c>
+      <c r="X40" t="n">
+        <v>7.68331393553926</v>
+      </c>
+      <c r="Y40" t="n">
+        <v>479.4387895776499</v>
+      </c>
+      <c r="Z40" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA40" t="n">
+        <v>27</v>
+      </c>
+      <c r="AB40" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="n">
+        <v>259.430510137401</v>
+      </c>
+      <c r="C41" t="n">
+        <v>34.72697403083299</v>
+      </c>
+      <c r="D41" t="n">
+        <v>40</v>
+      </c>
+      <c r="E41" t="n">
+        <v>264.4423746953465</v>
+      </c>
+      <c r="F41" t="n">
+        <v>39.99961494556895</v>
+      </c>
+      <c r="G41" t="n">
+        <v>40</v>
+      </c>
+      <c r="H41" t="n">
+        <v>261.9364424163738</v>
+      </c>
+      <c r="I41" t="n">
+        <v>37.28328476066929</v>
+      </c>
+      <c r="J41" t="n">
+        <v>40</v>
+      </c>
+      <c r="K41" t="n">
+        <v>38.64164238033464</v>
+      </c>
+      <c r="L41" t="n">
+        <v>5.011864557945557</v>
+      </c>
+      <c r="M41" t="n">
+        <v>-46.42480574440896</v>
+      </c>
+      <c r="N41" t="n">
+        <v>7.270885335185018</v>
+      </c>
+      <c r="O41" t="n">
+        <v>0</v>
+      </c>
+      <c r="P41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>2.716715239330711</v>
+      </c>
+      <c r="R41" t="n">
+        <v>1797.286764508247</v>
+      </c>
+      <c r="S41" t="n">
+        <v>0</v>
+      </c>
+      <c r="T41" t="n">
+        <v>1797.286764508247</v>
+      </c>
+      <c r="U41" t="n">
+        <v>0</v>
+      </c>
+      <c r="V41" t="n">
+        <v>0</v>
+      </c>
+      <c r="W41" t="n">
+        <v>40</v>
+      </c>
+      <c r="X41" t="n">
+        <v>2.716715239330711</v>
+      </c>
+      <c r="Y41" t="n">
+        <v>169.5230309342363</v>
+      </c>
+      <c r="Z41" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA41" t="n">
+        <v>27</v>
+      </c>
+      <c r="AB41" t="n">
         <v>400</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finally conquered the line of thrust problem.
</commit_message>
<xml_diff>
--- a/slices.xlsx
+++ b/slices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB21"/>
+  <dimension ref="A1:AB42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -589,52 +589,52 @@
         <v>40.21936727790366</v>
       </c>
       <c r="E2" t="n">
-        <v>118.903497678473</v>
+        <v>117.4370253272771</v>
       </c>
       <c r="F2" t="n">
-        <v>40.8545666849556</v>
+        <v>40.51964175793073</v>
       </c>
       <c r="G2" t="n">
-        <v>42.59743055011329</v>
+        <v>41.40839891400848</v>
       </c>
       <c r="H2" t="n">
-        <v>117.4370253272771</v>
+        <v>116.7037891516791</v>
       </c>
       <c r="I2" t="n">
-        <v>40.51964175793073</v>
+        <v>40.36214511739084</v>
       </c>
       <c r="J2" t="n">
-        <v>41.40839891400847</v>
+        <v>40.81388309595606</v>
       </c>
       <c r="K2" t="n">
-        <v>40.9640203359696</v>
+        <v>40.58801410667345</v>
       </c>
       <c r="L2" t="n">
-        <v>2.932944702391879</v>
+        <v>1.466472351195947</v>
       </c>
       <c r="M2" t="n">
-        <v>12.36969322478999</v>
+        <v>11.87578869033491</v>
       </c>
       <c r="N2" t="n">
-        <v>3.002649017626326</v>
+        <v>1.498547206397035</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>0.8887571560777374</v>
+        <v>0.4517379785652196</v>
       </c>
       <c r="Q2" t="n">
         <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>312.8010711157287</v>
+        <v>79.49535066612499</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>312.8010711157287</v>
+        <v>79.49535066612499</v>
       </c>
       <c r="U2" t="n">
         <v>0</v>
@@ -643,13 +643,13 @@
         <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>41.40839891400847</v>
+        <v>40.81388309595606</v>
       </c>
       <c r="X2" t="n">
-        <v>0.8887571560777374</v>
+        <v>0.4517379785652196</v>
       </c>
       <c r="Y2" t="n">
-        <v>55.45844653925082</v>
+        <v>28.1884498624697</v>
       </c>
       <c r="Z2" t="n">
         <v>2</v>
@@ -666,61 +666,61 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
+        <v>117.4370253272771</v>
+      </c>
+      <c r="C3" t="n">
+        <v>40.51964175793073</v>
+      </c>
+      <c r="D3" t="n">
+        <v>41.40839891400848</v>
+      </c>
+      <c r="E3" t="n">
         <v>118.903497678473</v>
       </c>
-      <c r="C3" t="n">
+      <c r="F3" t="n">
         <v>40.8545666849556</v>
       </c>
-      <c r="D3" t="n">
+      <c r="G3" t="n">
         <v>42.59743055011329</v>
       </c>
-      <c r="E3" t="n">
-        <v>121.8364423808649</v>
-      </c>
-      <c r="F3" t="n">
-        <v>41.60529025955755</v>
-      </c>
-      <c r="G3" t="n">
-        <v>44.97549382232293</v>
-      </c>
       <c r="H3" t="n">
-        <v>120.369970029669</v>
+        <v>118.1702615028751</v>
       </c>
       <c r="I3" t="n">
-        <v>41.21633377148819</v>
+        <v>40.6837694228856</v>
       </c>
       <c r="J3" t="n">
-        <v>43.78646218621811</v>
+        <v>42.00291473206088</v>
       </c>
       <c r="K3" t="n">
-        <v>42.50139797885315</v>
+        <v>41.34334207747324</v>
       </c>
       <c r="L3" t="n">
-        <v>2.932944702391893</v>
+        <v>1.466472351195932</v>
       </c>
       <c r="M3" t="n">
-        <v>14.35509490194034</v>
+        <v>12.86453328886096</v>
       </c>
       <c r="N3" t="n">
-        <v>3.02746902981108</v>
+        <v>1.504229717970171</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>2.570128414729915</v>
+        <v>1.319145309175276</v>
       </c>
       <c r="Q3" t="n">
         <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>904.5653422138773</v>
+        <v>232.1388147738423</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>904.5653422138773</v>
+        <v>232.1388147738423</v>
       </c>
       <c r="U3" t="n">
         <v>0</v>
@@ -729,13 +729,13 @@
         <v>0</v>
       </c>
       <c r="W3" t="n">
-        <v>43.78646218621811</v>
+        <v>42.00291473206088</v>
       </c>
       <c r="X3" t="n">
-        <v>2.570128414729915</v>
+        <v>1.319145309175276</v>
       </c>
       <c r="Y3" t="n">
-        <v>160.3760130791467</v>
+        <v>82.31466729253724</v>
       </c>
       <c r="Z3" t="n">
         <v>2</v>
@@ -752,61 +752,61 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>121.8364423808649</v>
+        <v>118.903497678473</v>
       </c>
       <c r="C4" t="n">
-        <v>41.60529025955755</v>
+        <v>40.8545666849556</v>
       </c>
       <c r="D4" t="n">
-        <v>44.97549382232293</v>
+        <v>42.59743055011329</v>
       </c>
       <c r="E4" t="n">
-        <v>124.7693870832568</v>
+        <v>120.369970029669</v>
       </c>
       <c r="F4" t="n">
-        <v>42.46632650231609</v>
+        <v>41.21633377148819</v>
       </c>
       <c r="G4" t="n">
-        <v>47.35355709453255</v>
+        <v>43.78646218621811</v>
       </c>
       <c r="H4" t="n">
-        <v>123.3029147320609</v>
+        <v>119.636733854071</v>
       </c>
       <c r="I4" t="n">
-        <v>42.02181620546986</v>
+        <v>41.03207400264517</v>
       </c>
       <c r="J4" t="n">
-        <v>46.16452545842775</v>
+        <v>43.1919463681657</v>
       </c>
       <c r="K4" t="n">
-        <v>44.0931708319488</v>
+        <v>42.11201018540544</v>
       </c>
       <c r="L4" t="n">
-        <v>2.932944702391879</v>
+        <v>1.466472351195947</v>
       </c>
       <c r="M4" t="n">
-        <v>16.35827067366206</v>
+        <v>13.85719057210321</v>
       </c>
       <c r="N4" t="n">
-        <v>3.056681131130836</v>
+        <v>1.510432428664756</v>
       </c>
       <c r="O4" t="n">
         <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>4.142709252957886</v>
+        <v>2.159872365520528</v>
       </c>
       <c r="Q4" t="n">
         <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>1458.040458841518</v>
+        <v>380.0871727377647</v>
       </c>
       <c r="S4" t="n">
         <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>1458.040458841518</v>
+        <v>380.0871727377647</v>
       </c>
       <c r="U4" t="n">
         <v>0</v>
@@ -815,13 +815,13 @@
         <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>46.16452545842775</v>
+        <v>43.1919463681657</v>
       </c>
       <c r="X4" t="n">
-        <v>4.142709252957886</v>
+        <v>2.159872365520528</v>
       </c>
       <c r="Y4" t="n">
-        <v>258.5050573845721</v>
+        <v>134.7760356084809</v>
       </c>
       <c r="Z4" t="n">
         <v>2</v>
@@ -838,61 +838,61 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>124.7693870832568</v>
+        <v>120.369970029669</v>
       </c>
       <c r="C5" t="n">
-        <v>42.46632650231609</v>
+        <v>41.21633377148819</v>
       </c>
       <c r="D5" t="n">
-        <v>47.35355709453255</v>
+        <v>43.78646218621811</v>
       </c>
       <c r="E5" t="n">
-        <v>127.7023317856487</v>
+        <v>121.8364423808649</v>
       </c>
       <c r="F5" t="n">
-        <v>43.44114784283002</v>
+        <v>41.60529025955755</v>
       </c>
       <c r="G5" t="n">
-        <v>49.7316203667422</v>
+        <v>44.97549382232293</v>
       </c>
       <c r="H5" t="n">
-        <v>126.2358594344528</v>
+        <v>121.103206205267</v>
       </c>
       <c r="I5" t="n">
-        <v>42.93927315549512</v>
+        <v>41.40739037843254</v>
       </c>
       <c r="J5" t="n">
-        <v>48.54258873063738</v>
+        <v>44.38097800427051</v>
       </c>
       <c r="K5" t="n">
-        <v>45.74093094306625</v>
+        <v>42.89418419135153</v>
       </c>
       <c r="L5" t="n">
-        <v>2.932944702391893</v>
+        <v>1.466472351195947</v>
       </c>
       <c r="M5" t="n">
-        <v>18.38222854153053</v>
+        <v>14.85410906326754</v>
       </c>
       <c r="N5" t="n">
-        <v>3.090648533113749</v>
+        <v>1.51717368733887</v>
       </c>
       <c r="O5" t="n">
         <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>5.603315575142261</v>
+        <v>2.973587625837972</v>
       </c>
       <c r="Q5" t="n">
         <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>1972.105767833217</v>
+        <v>523.282084457974</v>
       </c>
       <c r="S5" t="n">
         <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>1972.105767833217</v>
+        <v>523.282084457974</v>
       </c>
       <c r="U5" t="n">
         <v>0</v>
@@ -901,13 +901,13 @@
         <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>48.54258873063738</v>
+        <v>44.38097800427051</v>
       </c>
       <c r="X5" t="n">
-        <v>5.603315575142261</v>
+        <v>2.973587625837972</v>
       </c>
       <c r="Y5" t="n">
-        <v>349.6468918888771</v>
+        <v>185.5518678522894</v>
       </c>
       <c r="Z5" t="n">
         <v>2</v>
@@ -924,61 +924,61 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>127.7023317856487</v>
+        <v>121.8364423808649</v>
       </c>
       <c r="C6" t="n">
-        <v>43.44114784283002</v>
+        <v>41.60529025955755</v>
       </c>
       <c r="D6" t="n">
-        <v>49.7316203667422</v>
+        <v>44.97549382232293</v>
       </c>
       <c r="E6" t="n">
-        <v>130.6352764880406</v>
+        <v>123.3029147320609</v>
       </c>
       <c r="F6" t="n">
-        <v>44.53386404841829</v>
+        <v>42.02181620546986</v>
       </c>
       <c r="G6" t="n">
-        <v>52.10968363895181</v>
+        <v>46.16452545842775</v>
       </c>
       <c r="H6" t="n">
-        <v>129.1688041368446</v>
+        <v>122.5696785564629</v>
       </c>
       <c r="I6" t="n">
-        <v>43.97248479624828</v>
+        <v>41.81008196131133</v>
       </c>
       <c r="J6" t="n">
-        <v>50.92065200284701</v>
+        <v>45.57000964037535</v>
       </c>
       <c r="K6" t="n">
-        <v>47.44656839954765</v>
+        <v>43.69004580084334</v>
       </c>
       <c r="L6" t="n">
-        <v>2.932944702391865</v>
+        <v>1.466472351195947</v>
       </c>
       <c r="M6" t="n">
-        <v>20.43024197568106</v>
+        <v>15.85565003315322</v>
       </c>
       <c r="N6" t="n">
-        <v>3.129816832228253</v>
+        <v>1.524473886669827</v>
       </c>
       <c r="O6" t="n">
         <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>6.948167206598725</v>
+        <v>3.75992767906402</v>
       </c>
       <c r="Q6" t="n">
         <v>0</v>
       </c>
       <c r="R6" t="n">
-        <v>2445.430823991193</v>
+        <v>661.6595980612478</v>
       </c>
       <c r="S6" t="n">
         <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>2445.430823991193</v>
+        <v>661.6595980612478</v>
       </c>
       <c r="U6" t="n">
         <v>0</v>
@@ -987,13 +987,13 @@
         <v>0</v>
       </c>
       <c r="W6" t="n">
-        <v>50.92065200284701</v>
+        <v>45.57000964037535</v>
       </c>
       <c r="X6" t="n">
-        <v>6.948167206598725</v>
+        <v>3.75992767906402</v>
       </c>
       <c r="Y6" t="n">
-        <v>433.5656336917605</v>
+        <v>234.6194871735949</v>
       </c>
       <c r="Z6" t="n">
         <v>2</v>
@@ -1010,61 +1010,61 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>130.6352764880406</v>
+        <v>123.3029147320609</v>
       </c>
       <c r="C7" t="n">
-        <v>44.53386404841829</v>
+        <v>42.02181620546986</v>
       </c>
       <c r="D7" t="n">
-        <v>52.10968363895181</v>
+        <v>46.16452545842775</v>
       </c>
       <c r="E7" t="n">
-        <v>133.5682211904325</v>
+        <v>124.7693870832568</v>
       </c>
       <c r="F7" t="n">
-        <v>45.74932103578577</v>
+        <v>42.46632650231609</v>
       </c>
       <c r="G7" t="n">
-        <v>54.48774691116146</v>
+        <v>47.35355709453255</v>
       </c>
       <c r="H7" t="n">
-        <v>132.1017488392365</v>
+        <v>124.0361509076589</v>
       </c>
       <c r="I7" t="n">
-        <v>45.1259150954214</v>
+        <v>42.24054595803628</v>
       </c>
       <c r="J7" t="n">
-        <v>53.29871527505662</v>
+        <v>46.75904127648015</v>
       </c>
       <c r="K7" t="n">
-        <v>49.21231518523901</v>
+        <v>44.49979361725822</v>
       </c>
       <c r="L7" t="n">
-        <v>2.932944702391893</v>
+        <v>1.466472351195932</v>
       </c>
       <c r="M7" t="n">
-        <v>22.50590985809011</v>
+        <v>16.86218890555249</v>
       </c>
       <c r="N7" t="n">
-        <v>3.174732126033935</v>
+        <v>1.532355647855679</v>
       </c>
       <c r="O7" t="n">
         <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>8.172800179635217</v>
+        <v>4.518495318443875</v>
       </c>
       <c r="Q7" t="n">
         <v>0</v>
       </c>
       <c r="R7" t="n">
-        <v>2876.444518868235</v>
+        <v>795.1498144207443</v>
       </c>
       <c r="S7" t="n">
         <v>0</v>
       </c>
       <c r="T7" t="n">
-        <v>2876.444518868235</v>
+        <v>795.1498144207443</v>
       </c>
       <c r="U7" t="n">
         <v>0</v>
@@ -1073,13 +1073,13 @@
         <v>0</v>
       </c>
       <c r="W7" t="n">
-        <v>52.73926869503224</v>
+        <v>46.75904127648015</v>
       </c>
       <c r="X7" t="n">
-        <v>7.613353599610832</v>
+        <v>4.518495318443875</v>
       </c>
       <c r="Y7" t="n">
-        <v>475.0732646157159</v>
+        <v>281.9541078708978</v>
       </c>
       <c r="Z7" t="n">
         <v>2</v>
@@ -1096,61 +1096,61 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>133.5682211904325</v>
+        <v>124.7693870832568</v>
       </c>
       <c r="C8" t="n">
-        <v>45.74932103578577</v>
+        <v>42.46632650231609</v>
       </c>
       <c r="D8" t="n">
-        <v>54.48774691116146</v>
+        <v>47.35355709453255</v>
       </c>
       <c r="E8" t="n">
-        <v>136.5011658928244</v>
+        <v>126.2358594344528</v>
       </c>
       <c r="F8" t="n">
-        <v>47.09322675736657</v>
+        <v>42.93927315549512</v>
       </c>
       <c r="G8" t="n">
-        <v>56.8658101833711</v>
+        <v>48.54258873063738</v>
       </c>
       <c r="H8" t="n">
-        <v>135.0346935416284</v>
+        <v>125.5026232588548</v>
       </c>
       <c r="I8" t="n">
-        <v>46.40482325739281</v>
+        <v>42.69921551642359</v>
       </c>
       <c r="J8" t="n">
-        <v>55.67677854726629</v>
+        <v>47.94807291258496</v>
       </c>
       <c r="K8" t="n">
-        <v>51.04080090232955</v>
+        <v>45.32364421450428</v>
       </c>
       <c r="L8" t="n">
-        <v>2.932944702391893</v>
+        <v>1.466472351195947</v>
       </c>
       <c r="M8" t="n">
-        <v>24.61323022023543</v>
+        <v>17.87411679315489</v>
       </c>
       <c r="N8" t="n">
-        <v>3.226065103393914</v>
+        <v>1.540844032415425</v>
       </c>
       <c r="O8" t="n">
         <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>9.271955289873482</v>
+        <v>5.24885739616137</v>
       </c>
       <c r="Q8" t="n">
         <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>3263.29585778987</v>
+        <v>923.6765096209197</v>
       </c>
       <c r="S8" t="n">
         <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>3263.29585778987</v>
+        <v>923.6765096209197</v>
       </c>
       <c r="U8" t="n">
         <v>0</v>
@@ -1159,13 +1159,13 @@
         <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>54.09293548075158</v>
+        <v>47.94807291258496</v>
       </c>
       <c r="X8" t="n">
-        <v>7.688112223358779</v>
+        <v>5.24885739616137</v>
       </c>
       <c r="Y8" t="n">
-        <v>479.7382027375878</v>
+        <v>327.5287015204694</v>
       </c>
       <c r="Z8" t="n">
         <v>2</v>
@@ -1182,61 +1182,61 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>136.5011658928244</v>
+        <v>126.2358594344528</v>
       </c>
       <c r="C9" t="n">
-        <v>47.09322675736657</v>
+        <v>42.93927315549512</v>
       </c>
       <c r="D9" t="n">
-        <v>56.8658101833711</v>
+        <v>48.54258873063738</v>
       </c>
       <c r="E9" t="n">
-        <v>139.4341105952163</v>
+        <v>127.7023317856487</v>
       </c>
       <c r="F9" t="n">
-        <v>48.57231281173381</v>
+        <v>43.44114784283002</v>
       </c>
       <c r="G9" t="n">
-        <v>59.24387345558074</v>
+        <v>49.7316203667422</v>
       </c>
       <c r="H9" t="n">
-        <v>137.9676382440203</v>
+        <v>126.9690956100507</v>
       </c>
       <c r="I9" t="n">
-        <v>47.81540619668814</v>
+        <v>43.1865621389082</v>
       </c>
       <c r="J9" t="n">
-        <v>58.05484181947591</v>
+        <v>49.13710454868979</v>
       </c>
       <c r="K9" t="n">
-        <v>52.93512400808203</v>
+        <v>46.161833343799</v>
       </c>
       <c r="L9" t="n">
-        <v>2.932944702391893</v>
+        <v>1.466472351195947</v>
       </c>
       <c r="M9" t="n">
-        <v>26.75669242036603</v>
+        <v>18.89184218266112</v>
       </c>
       <c r="N9" t="n">
-        <v>3.284643417092181</v>
+        <v>1.54996678524872</v>
       </c>
       <c r="O9" t="n">
         <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>10.23943562278777</v>
+        <v>5.95054240978159</v>
       </c>
       <c r="Q9" t="n">
         <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>3603.803815840586</v>
+        <v>1047.156710227632</v>
       </c>
       <c r="S9" t="n">
         <v>0</v>
       </c>
       <c r="T9" t="n">
-        <v>3603.803815840586</v>
+        <v>1047.156710227632</v>
       </c>
       <c r="U9" t="n">
         <v>0</v>
@@ -1245,13 +1245,13 @@
         <v>0</v>
       </c>
       <c r="W9" t="n">
-        <v>55.4466022664709</v>
+        <v>49.13710454868979</v>
       </c>
       <c r="X9" t="n">
-        <v>7.63119606978276</v>
+        <v>5.95054240978159</v>
       </c>
       <c r="Y9" t="n">
-        <v>476.1866347544442</v>
+        <v>371.3138463703712</v>
       </c>
       <c r="Z9" t="n">
         <v>2</v>
@@ -1268,61 +1268,61 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>139.4341105952163</v>
+        <v>127.7023317856487</v>
       </c>
       <c r="C10" t="n">
-        <v>48.57231281173381</v>
+        <v>43.44114784283002</v>
       </c>
       <c r="D10" t="n">
-        <v>59.24387345558074</v>
+        <v>49.7316203667422</v>
       </c>
       <c r="E10" t="n">
-        <v>142.3670552976081</v>
+        <v>129.1688041368446</v>
       </c>
       <c r="F10" t="n">
-        <v>50.19454407086326</v>
+        <v>43.97248479624828</v>
       </c>
       <c r="G10" t="n">
-        <v>61.62193672779036</v>
+        <v>50.92065200284701</v>
       </c>
       <c r="H10" t="n">
-        <v>140.9005829464122</v>
+        <v>128.4355679612467</v>
       </c>
       <c r="I10" t="n">
-        <v>49.36498233025576</v>
+        <v>43.70309839844586</v>
       </c>
       <c r="J10" t="n">
-        <v>60.43290509168555</v>
+        <v>50.32613618479461</v>
       </c>
       <c r="K10" t="n">
-        <v>54.89894371097065</v>
+        <v>47.01461729162023</v>
       </c>
       <c r="L10" t="n">
-        <v>2.932944702391865</v>
+        <v>1.466472351195932</v>
       </c>
       <c r="M10" t="n">
-        <v>28.94139426941132</v>
+        <v>19.91579279204961</v>
       </c>
       <c r="N10" t="n">
-        <v>3.351495771472501</v>
+        <v>1.559754613942271</v>
       </c>
       <c r="O10" t="n">
         <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>11.06792276142979</v>
+        <v>6.623037786348746</v>
       </c>
       <c r="Q10" t="n">
         <v>0</v>
       </c>
       <c r="R10" t="n">
-        <v>3895.392651554141</v>
+        <v>1165.500215352762</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
       </c>
       <c r="T10" t="n">
-        <v>3895.392651554141</v>
+        <v>1165.500215352762</v>
       </c>
       <c r="U10" t="n">
         <v>0</v>
@@ -1331,13 +1331,13 @@
         <v>0</v>
       </c>
       <c r="W10" t="n">
-        <v>56.80026905219024</v>
+        <v>50.32613618479461</v>
       </c>
       <c r="X10" t="n">
-        <v>7.435286721934482</v>
+        <v>6.623037786348746</v>
       </c>
       <c r="Y10" t="n">
-        <v>463.9618914487116</v>
+        <v>413.2775578681618</v>
       </c>
       <c r="Z10" t="n">
         <v>2</v>
@@ -1354,61 +1354,61 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>142.3670552976081</v>
+        <v>129.1688041368446</v>
       </c>
       <c r="C11" t="n">
-        <v>50.19454407086326</v>
+        <v>43.97248479624828</v>
       </c>
       <c r="D11" t="n">
-        <v>61.62193672779036</v>
+        <v>50.92065200284701</v>
       </c>
       <c r="E11" t="n">
-        <v>145.3</v>
+        <v>130.6352764880406</v>
       </c>
       <c r="F11" t="n">
-        <v>51.96939412734315</v>
+        <v>44.53386404841829</v>
       </c>
       <c r="G11" t="n">
-        <v>64</v>
+        <v>52.10968363895181</v>
       </c>
       <c r="H11" t="n">
-        <v>143.8335276488041</v>
+        <v>129.9020403124426</v>
       </c>
       <c r="I11" t="n">
-        <v>51.06223144461947</v>
+        <v>44.24938099679981</v>
       </c>
       <c r="J11" t="n">
-        <v>62.81096836389519</v>
+        <v>51.51516782089941</v>
       </c>
       <c r="K11" t="n">
-        <v>56.93659990425733</v>
+        <v>47.88227440884962</v>
       </c>
       <c r="L11" t="n">
-        <v>2.932944702391893</v>
+        <v>1.466472351195932</v>
       </c>
       <c r="M11" t="n">
-        <v>31.17319341485867</v>
+        <v>20.94641762494726</v>
       </c>
       <c r="N11" t="n">
-        <v>3.427912938590898</v>
+        <v>1.570241510290336</v>
       </c>
       <c r="O11" t="n">
         <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>11.74873691927572</v>
+        <v>7.2657868240996</v>
       </c>
       <c r="Q11" t="n">
         <v>0</v>
       </c>
       <c r="R11" t="n">
-        <v>4135.007484862293</v>
+        <v>1278.609058467092</v>
       </c>
       <c r="S11" t="n">
         <v>0</v>
       </c>
       <c r="T11" t="n">
-        <v>4135.007484862293</v>
+        <v>1278.609058467092</v>
       </c>
       <c r="U11" t="n">
         <v>0</v>
@@ -1417,13 +1417,13 @@
         <v>0</v>
       </c>
       <c r="W11" t="n">
-        <v>58.15393583790957</v>
+        <v>51.51516782089941</v>
       </c>
       <c r="X11" t="n">
-        <v>7.091704393290101</v>
+        <v>7.2657868240996</v>
       </c>
       <c r="Y11" t="n">
-        <v>442.5223541413023</v>
+        <v>453.385097823815</v>
       </c>
       <c r="Z11" t="n">
         <v>2</v>
@@ -1440,61 +1440,61 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>145.3</v>
+        <v>130.6352764880406</v>
       </c>
       <c r="C12" t="n">
-        <v>51.96939412734315</v>
+        <v>44.53386404841829</v>
       </c>
       <c r="D12" t="n">
-        <v>64</v>
+        <v>52.10968363895181</v>
       </c>
       <c r="E12" t="n">
-        <v>148.3875</v>
+        <v>132.1017488392365</v>
       </c>
       <c r="F12" t="n">
-        <v>54.01517752872294</v>
+        <v>45.1259150954214</v>
       </c>
       <c r="G12" t="n">
-        <v>66.5</v>
+        <v>53.29871527505665</v>
       </c>
       <c r="H12" t="n">
-        <v>146.84375</v>
+        <v>131.3685126636386</v>
       </c>
       <c r="I12" t="n">
-        <v>52.96864067220648</v>
+        <v>44.82601421227278</v>
       </c>
       <c r="J12" t="n">
-        <v>65.24999999999999</v>
+        <v>52.70419945700424</v>
       </c>
       <c r="K12" t="n">
-        <v>59.15570915844685</v>
+        <v>48.76510683463852</v>
       </c>
       <c r="L12" t="n">
-        <v>3.087500000000006</v>
+        <v>1.466472351195961</v>
       </c>
       <c r="M12" t="n">
-        <v>33.51993017508019</v>
+        <v>21.98418925285722</v>
       </c>
       <c r="N12" t="n">
-        <v>3.703398138537016</v>
+        <v>1.58146512122851</v>
       </c>
       <c r="O12" t="n">
-        <v>1.249999999999986</v>
+        <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>11.03135932779352</v>
+        <v>7.878185244731462</v>
       </c>
       <c r="Q12" t="n">
         <v>0</v>
       </c>
       <c r="R12" t="n">
-        <v>4588.837380947503</v>
+        <v>1386.376900679841</v>
       </c>
       <c r="S12" t="n">
         <v>0</v>
       </c>
       <c r="T12" t="n">
-        <v>4588.837380947503</v>
+        <v>1386.376900679841</v>
       </c>
       <c r="U12" t="n">
         <v>0</v>
@@ -1503,22 +1503,22 @@
         <v>0</v>
       </c>
       <c r="W12" t="n">
-        <v>59.54326923076923</v>
+        <v>52.40085199860242</v>
       </c>
       <c r="X12" t="n">
-        <v>6.574628558562758</v>
+        <v>7.574837786329638</v>
       </c>
       <c r="Y12" t="n">
-        <v>410.256822054316</v>
+        <v>472.6698778669694</v>
       </c>
       <c r="Z12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA12" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AB12" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13">
@@ -1526,61 +1526,61 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>148.3875</v>
+        <v>132.1017488392365</v>
       </c>
       <c r="C13" t="n">
-        <v>54.01517752872294</v>
+        <v>45.1259150954214</v>
       </c>
       <c r="D13" t="n">
-        <v>66.5</v>
+        <v>53.29871527505665</v>
       </c>
       <c r="E13" t="n">
-        <v>151.475</v>
+        <v>133.5682211904325</v>
       </c>
       <c r="F13" t="n">
-        <v>56.25879568493919</v>
+        <v>45.74932103578577</v>
       </c>
       <c r="G13" t="n">
-        <v>69.00000000000001</v>
+        <v>54.48774691116146</v>
       </c>
       <c r="H13" t="n">
-        <v>149.93125</v>
+        <v>132.8349850148345</v>
       </c>
       <c r="I13" t="n">
-        <v>55.11111399206905</v>
+        <v>45.43365379237048</v>
       </c>
       <c r="J13" t="n">
-        <v>67.75000000000001</v>
+        <v>53.89323109310905</v>
       </c>
       <c r="K13" t="n">
-        <v>61.53779559103037</v>
+        <v>49.66344244273976</v>
       </c>
       <c r="L13" t="n">
-        <v>3.087500000000006</v>
+        <v>1.466472351195932</v>
       </c>
       <c r="M13" t="n">
-        <v>35.99506183523606</v>
+        <v>23.02960635994756</v>
       </c>
       <c r="N13" t="n">
-        <v>3.816120934206944</v>
+        <v>1.593467177870363</v>
       </c>
       <c r="O13" t="n">
-        <v>3.750000000000014</v>
+        <v>0</v>
       </c>
       <c r="P13" t="n">
-        <v>8.88888600793095</v>
+        <v>8.459577300738573</v>
       </c>
       <c r="Q13" t="n">
         <v>0</v>
       </c>
       <c r="R13" t="n">
-        <v>4798.488515938431</v>
+        <v>1488.68834572054</v>
       </c>
       <c r="S13" t="n">
         <v>0</v>
       </c>
       <c r="T13" t="n">
-        <v>4798.488515938431</v>
+        <v>1488.68834572054</v>
       </c>
       <c r="U13" t="n">
         <v>0</v>
@@ -1589,22 +1589,22 @@
         <v>0</v>
       </c>
       <c r="W13" t="n">
-        <v>60.96826923076924</v>
+        <v>53.07768539146208</v>
       </c>
       <c r="X13" t="n">
-        <v>5.857155238700194</v>
+        <v>7.644031599091598</v>
       </c>
       <c r="Y13" t="n">
-        <v>365.4864868948921</v>
+        <v>476.9875717833157</v>
       </c>
       <c r="Z13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA13" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AB13" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14">
@@ -1612,61 +1612,61 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>151.475</v>
+        <v>133.5682211904325</v>
       </c>
       <c r="C14" t="n">
-        <v>56.25879568493919</v>
+        <v>45.74932103578577</v>
       </c>
       <c r="D14" t="n">
-        <v>69.00000000000001</v>
+        <v>54.48774691116146</v>
       </c>
       <c r="E14" t="n">
-        <v>154.5625</v>
+        <v>135.0346935416284</v>
       </c>
       <c r="F14" t="n">
-        <v>58.72018573139036</v>
+        <v>46.40482325739281</v>
       </c>
       <c r="G14" t="n">
-        <v>71.5</v>
+        <v>55.67677854726629</v>
       </c>
       <c r="H14" t="n">
-        <v>153.01875</v>
+        <v>134.3014573660304</v>
       </c>
       <c r="I14" t="n">
-        <v>57.4608410660633</v>
+        <v>46.07301135704613</v>
       </c>
       <c r="J14" t="n">
-        <v>70.25</v>
+        <v>55.08226272921387</v>
       </c>
       <c r="K14" t="n">
-        <v>63.98336245352148</v>
+        <v>50.57763704313</v>
       </c>
       <c r="L14" t="n">
-        <v>3.087499999999977</v>
+        <v>1.466472351195961</v>
       </c>
       <c r="M14" t="n">
-        <v>38.55048908183519</v>
+        <v>24.08319659267862</v>
       </c>
       <c r="N14" t="n">
-        <v>3.947910380595018</v>
+        <v>1.606293993211679</v>
       </c>
       <c r="O14" t="n">
-        <v>6.25</v>
+        <v>0</v>
       </c>
       <c r="P14" t="n">
-        <v>6.539158933936704</v>
+        <v>9.009251372167739</v>
       </c>
       <c r="Q14" t="n">
         <v>0</v>
       </c>
       <c r="R14" t="n">
-        <v>4931.352135023512</v>
+        <v>1585.418165070991</v>
       </c>
       <c r="S14" t="n">
         <v>0</v>
       </c>
       <c r="T14" t="n">
-        <v>4931.352135023512</v>
+        <v>1585.418165070991</v>
       </c>
       <c r="U14" t="n">
         <v>0</v>
@@ -1675,22 +1675,22 @@
         <v>0</v>
       </c>
       <c r="W14" t="n">
-        <v>61.905625</v>
+        <v>53.75451878432174</v>
       </c>
       <c r="X14" t="n">
-        <v>4.444783933936705</v>
+        <v>7.681507427275612</v>
       </c>
       <c r="Y14" t="n">
-        <v>277.3545174776504</v>
+        <v>479.3260634619982</v>
       </c>
       <c r="Z14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA14" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AB14" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15">
@@ -1698,61 +1698,61 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>154.5625</v>
+        <v>135.0346935416284</v>
       </c>
       <c r="C15" t="n">
-        <v>58.72018573139036</v>
+        <v>46.40482325739281</v>
       </c>
       <c r="D15" t="n">
-        <v>71.5</v>
+        <v>55.67677854726629</v>
       </c>
       <c r="E15" t="n">
-        <v>157.65</v>
+        <v>136.5011658928244</v>
       </c>
       <c r="F15" t="n">
-        <v>61.42443913628225</v>
+        <v>47.09322675736657</v>
       </c>
       <c r="G15" t="n">
-        <v>74</v>
+        <v>56.8658101833711</v>
       </c>
       <c r="H15" t="n">
-        <v>156.10625</v>
+        <v>135.7679297172264</v>
       </c>
       <c r="I15" t="n">
-        <v>60.04013664131661</v>
+        <v>46.7448593904994</v>
       </c>
       <c r="J15" t="n">
-        <v>72.74999999999999</v>
+        <v>56.2712943653187</v>
       </c>
       <c r="K15" t="n">
-        <v>66.50249424203282</v>
+        <v>51.50807687790905</v>
       </c>
       <c r="L15" t="n">
-        <v>3.087500000000006</v>
+        <v>1.466472351195932</v>
       </c>
       <c r="M15" t="n">
-        <v>41.20023425836374</v>
+        <v>25.14551976323153</v>
       </c>
       <c r="N15" t="n">
-        <v>4.10346873060611</v>
+        <v>1.619997041377506</v>
       </c>
       <c r="O15" t="n">
-        <v>8.749999999999986</v>
+        <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>3.959863358683393</v>
+        <v>9.526434974819296</v>
       </c>
       <c r="Q15" t="n">
         <v>0</v>
       </c>
       <c r="R15" t="n">
-        <v>4979.160624392201</v>
+        <v>1676.43041952461</v>
       </c>
       <c r="S15" t="n">
         <v>0</v>
       </c>
       <c r="T15" t="n">
-        <v>4979.160624392201</v>
+        <v>1676.43041952461</v>
       </c>
       <c r="U15" t="n">
         <v>0</v>
@@ -1761,22 +1761,22 @@
         <v>0</v>
       </c>
       <c r="W15" t="n">
-        <v>62.831875</v>
+        <v>54.43135217718141</v>
       </c>
       <c r="X15" t="n">
-        <v>2.791738358683389</v>
+        <v>7.68649278668201</v>
       </c>
       <c r="Y15" t="n">
-        <v>174.2044735818435</v>
+        <v>479.6371498889574</v>
       </c>
       <c r="Z15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA15" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AB15" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16">
@@ -1784,61 +1784,61 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>157.65</v>
+        <v>136.5011658928244</v>
       </c>
       <c r="C16" t="n">
-        <v>61.42443913628225</v>
+        <v>47.09322675736657</v>
       </c>
       <c r="D16" t="n">
-        <v>74</v>
+        <v>56.8658101833711</v>
       </c>
       <c r="E16" t="n">
-        <v>160.7375</v>
+        <v>137.9676382440203</v>
       </c>
       <c r="F16" t="n">
-        <v>64.40379640476834</v>
+        <v>47.81540619668814</v>
       </c>
       <c r="G16" t="n">
-        <v>76.5</v>
+        <v>58.05484181947591</v>
       </c>
       <c r="H16" t="n">
-        <v>159.19375</v>
+        <v>137.2344020684223</v>
       </c>
       <c r="I16" t="n">
-        <v>62.87736063580922</v>
+        <v>47.4500369145324</v>
       </c>
       <c r="J16" t="n">
-        <v>75.25000000000001</v>
+        <v>57.4603260014235</v>
       </c>
       <c r="K16" t="n">
-        <v>69.10321688379364</v>
+        <v>52.45518145797796</v>
       </c>
       <c r="L16" t="n">
-        <v>3.087500000000006</v>
+        <v>1.466472351195932</v>
       </c>
       <c r="M16" t="n">
-        <v>43.96199282336407</v>
+        <v>26.21717146540865</v>
       </c>
       <c r="N16" t="n">
-        <v>4.289383295124071</v>
+        <v>1.63463363420544</v>
       </c>
       <c r="O16" t="n">
-        <v>11.25000000000001</v>
+        <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>1.122639364190782</v>
+        <v>10.0102890868911</v>
       </c>
       <c r="Q16" t="n">
         <v>0</v>
       </c>
       <c r="R16" t="n">
-        <v>4931.406634432699</v>
+        <v>1761.577460808501</v>
       </c>
       <c r="S16" t="n">
         <v>0</v>
       </c>
       <c r="T16" t="n">
-        <v>4931.406634432699</v>
+        <v>1761.577460808501</v>
       </c>
       <c r="U16" t="n">
         <v>0</v>
@@ -1847,22 +1847,22 @@
         <v>0</v>
       </c>
       <c r="W16" t="n">
-        <v>63.75812500000001</v>
+        <v>55.10818557004107</v>
       </c>
       <c r="X16" t="n">
-        <v>0.8807643641907887</v>
+        <v>7.658148655508668</v>
       </c>
       <c r="Y16" t="n">
-        <v>54.95969632550521</v>
+        <v>477.8684761037409</v>
       </c>
       <c r="Z16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA16" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AB16" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17">
@@ -1870,61 +1870,61 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>160.7375</v>
+        <v>137.9676382440203</v>
       </c>
       <c r="C17" t="n">
-        <v>64.40379640476834</v>
+        <v>47.81540619668814</v>
       </c>
       <c r="D17" t="n">
-        <v>76.5</v>
+        <v>58.05484181947591</v>
       </c>
       <c r="E17" t="n">
-        <v>163.825</v>
+        <v>139.4341105952163</v>
       </c>
       <c r="F17" t="n">
-        <v>67.70078395860372</v>
+        <v>48.57231281173381</v>
       </c>
       <c r="G17" t="n">
-        <v>78.99999999999999</v>
+        <v>59.24387345558074</v>
       </c>
       <c r="H17" t="n">
-        <v>162.28125</v>
+        <v>138.7008744196183</v>
       </c>
       <c r="I17" t="n">
-        <v>66.00940495811544</v>
+        <v>48.18945595489674</v>
       </c>
       <c r="J17" t="n">
-        <v>77.75</v>
+        <v>58.64935763752834</v>
       </c>
       <c r="K17" t="n">
-        <v>71.87970247905773</v>
+        <v>53.41940679621253</v>
       </c>
       <c r="L17" t="n">
-        <v>3.087499999999977</v>
+        <v>1.466472351195961</v>
       </c>
       <c r="M17" t="n">
-        <v>46.85869846135417</v>
+        <v>27.29878717327239</v>
       </c>
       <c r="N17" t="n">
-        <v>4.515209574421058</v>
+        <v>1.650267714633164</v>
       </c>
       <c r="O17" t="n">
-        <v>11.74059504188456</v>
+        <v>0</v>
       </c>
       <c r="P17" t="n">
-        <v>0</v>
+        <v>10.4599016826316</v>
       </c>
       <c r="Q17" t="n">
         <v>0</v>
       </c>
       <c r="R17" t="n">
-        <v>4712.381334936381</v>
+        <v>1840.698793656881</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
       </c>
       <c r="T17" t="n">
-        <v>4712.381334936381</v>
+        <v>1840.698793656881</v>
       </c>
       <c r="U17" t="n">
         <v>0</v>
@@ -1933,22 +1933,22 @@
         <v>0</v>
       </c>
       <c r="W17" t="n">
-        <v>64.684375</v>
+        <v>55.78501896290075</v>
       </c>
       <c r="X17" t="n">
-        <v>0</v>
+        <v>7.595563008004007</v>
       </c>
       <c r="Y17" t="n">
-        <v>0</v>
+        <v>473.96313169945</v>
       </c>
       <c r="Z17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA17" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AB17" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18">
@@ -1956,61 +1956,61 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>163.825</v>
+        <v>139.4341105952163</v>
       </c>
       <c r="C18" t="n">
-        <v>67.70078395860372</v>
+        <v>48.57231281173381</v>
       </c>
       <c r="D18" t="n">
-        <v>78.99999999999999</v>
+        <v>59.24387345558074</v>
       </c>
       <c r="E18" t="n">
-        <v>166.9125</v>
+        <v>140.9005829464122</v>
       </c>
       <c r="F18" t="n">
-        <v>71.37341370684827</v>
+        <v>49.36498233025576</v>
       </c>
       <c r="G18" t="n">
-        <v>81.5</v>
+        <v>60.43290509168555</v>
       </c>
       <c r="H18" t="n">
-        <v>165.36875</v>
+        <v>140.1673467708142</v>
       </c>
       <c r="I18" t="n">
-        <v>69.48570250875673</v>
+        <v>48.96410893480623</v>
       </c>
       <c r="J18" t="n">
-        <v>80.24999999999999</v>
+        <v>59.83838927363315</v>
       </c>
       <c r="K18" t="n">
-        <v>74.86785125437837</v>
+        <v>54.40124910421969</v>
       </c>
       <c r="L18" t="n">
-        <v>3.087500000000006</v>
+        <v>1.466472351195932</v>
       </c>
       <c r="M18" t="n">
-        <v>49.92105561848282</v>
+        <v>28.39104690759883</v>
       </c>
       <c r="N18" t="n">
-        <v>4.795427561821701</v>
+        <v>1.666970791043669</v>
       </c>
       <c r="O18" t="n">
-        <v>10.76429749124325</v>
+        <v>0</v>
       </c>
       <c r="P18" t="n">
-        <v>0</v>
+        <v>10.87428033882691</v>
       </c>
       <c r="Q18" t="n">
         <v>0</v>
       </c>
       <c r="R18" t="n">
-        <v>4320.51990554777</v>
+        <v>1913.619774725184</v>
       </c>
       <c r="S18" t="n">
         <v>0</v>
       </c>
       <c r="T18" t="n">
-        <v>4320.51990554777</v>
+        <v>1913.619774725184</v>
       </c>
       <c r="U18" t="n">
         <v>0</v>
@@ -2019,22 +2019,22 @@
         <v>0</v>
       </c>
       <c r="W18" t="n">
-        <v>65.610625</v>
+        <v>56.46185235576041</v>
       </c>
       <c r="X18" t="n">
-        <v>0</v>
+        <v>7.497743420954173</v>
       </c>
       <c r="Y18" t="n">
-        <v>0</v>
+        <v>467.8591894675404</v>
       </c>
       <c r="Z18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA18" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AB18" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19">
@@ -2042,61 +2042,61 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>166.9125</v>
+        <v>140.9005829464122</v>
       </c>
       <c r="C19" t="n">
-        <v>71.37341370684827</v>
+        <v>49.36498233025576</v>
       </c>
       <c r="D19" t="n">
-        <v>81.5</v>
+        <v>60.43290509168555</v>
       </c>
       <c r="E19" t="n">
-        <v>170</v>
+        <v>142.3670552976081</v>
       </c>
       <c r="F19" t="n">
-        <v>75.50440019361704</v>
+        <v>50.19454407086326</v>
       </c>
       <c r="G19" t="n">
-        <v>84</v>
+        <v>61.62193672779036</v>
       </c>
       <c r="H19" t="n">
-        <v>168.45625</v>
+        <v>141.6338191220102</v>
       </c>
       <c r="I19" t="n">
-        <v>73.37508430762216</v>
+        <v>49.77507715802599</v>
       </c>
       <c r="J19" t="n">
-        <v>82.75000000000001</v>
+        <v>61.02742090973796</v>
       </c>
       <c r="K19" t="n">
-        <v>78.06254215381108</v>
+        <v>55.40124903388197</v>
       </c>
       <c r="L19" t="n">
-        <v>3.087500000000006</v>
+        <v>1.466472351195932</v>
       </c>
       <c r="M19" t="n">
-        <v>53.19188933498902</v>
+        <v>29.49468057184322</v>
       </c>
       <c r="N19" t="n">
-        <v>5.153245914347297</v>
+        <v>1.684823042688945</v>
       </c>
       <c r="O19" t="n">
-        <v>9.374915692377854</v>
+        <v>0</v>
       </c>
       <c r="P19" t="n">
-        <v>0</v>
+        <v>11.25234375171196</v>
       </c>
       <c r="Q19" t="n">
         <v>0</v>
       </c>
       <c r="R19" t="n">
-        <v>3762.856786028168</v>
+        <v>1980.150119764548</v>
       </c>
       <c r="S19" t="n">
         <v>0</v>
       </c>
       <c r="T19" t="n">
-        <v>3762.856786028168</v>
+        <v>1980.150119764548</v>
       </c>
       <c r="U19" t="n">
         <v>0</v>
@@ -2105,22 +2105,22 @@
         <v>0</v>
       </c>
       <c r="W19" t="n">
-        <v>66.53687500000001</v>
+        <v>57.13868574862007</v>
       </c>
       <c r="X19" t="n">
-        <v>0</v>
+        <v>7.363608590594076</v>
       </c>
       <c r="Y19" t="n">
-        <v>0</v>
+        <v>459.4891760530703</v>
       </c>
       <c r="Z19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA19" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AB19" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20">
@@ -2128,61 +2128,61 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>170</v>
+        <v>142.3670552976081</v>
       </c>
       <c r="C20" t="n">
-        <v>75.50440019361704</v>
+        <v>50.19454407086326</v>
       </c>
       <c r="D20" t="n">
-        <v>84</v>
+        <v>61.62193672779036</v>
       </c>
       <c r="E20" t="n">
-        <v>172.6265258146969</v>
+        <v>143.8335276488041</v>
       </c>
       <c r="F20" t="n">
-        <v>79.47126890591167</v>
+        <v>51.06223144461947</v>
       </c>
       <c r="G20" t="n">
-        <v>84</v>
+        <v>62.81096836389519</v>
       </c>
       <c r="H20" t="n">
-        <v>171.3132629073484</v>
+        <v>143.1002914732061</v>
       </c>
       <c r="I20" t="n">
-        <v>77.42894111287163</v>
+        <v>50.62354057923822</v>
       </c>
       <c r="J20" t="n">
-        <v>84</v>
+        <v>62.21645254584276</v>
       </c>
       <c r="K20" t="n">
-        <v>80.71447055643581</v>
+        <v>56.41999656254048</v>
       </c>
       <c r="L20" t="n">
-        <v>2.62652581469689</v>
+        <v>1.466472351195961</v>
       </c>
       <c r="M20" t="n">
-        <v>56.45849684755021</v>
+        <v>30.61047408253977</v>
       </c>
       <c r="N20" t="n">
-        <v>4.753541162170476</v>
+        <v>1.703914634042265</v>
       </c>
       <c r="O20" t="n">
-        <v>6.571058887128373</v>
+        <v>0</v>
       </c>
       <c r="P20" t="n">
-        <v>0</v>
+        <v>11.59291196660454</v>
       </c>
       <c r="Q20" t="n">
         <v>0</v>
       </c>
       <c r="R20" t="n">
-        <v>2243.677253601692</v>
+        <v>2040.082184264922</v>
       </c>
       <c r="S20" t="n">
         <v>0</v>
       </c>
       <c r="T20" t="n">
-        <v>2243.677253601692</v>
+        <v>2040.082184264922</v>
       </c>
       <c r="U20" t="n">
         <v>0</v>
@@ -2191,22 +2191,22 @@
         <v>0</v>
       </c>
       <c r="W20" t="n">
-        <v>67.39397887220453</v>
+        <v>57.81551914147973</v>
       </c>
       <c r="X20" t="n">
-        <v>0</v>
+        <v>7.191978562241509</v>
       </c>
       <c r="Y20" t="n">
-        <v>0</v>
+        <v>448.7794622838701</v>
       </c>
       <c r="Z20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA20" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AB20" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21">
@@ -2214,84 +2214,1890 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
+        <v>143.8335276488041</v>
+      </c>
+      <c r="C21" t="n">
+        <v>51.06223144461947</v>
+      </c>
+      <c r="D21" t="n">
+        <v>62.81096836389519</v>
+      </c>
+      <c r="E21" t="n">
+        <v>145.3</v>
+      </c>
+      <c r="F21" t="n">
+        <v>51.96939412734315</v>
+      </c>
+      <c r="G21" t="n">
+        <v>64</v>
+      </c>
+      <c r="H21" t="n">
+        <v>144.566763824402</v>
+      </c>
+      <c r="I21" t="n">
+        <v>51.51078910380646</v>
+      </c>
+      <c r="J21" t="n">
+        <v>63.4054841819476</v>
+      </c>
+      <c r="K21" t="n">
+        <v>57.45813664287703</v>
+      </c>
+      <c r="L21" t="n">
+        <v>1.466472351195932</v>
+      </c>
+      <c r="M21" t="n">
+        <v>31.73927644732163</v>
+      </c>
+      <c r="N21" t="n">
+        <v>1.724347285969732</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" t="n">
+        <v>11.89469507814114</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0</v>
+      </c>
+      <c r="R21" t="n">
+        <v>2093.188974960039</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" t="n">
+        <v>2093.188974960039</v>
+      </c>
+      <c r="U21" t="n">
+        <v>0</v>
+      </c>
+      <c r="V21" t="n">
+        <v>0</v>
+      </c>
+      <c r="W21" t="n">
+        <v>58.4923525343394</v>
+      </c>
+      <c r="X21" t="n">
+        <v>6.981563430532944</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>435.6495580652557</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>145.3</v>
+      </c>
+      <c r="C22" t="n">
+        <v>51.96939412734315</v>
+      </c>
+      <c r="D22" t="n">
+        <v>64</v>
+      </c>
+      <c r="E22" t="n">
+        <v>146.7529411764706</v>
+      </c>
+      <c r="F22" t="n">
+        <v>52.90857190738048</v>
+      </c>
+      <c r="G22" t="n">
+        <v>65.17647058823528</v>
+      </c>
+      <c r="H22" t="n">
+        <v>146.0264705882353</v>
+      </c>
+      <c r="I22" t="n">
+        <v>52.43386231790717</v>
+      </c>
+      <c r="J22" t="n">
+        <v>64.58823529411764</v>
+      </c>
+      <c r="K22" t="n">
+        <v>58.53427872054358</v>
+      </c>
+      <c r="L22" t="n">
+        <v>1.452941176470574</v>
+      </c>
+      <c r="M22" t="n">
+        <v>32.8767024941475</v>
+      </c>
+      <c r="N22" t="n">
+        <v>1.730020045640405</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0.5882352941176379</v>
+      </c>
+      <c r="P22" t="n">
+        <v>11.56613768209283</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" t="n">
+        <v>2127.697389360855</v>
+      </c>
+      <c r="S22" t="n">
+        <v>0</v>
+      </c>
+      <c r="T22" t="n">
+        <v>2127.697389360855</v>
+      </c>
+      <c r="U22" t="n">
+        <v>0</v>
+      </c>
+      <c r="V22" t="n">
+        <v>0</v>
+      </c>
+      <c r="W22" t="n">
+        <v>59.16606334841629</v>
+      </c>
+      <c r="X22" t="n">
+        <v>6.732201030509124</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>420.0893443037693</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>146.7529411764706</v>
+      </c>
+      <c r="C23" t="n">
+        <v>52.90857190738048</v>
+      </c>
+      <c r="D23" t="n">
+        <v>65.17647058823528</v>
+      </c>
+      <c r="E23" t="n">
+        <v>148.2058823529412</v>
+      </c>
+      <c r="F23" t="n">
+        <v>53.88953436174755</v>
+      </c>
+      <c r="G23" t="n">
+        <v>66.35294117647059</v>
+      </c>
+      <c r="H23" t="n">
+        <v>147.4794117647059</v>
+      </c>
+      <c r="I23" t="n">
+        <v>53.39372516734613</v>
+      </c>
+      <c r="J23" t="n">
+        <v>65.76470588235294</v>
+      </c>
+      <c r="K23" t="n">
+        <v>59.64151546782855</v>
+      </c>
+      <c r="L23" t="n">
+        <v>1.452941176470603</v>
+      </c>
+      <c r="M23" t="n">
+        <v>34.02354049559441</v>
+      </c>
+      <c r="N23" t="n">
+        <v>1.753049692282183</v>
+      </c>
+      <c r="O23" t="n">
+        <v>1.764705882352942</v>
+      </c>
+      <c r="P23" t="n">
+        <v>10.60627483265387</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" t="n">
+        <v>2182.55701130716</v>
+      </c>
+      <c r="S23" t="n">
+        <v>0</v>
+      </c>
+      <c r="T23" t="n">
+        <v>2182.55701130716</v>
+      </c>
+      <c r="U23" t="n">
+        <v>0</v>
+      </c>
+      <c r="V23" t="n">
+        <v>0</v>
+      </c>
+      <c r="W23" t="n">
+        <v>59.83665158371041</v>
+      </c>
+      <c r="X23" t="n">
+        <v>6.44292641636428</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>402.038608381131</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB23" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
+        <v>148.2058823529412</v>
+      </c>
+      <c r="C24" t="n">
+        <v>53.88953436174755</v>
+      </c>
+      <c r="D24" t="n">
+        <v>66.35294117647059</v>
+      </c>
+      <c r="E24" t="n">
+        <v>149.6588235294118</v>
+      </c>
+      <c r="F24" t="n">
+        <v>54.9140235655541</v>
+      </c>
+      <c r="G24" t="n">
+        <v>67.52941176470587</v>
+      </c>
+      <c r="H24" t="n">
+        <v>148.9323529411765</v>
+      </c>
+      <c r="I24" t="n">
+        <v>54.39622240287571</v>
+      </c>
+      <c r="J24" t="n">
+        <v>66.94117647058823</v>
+      </c>
+      <c r="K24" t="n">
+        <v>60.76071888428542</v>
+      </c>
+      <c r="L24" t="n">
+        <v>1.452941176470574</v>
+      </c>
+      <c r="M24" t="n">
+        <v>35.18609217075181</v>
+      </c>
+      <c r="N24" t="n">
+        <v>1.777766065969487</v>
+      </c>
+      <c r="O24" t="n">
+        <v>2.941176470588232</v>
+      </c>
+      <c r="P24" t="n">
+        <v>9.603777597124292</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" t="n">
+        <v>2229.983202643226</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T24" t="n">
+        <v>2229.983202643226</v>
+      </c>
+      <c r="U24" t="n">
+        <v>0</v>
+      </c>
+      <c r="V24" t="n">
+        <v>0</v>
+      </c>
+      <c r="W24" t="n">
+        <v>60.50723981900452</v>
+      </c>
+      <c r="X24" t="n">
+        <v>6.111017416128817</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>381.3274867664382</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>149.6588235294118</v>
+      </c>
+      <c r="C25" t="n">
+        <v>54.9140235655541</v>
+      </c>
+      <c r="D25" t="n">
+        <v>67.52941176470587</v>
+      </c>
+      <c r="E25" t="n">
+        <v>151.1117647058824</v>
+      </c>
+      <c r="F25" t="n">
+        <v>55.98396391222813</v>
+      </c>
+      <c r="G25" t="n">
+        <v>68.70588235294117</v>
+      </c>
+      <c r="H25" t="n">
+        <v>150.385294117647</v>
+      </c>
+      <c r="I25" t="n">
+        <v>55.44318426594134</v>
+      </c>
+      <c r="J25" t="n">
+        <v>68.11764705882351</v>
+      </c>
+      <c r="K25" t="n">
+        <v>61.89319229751136</v>
+      </c>
+      <c r="L25" t="n">
+        <v>1.452941176470603</v>
+      </c>
+      <c r="M25" t="n">
+        <v>36.36552132794861</v>
+      </c>
+      <c r="N25" t="n">
+        <v>1.804333835711337</v>
+      </c>
+      <c r="O25" t="n">
+        <v>4.117647058823508</v>
+      </c>
+      <c r="P25" t="n">
+        <v>8.556815734058659</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0</v>
+      </c>
+      <c r="R25" t="n">
+        <v>2269.656855390149</v>
+      </c>
+      <c r="S25" t="n">
+        <v>0</v>
+      </c>
+      <c r="T25" t="n">
+        <v>2269.656855390149</v>
+      </c>
+      <c r="U25" t="n">
+        <v>0</v>
+      </c>
+      <c r="V25" t="n">
+        <v>0</v>
+      </c>
+      <c r="W25" t="n">
+        <v>61.11558823529411</v>
+      </c>
+      <c r="X25" t="n">
+        <v>5.672403969352771</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>353.9580076876129</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>151.1117647058824</v>
+      </c>
+      <c r="C26" t="n">
+        <v>55.98396391222813</v>
+      </c>
+      <c r="D26" t="n">
+        <v>68.70588235294117</v>
+      </c>
+      <c r="E26" t="n">
+        <v>152.5647058823529</v>
+      </c>
+      <c r="F26" t="n">
+        <v>57.10148831016802</v>
+      </c>
+      <c r="G26" t="n">
+        <v>69.88235294117646</v>
+      </c>
+      <c r="H26" t="n">
+        <v>151.8382352941177</v>
+      </c>
+      <c r="I26" t="n">
+        <v>56.53663583549732</v>
+      </c>
+      <c r="J26" t="n">
+        <v>69.29411764705883</v>
+      </c>
+      <c r="K26" t="n">
+        <v>63.04011141469798</v>
+      </c>
+      <c r="L26" t="n">
+        <v>1.452941176470574</v>
+      </c>
+      <c r="M26" t="n">
+        <v>37.56310816536429</v>
+      </c>
+      <c r="N26" t="n">
+        <v>1.832942529274935</v>
+      </c>
+      <c r="O26" t="n">
+        <v>5.294117647058826</v>
+      </c>
+      <c r="P26" t="n">
+        <v>7.463364164502678</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" t="n">
+        <v>2301.224891075968</v>
+      </c>
+      <c r="S26" t="n">
+        <v>0</v>
+      </c>
+      <c r="T26" t="n">
+        <v>2301.224891075968</v>
+      </c>
+      <c r="U26" t="n">
+        <v>0</v>
+      </c>
+      <c r="V26" t="n">
+        <v>0</v>
+      </c>
+      <c r="W26" t="n">
+        <v>61.5514705882353</v>
+      </c>
+      <c r="X26" t="n">
+        <v>5.014834752737976</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>312.9256885708497</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
+        <v>152.5647058823529</v>
+      </c>
+      <c r="C27" t="n">
+        <v>57.10148831016802</v>
+      </c>
+      <c r="D27" t="n">
+        <v>69.88235294117646</v>
+      </c>
+      <c r="E27" t="n">
+        <v>154.0176470588235</v>
+      </c>
+      <c r="F27" t="n">
+        <v>58.26896956548119</v>
+      </c>
+      <c r="G27" t="n">
+        <v>71.05882352941177</v>
+      </c>
+      <c r="H27" t="n">
+        <v>153.2911764705883</v>
+      </c>
+      <c r="I27" t="n">
+        <v>57.67882567478496</v>
+      </c>
+      <c r="J27" t="n">
+        <v>70.47058823529413</v>
+      </c>
+      <c r="K27" t="n">
+        <v>64.20254739888148</v>
+      </c>
+      <c r="L27" t="n">
+        <v>1.452941176470603</v>
+      </c>
+      <c r="M27" t="n">
+        <v>38.7802672104985</v>
+      </c>
+      <c r="N27" t="n">
+        <v>1.86381147919721</v>
+      </c>
+      <c r="O27" t="n">
+        <v>6.47058823529413</v>
+      </c>
+      <c r="P27" t="n">
+        <v>6.32117432521504</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" t="n">
+        <v>2324.295266086307</v>
+      </c>
+      <c r="S27" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" t="n">
+        <v>2324.295266086307</v>
+      </c>
+      <c r="U27" t="n">
+        <v>0</v>
+      </c>
+      <c r="V27" t="n">
+        <v>0</v>
+      </c>
+      <c r="W27" t="n">
+        <v>61.98735294117647</v>
+      </c>
+      <c r="X27" t="n">
+        <v>4.308527266391515</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>268.8521014228305</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>154.0176470588235</v>
+      </c>
+      <c r="C28" t="n">
+        <v>58.26896956548119</v>
+      </c>
+      <c r="D28" t="n">
+        <v>71.05882352941177</v>
+      </c>
+      <c r="E28" t="n">
+        <v>155.4705882352941</v>
+      </c>
+      <c r="F28" t="n">
+        <v>59.4890582625445</v>
+      </c>
+      <c r="G28" t="n">
+        <v>72.23529411764706</v>
+      </c>
+      <c r="H28" t="n">
+        <v>154.7441176470588</v>
+      </c>
+      <c r="I28" t="n">
+        <v>58.87226027627801</v>
+      </c>
+      <c r="J28" t="n">
+        <v>71.64705882352941</v>
+      </c>
+      <c r="K28" t="n">
+        <v>65.38147822917212</v>
+      </c>
+      <c r="L28" t="n">
+        <v>1.452941176470574</v>
+      </c>
+      <c r="M28" t="n">
+        <v>40.01856891423017</v>
+      </c>
+      <c r="N28" t="n">
+        <v>1.897196030975709</v>
+      </c>
+      <c r="O28" t="n">
+        <v>7.647058823529406</v>
+      </c>
+      <c r="P28" t="n">
+        <v>5.127739723721987</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" t="n">
+        <v>2338.430966086148</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0</v>
+      </c>
+      <c r="T28" t="n">
+        <v>2338.430966086148</v>
+      </c>
+      <c r="U28" t="n">
+        <v>0</v>
+      </c>
+      <c r="V28" t="n">
+        <v>0</v>
+      </c>
+      <c r="W28" t="n">
+        <v>62.42323529411765</v>
+      </c>
+      <c r="X28" t="n">
+        <v>3.550975017839633</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>221.5808411131931</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>155.4705882352941</v>
+      </c>
+      <c r="C29" t="n">
+        <v>59.4890582625445</v>
+      </c>
+      <c r="D29" t="n">
+        <v>72.23529411764706</v>
+      </c>
+      <c r="E29" t="n">
+        <v>156.9235294117647</v>
+      </c>
+      <c r="F29" t="n">
+        <v>60.76472886656208</v>
+      </c>
+      <c r="G29" t="n">
+        <v>73.41176470588236</v>
+      </c>
+      <c r="H29" t="n">
+        <v>156.1970588235294</v>
+      </c>
+      <c r="I29" t="n">
+        <v>60.11974580648753</v>
+      </c>
+      <c r="J29" t="n">
+        <v>72.8235294117647</v>
+      </c>
+      <c r="K29" t="n">
+        <v>66.57778805122818</v>
+      </c>
+      <c r="L29" t="n">
+        <v>1.452941176470603</v>
+      </c>
+      <c r="M29" t="n">
+        <v>41.27976585456518</v>
+      </c>
+      <c r="N29" t="n">
+        <v>1.933395411990592</v>
+      </c>
+      <c r="O29" t="n">
+        <v>8.823529411764696</v>
+      </c>
+      <c r="P29" t="n">
+        <v>3.880254193512471</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" t="n">
+        <v>2343.142727691047</v>
+      </c>
+      <c r="S29" t="n">
+        <v>0</v>
+      </c>
+      <c r="T29" t="n">
+        <v>2343.142727691047</v>
+      </c>
+      <c r="U29" t="n">
+        <v>0</v>
+      </c>
+      <c r="V29" t="n">
+        <v>0</v>
+      </c>
+      <c r="W29" t="n">
+        <v>62.85911764705882</v>
+      </c>
+      <c r="X29" t="n">
+        <v>2.739371840571295</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>170.9368028516488</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>156.9235294117647</v>
+      </c>
+      <c r="C30" t="n">
+        <v>60.76472886656208</v>
+      </c>
+      <c r="D30" t="n">
+        <v>73.41176470588236</v>
+      </c>
+      <c r="E30" t="n">
+        <v>158.3764705882353</v>
+      </c>
+      <c r="F30" t="n">
+        <v>62.09933634220274</v>
+      </c>
+      <c r="G30" t="n">
+        <v>74.58823529411764</v>
+      </c>
+      <c r="H30" t="n">
+        <v>157.65</v>
+      </c>
+      <c r="I30" t="n">
+        <v>61.42443913628225</v>
+      </c>
+      <c r="J30" t="n">
+        <v>74</v>
+      </c>
+      <c r="K30" t="n">
+        <v>67.79225229448767</v>
+      </c>
+      <c r="L30" t="n">
+        <v>1.452941176470574</v>
+      </c>
+      <c r="M30" t="n">
+        <v>42.56582481565094</v>
+      </c>
+      <c r="N30" t="n">
+        <v>1.97276281233556</v>
+      </c>
+      <c r="O30" t="n">
+        <v>10</v>
+      </c>
+      <c r="P30" t="n">
+        <v>2.575560863717755</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>0</v>
+      </c>
+      <c r="R30" t="n">
+        <v>2337.880141179944</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0</v>
+      </c>
+      <c r="T30" t="n">
+        <v>2337.880141179944</v>
+      </c>
+      <c r="U30" t="n">
+        <v>0</v>
+      </c>
+      <c r="V30" t="n">
+        <v>0</v>
+      </c>
+      <c r="W30" t="n">
+        <v>63.295</v>
+      </c>
+      <c r="X30" t="n">
+        <v>1.870560863717756</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>116.722997895988</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB30" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>158.3764705882353</v>
+      </c>
+      <c r="C31" t="n">
+        <v>62.09933634220274</v>
+      </c>
+      <c r="D31" t="n">
+        <v>74.58823529411764</v>
+      </c>
+      <c r="E31" t="n">
+        <v>159.8294117647059</v>
+      </c>
+      <c r="F31" t="n">
+        <v>63.49668638166201</v>
+      </c>
+      <c r="G31" t="n">
+        <v>75.76470588235294</v>
+      </c>
+      <c r="H31" t="n">
+        <v>159.1029411764706</v>
+      </c>
+      <c r="I31" t="n">
+        <v>62.78991081598492</v>
+      </c>
+      <c r="J31" t="n">
+        <v>75.1764705882353</v>
+      </c>
+      <c r="K31" t="n">
+        <v>69.02550372115351</v>
+      </c>
+      <c r="L31" t="n">
+        <v>1.452941176470603</v>
+      </c>
+      <c r="M31" t="n">
+        <v>43.87896643861341</v>
+      </c>
+      <c r="N31" t="n">
+        <v>2.015718451111918</v>
+      </c>
+      <c r="O31" t="n">
+        <v>11.1764705882353</v>
+      </c>
+      <c r="P31" t="n">
+        <v>1.210089184015082</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" t="n">
+        <v>2322.020670602627</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0</v>
+      </c>
+      <c r="T31" t="n">
+        <v>2322.020670602627</v>
+      </c>
+      <c r="U31" t="n">
+        <v>0</v>
+      </c>
+      <c r="V31" t="n">
+        <v>0</v>
+      </c>
+      <c r="W31" t="n">
+        <v>63.73088235294118</v>
+      </c>
+      <c r="X31" t="n">
+        <v>0.9409715369562619</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>58.71662390607074</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="n">
+        <v>159.8294117647059</v>
+      </c>
+      <c r="C32" t="n">
+        <v>63.49668638166201</v>
+      </c>
+      <c r="D32" t="n">
+        <v>75.76470588235294</v>
+      </c>
+      <c r="E32" t="n">
+        <v>161.2823529411765</v>
+      </c>
+      <c r="F32" t="n">
+        <v>64.96112347479303</v>
+      </c>
+      <c r="G32" t="n">
+        <v>76.94117647058823</v>
+      </c>
+      <c r="H32" t="n">
+        <v>160.5558823529412</v>
+      </c>
+      <c r="I32" t="n">
+        <v>64.2202236067258</v>
+      </c>
+      <c r="J32" t="n">
+        <v>76.35294117647059</v>
+      </c>
+      <c r="K32" t="n">
+        <v>70.28658239159819</v>
+      </c>
+      <c r="L32" t="n">
+        <v>1.452941176470574</v>
+      </c>
+      <c r="M32" t="n">
+        <v>45.22171475164012</v>
+      </c>
+      <c r="N32" t="n">
+        <v>2.062766731572732</v>
+      </c>
+      <c r="O32" t="n">
+        <v>12.1327175697448</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" t="n">
+        <v>2291.656242144128</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" t="n">
+        <v>2291.656242144128</v>
+      </c>
+      <c r="U32" t="n">
+        <v>0</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0</v>
+      </c>
+      <c r="W32" t="n">
+        <v>64.16676470588236</v>
+      </c>
+      <c r="X32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="n">
+        <v>161.2823529411765</v>
+      </c>
+      <c r="C33" t="n">
+        <v>64.96112347479303</v>
+      </c>
+      <c r="D33" t="n">
+        <v>76.94117647058823</v>
+      </c>
+      <c r="E33" t="n">
+        <v>162.7352941176471</v>
+      </c>
+      <c r="F33" t="n">
+        <v>66.49764270734632</v>
+      </c>
+      <c r="G33" t="n">
+        <v>78.11764705882354</v>
+      </c>
+      <c r="H33" t="n">
+        <v>162.0088235294118</v>
+      </c>
+      <c r="I33" t="n">
+        <v>65.72003154878985</v>
+      </c>
+      <c r="J33" t="n">
+        <v>77.52941176470587</v>
+      </c>
+      <c r="K33" t="n">
+        <v>71.62472165674785</v>
+      </c>
+      <c r="L33" t="n">
+        <v>1.452941176470603</v>
+      </c>
+      <c r="M33" t="n">
+        <v>46.59695976651698</v>
+      </c>
+      <c r="N33" t="n">
+        <v>2.114519087332646</v>
+      </c>
+      <c r="O33" t="n">
+        <v>11.80938021591602</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0</v>
+      </c>
+      <c r="R33" t="n">
+        <v>2230.583521959219</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0</v>
+      </c>
+      <c r="T33" t="n">
+        <v>2230.583521959219</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0</v>
+      </c>
+      <c r="V33" t="n">
+        <v>0</v>
+      </c>
+      <c r="W33" t="n">
+        <v>64.60264705882352</v>
+      </c>
+      <c r="X33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="n">
+        <v>162.7352941176471</v>
+      </c>
+      <c r="C34" t="n">
+        <v>66.49764270734632</v>
+      </c>
+      <c r="D34" t="n">
+        <v>78.11764705882354</v>
+      </c>
+      <c r="E34" t="n">
+        <v>164.1882352941176</v>
+      </c>
+      <c r="F34" t="n">
+        <v>68.11203362096626</v>
+      </c>
+      <c r="G34" t="n">
+        <v>79.29411764705883</v>
+      </c>
+      <c r="H34" t="n">
+        <v>163.4617647058824</v>
+      </c>
+      <c r="I34" t="n">
+        <v>67.2947065541191</v>
+      </c>
+      <c r="J34" t="n">
+        <v>78.70588235294117</v>
+      </c>
+      <c r="K34" t="n">
+        <v>73.00029445353013</v>
+      </c>
+      <c r="L34" t="n">
+        <v>1.452941176470574</v>
+      </c>
+      <c r="M34" t="n">
+        <v>48.00803761833639</v>
+      </c>
+      <c r="N34" t="n">
+        <v>2.171724892562904</v>
+      </c>
+      <c r="O34" t="n">
+        <v>11.41117579882207</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0</v>
+      </c>
+      <c r="R34" t="n">
+        <v>2155.369734706901</v>
+      </c>
+      <c r="S34" t="n">
+        <v>0</v>
+      </c>
+      <c r="T34" t="n">
+        <v>2155.369734706901</v>
+      </c>
+      <c r="U34" t="n">
+        <v>0</v>
+      </c>
+      <c r="V34" t="n">
+        <v>0</v>
+      </c>
+      <c r="W34" t="n">
+        <v>65.03852941176471</v>
+      </c>
+      <c r="X34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB34" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="n">
+        <v>164.1882352941176</v>
+      </c>
+      <c r="C35" t="n">
+        <v>68.11203362096626</v>
+      </c>
+      <c r="D35" t="n">
+        <v>79.29411764705883</v>
+      </c>
+      <c r="E35" t="n">
+        <v>165.6411764705882</v>
+      </c>
+      <c r="F35" t="n">
+        <v>69.81106817304104</v>
+      </c>
+      <c r="G35" t="n">
+        <v>80.4705882352941</v>
+      </c>
+      <c r="H35" t="n">
+        <v>164.9147058823529</v>
+      </c>
+      <c r="I35" t="n">
+        <v>68.95050251248941</v>
+      </c>
+      <c r="J35" t="n">
+        <v>79.88235294117646</v>
+      </c>
+      <c r="K35" t="n">
+        <v>74.41642772683294</v>
+      </c>
+      <c r="L35" t="n">
+        <v>1.452941176470574</v>
+      </c>
+      <c r="M35" t="n">
+        <v>49.45883465850059</v>
+      </c>
+      <c r="N35" t="n">
+        <v>2.235314028783751</v>
+      </c>
+      <c r="O35" t="n">
+        <v>10.93185042868706</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0</v>
+      </c>
+      <c r="R35" t="n">
+        <v>2064.8336309714</v>
+      </c>
+      <c r="S35" t="n">
+        <v>0</v>
+      </c>
+      <c r="T35" t="n">
+        <v>2064.8336309714</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0</v>
+      </c>
+      <c r="V35" t="n">
+        <v>0</v>
+      </c>
+      <c r="W35" t="n">
+        <v>65.47441176470588</v>
+      </c>
+      <c r="X35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB35" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="n">
+        <v>165.6411764705882</v>
+      </c>
+      <c r="C36" t="n">
+        <v>69.81106817304104</v>
+      </c>
+      <c r="D36" t="n">
+        <v>80.4705882352941</v>
+      </c>
+      <c r="E36" t="n">
+        <v>167.0941176470588</v>
+      </c>
+      <c r="F36" t="n">
+        <v>71.60275058215227</v>
+      </c>
+      <c r="G36" t="n">
+        <v>81.64705882352941</v>
+      </c>
+      <c r="H36" t="n">
+        <v>166.3676470588235</v>
+      </c>
+      <c r="I36" t="n">
+        <v>70.69477150002697</v>
+      </c>
+      <c r="J36" t="n">
+        <v>81.05882352941177</v>
+      </c>
+      <c r="K36" t="n">
+        <v>75.87679751471937</v>
+      </c>
+      <c r="L36" t="n">
+        <v>1.452941176470603</v>
+      </c>
+      <c r="M36" t="n">
+        <v>50.95392487570476</v>
+      </c>
+      <c r="N36" t="n">
+        <v>2.306456683259107</v>
+      </c>
+      <c r="O36" t="n">
+        <v>10.36405202938479</v>
+      </c>
+      <c r="P36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>0</v>
+      </c>
+      <c r="R36" t="n">
+        <v>1957.586533314994</v>
+      </c>
+      <c r="S36" t="n">
+        <v>0</v>
+      </c>
+      <c r="T36" t="n">
+        <v>1957.586533314994</v>
+      </c>
+      <c r="U36" t="n">
+        <v>0</v>
+      </c>
+      <c r="V36" t="n">
+        <v>0</v>
+      </c>
+      <c r="W36" t="n">
+        <v>65.91029411764706</v>
+      </c>
+      <c r="X36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA36" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB36" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="n">
+        <v>167.0941176470588</v>
+      </c>
+      <c r="C37" t="n">
+        <v>71.60275058215227</v>
+      </c>
+      <c r="D37" t="n">
+        <v>81.64705882352941</v>
+      </c>
+      <c r="E37" t="n">
+        <v>168.5470588235294</v>
+      </c>
+      <c r="F37" t="n">
+        <v>73.49665601649136</v>
+      </c>
+      <c r="G37" t="n">
+        <v>82.82352941176472</v>
+      </c>
+      <c r="H37" t="n">
+        <v>167.8205882352941</v>
+      </c>
+      <c r="I37" t="n">
+        <v>72.53625391219026</v>
+      </c>
+      <c r="J37" t="n">
+        <v>82.23529411764706</v>
+      </c>
+      <c r="K37" t="n">
+        <v>77.38577401491867</v>
+      </c>
+      <c r="L37" t="n">
+        <v>1.452941176470603</v>
+      </c>
+      <c r="M37" t="n">
+        <v>52.49875468800307</v>
+      </c>
+      <c r="N37" t="n">
+        <v>2.386649274574875</v>
+      </c>
+      <c r="O37" t="n">
+        <v>9.699040205456797</v>
+      </c>
+      <c r="P37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>0</v>
+      </c>
+      <c r="R37" t="n">
+        <v>1831.977535277769</v>
+      </c>
+      <c r="S37" t="n">
+        <v>0</v>
+      </c>
+      <c r="T37" t="n">
+        <v>1831.977535277769</v>
+      </c>
+      <c r="U37" t="n">
+        <v>0</v>
+      </c>
+      <c r="V37" t="n">
+        <v>0</v>
+      </c>
+      <c r="W37" t="n">
+        <v>66.34617647058823</v>
+      </c>
+      <c r="X37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA37" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB37" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="n">
+        <v>168.5470588235294</v>
+      </c>
+      <c r="C38" t="n">
+        <v>73.49665601649136</v>
+      </c>
+      <c r="D38" t="n">
+        <v>82.82352941176472</v>
+      </c>
+      <c r="E38" t="n">
+        <v>170</v>
+      </c>
+      <c r="F38" t="n">
+        <v>75.50440019361704</v>
+      </c>
+      <c r="G38" t="n">
+        <v>84</v>
+      </c>
+      <c r="H38" t="n">
+        <v>169.2735294117647</v>
+      </c>
+      <c r="I38" t="n">
+        <v>74.4854760656425</v>
+      </c>
+      <c r="J38" t="n">
+        <v>83.41176470588236</v>
+      </c>
+      <c r="K38" t="n">
+        <v>78.94862038576244</v>
+      </c>
+      <c r="L38" t="n">
+        <v>1.452941176470574</v>
+      </c>
+      <c r="M38" t="n">
+        <v>54.09989672493607</v>
+      </c>
+      <c r="N38" t="n">
+        <v>2.477841156573934</v>
+      </c>
+      <c r="O38" t="n">
+        <v>8.926288640239861</v>
+      </c>
+      <c r="P38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>0</v>
+      </c>
+      <c r="R38" t="n">
+        <v>1686.018401400583</v>
+      </c>
+      <c r="S38" t="n">
+        <v>0</v>
+      </c>
+      <c r="T38" t="n">
+        <v>1686.018401400583</v>
+      </c>
+      <c r="U38" t="n">
+        <v>0</v>
+      </c>
+      <c r="V38" t="n">
+        <v>0</v>
+      </c>
+      <c r="W38" t="n">
+        <v>66.78205882352941</v>
+      </c>
+      <c r="X38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z38" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA38" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB38" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="n">
+        <v>170</v>
+      </c>
+      <c r="C39" t="n">
+        <v>75.50440019361704</v>
+      </c>
+      <c r="D39" t="n">
+        <v>84</v>
+      </c>
+      <c r="E39" t="n">
+        <v>171.3132629073484</v>
+      </c>
+      <c r="F39" t="n">
+        <v>77.42894111287163</v>
+      </c>
+      <c r="G39" t="n">
+        <v>84</v>
+      </c>
+      <c r="H39" t="n">
+        <v>170.6566314536742</v>
+      </c>
+      <c r="I39" t="n">
+        <v>76.452833760442</v>
+      </c>
+      <c r="J39" t="n">
+        <v>84</v>
+      </c>
+      <c r="K39" t="n">
+        <v>80.226416880221</v>
+      </c>
+      <c r="L39" t="n">
+        <v>1.313262907348445</v>
+      </c>
+      <c r="M39" t="n">
+        <v>55.68373714062625</v>
+      </c>
+      <c r="N39" t="n">
+        <v>2.329469504482719</v>
+      </c>
+      <c r="O39" t="n">
+        <v>7.547166239557995</v>
+      </c>
+      <c r="P39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>0</v>
+      </c>
+      <c r="R39" t="n">
+        <v>1288.483752140515</v>
+      </c>
+      <c r="S39" t="n">
+        <v>0</v>
+      </c>
+      <c r="T39" t="n">
+        <v>1288.483752140515</v>
+      </c>
+      <c r="U39" t="n">
+        <v>0</v>
+      </c>
+      <c r="V39" t="n">
+        <v>0</v>
+      </c>
+      <c r="W39" t="n">
+        <v>67.19698943610226</v>
+      </c>
+      <c r="X39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z39" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA39" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB39" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="n">
+        <v>171.3132629073484</v>
+      </c>
+      <c r="C40" t="n">
+        <v>77.42894111287163</v>
+      </c>
+      <c r="D40" t="n">
+        <v>84</v>
+      </c>
+      <c r="E40" t="n">
         <v>172.6265258146969</v>
       </c>
-      <c r="C21" t="n">
+      <c r="F40" t="n">
         <v>79.47126890591167</v>
       </c>
-      <c r="D21" t="n">
+      <c r="G40" t="n">
         <v>84</v>
       </c>
-      <c r="E21" t="n">
+      <c r="H40" t="n">
+        <v>171.9698943610227</v>
+      </c>
+      <c r="I40" t="n">
+        <v>78.43444402541515</v>
+      </c>
+      <c r="J40" t="n">
+        <v>84</v>
+      </c>
+      <c r="K40" t="n">
+        <v>81.21722201270757</v>
+      </c>
+      <c r="L40" t="n">
+        <v>1.313262907348445</v>
+      </c>
+      <c r="M40" t="n">
+        <v>57.24939360874781</v>
+      </c>
+      <c r="N40" t="n">
+        <v>2.427547636618971</v>
+      </c>
+      <c r="O40" t="n">
+        <v>5.565555974584854</v>
+      </c>
+      <c r="P40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>0</v>
+      </c>
+      <c r="R40" t="n">
+        <v>950.1749686251959</v>
+      </c>
+      <c r="S40" t="n">
+        <v>0</v>
+      </c>
+      <c r="T40" t="n">
+        <v>950.1749686251959</v>
+      </c>
+      <c r="U40" t="n">
+        <v>0</v>
+      </c>
+      <c r="V40" t="n">
+        <v>0</v>
+      </c>
+      <c r="W40" t="n">
+        <v>67.5909683083068</v>
+      </c>
+      <c r="X40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z40" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA40" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB40" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="n">
+        <v>172.6265258146969</v>
+      </c>
+      <c r="C41" t="n">
+        <v>79.47126890591167</v>
+      </c>
+      <c r="D41" t="n">
+        <v>84</v>
+      </c>
+      <c r="E41" t="n">
+        <v>173.9397887220453</v>
+      </c>
+      <c r="F41" t="n">
+        <v>81.64783755837817</v>
+      </c>
+      <c r="G41" t="n">
+        <v>84</v>
+      </c>
+      <c r="H41" t="n">
+        <v>173.2831572683711</v>
+      </c>
+      <c r="I41" t="n">
+        <v>80.54158273098243</v>
+      </c>
+      <c r="J41" t="n">
+        <v>84</v>
+      </c>
+      <c r="K41" t="n">
+        <v>82.27079136549122</v>
+      </c>
+      <c r="L41" t="n">
+        <v>1.313262907348445</v>
+      </c>
+      <c r="M41" t="n">
+        <v>58.88460511817222</v>
+      </c>
+      <c r="N41" t="n">
+        <v>2.541323463701519</v>
+      </c>
+      <c r="O41" t="n">
+        <v>3.458417269017573</v>
+      </c>
+      <c r="P41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>0</v>
+      </c>
+      <c r="R41" t="n">
+        <v>590.4354452794314</v>
+      </c>
+      <c r="S41" t="n">
+        <v>0</v>
+      </c>
+      <c r="T41" t="n">
+        <v>590.4354452794314</v>
+      </c>
+      <c r="U41" t="n">
+        <v>0</v>
+      </c>
+      <c r="V41" t="n">
+        <v>0</v>
+      </c>
+      <c r="W41" t="n">
+        <v>67.98494718051133</v>
+      </c>
+      <c r="X41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z41" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA41" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB41" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="n">
+        <v>173.9397887220453</v>
+      </c>
+      <c r="C42" t="n">
+        <v>81.64783755837817</v>
+      </c>
+      <c r="D42" t="n">
+        <v>84</v>
+      </c>
+      <c r="E42" t="n">
         <v>175.2530516293938</v>
       </c>
-      <c r="F21" t="n">
+      <c r="F42" t="n">
         <v>83.97975317326198</v>
       </c>
-      <c r="G21" t="n">
+      <c r="G42" t="n">
         <v>84</v>
       </c>
-      <c r="H21" t="n">
-        <v>173.9397887220453</v>
-      </c>
-      <c r="I21" t="n">
-        <v>81.64783755837817</v>
-      </c>
-      <c r="J21" t="n">
+      <c r="H42" t="n">
+        <v>174.5964201757196</v>
+      </c>
+      <c r="I42" t="n">
+        <v>82.79282626366185</v>
+      </c>
+      <c r="J42" t="n">
         <v>84</v>
       </c>
-      <c r="K21" t="n">
-        <v>82.82391877918909</v>
-      </c>
-      <c r="L21" t="n">
-        <v>2.62652581469689</v>
-      </c>
-      <c r="M21" t="n">
-        <v>59.73183603755096</v>
-      </c>
-      <c r="N21" t="n">
-        <v>5.210866479545521</v>
-      </c>
-      <c r="O21" t="n">
-        <v>2.352162441621829</v>
-      </c>
-      <c r="P21" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q21" t="n">
-        <v>0</v>
-      </c>
-      <c r="R21" t="n">
-        <v>803.1419985264261</v>
-      </c>
-      <c r="S21" t="n">
-        <v>0</v>
-      </c>
-      <c r="T21" t="n">
-        <v>803.1419985264261</v>
-      </c>
-      <c r="U21" t="n">
-        <v>0</v>
-      </c>
-      <c r="V21" t="n">
-        <v>0</v>
-      </c>
-      <c r="W21" t="n">
-        <v>68.1819366166136</v>
-      </c>
-      <c r="X21" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y21" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z21" t="n">
+      <c r="K42" t="n">
+        <v>83.39641313183093</v>
+      </c>
+      <c r="L42" t="n">
+        <v>1.313262907348445</v>
+      </c>
+      <c r="M42" t="n">
+        <v>60.60110101066249</v>
+      </c>
+      <c r="N42" t="n">
+        <v>2.675285503802047</v>
+      </c>
+      <c r="O42" t="n">
+        <v>1.207173736338149</v>
+      </c>
+      <c r="P42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>0</v>
+      </c>
+      <c r="R42" t="n">
+        <v>206.0937437855559</v>
+      </c>
+      <c r="S42" t="n">
+        <v>0</v>
+      </c>
+      <c r="T42" t="n">
+        <v>206.0937437855559</v>
+      </c>
+      <c r="U42" t="n">
+        <v>0</v>
+      </c>
+      <c r="V42" t="n">
+        <v>0</v>
+      </c>
+      <c r="W42" t="n">
+        <v>68.37892605271587</v>
+      </c>
+      <c r="X42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z42" t="n">
         <v>1</v>
       </c>
-      <c r="AA21" t="n">
+      <c r="AA42" t="n">
         <v>28</v>
       </c>
-      <c r="AB21" t="n">
+      <c r="AB42" t="n">
         <v>200</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates slice.py to include dload, kw, T, and P in the slice df in order to enable complete formulations.
</commit_message>
<xml_diff>
--- a/slices.xlsx
+++ b/slices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE21"/>
+  <dimension ref="A1:AK21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,70 +521,100 @@
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>w_s</t>
+          <t>w</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>dload</t>
+          <t>qL</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>w</t>
+          <t>qR</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>d_x</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>d_y</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>kw</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>y_t</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>beta</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>p</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
           <t>n_eff</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>z</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>theta</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>shear_reinf</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>normal_reinf</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>piezo_y</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>hw</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>u</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>mat</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>phi</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>c</t>
         </is>
@@ -649,16 +679,16 @@
         <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>6976.910679550587</v>
+        <v>0</v>
       </c>
       <c r="U2" t="n">
         <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>0</v>
+        <v>60.56948986259904</v>
       </c>
       <c r="W2" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="X2" t="n">
         <v>0</v>
@@ -667,21 +697,39 @@
         <v>0</v>
       </c>
       <c r="Z2" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>40</v>
+      </c>
+      <c r="AG2" t="n">
         <v>5.273025969167023</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="AH2" t="n">
         <v>329.0368204760222</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AI2" t="n">
         <v>3</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="AJ2" t="n">
         <v>27</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="AK2" t="n">
         <v>400</v>
       </c>
     </row>
@@ -744,16 +792,16 @@
         <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>18718.16443016667</v>
+        <v>0</v>
       </c>
       <c r="U3" t="n">
         <v>0</v>
       </c>
       <c r="V3" t="n">
-        <v>0</v>
+        <v>70.59321897849011</v>
       </c>
       <c r="W3" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="X3" t="n">
         <v>0</v>
@@ -762,21 +810,39 @@
         <v>0</v>
       </c>
       <c r="Z3" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AA3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>40</v>
+      </c>
+      <c r="AG3" t="n">
         <v>14.14685835447233</v>
       </c>
-      <c r="AB3" t="n">
+      <c r="AH3" t="n">
         <v>882.7639613190732</v>
       </c>
-      <c r="AC3" t="n">
+      <c r="AI3" t="n">
         <v>3</v>
       </c>
-      <c r="AD3" t="n">
+      <c r="AJ3" t="n">
         <v>27</v>
       </c>
-      <c r="AE3" t="n">
+      <c r="AK3" t="n">
         <v>400</v>
       </c>
     </row>
@@ -839,16 +905,16 @@
         <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>28137.86010431374</v>
+        <v>0</v>
       </c>
       <c r="U4" t="n">
         <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>0</v>
+        <v>80.6169480943812</v>
       </c>
       <c r="W4" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="X4" t="n">
         <v>0</v>
@@ -857,21 +923,39 @@
         <v>0</v>
       </c>
       <c r="Z4" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AA4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>40</v>
+      </c>
+      <c r="AG4" t="n">
         <v>21.26609811441534</v>
       </c>
-      <c r="AB4" t="n">
+      <c r="AH4" t="n">
         <v>1327.004522339517</v>
       </c>
-      <c r="AC4" t="n">
+      <c r="AI4" t="n">
         <v>3</v>
       </c>
-      <c r="AD4" t="n">
+      <c r="AJ4" t="n">
         <v>27</v>
       </c>
-      <c r="AE4" t="n">
+      <c r="AK4" t="n">
         <v>400</v>
       </c>
     </row>
@@ -934,16 +1018,16 @@
         <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>35700.23289621456</v>
+        <v>0</v>
       </c>
       <c r="U5" t="n">
         <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>0</v>
+        <v>90.64067721027229</v>
       </c>
       <c r="W5" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="X5" t="n">
         <v>0</v>
@@ -952,21 +1036,39 @@
         <v>0</v>
       </c>
       <c r="Z5" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AA5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AG5" t="n">
         <v>26.98160601637176</v>
       </c>
-      <c r="AB5" t="n">
+      <c r="AH5" t="n">
         <v>1683.652215421597</v>
       </c>
-      <c r="AC5" t="n">
+      <c r="AI5" t="n">
         <v>3</v>
       </c>
-      <c r="AD5" t="n">
+      <c r="AJ5" t="n">
         <v>27</v>
       </c>
-      <c r="AE5" t="n">
+      <c r="AK5" t="n">
         <v>400</v>
       </c>
     </row>
@@ -1029,16 +1131,16 @@
         <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>41691.15558417432</v>
+        <v>0</v>
       </c>
       <c r="U6" t="n">
         <v>0</v>
       </c>
       <c r="V6" t="n">
-        <v>0</v>
+        <v>100.6644063261634</v>
       </c>
       <c r="W6" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="X6" t="n">
         <v>0</v>
@@ -1047,21 +1149,39 @@
         <v>0</v>
       </c>
       <c r="Z6" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AA6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>40</v>
+      </c>
+      <c r="AG6" t="n">
         <v>31.5094396613509</v>
       </c>
-      <c r="AB6" t="n">
+      <c r="AH6" t="n">
         <v>1966.189034868296</v>
       </c>
-      <c r="AC6" t="n">
+      <c r="AI6" t="n">
         <v>3</v>
       </c>
-      <c r="AD6" t="n">
+      <c r="AJ6" t="n">
         <v>27</v>
       </c>
-      <c r="AE6" t="n">
+      <c r="AK6" t="n">
         <v>400</v>
       </c>
     </row>
@@ -1124,16 +1244,16 @@
         <v>0</v>
       </c>
       <c r="T7" t="n">
-        <v>46296.37332020365</v>
+        <v>0</v>
       </c>
       <c r="U7" t="n">
         <v>0</v>
       </c>
       <c r="V7" t="n">
-        <v>0</v>
+        <v>110.6881354420544</v>
       </c>
       <c r="W7" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="X7" t="n">
         <v>0</v>
@@ -1142,21 +1262,39 @@
         <v>0</v>
       </c>
       <c r="Z7" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AA7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>40</v>
+      </c>
+      <c r="AG7" t="n">
         <v>34.98998195737401</v>
       </c>
-      <c r="AB7" t="n">
+      <c r="AH7" t="n">
         <v>2183.374874140138</v>
       </c>
-      <c r="AC7" t="n">
+      <c r="AI7" t="n">
         <v>3</v>
       </c>
-      <c r="AD7" t="n">
+      <c r="AJ7" t="n">
         <v>27</v>
       </c>
-      <c r="AE7" t="n">
+      <c r="AK7" t="n">
         <v>400</v>
       </c>
     </row>
@@ -1219,16 +1357,16 @@
         <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>53576.08621085047</v>
+        <v>0</v>
       </c>
       <c r="U8" t="n">
         <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>0</v>
+        <v>120.6333333333333</v>
       </c>
       <c r="W8" t="n">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="X8" t="n">
         <v>0</v>
@@ -1237,21 +1375,39 @@
         <v>0</v>
       </c>
       <c r="Z8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>39.03551289874686</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF8" t="n">
         <v>44</v>
       </c>
-      <c r="AA8" t="n">
+      <c r="AG8" t="n">
         <v>41.50006619383478</v>
       </c>
-      <c r="AB8" t="n">
+      <c r="AH8" t="n">
         <v>2589.604130495291</v>
       </c>
-      <c r="AC8" t="n">
+      <c r="AI8" t="n">
         <v>2</v>
       </c>
-      <c r="AD8" t="n">
+      <c r="AJ8" t="n">
         <v>32</v>
       </c>
-      <c r="AE8" t="n">
+      <c r="AK8" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1314,16 +1470,16 @@
         <v>0</v>
       </c>
       <c r="T9" t="n">
-        <v>65158.84795942099</v>
+        <v>0</v>
       </c>
       <c r="U9" t="n">
         <v>0</v>
       </c>
       <c r="V9" t="n">
-        <v>0</v>
+        <v>130.5</v>
       </c>
       <c r="W9" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="X9" t="n">
         <v>0</v>
@@ -1332,21 +1488,39 @@
         <v>0</v>
       </c>
       <c r="Z9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>39.03551289874686</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF9" t="n">
         <v>52</v>
       </c>
-      <c r="AA9" t="n">
+      <c r="AG9" t="n">
         <v>51.12073706957996</v>
       </c>
-      <c r="AB9" t="n">
+      <c r="AH9" t="n">
         <v>3189.933993141789</v>
       </c>
-      <c r="AC9" t="n">
+      <c r="AI9" t="n">
         <v>2</v>
       </c>
-      <c r="AD9" t="n">
+      <c r="AJ9" t="n">
         <v>32</v>
       </c>
-      <c r="AE9" t="n">
+      <c r="AK9" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1409,16 +1583,16 @@
         <v>0</v>
       </c>
       <c r="T10" t="n">
-        <v>75659.45807402786</v>
+        <v>0</v>
       </c>
       <c r="U10" t="n">
         <v>0</v>
       </c>
       <c r="V10" t="n">
-        <v>0</v>
+        <v>140.3666666666667</v>
       </c>
       <c r="W10" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="X10" t="n">
         <v>0</v>
@@ -1427,21 +1601,39 @@
         <v>0</v>
       </c>
       <c r="Z10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>39.03551289874686</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF10" t="n">
         <v>56.55384615384616</v>
       </c>
-      <c r="AA10" t="n">
+      <c r="AG10" t="n">
         <v>56.4643637168282</v>
       </c>
-      <c r="AB10" t="n">
+      <c r="AH10" t="n">
         <v>3523.376295930079</v>
       </c>
-      <c r="AC10" t="n">
+      <c r="AI10" t="n">
         <v>2</v>
       </c>
-      <c r="AD10" t="n">
+      <c r="AJ10" t="n">
         <v>32</v>
       </c>
-      <c r="AE10" t="n">
+      <c r="AK10" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1504,16 +1696,16 @@
         <v>0</v>
       </c>
       <c r="T11" t="n">
-        <v>108518.5126056569</v>
+        <v>0</v>
       </c>
       <c r="U11" t="n">
         <v>0</v>
       </c>
       <c r="V11" t="n">
-        <v>0</v>
+        <v>151.475</v>
       </c>
       <c r="W11" t="n">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="X11" t="n">
         <v>0</v>
@@ -1522,21 +1714,39 @@
         <v>0</v>
       </c>
       <c r="Z11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>38.99766642858376</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF11" t="n">
         <v>61.44250000000001</v>
       </c>
-      <c r="AA11" t="n">
+      <c r="AG11" t="n">
         <v>61.26768255775788</v>
       </c>
-      <c r="AB11" t="n">
+      <c r="AH11" t="n">
         <v>3823.103391604091</v>
       </c>
-      <c r="AC11" t="n">
+      <c r="AI11" t="n">
         <v>1</v>
       </c>
-      <c r="AD11" t="n">
+      <c r="AJ11" t="n">
         <v>28</v>
       </c>
-      <c r="AE11" t="n">
+      <c r="AK11" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1599,16 +1809,16 @@
         <v>0</v>
       </c>
       <c r="T12" t="n">
-        <v>122436.3747918735</v>
+        <v>0</v>
       </c>
       <c r="U12" t="n">
         <v>0</v>
       </c>
       <c r="V12" t="n">
-        <v>0</v>
+        <v>163.825</v>
       </c>
       <c r="W12" t="n">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="X12" t="n">
         <v>0</v>
@@ -1617,21 +1827,39 @@
         <v>0</v>
       </c>
       <c r="Z12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>38.99766642858376</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF12" t="n">
         <v>65.14749999999999</v>
       </c>
-      <c r="AA12" t="n">
+      <c r="AG12" t="n">
         <v>63.66171591944149</v>
       </c>
-      <c r="AB12" t="n">
+      <c r="AH12" t="n">
         <v>3972.491073373149</v>
       </c>
-      <c r="AC12" t="n">
+      <c r="AI12" t="n">
         <v>1</v>
       </c>
-      <c r="AD12" t="n">
+      <c r="AJ12" t="n">
         <v>28</v>
       </c>
-      <c r="AE12" t="n">
+      <c r="AK12" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1694,16 +1922,16 @@
         <v>0</v>
       </c>
       <c r="T13" t="n">
-        <v>101962.1203276141</v>
+        <v>0</v>
       </c>
       <c r="U13" t="n">
         <v>0</v>
       </c>
       <c r="V13" t="n">
-        <v>0</v>
+        <v>174.969863351536</v>
       </c>
       <c r="W13" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="X13" t="n">
         <v>0</v>
@@ -1712,21 +1940,39 @@
         <v>0</v>
       </c>
       <c r="Z13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF13" t="n">
         <v>68.49095900546081</v>
       </c>
-      <c r="AA13" t="n">
+      <c r="AG13" t="n">
         <v>64.68823647223391</v>
       </c>
-      <c r="AB13" t="n">
+      <c r="AH13" t="n">
         <v>4036.545955867396</v>
       </c>
-      <c r="AC13" t="n">
+      <c r="AI13" t="n">
         <v>1</v>
       </c>
-      <c r="AD13" t="n">
+      <c r="AJ13" t="n">
         <v>28</v>
       </c>
-      <c r="AE13" t="n">
+      <c r="AK13" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1789,16 +2035,16 @@
         <v>0</v>
       </c>
       <c r="T14" t="n">
-        <v>97988.89922008957</v>
+        <v>0</v>
       </c>
       <c r="U14" t="n">
         <v>0</v>
       </c>
       <c r="V14" t="n">
-        <v>0</v>
+        <v>184.9095900546081</v>
       </c>
       <c r="W14" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="X14" t="n">
         <v>0</v>
@@ -1807,21 +2053,39 @@
         <v>0</v>
       </c>
       <c r="Z14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF14" t="n">
         <v>71.05205501170174</v>
       </c>
-      <c r="AA14" t="n">
+      <c r="AG14" t="n">
         <v>64.22106411610774</v>
       </c>
-      <c r="AB14" t="n">
+      <c r="AH14" t="n">
         <v>4007.394400845123</v>
       </c>
-      <c r="AC14" t="n">
+      <c r="AI14" t="n">
         <v>1</v>
       </c>
-      <c r="AD14" t="n">
+      <c r="AJ14" t="n">
         <v>28</v>
       </c>
-      <c r="AE14" t="n">
+      <c r="AK14" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1884,16 +2148,16 @@
         <v>0</v>
       </c>
       <c r="T15" t="n">
-        <v>92723.7348333438</v>
+        <v>0</v>
       </c>
       <c r="U15" t="n">
         <v>0</v>
       </c>
       <c r="V15" t="n">
-        <v>0</v>
+        <v>194.8493167576802</v>
       </c>
       <c r="W15" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="X15" t="n">
         <v>0</v>
@@ -1902,21 +2166,39 @@
         <v>0</v>
       </c>
       <c r="Z15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF15" t="n">
         <v>73.18199644807433</v>
       </c>
-      <c r="AA15" t="n">
+      <c r="AG15" t="n">
         <v>62.33805729121976</v>
       </c>
-      <c r="AB15" t="n">
+      <c r="AH15" t="n">
         <v>3889.894774972113</v>
       </c>
-      <c r="AC15" t="n">
+      <c r="AI15" t="n">
         <v>1</v>
       </c>
-      <c r="AD15" t="n">
+      <c r="AJ15" t="n">
         <v>28</v>
       </c>
-      <c r="AE15" t="n">
+      <c r="AK15" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1979,16 +2261,16 @@
         <v>0</v>
       </c>
       <c r="T16" t="n">
-        <v>86017.22004816629</v>
+        <v>0</v>
       </c>
       <c r="U16" t="n">
         <v>0</v>
       </c>
       <c r="V16" t="n">
-        <v>0</v>
+        <v>204.7890434607522</v>
       </c>
       <c r="W16" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="X16" t="n">
         <v>0</v>
@@ -1997,21 +2279,39 @@
         <v>0</v>
       </c>
       <c r="Z16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF16" t="n">
         <v>75.31193788444691</v>
       </c>
-      <c r="AA16" t="n">
+      <c r="AG16" t="n">
         <v>59.35649700239541</v>
       </c>
-      <c r="AB16" t="n">
+      <c r="AH16" t="n">
         <v>3703.845412949474</v>
       </c>
-      <c r="AC16" t="n">
+      <c r="AI16" t="n">
         <v>1</v>
       </c>
-      <c r="AD16" t="n">
+      <c r="AJ16" t="n">
         <v>28</v>
       </c>
-      <c r="AE16" t="n">
+      <c r="AK16" t="n">
         <v>200</v>
       </c>
     </row>
@@ -2074,16 +2374,16 @@
         <v>0</v>
       </c>
       <c r="T17" t="n">
-        <v>77643.23955338272</v>
+        <v>0</v>
       </c>
       <c r="U17" t="n">
         <v>0</v>
       </c>
       <c r="V17" t="n">
-        <v>0</v>
+        <v>214.7287701638243</v>
       </c>
       <c r="W17" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="X17" t="n">
         <v>0</v>
@@ -2092,21 +2392,39 @@
         <v>0</v>
       </c>
       <c r="Z17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF17" t="n">
         <v>76.545575959229</v>
       </c>
-      <c r="AA17" t="n">
+      <c r="AG17" t="n">
         <v>54.20774167062702</v>
       </c>
-      <c r="AB17" t="n">
+      <c r="AH17" t="n">
         <v>3382.563080247126</v>
       </c>
-      <c r="AC17" t="n">
+      <c r="AI17" t="n">
         <v>1</v>
       </c>
-      <c r="AD17" t="n">
+      <c r="AJ17" t="n">
         <v>28</v>
       </c>
-      <c r="AE17" t="n">
+      <c r="AK17" t="n">
         <v>200</v>
       </c>
     </row>
@@ -2169,16 +2487,16 @@
         <v>0</v>
       </c>
       <c r="T18" t="n">
-        <v>67246.54663088753</v>
+        <v>0</v>
       </c>
       <c r="U18" t="n">
         <v>0</v>
       </c>
       <c r="V18" t="n">
-        <v>0</v>
+        <v>224.6684968668964</v>
       </c>
       <c r="W18" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="X18" t="n">
         <v>0</v>
@@ -2187,21 +2505,39 @@
         <v>0</v>
       </c>
       <c r="Z18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF18" t="n">
         <v>77.35149974596457</v>
       </c>
-      <c r="AA18" t="n">
+      <c r="AG18" t="n">
         <v>47.08962211861802</v>
       </c>
-      <c r="AB18" t="n">
+      <c r="AH18" t="n">
         <v>2938.392420201765</v>
       </c>
-      <c r="AC18" t="n">
+      <c r="AI18" t="n">
         <v>1</v>
       </c>
-      <c r="AD18" t="n">
+      <c r="AJ18" t="n">
         <v>28</v>
       </c>
-      <c r="AE18" t="n">
+      <c r="AK18" t="n">
         <v>200</v>
       </c>
     </row>
@@ -2264,16 +2600,16 @@
         <v>0</v>
       </c>
       <c r="T19" t="n">
-        <v>54248.53262366771</v>
+        <v>0</v>
       </c>
       <c r="U19" t="n">
         <v>0</v>
       </c>
       <c r="V19" t="n">
-        <v>0</v>
+        <v>234.6082235699684</v>
       </c>
       <c r="W19" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="X19" t="n">
         <v>0</v>
@@ -2282,21 +2618,39 @@
         <v>0</v>
       </c>
       <c r="Z19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF19" t="n">
         <v>78.15742353270014</v>
       </c>
-      <c r="AA19" t="n">
+      <c r="AG19" t="n">
         <v>37.97199781982241</v>
       </c>
-      <c r="AB19" t="n">
+      <c r="AH19" t="n">
         <v>2369.452663956918</v>
       </c>
-      <c r="AC19" t="n">
+      <c r="AI19" t="n">
         <v>1</v>
       </c>
-      <c r="AD19" t="n">
+      <c r="AJ19" t="n">
         <v>28</v>
       </c>
-      <c r="AE19" t="n">
+      <c r="AK19" t="n">
         <v>200</v>
       </c>
     </row>
@@ -2359,16 +2713,16 @@
         <v>0</v>
       </c>
       <c r="T20" t="n">
-        <v>38974.45926823906</v>
+        <v>0</v>
       </c>
       <c r="U20" t="n">
         <v>0</v>
       </c>
       <c r="V20" t="n">
-        <v>0</v>
+        <v>244.5479502730405</v>
       </c>
       <c r="W20" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="X20" t="n">
         <v>0</v>
@@ -2377,21 +2731,39 @@
         <v>0</v>
       </c>
       <c r="Z20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF20" t="n">
         <v>78.96334731943571</v>
       </c>
-      <c r="AA20" t="n">
+      <c r="AG20" t="n">
         <v>25.97234370377396</v>
       </c>
-      <c r="AB20" t="n">
+      <c r="AH20" t="n">
         <v>1620.674247115495</v>
       </c>
-      <c r="AC20" t="n">
+      <c r="AI20" t="n">
         <v>1</v>
       </c>
-      <c r="AD20" t="n">
+      <c r="AJ20" t="n">
         <v>28</v>
       </c>
-      <c r="AE20" t="n">
+      <c r="AK20" t="n">
         <v>200</v>
       </c>
     </row>
@@ -2454,16 +2826,16 @@
         <v>0</v>
       </c>
       <c r="T21" t="n">
-        <v>16948.91230046818</v>
+        <v>0</v>
       </c>
       <c r="U21" t="n">
         <v>0</v>
       </c>
       <c r="V21" t="n">
-        <v>0</v>
+        <v>254.4876769761125</v>
       </c>
       <c r="W21" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="X21" t="n">
         <v>0</v>
@@ -2472,21 +2844,39 @@
         <v>0</v>
       </c>
       <c r="Z21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF21" t="n">
         <v>79.1265023596815</v>
       </c>
-      <c r="AA21" t="n">
+      <c r="AG21" t="n">
         <v>8.243185781655711</v>
       </c>
-      <c r="AB21" t="n">
+      <c r="AH21" t="n">
         <v>514.3747927753163</v>
       </c>
-      <c r="AC21" t="n">
+      <c r="AI21" t="n">
         <v>1</v>
       </c>
-      <c r="AD21" t="n">
+      <c r="AJ21" t="n">
         <v>28</v>
       </c>
-      <c r="AE21" t="n">
+      <c r="AK21" t="n">
         <v>200</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added figure to home page of documentation
</commit_message>
<xml_diff>
--- a/slices.xlsx
+++ b/slices.xlsx
@@ -697,7 +697,7 @@
         <v>0</v>
       </c>
       <c r="Z2" t="n">
-        <v>30.04068289318306</v>
+        <v>0</v>
       </c>
       <c r="AA2" t="n">
         <v>0</v>
@@ -810,7 +810,7 @@
         <v>0</v>
       </c>
       <c r="Z3" t="n">
-        <v>22.10032906584962</v>
+        <v>0</v>
       </c>
       <c r="AA3" t="n">
         <v>0</v>
@@ -923,7 +923,7 @@
         <v>0</v>
       </c>
       <c r="Z4" t="n">
-        <v>15.71643411866143</v>
+        <v>0</v>
       </c>
       <c r="AA4" t="n">
         <v>0</v>
@@ -1036,7 +1036,7 @@
         <v>0</v>
       </c>
       <c r="Z5" t="n">
-        <v>10.6161421138269</v>
+        <v>0</v>
       </c>
       <c r="AA5" t="n">
         <v>0</v>
@@ -1149,7 +1149,7 @@
         <v>0</v>
       </c>
       <c r="Z6" t="n">
-        <v>6.62608620842262</v>
+        <v>0</v>
       </c>
       <c r="AA6" t="n">
         <v>0</v>
@@ -1262,7 +1262,7 @@
         <v>0</v>
       </c>
       <c r="Z7" t="n">
-        <v>3.632006118520721</v>
+        <v>0</v>
       </c>
       <c r="AA7" t="n">
         <v>0</v>
@@ -1375,7 +1375,7 @@
         <v>0</v>
       </c>
       <c r="Z8" t="n">
-        <v>1.58401478028587</v>
+        <v>0</v>
       </c>
       <c r="AA8" t="n">
         <v>39.03551289874686</v>
@@ -1488,7 +1488,7 @@
         <v>0</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.3819458071278916</v>
+        <v>0</v>
       </c>
       <c r="AA9" t="n">
         <v>39.03551289874686</v>
@@ -1601,7 +1601,7 @@
         <v>0</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.000375000585933094</v>
+        <v>0</v>
       </c>
       <c r="AA10" t="n">
         <v>39.03551289874686</v>
@@ -1714,7 +1714,7 @@
         <v>0</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.6686231538410539</v>
+        <v>0</v>
       </c>
       <c r="AA11" t="n">
         <v>38.99766642858376</v>
@@ -1827,7 +1827,7 @@
         <v>0</v>
       </c>
       <c r="Z12" t="n">
-        <v>2.633054056944971</v>
+        <v>0</v>
       </c>
       <c r="AA12" t="n">
         <v>38.99766642858376</v>
@@ -1940,7 +1940,7 @@
         <v>0</v>
       </c>
       <c r="Z13" t="n">
-        <v>5.217597167510036</v>
+        <v>0</v>
       </c>
       <c r="AA13" t="n">
         <v>0</v>
@@ -2053,7 +2053,7 @@
         <v>0</v>
       </c>
       <c r="Z14" t="n">
-        <v>8.757022693565062</v>
+        <v>0</v>
       </c>
       <c r="AA14" t="n">
         <v>0</v>
@@ -2166,7 +2166,7 @@
         <v>0</v>
       </c>
       <c r="Z15" t="n">
-        <v>13.3463549614923</v>
+        <v>0</v>
       </c>
       <c r="AA15" t="n">
         <v>0</v>
@@ -2279,7 +2279,7 @@
         <v>0</v>
       </c>
       <c r="Z16" t="n">
-        <v>19.12879499083992</v>
+        <v>0</v>
       </c>
       <c r="AA16" t="n">
         <v>0</v>
@@ -2392,7 +2392,7 @@
         <v>0</v>
       </c>
       <c r="Z17" t="n">
-        <v>26.32503002402403</v>
+        <v>0</v>
       </c>
       <c r="AA17" t="n">
         <v>0</v>
@@ -2442,34 +2442,34 @@
         <v>84</v>
       </c>
       <c r="E18" t="n">
-        <v>228.9543811126312</v>
+        <v>229.8643850819121</v>
       </c>
       <c r="F18" t="n">
-        <v>34.258167199464</v>
+        <v>35.15875917533425</v>
       </c>
       <c r="G18" t="n">
         <v>84</v>
       </c>
       <c r="H18" t="n">
-        <v>224.4771905563156</v>
+        <v>224.9321925409561</v>
       </c>
       <c r="I18" t="n">
-        <v>30.09240198250708</v>
+        <v>30.49667829853728</v>
       </c>
       <c r="J18" t="n">
         <v>84</v>
       </c>
       <c r="K18" t="n">
-        <v>57.16039905094622</v>
+        <v>57.37328724188009</v>
       </c>
       <c r="L18" t="n">
-        <v>8.954381112631211</v>
+        <v>9.864385081912133</v>
       </c>
       <c r="M18" t="n">
-        <v>41.47627967182778</v>
+        <v>41.76689339905241</v>
       </c>
       <c r="N18" t="n">
-        <v>11.95144528831471</v>
+        <v>13.22550038612207</v>
       </c>
       <c r="O18" t="n">
         <v>20</v>
@@ -2478,10 +2478,10 @@
         <v>24</v>
       </c>
       <c r="Q18" t="n">
-        <v>9.907598017492916</v>
+        <v>9.503321701462724</v>
       </c>
       <c r="R18" t="n">
-        <v>60780.57442705733</v>
+        <v>66431.09432518722</v>
       </c>
       <c r="S18" t="n">
         <v>0</v>
@@ -2493,7 +2493,7 @@
         <v>0</v>
       </c>
       <c r="V18" t="n">
-        <v>224.4771905563156</v>
+        <v>224.9321925409561</v>
       </c>
       <c r="W18" t="n">
         <v>84</v>
@@ -2505,7 +2505,7 @@
         <v>0</v>
       </c>
       <c r="Z18" t="n">
-        <v>34.258167199464</v>
+        <v>0</v>
       </c>
       <c r="AA18" t="n">
         <v>0</v>
@@ -2523,13 +2523,13 @@
         <v>0</v>
       </c>
       <c r="AF18" t="n">
-        <v>77.33598842348505</v>
+        <v>77.37288047629373</v>
       </c>
       <c r="AG18" t="n">
-        <v>47.24358644097796</v>
+        <v>46.87620217775645</v>
       </c>
       <c r="AH18" t="n">
-        <v>2947.999793917025</v>
+        <v>2925.075015892003</v>
       </c>
       <c r="AI18" t="n">
         <v>1</v>
@@ -2546,55 +2546,55 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>228.9543811126312</v>
+        <v>229.8643850819121</v>
       </c>
       <c r="C19" t="n">
-        <v>34.258167199464</v>
+        <v>35.15875917533425</v>
       </c>
       <c r="D19" t="n">
         <v>84</v>
       </c>
       <c r="E19" t="n">
-        <v>237.9087622252624</v>
+        <v>239.7287701638243</v>
       </c>
       <c r="F19" t="n">
-        <v>44.05290063623465</v>
+        <v>46.33548952684643</v>
       </c>
       <c r="G19" t="n">
         <v>84</v>
       </c>
       <c r="H19" t="n">
-        <v>233.4315716689468</v>
+        <v>234.7965776228682</v>
       </c>
       <c r="I19" t="n">
-        <v>38.88368146815391</v>
+        <v>40.39739547464413</v>
       </c>
       <c r="J19" t="n">
         <v>84</v>
       </c>
       <c r="K19" t="n">
-        <v>61.8357956447819</v>
+        <v>62.63318313075887</v>
       </c>
       <c r="L19" t="n">
-        <v>8.954381112631239</v>
+        <v>9.864385081912161</v>
       </c>
       <c r="M19" t="n">
-        <v>47.47053161366336</v>
+        <v>48.44374871983539</v>
       </c>
       <c r="N19" t="n">
-        <v>13.24672720197736</v>
+        <v>14.87044587012606</v>
       </c>
       <c r="O19" t="n">
         <v>20</v>
       </c>
       <c r="P19" t="n">
-        <v>24</v>
+        <v>23.60260452535587</v>
       </c>
       <c r="Q19" t="n">
-        <v>1.11631853184609</v>
+        <v>0</v>
       </c>
       <c r="R19" t="n">
-        <v>50389.47278541525</v>
+        <v>53586.42280987477</v>
       </c>
       <c r="S19" t="n">
         <v>0</v>
@@ -2606,7 +2606,7 @@
         <v>0</v>
       </c>
       <c r="V19" t="n">
-        <v>233.4315716689468</v>
+        <v>234.7965776228682</v>
       </c>
       <c r="W19" t="n">
         <v>84</v>
@@ -2618,7 +2618,7 @@
         <v>0</v>
       </c>
       <c r="Z19" t="n">
-        <v>44.05290063623465</v>
+        <v>0</v>
       </c>
       <c r="AA19" t="n">
         <v>0</v>
@@ -2636,13 +2636,13 @@
         <v>0</v>
       </c>
       <c r="AF19" t="n">
-        <v>78.06201932450921</v>
+        <v>78.17269548293525</v>
       </c>
       <c r="AG19" t="n">
-        <v>39.1783378563553</v>
+        <v>37.77530000829113</v>
       </c>
       <c r="AH19" t="n">
-        <v>2444.728282236571</v>
+        <v>2357.178720517366</v>
       </c>
       <c r="AI19" t="n">
         <v>1</v>
@@ -2659,55 +2659,55 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>237.9087622252624</v>
+        <v>239.7287701638243</v>
       </c>
       <c r="C20" t="n">
-        <v>44.05290063623465</v>
+        <v>46.33548952684643</v>
       </c>
       <c r="D20" t="n">
         <v>84</v>
       </c>
       <c r="E20" t="n">
-        <v>246.8631433378937</v>
+        <v>249.5931552457365</v>
       </c>
       <c r="F20" t="n">
-        <v>56.56578187347365</v>
+        <v>61.175924352853</v>
       </c>
       <c r="G20" t="n">
         <v>84</v>
       </c>
       <c r="H20" t="n">
-        <v>242.3859527815781</v>
+        <v>244.6609627047804</v>
       </c>
       <c r="I20" t="n">
-        <v>49.88597714562194</v>
+        <v>53.15920023850424</v>
       </c>
       <c r="J20" t="n">
         <v>84</v>
       </c>
       <c r="K20" t="n">
-        <v>67.27170458889177</v>
+        <v>68.85750549896575</v>
       </c>
       <c r="L20" t="n">
-        <v>8.954381112631239</v>
+        <v>9.864385081912161</v>
       </c>
       <c r="M20" t="n">
-        <v>54.24761044425681</v>
+        <v>56.15096057258316</v>
       </c>
       <c r="N20" t="n">
-        <v>15.32540440350763</v>
+        <v>17.7096360831204</v>
       </c>
       <c r="O20" t="n">
         <v>20</v>
       </c>
       <c r="P20" t="n">
-        <v>14.11402285437806</v>
+        <v>10.84079976149576</v>
       </c>
       <c r="Q20" t="n">
         <v>0</v>
       </c>
       <c r="R20" t="n">
-        <v>38447.27165329985</v>
+        <v>38479.9400261671</v>
       </c>
       <c r="S20" t="n">
         <v>0</v>
@@ -2719,7 +2719,7 @@
         <v>0</v>
       </c>
       <c r="V20" t="n">
-        <v>242.3859527815781</v>
+        <v>244.6609627047804</v>
       </c>
       <c r="W20" t="n">
         <v>84</v>
@@ -2731,7 +2731,7 @@
         <v>0</v>
       </c>
       <c r="Z20" t="n">
-        <v>56.56578187347365</v>
+        <v>0</v>
       </c>
       <c r="AA20" t="n">
         <v>0</v>
@@ -2749,13 +2749,13 @@
         <v>0</v>
       </c>
       <c r="AF20" t="n">
-        <v>78.78805022553335</v>
+        <v>78.97251048957679</v>
       </c>
       <c r="AG20" t="n">
-        <v>28.90207307991142</v>
+        <v>25.81331025107255</v>
       </c>
       <c r="AH20" t="n">
-        <v>1803.489360186472</v>
+        <v>1610.750559666927</v>
       </c>
       <c r="AI20" t="n">
         <v>1</v>
@@ -2772,46 +2772,46 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>246.8631433378937</v>
+        <v>249.5931552457365</v>
       </c>
       <c r="C21" t="n">
-        <v>56.56578187347365</v>
+        <v>61.175924352853</v>
       </c>
       <c r="D21" t="n">
         <v>84</v>
       </c>
       <c r="E21" t="n">
-        <v>255.8175244505249</v>
+        <v>259.4575403276486</v>
       </c>
       <c r="F21" t="n">
-        <v>73.96222991219801</v>
+        <v>83.95181749179723</v>
       </c>
       <c r="G21" t="n">
         <v>84</v>
       </c>
       <c r="H21" t="n">
-        <v>251.3403338942093</v>
+        <v>254.5253477866925</v>
       </c>
       <c r="I21" t="n">
-        <v>64.39664230221271</v>
+        <v>70.96737624597222</v>
       </c>
       <c r="J21" t="n">
         <v>84</v>
       </c>
       <c r="K21" t="n">
-        <v>74.19832115110636</v>
+        <v>77.48368812298611</v>
       </c>
       <c r="L21" t="n">
-        <v>8.954381112631211</v>
+        <v>9.864385081912133</v>
       </c>
       <c r="M21" t="n">
-        <v>62.3957812014332</v>
+        <v>65.8827570725098</v>
       </c>
       <c r="N21" t="n">
-        <v>19.32483651285239</v>
+        <v>24.14160699618116</v>
       </c>
       <c r="O21" t="n">
-        <v>19.60335769778729</v>
+        <v>13.03262375402778</v>
       </c>
       <c r="P21" t="n">
         <v>0</v>
@@ -2820,7 +2820,7 @@
         <v>0</v>
       </c>
       <c r="R21" t="n">
-        <v>22819.67166871862</v>
+        <v>16712.6465138627</v>
       </c>
       <c r="S21" t="n">
         <v>0</v>
@@ -2832,7 +2832,7 @@
         <v>0</v>
       </c>
       <c r="V21" t="n">
-        <v>251.3403338942093</v>
+        <v>254.5253477866925</v>
       </c>
       <c r="W21" t="n">
         <v>84</v>
@@ -2841,10 +2841,10 @@
         <v>0</v>
       </c>
       <c r="Y21" t="n">
-        <v>3120</v>
+        <v>0</v>
       </c>
       <c r="Z21" t="n">
-        <v>77.29556324553134</v>
+        <v>0</v>
       </c>
       <c r="AA21" t="n">
         <v>0</v>
@@ -2862,13 +2862,13 @@
         <v>0</v>
       </c>
       <c r="AF21" t="n">
-        <v>79.08453778525612</v>
+        <v>79.12700463715591</v>
       </c>
       <c r="AG21" t="n">
-        <v>14.68789548304341</v>
+        <v>8.159628391183688</v>
       </c>
       <c r="AH21" t="n">
-        <v>916.5246781419085</v>
+        <v>509.1608116098621</v>
       </c>
       <c r="AI21" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Got rid of circle argument. Put circle variables in df.
</commit_message>
<xml_diff>
--- a/slices.xlsx
+++ b/slices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK21"/>
+  <dimension ref="A1:AN21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -619,6 +619,21 @@
           <t>c</t>
         </is>
       </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>xo</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>yo</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -732,6 +747,15 @@
       <c r="AK2" t="n">
         <v>400</v>
       </c>
+      <c r="AL2" t="n">
+        <v>120</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>145</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -845,6 +869,15 @@
       <c r="AK3" t="n">
         <v>400</v>
       </c>
+      <c r="AL3" t="n">
+        <v>120</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>145</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -958,6 +991,15 @@
       <c r="AK4" t="n">
         <v>400</v>
       </c>
+      <c r="AL4" t="n">
+        <v>120</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>145</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -1071,6 +1113,15 @@
       <c r="AK5" t="n">
         <v>400</v>
       </c>
+      <c r="AL5" t="n">
+        <v>120</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>145</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1184,6 +1235,15 @@
       <c r="AK6" t="n">
         <v>400</v>
       </c>
+      <c r="AL6" t="n">
+        <v>120</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>145</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1297,6 +1357,15 @@
       <c r="AK7" t="n">
         <v>400</v>
       </c>
+      <c r="AL7" t="n">
+        <v>120</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>145</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1410,6 +1479,15 @@
       <c r="AK8" t="n">
         <v>100</v>
       </c>
+      <c r="AL8" t="n">
+        <v>120</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>145</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1523,6 +1601,15 @@
       <c r="AK9" t="n">
         <v>100</v>
       </c>
+      <c r="AL9" t="n">
+        <v>120</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>145</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1636,6 +1723,15 @@
       <c r="AK10" t="n">
         <v>100</v>
       </c>
+      <c r="AL10" t="n">
+        <v>120</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>145</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1749,6 +1845,15 @@
       <c r="AK11" t="n">
         <v>200</v>
       </c>
+      <c r="AL11" t="n">
+        <v>120</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>145</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1862,6 +1967,15 @@
       <c r="AK12" t="n">
         <v>200</v>
       </c>
+      <c r="AL12" t="n">
+        <v>120</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>145</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1975,6 +2089,15 @@
       <c r="AK13" t="n">
         <v>200</v>
       </c>
+      <c r="AL13" t="n">
+        <v>120</v>
+      </c>
+      <c r="AM13" t="n">
+        <v>145</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -2088,6 +2211,15 @@
       <c r="AK14" t="n">
         <v>200</v>
       </c>
+      <c r="AL14" t="n">
+        <v>120</v>
+      </c>
+      <c r="AM14" t="n">
+        <v>145</v>
+      </c>
+      <c r="AN14" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -2201,6 +2333,15 @@
       <c r="AK15" t="n">
         <v>200</v>
       </c>
+      <c r="AL15" t="n">
+        <v>120</v>
+      </c>
+      <c r="AM15" t="n">
+        <v>145</v>
+      </c>
+      <c r="AN15" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -2314,6 +2455,15 @@
       <c r="AK16" t="n">
         <v>200</v>
       </c>
+      <c r="AL16" t="n">
+        <v>120</v>
+      </c>
+      <c r="AM16" t="n">
+        <v>145</v>
+      </c>
+      <c r="AN16" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -2427,6 +2577,15 @@
       <c r="AK17" t="n">
         <v>200</v>
       </c>
+      <c r="AL17" t="n">
+        <v>120</v>
+      </c>
+      <c r="AM17" t="n">
+        <v>145</v>
+      </c>
+      <c r="AN17" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -2540,6 +2699,15 @@
       <c r="AK18" t="n">
         <v>200</v>
       </c>
+      <c r="AL18" t="n">
+        <v>120</v>
+      </c>
+      <c r="AM18" t="n">
+        <v>145</v>
+      </c>
+      <c r="AN18" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -2653,6 +2821,15 @@
       <c r="AK19" t="n">
         <v>200</v>
       </c>
+      <c r="AL19" t="n">
+        <v>120</v>
+      </c>
+      <c r="AM19" t="n">
+        <v>145</v>
+      </c>
+      <c r="AN19" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -2766,6 +2943,15 @@
       <c r="AK20" t="n">
         <v>200</v>
       </c>
+      <c r="AL20" t="n">
+        <v>120</v>
+      </c>
+      <c r="AM20" t="n">
+        <v>145</v>
+      </c>
+      <c r="AN20" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -2878,6 +3064,15 @@
       </c>
       <c r="AK21" t="n">
         <v>200</v>
+      </c>
+      <c r="AL21" t="n">
+        <v>120</v>
+      </c>
+      <c r="AM21" t="n">
+        <v>145</v>
+      </c>
+      <c r="AN21" t="n">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug in buid_ground_surface
</commit_message>
<xml_diff>
--- a/slices.xlsx
+++ b/slices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN21"/>
+  <dimension ref="A1:AO23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,115 +521,120 @@
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
+          <t>h4</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
           <t>w</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>qL</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>qR</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>d_x</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>d_y</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>kw</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>t</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>y_t</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>beta</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>p</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>n_eff</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>z</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>theta</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>piezo_y</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>hw</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>u</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>mat</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>phi</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>c</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>r</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>xo</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>yo</t>
         </is>
@@ -640,43 +645,41 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>55.5576253046535</v>
+        <v>-31.37176393847567</v>
       </c>
       <c r="C2" t="n">
-        <v>39.99961494556892</v>
+        <v>226.9606994594122</v>
       </c>
       <c r="D2" t="n">
-        <v>40</v>
+        <v>227</v>
       </c>
       <c r="E2" t="n">
-        <v>65.58135442054459</v>
+        <v>-15.68588196923784</v>
       </c>
       <c r="F2" t="n">
-        <v>30.04068289318306</v>
+        <v>219.9539739382121</v>
       </c>
       <c r="G2" t="n">
-        <v>40</v>
+        <v>227</v>
       </c>
       <c r="H2" t="n">
-        <v>60.56948986259904</v>
+        <v>-23.52882295385675</v>
       </c>
       <c r="I2" t="n">
-        <v>34.72697403083298</v>
+        <v>223.3239621874805</v>
       </c>
       <c r="J2" t="n">
-        <v>40</v>
-      </c>
-      <c r="K2" t="n">
-        <v>37.36348701541649</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="n">
-        <v>10.02372911589109</v>
+        <v>15.68588196923784</v>
       </c>
       <c r="M2" t="n">
-        <v>-44.71555019038</v>
+        <v>-24.05954835518347</v>
       </c>
       <c r="N2" t="n">
-        <v>14.10583813984129</v>
+        <v>17.17829370001035</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
@@ -685,28 +688,28 @@
         <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>5.273025969167023</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>6976.910679550587</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>0</v>
+        <v>4680</v>
       </c>
       <c r="U2" t="n">
-        <v>0</v>
+        <v>4680</v>
       </c>
       <c r="V2" t="n">
-        <v>60.56948986259904</v>
+        <v>73409.92761603308</v>
       </c>
       <c r="W2" t="n">
-        <v>40</v>
+        <v>-23.52882295385675</v>
       </c>
       <c r="X2" t="n">
-        <v>0</v>
+        <v>227</v>
       </c>
       <c r="Y2" t="n">
         <v>0</v>
@@ -730,31 +733,32 @@
         <v>0</v>
       </c>
       <c r="AF2" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AG2" t="n">
-        <v>5.273025969167023</v>
+        <v>302</v>
       </c>
       <c r="AH2" t="n">
-        <v>329.0368204760222</v>
+        <v>78.6760378125195</v>
       </c>
       <c r="AI2" t="n">
-        <v>3</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>27</v>
-      </c>
+        <v>4909.384759501217</v>
+      </c>
+      <c r="AJ2" t="inlineStr"/>
       <c r="AK2" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="AL2" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="AM2" t="n">
-        <v>145</v>
+        <v>303</v>
       </c>
       <c r="AN2" t="n">
-        <v>120</v>
+        <v>100</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="3">
@@ -762,43 +766,41 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>65.58135442054459</v>
+        <v>-15.68588196923784</v>
       </c>
       <c r="C3" t="n">
-        <v>30.04068289318306</v>
+        <v>219.9539739382121</v>
       </c>
       <c r="D3" t="n">
-        <v>40</v>
+        <v>227</v>
       </c>
       <c r="E3" t="n">
-        <v>75.60508353643566</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>22.10032906584962</v>
+        <v>213.9772736302236</v>
       </c>
       <c r="G3" t="n">
-        <v>40</v>
+        <v>227</v>
       </c>
       <c r="H3" t="n">
-        <v>70.59321897849011</v>
+        <v>-7.842940984618918</v>
       </c>
       <c r="I3" t="n">
-        <v>25.85314164552767</v>
+        <v>216.8412104846682</v>
       </c>
       <c r="J3" t="n">
-        <v>40</v>
-      </c>
-      <c r="K3" t="n">
-        <v>32.92657082276384</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="n">
-        <v>10.02372911589107</v>
+        <v>15.68588196923784</v>
       </c>
       <c r="M3" t="n">
-        <v>-38.3202613973887</v>
+        <v>-20.84967387725808</v>
       </c>
       <c r="N3" t="n">
-        <v>12.77628929067389</v>
+        <v>16.7850069045825</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
@@ -807,28 +809,28 @@
         <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>14.14685835447233</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>18718.16443016667</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>0</v>
+        <v>4680</v>
       </c>
       <c r="U3" t="n">
-        <v>0</v>
+        <v>4680</v>
       </c>
       <c r="V3" t="n">
-        <v>70.59321897849011</v>
+        <v>73409.92761603308</v>
       </c>
       <c r="W3" t="n">
-        <v>40</v>
+        <v>-7.842940984618918</v>
       </c>
       <c r="X3" t="n">
-        <v>0</v>
+        <v>227</v>
       </c>
       <c r="Y3" t="n">
         <v>0</v>
@@ -852,31 +854,32 @@
         <v>0</v>
       </c>
       <c r="AF3" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AG3" t="n">
-        <v>14.14685835447233</v>
+        <v>302</v>
       </c>
       <c r="AH3" t="n">
-        <v>882.7639613190732</v>
+        <v>85.15878951533182</v>
       </c>
       <c r="AI3" t="n">
-        <v>3</v>
-      </c>
-      <c r="AJ3" t="n">
-        <v>27</v>
-      </c>
+        <v>5313.908465756705</v>
+      </c>
+      <c r="AJ3" t="inlineStr"/>
       <c r="AK3" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="AL3" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="AM3" t="n">
-        <v>145</v>
+        <v>303</v>
       </c>
       <c r="AN3" t="n">
-        <v>120</v>
+        <v>100</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="4">
@@ -884,43 +887,41 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>75.60508353643566</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>22.10032906584962</v>
+        <v>213.9772736302236</v>
       </c>
       <c r="D4" t="n">
-        <v>40</v>
+        <v>227</v>
       </c>
       <c r="E4" t="n">
-        <v>85.62881265232674</v>
+        <v>18.75</v>
       </c>
       <c r="F4" t="n">
-        <v>15.71643411866143</v>
+        <v>208.0968696639243</v>
       </c>
       <c r="G4" t="n">
-        <v>40</v>
+        <v>233.25</v>
       </c>
       <c r="H4" t="n">
-        <v>80.6169480943812</v>
+        <v>9.375</v>
       </c>
       <c r="I4" t="n">
-        <v>18.73390188558466</v>
+        <v>210.8700821862255</v>
       </c>
       <c r="J4" t="n">
-        <v>40</v>
-      </c>
-      <c r="K4" t="n">
-        <v>29.36695094279233</v>
-      </c>
+        <v>230.125</v>
+      </c>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="n">
-        <v>10.02372911589109</v>
+        <v>18.75</v>
       </c>
       <c r="M4" t="n">
-        <v>-32.44742192315573</v>
+        <v>-17.40309929341838</v>
       </c>
       <c r="N4" t="n">
-        <v>11.87808673064982</v>
+        <v>19.64947122488833</v>
       </c>
       <c r="O4" t="n">
         <v>0</v>
@@ -929,28 +930,28 @@
         <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>21.26609811441534</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>28137.86010431374</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
         <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>0</v>
+        <v>4680</v>
       </c>
       <c r="U4" t="n">
-        <v>0</v>
+        <v>4290</v>
       </c>
       <c r="V4" t="n">
-        <v>80.6169480943812</v>
+        <v>84093.75</v>
       </c>
       <c r="W4" t="n">
-        <v>40</v>
+        <v>9.239130434782609</v>
       </c>
       <c r="X4" t="n">
-        <v>0</v>
+        <v>230.0797101449275</v>
       </c>
       <c r="Y4" t="n">
         <v>0</v>
@@ -962,7 +963,7 @@
         <v>0</v>
       </c>
       <c r="AB4" t="n">
-        <v>0</v>
+        <v>18.43494882292201</v>
       </c>
       <c r="AC4" t="n">
         <v>0</v>
@@ -974,31 +975,32 @@
         <v>0</v>
       </c>
       <c r="AF4" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AG4" t="n">
-        <v>21.26609811441534</v>
+        <v>302</v>
       </c>
       <c r="AH4" t="n">
-        <v>1327.004522339517</v>
+        <v>91.12991781377451</v>
       </c>
       <c r="AI4" t="n">
-        <v>3</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>27</v>
-      </c>
+        <v>5686.50687157953</v>
+      </c>
+      <c r="AJ4" t="inlineStr"/>
       <c r="AK4" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="AL4" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="AM4" t="n">
-        <v>145</v>
+        <v>303</v>
       </c>
       <c r="AN4" t="n">
-        <v>120</v>
+        <v>100</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="5">
@@ -1006,43 +1008,41 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>85.62881265232674</v>
+        <v>18.75</v>
       </c>
       <c r="C5" t="n">
-        <v>15.71643411866143</v>
+        <v>208.0968696639243</v>
       </c>
       <c r="D5" t="n">
-        <v>40</v>
+        <v>233.25</v>
       </c>
       <c r="E5" t="n">
-        <v>95.65254176821782</v>
+        <v>37.5</v>
       </c>
       <c r="F5" t="n">
-        <v>10.6161421138269</v>
+        <v>203.5160206689069</v>
       </c>
       <c r="G5" t="n">
-        <v>40</v>
+        <v>239.5</v>
       </c>
       <c r="H5" t="n">
-        <v>90.64067721027229</v>
+        <v>28.125</v>
       </c>
       <c r="I5" t="n">
-        <v>13.01839398362824</v>
+        <v>205.6481962429991</v>
       </c>
       <c r="J5" t="n">
-        <v>40</v>
-      </c>
-      <c r="K5" t="n">
-        <v>26.50919699181412</v>
-      </c>
+        <v>236.375</v>
+      </c>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="n">
-        <v>10.02372911589107</v>
+        <v>18.75</v>
       </c>
       <c r="M5" t="n">
-        <v>-26.9359618041506</v>
+        <v>-13.72200262919582</v>
       </c>
       <c r="N5" t="n">
-        <v>11.24349820547246</v>
+        <v>19.3008839343938</v>
       </c>
       <c r="O5" t="n">
         <v>0</v>
@@ -1051,28 +1051,28 @@
         <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>26.98160601637176</v>
+        <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>35700.23289621456</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
         <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>0</v>
+        <v>4290</v>
       </c>
       <c r="U5" t="n">
-        <v>0</v>
+        <v>3900</v>
       </c>
       <c r="V5" t="n">
-        <v>90.64067721027229</v>
+        <v>76781.25</v>
       </c>
       <c r="W5" t="n">
-        <v>40</v>
+        <v>27.97619047619047</v>
       </c>
       <c r="X5" t="n">
-        <v>0</v>
+        <v>236.3253968253968</v>
       </c>
       <c r="Y5" t="n">
         <v>0</v>
@@ -1084,7 +1084,7 @@
         <v>0</v>
       </c>
       <c r="AB5" t="n">
-        <v>0</v>
+        <v>18.43494882292201</v>
       </c>
       <c r="AC5" t="n">
         <v>0</v>
@@ -1096,31 +1096,32 @@
         <v>0</v>
       </c>
       <c r="AF5" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AG5" t="n">
-        <v>26.98160601637176</v>
+        <v>302</v>
       </c>
       <c r="AH5" t="n">
-        <v>1683.652215421597</v>
+        <v>96.35180375700094</v>
       </c>
       <c r="AI5" t="n">
-        <v>3</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>27</v>
-      </c>
+        <v>6012.352554436859</v>
+      </c>
+      <c r="AJ5" t="inlineStr"/>
       <c r="AK5" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="AL5" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="AM5" t="n">
-        <v>145</v>
+        <v>303</v>
       </c>
       <c r="AN5" t="n">
-        <v>120</v>
+        <v>100</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="6">
@@ -1128,43 +1129,41 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>95.65254176821782</v>
+        <v>37.5</v>
       </c>
       <c r="C6" t="n">
-        <v>10.6161421138269</v>
+        <v>203.5160206689069</v>
       </c>
       <c r="D6" t="n">
-        <v>40</v>
+        <v>239.5</v>
       </c>
       <c r="E6" t="n">
-        <v>105.6762708841089</v>
+        <v>56.25</v>
       </c>
       <c r="F6" t="n">
-        <v>6.62608620842262</v>
+        <v>200.1751552989646</v>
       </c>
       <c r="G6" t="n">
-        <v>40</v>
+        <v>245.75</v>
       </c>
       <c r="H6" t="n">
-        <v>100.6644063261634</v>
+        <v>46.875</v>
       </c>
       <c r="I6" t="n">
-        <v>8.490560338649104</v>
+        <v>201.6935562630267</v>
       </c>
       <c r="J6" t="n">
-        <v>40</v>
-      </c>
-      <c r="K6" t="n">
-        <v>24.24528016932455</v>
-      </c>
+        <v>242.625</v>
+      </c>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="n">
-        <v>10.02372911589109</v>
+        <v>18.75</v>
       </c>
       <c r="M6" t="n">
-        <v>-21.68252031424755</v>
+        <v>-10.09786456109964</v>
       </c>
       <c r="N6" t="n">
-        <v>10.78695667671407</v>
+        <v>19.0450126686252</v>
       </c>
       <c r="O6" t="n">
         <v>0</v>
@@ -1173,28 +1172,28 @@
         <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>31.5094396613509</v>
+        <v>0</v>
       </c>
       <c r="R6" t="n">
-        <v>41691.15558417432</v>
+        <v>0</v>
       </c>
       <c r="S6" t="n">
         <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>0</v>
+        <v>3900</v>
       </c>
       <c r="U6" t="n">
-        <v>0</v>
+        <v>3510</v>
       </c>
       <c r="V6" t="n">
-        <v>100.6644063261634</v>
+        <v>69468.75</v>
       </c>
       <c r="W6" t="n">
-        <v>40</v>
+        <v>46.71052631578947</v>
       </c>
       <c r="X6" t="n">
-        <v>0</v>
+        <v>242.5701754385965</v>
       </c>
       <c r="Y6" t="n">
         <v>0</v>
@@ -1206,7 +1205,7 @@
         <v>0</v>
       </c>
       <c r="AB6" t="n">
-        <v>0</v>
+        <v>18.43494882292201</v>
       </c>
       <c r="AC6" t="n">
         <v>0</v>
@@ -1218,31 +1217,32 @@
         <v>0</v>
       </c>
       <c r="AF6" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AG6" t="n">
-        <v>31.5094396613509</v>
+        <v>302</v>
       </c>
       <c r="AH6" t="n">
-        <v>1966.189034868296</v>
+        <v>100.3064437369733</v>
       </c>
       <c r="AI6" t="n">
-        <v>3</v>
-      </c>
-      <c r="AJ6" t="n">
-        <v>27</v>
-      </c>
+        <v>6259.122089187133</v>
+      </c>
+      <c r="AJ6" t="inlineStr"/>
       <c r="AK6" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="AL6" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="AM6" t="n">
-        <v>145</v>
+        <v>303</v>
       </c>
       <c r="AN6" t="n">
-        <v>120</v>
+        <v>100</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="7">
@@ -1250,43 +1250,41 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>105.6762708841089</v>
+        <v>56.25</v>
       </c>
       <c r="C7" t="n">
-        <v>6.62608620842262</v>
+        <v>200.1751552989646</v>
       </c>
       <c r="D7" t="n">
-        <v>40</v>
+        <v>245.75</v>
       </c>
       <c r="E7" t="n">
-        <v>115.7</v>
+        <v>75</v>
       </c>
       <c r="F7" t="n">
-        <v>3.632006118520721</v>
+        <v>198.0331143982837</v>
       </c>
       <c r="G7" t="n">
-        <v>40</v>
+        <v>252</v>
       </c>
       <c r="H7" t="n">
-        <v>110.6881354420544</v>
+        <v>65.625</v>
       </c>
       <c r="I7" t="n">
-        <v>5.010018042625987</v>
+        <v>198.956216847117</v>
       </c>
       <c r="J7" t="n">
-        <v>40</v>
-      </c>
-      <c r="K7" t="n">
-        <v>22.50500902131299</v>
-      </c>
+        <v>248.875</v>
+      </c>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="n">
-        <v>10.02372911589109</v>
+        <v>18.75</v>
       </c>
       <c r="M7" t="n">
-        <v>-16.61457905447066</v>
+        <v>-6.51416488206162</v>
       </c>
       <c r="N7" t="n">
-        <v>10.46045467471967</v>
+        <v>18.871839639202</v>
       </c>
       <c r="O7" t="n">
         <v>0</v>
@@ -1295,28 +1293,28 @@
         <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>34.98998195737401</v>
+        <v>0</v>
       </c>
       <c r="R7" t="n">
-        <v>46296.37332020365</v>
+        <v>0</v>
       </c>
       <c r="S7" t="n">
         <v>0</v>
       </c>
       <c r="T7" t="n">
-        <v>0</v>
+        <v>3510</v>
       </c>
       <c r="U7" t="n">
-        <v>0</v>
+        <v>3120</v>
       </c>
       <c r="V7" t="n">
-        <v>110.6881354420544</v>
+        <v>62156.25</v>
       </c>
       <c r="W7" t="n">
-        <v>40</v>
+        <v>65.44117647058823</v>
       </c>
       <c r="X7" t="n">
-        <v>0</v>
+        <v>248.8137254901961</v>
       </c>
       <c r="Y7" t="n">
         <v>0</v>
@@ -1328,7 +1326,7 @@
         <v>0</v>
       </c>
       <c r="AB7" t="n">
-        <v>0</v>
+        <v>18.43494882292201</v>
       </c>
       <c r="AC7" t="n">
         <v>0</v>
@@ -1340,31 +1338,32 @@
         <v>0</v>
       </c>
       <c r="AF7" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AG7" t="n">
-        <v>34.98998195737401</v>
+        <v>302</v>
       </c>
       <c r="AH7" t="n">
-        <v>2183.374874140138</v>
+        <v>103.043783152883</v>
       </c>
       <c r="AI7" t="n">
-        <v>3</v>
-      </c>
-      <c r="AJ7" t="n">
-        <v>27</v>
-      </c>
+        <v>6429.932068739896</v>
+      </c>
+      <c r="AJ7" t="inlineStr"/>
       <c r="AK7" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="AL7" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="AM7" t="n">
-        <v>145</v>
+        <v>303</v>
       </c>
       <c r="AN7" t="n">
-        <v>120</v>
+        <v>100</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="8">
@@ -1372,73 +1371,71 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>115.7</v>
+        <v>75</v>
       </c>
       <c r="C8" t="n">
-        <v>3.632006118520721</v>
+        <v>198.0331143982837</v>
       </c>
       <c r="D8" t="n">
-        <v>40</v>
+        <v>252</v>
       </c>
       <c r="E8" t="n">
-        <v>125.5666666666667</v>
+        <v>93.75</v>
       </c>
       <c r="F8" t="n">
-        <v>1.58401478028587</v>
+        <v>197.0644664289117</v>
       </c>
       <c r="G8" t="n">
-        <v>48</v>
+        <v>258.25</v>
       </c>
       <c r="H8" t="n">
-        <v>120.6333333333333</v>
+        <v>84.375</v>
       </c>
       <c r="I8" t="n">
-        <v>2.499933806165217</v>
+        <v>197.4031405070436</v>
       </c>
       <c r="J8" t="n">
-        <v>44</v>
-      </c>
-      <c r="K8" t="n">
-        <v>23.08422102086657</v>
-      </c>
+        <v>255.125</v>
+      </c>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="n">
-        <v>9.866666666666674</v>
+        <v>18.75</v>
       </c>
       <c r="M8" t="n">
-        <v>-11.71569679076375</v>
+        <v>-2.955920157288468</v>
       </c>
       <c r="N8" t="n">
-        <v>10.07659006958534</v>
+        <v>18.77498004945495</v>
       </c>
       <c r="O8" t="n">
         <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>37.50006619383478</v>
+        <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>53576.08621085047</v>
+        <v>0</v>
       </c>
       <c r="S8" t="n">
         <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>0</v>
+        <v>3120</v>
       </c>
       <c r="U8" t="n">
-        <v>0</v>
+        <v>2730</v>
       </c>
       <c r="V8" t="n">
-        <v>120.6333333333333</v>
+        <v>54843.75</v>
       </c>
       <c r="W8" t="n">
-        <v>44</v>
+        <v>84.16666666666667</v>
       </c>
       <c r="X8" t="n">
-        <v>0</v>
+        <v>255.0555555555555</v>
       </c>
       <c r="Y8" t="n">
         <v>0</v>
@@ -1447,10 +1444,10 @@
         <v>0</v>
       </c>
       <c r="AA8" t="n">
-        <v>39.03551289874686</v>
+        <v>0</v>
       </c>
       <c r="AB8" t="n">
-        <v>0</v>
+        <v>18.43494882292201</v>
       </c>
       <c r="AC8" t="n">
         <v>0</v>
@@ -1462,31 +1459,32 @@
         <v>0</v>
       </c>
       <c r="AF8" t="n">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="AG8" t="n">
-        <v>41.50006619383478</v>
+        <v>302</v>
       </c>
       <c r="AH8" t="n">
-        <v>2589.604130495291</v>
+        <v>104.5968594929564</v>
       </c>
       <c r="AI8" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ8" t="n">
-        <v>32</v>
-      </c>
+        <v>6526.84403236048</v>
+      </c>
+      <c r="AJ8" t="inlineStr"/>
       <c r="AK8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>303</v>
+      </c>
+      <c r="AN8" t="n">
         <v>100</v>
       </c>
-      <c r="AL8" t="n">
-        <v>120</v>
-      </c>
-      <c r="AM8" t="n">
-        <v>145</v>
-      </c>
-      <c r="AN8" t="n">
-        <v>120</v>
+      <c r="AO8" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="9">
@@ -1494,73 +1492,71 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>125.5666666666667</v>
+        <v>93.75</v>
       </c>
       <c r="C9" t="n">
-        <v>1.58401478028587</v>
+        <v>197.0644664289117</v>
       </c>
       <c r="D9" t="n">
-        <v>48</v>
+        <v>258.25</v>
       </c>
       <c r="E9" t="n">
-        <v>135.4333333333333</v>
+        <v>112.5</v>
       </c>
       <c r="F9" t="n">
-        <v>0.3819458071278916</v>
+        <v>197.2579480812089</v>
       </c>
       <c r="G9" t="n">
-        <v>56</v>
+        <v>264.5</v>
       </c>
       <c r="H9" t="n">
-        <v>130.5</v>
+        <v>103.125</v>
       </c>
       <c r="I9" t="n">
-        <v>0.8792629304200403</v>
+        <v>197.0161153212931</v>
       </c>
       <c r="J9" t="n">
-        <v>52</v>
-      </c>
-      <c r="K9" t="n">
-        <v>26.01311423102661</v>
-      </c>
+        <v>261.375</v>
+      </c>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" t="n">
-        <v>9.866666666666674</v>
+        <v>18.75</v>
       </c>
       <c r="M9" t="n">
-        <v>-6.940199065150054</v>
+        <v>0.5909322952925811</v>
       </c>
       <c r="N9" t="n">
-        <v>9.939495248171937</v>
+        <v>18.75099728827162</v>
       </c>
       <c r="O9" t="n">
         <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>39.12073706957996</v>
+        <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>65158.84795942099</v>
+        <v>0</v>
       </c>
       <c r="S9" t="n">
         <v>0</v>
       </c>
       <c r="T9" t="n">
-        <v>0</v>
+        <v>2730</v>
       </c>
       <c r="U9" t="n">
-        <v>0</v>
+        <v>2340</v>
       </c>
       <c r="V9" t="n">
-        <v>130.5</v>
+        <v>47531.25</v>
       </c>
       <c r="W9" t="n">
-        <v>52</v>
+        <v>102.8846153846154</v>
       </c>
       <c r="X9" t="n">
-        <v>0</v>
+        <v>261.2948717948718</v>
       </c>
       <c r="Y9" t="n">
         <v>0</v>
@@ -1569,10 +1565,10 @@
         <v>0</v>
       </c>
       <c r="AA9" t="n">
-        <v>39.03551289874686</v>
+        <v>0</v>
       </c>
       <c r="AB9" t="n">
-        <v>0</v>
+        <v>18.43494882292201</v>
       </c>
       <c r="AC9" t="n">
         <v>0</v>
@@ -1584,31 +1580,32 @@
         <v>0</v>
       </c>
       <c r="AF9" t="n">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="AG9" t="n">
-        <v>51.12073706957996</v>
+        <v>302</v>
       </c>
       <c r="AH9" t="n">
-        <v>3189.933993141789</v>
+        <v>104.9838846787069</v>
       </c>
       <c r="AI9" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ9" t="n">
-        <v>32</v>
-      </c>
+        <v>6550.994403951313</v>
+      </c>
+      <c r="AJ9" t="inlineStr"/>
       <c r="AK9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>303</v>
+      </c>
+      <c r="AN9" t="n">
         <v>100</v>
       </c>
-      <c r="AL9" t="n">
-        <v>120</v>
-      </c>
-      <c r="AM9" t="n">
-        <v>145</v>
-      </c>
-      <c r="AN9" t="n">
-        <v>120</v>
+      <c r="AO9" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="10">
@@ -1616,73 +1613,71 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>135.4333333333333</v>
+        <v>112.5</v>
       </c>
       <c r="C10" t="n">
-        <v>0.3819458071278916</v>
+        <v>197.2579480812089</v>
       </c>
       <c r="D10" t="n">
-        <v>56</v>
+        <v>264.5</v>
       </c>
       <c r="E10" t="n">
-        <v>145.3</v>
+        <v>131.25</v>
       </c>
       <c r="F10" t="n">
-        <v>0.000375000585933094</v>
+        <v>198.6157975274749</v>
       </c>
       <c r="G10" t="n">
-        <v>64</v>
+        <v>270.75</v>
       </c>
       <c r="H10" t="n">
-        <v>140.3666666666667</v>
+        <v>121.875</v>
       </c>
       <c r="I10" t="n">
-        <v>0.08948243701796343</v>
+        <v>197.7906613372115</v>
       </c>
       <c r="J10" t="n">
-        <v>60</v>
-      </c>
-      <c r="K10" t="n">
-        <v>29.4201788174892</v>
-      </c>
+        <v>267.625</v>
+      </c>
+      <c r="K10" t="inlineStr"/>
       <c r="L10" t="n">
-        <v>9.866666666666674</v>
+        <v>18.75</v>
       </c>
       <c r="M10" t="n">
-        <v>-2.212803763689251</v>
+        <v>4.140054437167695</v>
       </c>
       <c r="N10" t="n">
-        <v>9.874029601984471</v>
+        <v>18.79905506942506</v>
       </c>
       <c r="O10" t="n">
         <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>39.91051756298204</v>
+        <v>0</v>
       </c>
       <c r="R10" t="n">
-        <v>75659.45807402786</v>
+        <v>0</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
       </c>
       <c r="T10" t="n">
-        <v>0</v>
+        <v>2340</v>
       </c>
       <c r="U10" t="n">
-        <v>0</v>
+        <v>1950</v>
       </c>
       <c r="V10" t="n">
-        <v>140.3666666666667</v>
+        <v>40218.75</v>
       </c>
       <c r="W10" t="n">
-        <v>60</v>
+        <v>121.5909090909091</v>
       </c>
       <c r="X10" t="n">
-        <v>0</v>
+        <v>267.530303030303</v>
       </c>
       <c r="Y10" t="n">
         <v>0</v>
@@ -1691,10 +1686,10 @@
         <v>0</v>
       </c>
       <c r="AA10" t="n">
-        <v>39.03551289874686</v>
+        <v>0</v>
       </c>
       <c r="AB10" t="n">
-        <v>0</v>
+        <v>18.43494882292201</v>
       </c>
       <c r="AC10" t="n">
         <v>0</v>
@@ -1706,31 +1701,32 @@
         <v>0</v>
       </c>
       <c r="AF10" t="n">
-        <v>56.55384615384616</v>
+        <v>0</v>
       </c>
       <c r="AG10" t="n">
-        <v>56.4643637168282</v>
+        <v>302</v>
       </c>
       <c r="AH10" t="n">
-        <v>3523.376295930079</v>
+        <v>104.2093386627885</v>
       </c>
       <c r="AI10" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ10" t="n">
-        <v>32</v>
-      </c>
+        <v>6502.662732558004</v>
+      </c>
+      <c r="AJ10" t="inlineStr"/>
       <c r="AK10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>303</v>
+      </c>
+      <c r="AN10" t="n">
         <v>100</v>
       </c>
-      <c r="AL10" t="n">
-        <v>120</v>
-      </c>
-      <c r="AM10" t="n">
-        <v>145</v>
-      </c>
-      <c r="AN10" t="n">
-        <v>120</v>
+      <c r="AO10" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="11">
@@ -1738,73 +1734,71 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>145.3</v>
+        <v>131.25</v>
       </c>
       <c r="C11" t="n">
-        <v>0.000375000585933094</v>
+        <v>198.6157975274749</v>
       </c>
       <c r="D11" t="n">
-        <v>64</v>
+        <v>270.75</v>
       </c>
       <c r="E11" t="n">
-        <v>157.65</v>
+        <v>150</v>
       </c>
       <c r="F11" t="n">
-        <v>0.6686231538410539</v>
+        <v>201.1538857538884</v>
       </c>
       <c r="G11" t="n">
-        <v>74</v>
+        <v>277</v>
       </c>
       <c r="H11" t="n">
-        <v>151.475</v>
+        <v>140.625</v>
       </c>
       <c r="I11" t="n">
-        <v>0.17481744224213</v>
+        <v>199.7357674064392</v>
       </c>
       <c r="J11" t="n">
-        <v>69.00000000000001</v>
-      </c>
-      <c r="K11" t="n">
-        <v>33.98037580017571</v>
-      </c>
+        <v>273.875</v>
+      </c>
+      <c r="K11" t="inlineStr"/>
       <c r="L11" t="n">
-        <v>12.34999999999999</v>
+        <v>18.75</v>
       </c>
       <c r="M11" t="n">
-        <v>3.093086941691099</v>
+        <v>7.705187512178096</v>
       </c>
       <c r="N11" t="n">
-        <v>12.3680178772166</v>
+        <v>18.92083499584225</v>
       </c>
       <c r="O11" t="n">
-        <v>5.000000000000014</v>
+        <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="Q11" t="n">
-        <v>39.82518255775787</v>
+        <v>0</v>
       </c>
       <c r="R11" t="n">
-        <v>108518.5126056569</v>
+        <v>0</v>
       </c>
       <c r="S11" t="n">
         <v>0</v>
       </c>
       <c r="T11" t="n">
-        <v>0</v>
+        <v>1950</v>
       </c>
       <c r="U11" t="n">
-        <v>0</v>
+        <v>1560</v>
       </c>
       <c r="V11" t="n">
-        <v>151.475</v>
+        <v>32906.25</v>
       </c>
       <c r="W11" t="n">
-        <v>69</v>
+        <v>140.2777777777778</v>
       </c>
       <c r="X11" t="n">
-        <v>0</v>
+        <v>273.7592592592592</v>
       </c>
       <c r="Y11" t="n">
         <v>0</v>
@@ -1813,10 +1807,10 @@
         <v>0</v>
       </c>
       <c r="AA11" t="n">
-        <v>38.99766642858376</v>
+        <v>0</v>
       </c>
       <c r="AB11" t="n">
-        <v>0</v>
+        <v>18.43494882292201</v>
       </c>
       <c r="AC11" t="n">
         <v>0</v>
@@ -1828,31 +1822,32 @@
         <v>0</v>
       </c>
       <c r="AF11" t="n">
-        <v>61.44250000000001</v>
+        <v>0</v>
       </c>
       <c r="AG11" t="n">
-        <v>61.26768255775788</v>
+        <v>302</v>
       </c>
       <c r="AH11" t="n">
-        <v>3823.103391604091</v>
+        <v>102.2642325935608</v>
       </c>
       <c r="AI11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ11" t="n">
-        <v>28</v>
-      </c>
+        <v>6381.288113838197</v>
+      </c>
+      <c r="AJ11" t="inlineStr"/>
       <c r="AK11" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="AL11" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="AM11" t="n">
-        <v>145</v>
+        <v>303</v>
       </c>
       <c r="AN11" t="n">
-        <v>120</v>
+        <v>100</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="12">
@@ -1860,73 +1855,71 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>157.65</v>
+        <v>150</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6686231538410539</v>
+        <v>201.1538857538884</v>
       </c>
       <c r="D12" t="n">
-        <v>74</v>
+        <v>277</v>
       </c>
       <c r="E12" t="n">
-        <v>170</v>
+        <v>168.75</v>
       </c>
       <c r="F12" t="n">
-        <v>2.633054056944971</v>
+        <v>204.9026643630953</v>
       </c>
       <c r="G12" t="n">
-        <v>84</v>
+        <v>283.25</v>
       </c>
       <c r="H12" t="n">
-        <v>163.825</v>
+        <v>159.375</v>
       </c>
       <c r="I12" t="n">
-        <v>1.485784080558503</v>
+        <v>202.8744215403191</v>
       </c>
       <c r="J12" t="n">
-        <v>78.99999999999999</v>
-      </c>
-      <c r="K12" t="n">
-        <v>39.80675988444744</v>
-      </c>
+        <v>280.125</v>
+      </c>
+      <c r="K12" t="inlineStr"/>
       <c r="L12" t="n">
-        <v>12.34999999999999</v>
+        <v>18.75</v>
       </c>
       <c r="M12" t="n">
-        <v>9.025556359556186</v>
+        <v>11.30063988423298</v>
       </c>
       <c r="N12" t="n">
-        <v>12.50482896617596</v>
+        <v>19.12070320428024</v>
       </c>
       <c r="O12" t="n">
-        <v>14.99999999999999</v>
+        <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="Q12" t="n">
-        <v>38.5142159194415</v>
+        <v>0</v>
       </c>
       <c r="R12" t="n">
-        <v>122436.3747918735</v>
+        <v>0</v>
       </c>
       <c r="S12" t="n">
         <v>0</v>
       </c>
       <c r="T12" t="n">
-        <v>0</v>
+        <v>1560</v>
       </c>
       <c r="U12" t="n">
-        <v>0</v>
+        <v>1170</v>
       </c>
       <c r="V12" t="n">
-        <v>163.825</v>
+        <v>25593.75</v>
       </c>
       <c r="W12" t="n">
-        <v>79</v>
+        <v>158.9285714285714</v>
       </c>
       <c r="X12" t="n">
-        <v>0</v>
+        <v>279.9761904761905</v>
       </c>
       <c r="Y12" t="n">
         <v>0</v>
@@ -1935,10 +1928,10 @@
         <v>0</v>
       </c>
       <c r="AA12" t="n">
-        <v>38.99766642858376</v>
+        <v>0</v>
       </c>
       <c r="AB12" t="n">
-        <v>0</v>
+        <v>18.43494882292201</v>
       </c>
       <c r="AC12" t="n">
         <v>0</v>
@@ -1950,31 +1943,32 @@
         <v>0</v>
       </c>
       <c r="AF12" t="n">
-        <v>65.14749999999999</v>
+        <v>0</v>
       </c>
       <c r="AG12" t="n">
-        <v>63.66171591944149</v>
+        <v>302</v>
       </c>
       <c r="AH12" t="n">
-        <v>3972.491073373149</v>
+        <v>99.12557845968092</v>
       </c>
       <c r="AI12" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ12" t="n">
-        <v>28</v>
-      </c>
+        <v>6185.43609588409</v>
+      </c>
+      <c r="AJ12" t="inlineStr"/>
       <c r="AK12" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="AL12" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="AM12" t="n">
-        <v>145</v>
+        <v>303</v>
       </c>
       <c r="AN12" t="n">
-        <v>120</v>
+        <v>100</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="13">
@@ -1982,73 +1976,71 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>170</v>
+        <v>168.75</v>
       </c>
       <c r="C13" t="n">
-        <v>2.633054056944971</v>
+        <v>204.9026643630953</v>
       </c>
       <c r="D13" t="n">
-        <v>84</v>
+        <v>283.25</v>
       </c>
       <c r="E13" t="n">
-        <v>179.9397267030721</v>
+        <v>187.5</v>
       </c>
       <c r="F13" t="n">
-        <v>5.19923563880495</v>
+        <v>209.9090659810273</v>
       </c>
       <c r="G13" t="n">
-        <v>84</v>
+        <v>289.5</v>
       </c>
       <c r="H13" t="n">
-        <v>174.969863351536</v>
+        <v>178.125</v>
       </c>
       <c r="I13" t="n">
-        <v>3.802722533226898</v>
+        <v>207.2450096497072</v>
       </c>
       <c r="J13" t="n">
-        <v>84</v>
-      </c>
-      <c r="K13" t="n">
-        <v>43.55662160008098</v>
-      </c>
+        <v>286.375</v>
+      </c>
+      <c r="K13" t="inlineStr"/>
       <c r="L13" t="n">
-        <v>9.939726703072068</v>
+        <v>18.75</v>
       </c>
       <c r="M13" t="n">
-        <v>14.4626516468614</v>
+        <v>14.94183213748511</v>
       </c>
       <c r="N13" t="n">
-        <v>10.26501851563292</v>
+        <v>19.40615937388218</v>
       </c>
       <c r="O13" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="P13" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="Q13" t="n">
-        <v>36.1972774667731</v>
+        <v>0</v>
       </c>
       <c r="R13" t="n">
-        <v>101962.1203276141</v>
+        <v>0</v>
       </c>
       <c r="S13" t="n">
         <v>0</v>
       </c>
       <c r="T13" t="n">
-        <v>0</v>
+        <v>1170</v>
       </c>
       <c r="U13" t="n">
-        <v>0</v>
+        <v>779.9999999999999</v>
       </c>
       <c r="V13" t="n">
-        <v>174.969863351536</v>
+        <v>18281.25</v>
       </c>
       <c r="W13" t="n">
-        <v>84</v>
+        <v>177.5</v>
       </c>
       <c r="X13" t="n">
-        <v>0</v>
+        <v>286.1666666666667</v>
       </c>
       <c r="Y13" t="n">
         <v>0</v>
@@ -2060,7 +2052,7 @@
         <v>0</v>
       </c>
       <c r="AB13" t="n">
-        <v>0</v>
+        <v>18.43494882292201</v>
       </c>
       <c r="AC13" t="n">
         <v>0</v>
@@ -2072,31 +2064,32 @@
         <v>0</v>
       </c>
       <c r="AF13" t="n">
-        <v>68.49095900546081</v>
+        <v>0</v>
       </c>
       <c r="AG13" t="n">
-        <v>64.68823647223391</v>
+        <v>302</v>
       </c>
       <c r="AH13" t="n">
-        <v>4036.545955867396</v>
+        <v>94.75499035029276</v>
       </c>
       <c r="AI13" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ13" t="n">
-        <v>28</v>
-      </c>
+        <v>5912.711397858268</v>
+      </c>
+      <c r="AJ13" t="inlineStr"/>
       <c r="AK13" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="AL13" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="AM13" t="n">
-        <v>145</v>
+        <v>303</v>
       </c>
       <c r="AN13" t="n">
-        <v>120</v>
+        <v>100</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="14">
@@ -2104,73 +2097,71 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>179.9397267030721</v>
+        <v>187.5</v>
       </c>
       <c r="C14" t="n">
-        <v>5.19923563880495</v>
+        <v>209.9090659810273</v>
       </c>
       <c r="D14" t="n">
-        <v>84</v>
+        <v>289.5</v>
       </c>
       <c r="E14" t="n">
-        <v>189.8794534061441</v>
+        <v>206.25</v>
       </c>
       <c r="F14" t="n">
-        <v>8.708335164012681</v>
+        <v>216.2396477659361</v>
       </c>
       <c r="G14" t="n">
-        <v>84</v>
+        <v>295.75</v>
       </c>
       <c r="H14" t="n">
-        <v>184.9095900546081</v>
+        <v>196.875</v>
       </c>
       <c r="I14" t="n">
-        <v>6.830990895593999</v>
+        <v>212.9037889922614</v>
       </c>
       <c r="J14" t="n">
-        <v>84</v>
-      </c>
-      <c r="K14" t="n">
-        <v>45.10715479516529</v>
-      </c>
+        <v>292.625</v>
+      </c>
+      <c r="K14" t="inlineStr"/>
       <c r="L14" t="n">
-        <v>9.939726703072068</v>
+        <v>18.75</v>
       </c>
       <c r="M14" t="n">
-        <v>19.42544105333852</v>
+        <v>18.64596060234503</v>
       </c>
       <c r="N14" t="n">
-        <v>10.53969822999045</v>
+        <v>19.78866241546906</v>
       </c>
       <c r="O14" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="P14" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="Q14" t="n">
-        <v>33.169009104406</v>
+        <v>0</v>
       </c>
       <c r="R14" t="n">
-        <v>97988.89922008957</v>
+        <v>0</v>
       </c>
       <c r="S14" t="n">
         <v>0</v>
       </c>
       <c r="T14" t="n">
-        <v>0</v>
+        <v>779.9999999999999</v>
       </c>
       <c r="U14" t="n">
-        <v>0</v>
+        <v>389.9999999999998</v>
       </c>
       <c r="V14" t="n">
-        <v>184.9095900546081</v>
+        <v>10968.75</v>
       </c>
       <c r="W14" t="n">
-        <v>84</v>
+        <v>195.8333333333333</v>
       </c>
       <c r="X14" t="n">
-        <v>0</v>
+        <v>292.2777777777778</v>
       </c>
       <c r="Y14" t="n">
         <v>0</v>
@@ -2182,7 +2173,7 @@
         <v>0</v>
       </c>
       <c r="AB14" t="n">
-        <v>0</v>
+        <v>18.43494882292201</v>
       </c>
       <c r="AC14" t="n">
         <v>0</v>
@@ -2194,31 +2185,32 @@
         <v>0</v>
       </c>
       <c r="AF14" t="n">
-        <v>71.05205501170174</v>
+        <v>0</v>
       </c>
       <c r="AG14" t="n">
-        <v>64.22106411610774</v>
+        <v>302</v>
       </c>
       <c r="AH14" t="n">
-        <v>4007.394400845123</v>
+        <v>89.09621100773865</v>
       </c>
       <c r="AI14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ14" t="n">
-        <v>28</v>
-      </c>
+        <v>5559.603566882892</v>
+      </c>
+      <c r="AJ14" t="inlineStr"/>
       <c r="AK14" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="AL14" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="AM14" t="n">
-        <v>145</v>
+        <v>303</v>
       </c>
       <c r="AN14" t="n">
-        <v>120</v>
+        <v>100</v>
+      </c>
+      <c r="AO14" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="15">
@@ -2226,73 +2218,71 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>189.8794534061441</v>
+        <v>206.25</v>
       </c>
       <c r="C15" t="n">
-        <v>8.708335164012681</v>
+        <v>216.2396477659361</v>
       </c>
       <c r="D15" t="n">
-        <v>84</v>
+        <v>295.75</v>
       </c>
       <c r="E15" t="n">
-        <v>199.8191801092162</v>
+        <v>225</v>
       </c>
       <c r="F15" t="n">
-        <v>13.25330219555589</v>
+        <v>223.9855076268639</v>
       </c>
       <c r="G15" t="n">
-        <v>84</v>
+        <v>302</v>
       </c>
       <c r="H15" t="n">
-        <v>194.8493167576802</v>
+        <v>215.625</v>
       </c>
       <c r="I15" t="n">
-        <v>10.84393915685457</v>
+        <v>219.9288315891834</v>
       </c>
       <c r="J15" t="n">
-        <v>84</v>
-      </c>
-      <c r="K15" t="n">
-        <v>47.16666932219525</v>
-      </c>
+        <v>298.875</v>
+      </c>
+      <c r="K15" t="inlineStr"/>
       <c r="L15" t="n">
-        <v>9.939726703072068</v>
+        <v>18.75</v>
       </c>
       <c r="M15" t="n">
-        <v>24.54520018318539</v>
+        <v>22.43286653732118</v>
       </c>
       <c r="N15" t="n">
-        <v>10.92717340841417</v>
+        <v>20.2850226706894</v>
       </c>
       <c r="O15" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="Q15" t="n">
-        <v>29.15606084314543</v>
+        <v>0</v>
       </c>
       <c r="R15" t="n">
-        <v>92723.7348333438</v>
+        <v>0</v>
       </c>
       <c r="S15" t="n">
         <v>0</v>
       </c>
       <c r="T15" t="n">
-        <v>0</v>
+        <v>389.9999999999998</v>
       </c>
       <c r="U15" t="n">
         <v>0</v>
       </c>
       <c r="V15" t="n">
-        <v>194.8493167576802</v>
+        <v>3656.249999999998</v>
       </c>
       <c r="W15" t="n">
-        <v>84</v>
+        <v>212.5</v>
       </c>
       <c r="X15" t="n">
-        <v>0</v>
+        <v>297.8333333333333</v>
       </c>
       <c r="Y15" t="n">
         <v>0</v>
@@ -2304,7 +2294,7 @@
         <v>0</v>
       </c>
       <c r="AB15" t="n">
-        <v>0</v>
+        <v>18.43494882292201</v>
       </c>
       <c r="AC15" t="n">
         <v>0</v>
@@ -2316,31 +2306,32 @@
         <v>0</v>
       </c>
       <c r="AF15" t="n">
-        <v>73.18199644807433</v>
+        <v>0</v>
       </c>
       <c r="AG15" t="n">
-        <v>62.33805729121976</v>
+        <v>302</v>
       </c>
       <c r="AH15" t="n">
-        <v>3889.894774972113</v>
+        <v>82.0711684108166</v>
       </c>
       <c r="AI15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ15" t="n">
-        <v>28</v>
-      </c>
+        <v>5121.240908834956</v>
+      </c>
+      <c r="AJ15" t="inlineStr"/>
       <c r="AK15" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="AL15" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="AM15" t="n">
-        <v>145</v>
+        <v>303</v>
       </c>
       <c r="AN15" t="n">
-        <v>120</v>
+        <v>100</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="16">
@@ -2348,55 +2339,53 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>199.8191801092162</v>
+        <v>225</v>
       </c>
       <c r="C16" t="n">
-        <v>13.25330219555589</v>
+        <v>223.9855076268639</v>
       </c>
       <c r="D16" t="n">
-        <v>84</v>
+        <v>302</v>
       </c>
       <c r="E16" t="n">
-        <v>209.7589068122883</v>
+        <v>240</v>
       </c>
       <c r="F16" t="n">
-        <v>18.97384502774857</v>
+        <v>231.2826764051115</v>
       </c>
       <c r="G16" t="n">
-        <v>84</v>
+        <v>307</v>
       </c>
       <c r="H16" t="n">
-        <v>204.7890434607522</v>
+        <v>232.5</v>
       </c>
       <c r="I16" t="n">
-        <v>15.95544088205149</v>
+        <v>227.5064220940244</v>
       </c>
       <c r="J16" t="n">
-        <v>84</v>
-      </c>
-      <c r="K16" t="n">
-        <v>49.79938339756081</v>
-      </c>
+        <v>304.5</v>
+      </c>
+      <c r="K16" t="inlineStr"/>
       <c r="L16" t="n">
-        <v>9.939726703072068</v>
+        <v>15</v>
       </c>
       <c r="M16" t="n">
-        <v>29.8837617113602</v>
+        <v>25.9313375145285</v>
       </c>
       <c r="N16" t="n">
-        <v>11.46400365670253</v>
+        <v>16.67929217139375</v>
       </c>
       <c r="O16" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="Q16" t="n">
-        <v>24.04455911794851</v>
+        <v>0</v>
       </c>
       <c r="R16" t="n">
-        <v>86017.22004816629</v>
+        <v>0</v>
       </c>
       <c r="S16" t="n">
         <v>0</v>
@@ -2408,13 +2397,13 @@
         <v>0</v>
       </c>
       <c r="V16" t="n">
-        <v>204.7890434607522</v>
+        <v>0</v>
       </c>
       <c r="W16" t="n">
-        <v>84</v>
+        <v>232.5</v>
       </c>
       <c r="X16" t="n">
-        <v>0</v>
+        <v>304.5</v>
       </c>
       <c r="Y16" t="n">
         <v>0</v>
@@ -2426,7 +2415,7 @@
         <v>0</v>
       </c>
       <c r="AB16" t="n">
-        <v>0</v>
+        <v>18.43494882292201</v>
       </c>
       <c r="AC16" t="n">
         <v>0</v>
@@ -2438,31 +2427,32 @@
         <v>0</v>
       </c>
       <c r="AF16" t="n">
-        <v>75.31193788444691</v>
+        <v>0</v>
       </c>
       <c r="AG16" t="n">
-        <v>59.35649700239541</v>
+        <v>302</v>
       </c>
       <c r="AH16" t="n">
-        <v>3703.845412949474</v>
+        <v>74.4935779059756</v>
       </c>
       <c r="AI16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ16" t="n">
-        <v>28</v>
-      </c>
+        <v>4648.399261332877</v>
+      </c>
+      <c r="AJ16" t="inlineStr"/>
       <c r="AK16" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="AL16" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="AM16" t="n">
-        <v>145</v>
+        <v>303</v>
       </c>
       <c r="AN16" t="n">
-        <v>120</v>
+        <v>100</v>
+      </c>
+      <c r="AO16" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="17">
@@ -2470,58 +2460,58 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>209.7589068122883</v>
+        <v>240</v>
       </c>
       <c r="C17" t="n">
-        <v>18.97384502774857</v>
+        <v>231.2826764051115</v>
       </c>
       <c r="D17" t="n">
-        <v>84</v>
+        <v>307</v>
       </c>
       <c r="E17" t="n">
-        <v>219.6986335153603</v>
+        <v>255</v>
       </c>
       <c r="F17" t="n">
-        <v>26.08453721064944</v>
+        <v>239.6463943019033</v>
       </c>
       <c r="G17" t="n">
-        <v>84</v>
+        <v>312</v>
       </c>
       <c r="H17" t="n">
-        <v>214.7287701638243</v>
+        <v>247.5</v>
       </c>
       <c r="I17" t="n">
-        <v>22.33783428860198</v>
+        <v>235.3251995372435</v>
       </c>
       <c r="J17" t="n">
-        <v>84</v>
+        <v>309.5</v>
       </c>
       <c r="K17" t="n">
-        <v>53.10534405839487</v>
+        <v>272.3877240503961</v>
       </c>
       <c r="L17" t="n">
-        <v>9.93972670307204</v>
+        <v>15</v>
       </c>
       <c r="M17" t="n">
-        <v>35.52605335902853</v>
+        <v>29.13038439711123</v>
       </c>
       <c r="N17" t="n">
-        <v>12.21319636798589</v>
+        <v>17.17201635011672</v>
       </c>
       <c r="O17" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="P17" t="n">
-        <v>24</v>
+        <v>67.5</v>
       </c>
       <c r="Q17" t="n">
-        <v>17.66216571139802</v>
+        <v>6.674800462756536</v>
       </c>
       <c r="R17" t="n">
-        <v>77643.23955338272</v>
+        <v>0</v>
       </c>
       <c r="S17" t="n">
-        <v>0</v>
+        <v>135840.0068537858</v>
       </c>
       <c r="T17" t="n">
         <v>0</v>
@@ -2530,13 +2520,13 @@
         <v>0</v>
       </c>
       <c r="V17" t="n">
-        <v>214.7287701638243</v>
+        <v>0</v>
       </c>
       <c r="W17" t="n">
-        <v>84</v>
+        <v>247.5</v>
       </c>
       <c r="X17" t="n">
-        <v>0</v>
+        <v>309.5</v>
       </c>
       <c r="Y17" t="n">
         <v>0</v>
@@ -2548,7 +2538,7 @@
         <v>0</v>
       </c>
       <c r="AB17" t="n">
-        <v>0</v>
+        <v>18.43494882292201</v>
       </c>
       <c r="AC17" t="n">
         <v>0</v>
@@ -2560,31 +2550,34 @@
         <v>0</v>
       </c>
       <c r="AF17" t="n">
-        <v>76.545575959229</v>
+        <v>0</v>
       </c>
       <c r="AG17" t="n">
-        <v>54.20774167062702</v>
+        <v>302</v>
       </c>
       <c r="AH17" t="n">
-        <v>3382.563080247126</v>
+        <v>66.67480046275654</v>
       </c>
       <c r="AI17" t="n">
-        <v>1</v>
+        <v>4160.507548876008</v>
       </c>
       <c r="AJ17" t="n">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="AK17" t="n">
-        <v>200</v>
+        <v>26</v>
       </c>
       <c r="AL17" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="AM17" t="n">
-        <v>145</v>
+        <v>303</v>
       </c>
       <c r="AN17" t="n">
-        <v>120</v>
+        <v>100</v>
+      </c>
+      <c r="AO17" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="18">
@@ -2592,58 +2585,58 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>219.6986335153603</v>
+        <v>255</v>
       </c>
       <c r="C18" t="n">
-        <v>26.08453721064944</v>
+        <v>239.6463943019033</v>
       </c>
       <c r="D18" t="n">
-        <v>84</v>
+        <v>312</v>
       </c>
       <c r="E18" t="n">
-        <v>229.6383602184324</v>
+        <v>270</v>
       </c>
       <c r="F18" t="n">
-        <v>34.9332733700486</v>
+        <v>249.18333388708</v>
       </c>
       <c r="G18" t="n">
-        <v>84</v>
+        <v>317</v>
       </c>
       <c r="H18" t="n">
-        <v>224.6684968668964</v>
+        <v>262.5</v>
       </c>
       <c r="I18" t="n">
-        <v>30.26187762734655</v>
+        <v>244.2603863301581</v>
       </c>
       <c r="J18" t="n">
-        <v>84</v>
+        <v>314.5</v>
       </c>
       <c r="K18" t="n">
-        <v>57.24962272221062</v>
+        <v>279.3116263769731</v>
       </c>
       <c r="L18" t="n">
-        <v>9.939726703072068</v>
+        <v>15</v>
       </c>
       <c r="M18" t="n">
-        <v>41.59830918914744</v>
+        <v>32.43236370231759</v>
       </c>
       <c r="N18" t="n">
-        <v>13.291644383338</v>
+        <v>17.77198274519629</v>
       </c>
       <c r="O18" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="P18" t="n">
-        <v>24</v>
+        <v>42.5</v>
       </c>
       <c r="Q18" t="n">
-        <v>9.73812237265345</v>
+        <v>27.73961366984193</v>
       </c>
       <c r="R18" t="n">
-        <v>67246.54663088753</v>
+        <v>0</v>
       </c>
       <c r="S18" t="n">
-        <v>0</v>
+        <v>128954.5872208584</v>
       </c>
       <c r="T18" t="n">
         <v>0</v>
@@ -2652,13 +2645,13 @@
         <v>0</v>
       </c>
       <c r="V18" t="n">
-        <v>224.6684968668964</v>
+        <v>0</v>
       </c>
       <c r="W18" t="n">
-        <v>84</v>
+        <v>262.5</v>
       </c>
       <c r="X18" t="n">
-        <v>0</v>
+        <v>314.5</v>
       </c>
       <c r="Y18" t="n">
         <v>0</v>
@@ -2670,7 +2663,7 @@
         <v>0</v>
       </c>
       <c r="AB18" t="n">
-        <v>0</v>
+        <v>18.43494882292201</v>
       </c>
       <c r="AC18" t="n">
         <v>0</v>
@@ -2682,31 +2675,34 @@
         <v>0</v>
       </c>
       <c r="AF18" t="n">
-        <v>77.35149974596457</v>
+        <v>0</v>
       </c>
       <c r="AG18" t="n">
-        <v>47.08962211861802</v>
+        <v>302</v>
       </c>
       <c r="AH18" t="n">
-        <v>2938.392420201765</v>
+        <v>57.73961366984193</v>
       </c>
       <c r="AI18" t="n">
-        <v>1</v>
+        <v>3602.951892998136</v>
       </c>
       <c r="AJ18" t="n">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="AK18" t="n">
-        <v>200</v>
+        <v>26</v>
       </c>
       <c r="AL18" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="AM18" t="n">
-        <v>145</v>
+        <v>303</v>
       </c>
       <c r="AN18" t="n">
-        <v>120</v>
+        <v>100</v>
+      </c>
+      <c r="AO18" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="19">
@@ -2714,58 +2710,58 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>229.6383602184324</v>
+        <v>270</v>
       </c>
       <c r="C19" t="n">
-        <v>34.9332733700486</v>
+        <v>249.18333388708</v>
       </c>
       <c r="D19" t="n">
-        <v>84</v>
+        <v>317</v>
       </c>
       <c r="E19" t="n">
-        <v>239.5780869215045</v>
+        <v>280</v>
       </c>
       <c r="F19" t="n">
-        <v>46.14212652486975</v>
+        <v>256.2603848366048</v>
       </c>
       <c r="G19" t="n">
-        <v>84</v>
+        <v>307</v>
       </c>
       <c r="H19" t="n">
-        <v>234.6082235699684</v>
+        <v>275</v>
       </c>
       <c r="I19" t="n">
-        <v>40.18542571287773</v>
+        <v>252.6460026601551</v>
       </c>
       <c r="J19" t="n">
-        <v>84</v>
+        <v>312</v>
       </c>
       <c r="K19" t="n">
-        <v>62.52905711962126</v>
+        <v>282.2773417216382</v>
       </c>
       <c r="L19" t="n">
-        <v>9.939726703072068</v>
+        <v>10</v>
       </c>
       <c r="M19" t="n">
-        <v>48.30835694146017</v>
+        <v>35.27895092088615</v>
       </c>
       <c r="N19" t="n">
-        <v>14.94422825432905</v>
+        <v>12.24965043551492</v>
       </c>
       <c r="O19" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="P19" t="n">
-        <v>23.81457428712227</v>
+        <v>15</v>
       </c>
       <c r="Q19" t="n">
-        <v>0</v>
+        <v>44.35399733984491</v>
       </c>
       <c r="R19" t="n">
-        <v>54248.53262366771</v>
+        <v>0</v>
       </c>
       <c r="S19" t="n">
-        <v>0</v>
+        <v>72855.41672800924</v>
       </c>
       <c r="T19" t="n">
         <v>0</v>
@@ -2774,13 +2770,13 @@
         <v>0</v>
       </c>
       <c r="V19" t="n">
-        <v>234.6082235699684</v>
+        <v>0</v>
       </c>
       <c r="W19" t="n">
-        <v>84</v>
+        <v>275</v>
       </c>
       <c r="X19" t="n">
-        <v>0</v>
+        <v>312</v>
       </c>
       <c r="Y19" t="n">
         <v>0</v>
@@ -2792,7 +2788,7 @@
         <v>0</v>
       </c>
       <c r="AB19" t="n">
-        <v>0</v>
+        <v>-45</v>
       </c>
       <c r="AC19" t="n">
         <v>0</v>
@@ -2804,31 +2800,34 @@
         <v>0</v>
       </c>
       <c r="AF19" t="n">
-        <v>78.15742353270014</v>
+        <v>0</v>
       </c>
       <c r="AG19" t="n">
-        <v>37.97199781982241</v>
+        <v>302</v>
       </c>
       <c r="AH19" t="n">
-        <v>2369.452663956918</v>
+        <v>49.35399733984491</v>
       </c>
       <c r="AI19" t="n">
-        <v>1</v>
+        <v>3079.689434006322</v>
       </c>
       <c r="AJ19" t="n">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="AK19" t="n">
-        <v>200</v>
+        <v>26</v>
       </c>
       <c r="AL19" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="AM19" t="n">
-        <v>145</v>
+        <v>303</v>
       </c>
       <c r="AN19" t="n">
-        <v>120</v>
+        <v>100</v>
+      </c>
+      <c r="AO19" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="20">
@@ -2836,58 +2835,58 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>239.5780869215045</v>
+        <v>280</v>
       </c>
       <c r="C20" t="n">
-        <v>46.14212652486975</v>
+        <v>256.2603848366048</v>
       </c>
       <c r="D20" t="n">
-        <v>84</v>
+        <v>307</v>
       </c>
       <c r="E20" t="n">
-        <v>249.5178136245765</v>
+        <v>295</v>
       </c>
       <c r="F20" t="n">
-        <v>61.04216222470259</v>
+        <v>268.0862229189478</v>
       </c>
       <c r="G20" t="n">
-        <v>84</v>
+        <v>307</v>
       </c>
       <c r="H20" t="n">
-        <v>244.5479502730405</v>
+        <v>287.5</v>
       </c>
       <c r="I20" t="n">
-        <v>52.99100361566175</v>
+        <v>261.9816183569009</v>
       </c>
       <c r="J20" t="n">
-        <v>84</v>
+        <v>307</v>
       </c>
       <c r="K20" t="n">
-        <v>68.77626622994207</v>
+        <v>284.4908091784504</v>
       </c>
       <c r="L20" t="n">
-        <v>9.939726703072068</v>
+        <v>15</v>
       </c>
       <c r="M20" t="n">
-        <v>56.05420832385308</v>
+        <v>38.22942360091947</v>
       </c>
       <c r="N20" t="n">
-        <v>17.80010592668061</v>
+        <v>19.09516387395373</v>
       </c>
       <c r="O20" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="P20" t="n">
-        <v>11.00899638433825</v>
+        <v>0</v>
       </c>
       <c r="Q20" t="n">
-        <v>0</v>
+        <v>45.01838164309913</v>
       </c>
       <c r="R20" t="n">
-        <v>38974.45926823906</v>
+        <v>0</v>
       </c>
       <c r="S20" t="n">
-        <v>0</v>
+        <v>83058.9141315179</v>
       </c>
       <c r="T20" t="n">
         <v>0</v>
@@ -2896,13 +2895,13 @@
         <v>0</v>
       </c>
       <c r="V20" t="n">
-        <v>244.5479502730405</v>
+        <v>0</v>
       </c>
       <c r="W20" t="n">
-        <v>84</v>
+        <v>287.5</v>
       </c>
       <c r="X20" t="n">
-        <v>0</v>
+        <v>307</v>
       </c>
       <c r="Y20" t="n">
         <v>0</v>
@@ -2926,31 +2925,34 @@
         <v>0</v>
       </c>
       <c r="AF20" t="n">
-        <v>78.96334731943571</v>
+        <v>0</v>
       </c>
       <c r="AG20" t="n">
-        <v>25.97234370377396</v>
+        <v>294.8</v>
       </c>
       <c r="AH20" t="n">
-        <v>1620.674247115495</v>
+        <v>32.81838164309914</v>
       </c>
       <c r="AI20" t="n">
-        <v>1</v>
+        <v>2047.867014529387</v>
       </c>
       <c r="AJ20" t="n">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="AK20" t="n">
-        <v>200</v>
+        <v>24</v>
       </c>
       <c r="AL20" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="AM20" t="n">
-        <v>145</v>
+        <v>303</v>
       </c>
       <c r="AN20" t="n">
-        <v>120</v>
+        <v>100</v>
+      </c>
+      <c r="AO20" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="21">
@@ -2958,58 +2960,58 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>249.5178136245765</v>
+        <v>295</v>
       </c>
       <c r="C21" t="n">
-        <v>61.04216222470259</v>
+        <v>268.0862229189478</v>
       </c>
       <c r="D21" t="n">
-        <v>84</v>
+        <v>307</v>
       </c>
       <c r="E21" t="n">
-        <v>259.4575403276486</v>
+        <v>310</v>
       </c>
       <c r="F21" t="n">
-        <v>83.95181749179723</v>
+        <v>281.5761002087912</v>
       </c>
       <c r="G21" t="n">
-        <v>84</v>
+        <v>307</v>
       </c>
       <c r="H21" t="n">
-        <v>254.4876769761125</v>
+        <v>302.5</v>
       </c>
       <c r="I21" t="n">
-        <v>70.88331657802578</v>
+        <v>274.6053461148646</v>
       </c>
       <c r="J21" t="n">
-        <v>84</v>
+        <v>307</v>
       </c>
       <c r="K21" t="n">
-        <v>77.44165828901289</v>
+        <v>290.8026730574323</v>
       </c>
       <c r="L21" t="n">
-        <v>9.939726703072068</v>
+        <v>15</v>
       </c>
       <c r="M21" t="n">
-        <v>65.83877552790588</v>
+        <v>41.93728966273724</v>
       </c>
       <c r="N21" t="n">
-        <v>24.28436213742816</v>
+        <v>20.16463090523105</v>
       </c>
       <c r="O21" t="n">
-        <v>13.11668342197422</v>
+        <v>0</v>
       </c>
       <c r="P21" t="n">
         <v>0</v>
       </c>
       <c r="Q21" t="n">
-        <v>0</v>
+        <v>32.39465388513543</v>
       </c>
       <c r="R21" t="n">
-        <v>16948.91230046818</v>
+        <v>0</v>
       </c>
       <c r="S21" t="n">
-        <v>0</v>
+        <v>59768.13641807486</v>
       </c>
       <c r="T21" t="n">
         <v>0</v>
@@ -3018,13 +3020,13 @@
         <v>0</v>
       </c>
       <c r="V21" t="n">
-        <v>254.4876769761125</v>
+        <v>0</v>
       </c>
       <c r="W21" t="n">
-        <v>84</v>
+        <v>302.5</v>
       </c>
       <c r="X21" t="n">
-        <v>0</v>
+        <v>307</v>
       </c>
       <c r="Y21" t="n">
         <v>0</v>
@@ -3048,31 +3050,284 @@
         <v>0</v>
       </c>
       <c r="AF21" t="n">
-        <v>79.1265023596815</v>
+        <v>0</v>
       </c>
       <c r="AG21" t="n">
-        <v>8.243185781655711</v>
+        <v>284</v>
       </c>
       <c r="AH21" t="n">
-        <v>514.3747927753163</v>
+        <v>9.394653885135426</v>
       </c>
       <c r="AI21" t="n">
-        <v>1</v>
+        <v>586.2264024324505</v>
       </c>
       <c r="AJ21" t="n">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="AK21" t="n">
-        <v>200</v>
+        <v>24</v>
       </c>
       <c r="AL21" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="AM21" t="n">
-        <v>145</v>
+        <v>303</v>
       </c>
       <c r="AN21" t="n">
-        <v>120</v>
+        <v>100</v>
+      </c>
+      <c r="AO21" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>310</v>
+      </c>
+      <c r="C22" t="n">
+        <v>281.5761002087912</v>
+      </c>
+      <c r="D22" t="n">
+        <v>307</v>
+      </c>
+      <c r="E22" t="n">
+        <v>320</v>
+      </c>
+      <c r="F22" t="n">
+        <v>291.6517338685056</v>
+      </c>
+      <c r="G22" t="n">
+        <v>317</v>
+      </c>
+      <c r="H22" t="n">
+        <v>315</v>
+      </c>
+      <c r="I22" t="n">
+        <v>286.4959016786797</v>
+      </c>
+      <c r="J22" t="n">
+        <v>312</v>
+      </c>
+      <c r="K22" t="n">
+        <v>299.2227168117569</v>
+      </c>
+      <c r="L22" t="n">
+        <v>10</v>
+      </c>
+      <c r="M22" t="n">
+        <v>45.2000179975562</v>
+      </c>
+      <c r="N22" t="n">
+        <v>14.19176506302563</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>10.50409832132027</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0</v>
+      </c>
+      <c r="S22" t="n">
+        <v>31220.04093522393</v>
+      </c>
+      <c r="T22" t="n">
+        <v>0</v>
+      </c>
+      <c r="U22" t="n">
+        <v>0</v>
+      </c>
+      <c r="V22" t="n">
+        <v>0</v>
+      </c>
+      <c r="W22" t="n">
+        <v>315</v>
+      </c>
+      <c r="X22" t="n">
+        <v>312</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>45</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>275</v>
+      </c>
+      <c r="AH22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ22" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK22" t="n">
+        <v>26</v>
+      </c>
+      <c r="AL22" t="n">
+        <v>100</v>
+      </c>
+      <c r="AM22" t="n">
+        <v>303</v>
+      </c>
+      <c r="AN22" t="n">
+        <v>100</v>
+      </c>
+      <c r="AO22" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>320</v>
+      </c>
+      <c r="C23" t="n">
+        <v>291.6517338685056</v>
+      </c>
+      <c r="D23" t="n">
+        <v>317</v>
+      </c>
+      <c r="E23" t="n">
+        <v>337.051583908027</v>
+      </c>
+      <c r="F23" t="n">
+        <v>311.2791835363793</v>
+      </c>
+      <c r="G23" t="n">
+        <v>311.3161386973243</v>
+      </c>
+      <c r="H23" t="n">
+        <v>328.5257919540135</v>
+      </c>
+      <c r="I23" t="n">
+        <v>301.040299528294</v>
+      </c>
+      <c r="J23" t="n">
+        <v>314.1580693486621</v>
+      </c>
+      <c r="K23" t="n">
+        <v>307.5991844384781</v>
+      </c>
+      <c r="L23" t="n">
+        <v>17.051583908027</v>
+      </c>
+      <c r="M23" t="n">
+        <v>48.95643583704144</v>
+      </c>
+      <c r="N23" t="n">
+        <v>25.96822331605339</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" t="n">
+        <v>13.1177698203681</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0</v>
+      </c>
+      <c r="S23" t="n">
+        <v>27288.80783893928</v>
+      </c>
+      <c r="T23" t="n">
+        <v>0</v>
+      </c>
+      <c r="U23" t="n">
+        <v>0</v>
+      </c>
+      <c r="V23" t="n">
+        <v>0</v>
+      </c>
+      <c r="W23" t="n">
+        <v>328.5257919540135</v>
+      </c>
+      <c r="X23" t="n">
+        <v>314.1580693486621</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB23" t="n">
+        <v>-18.43494882292201</v>
+      </c>
+      <c r="AC23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG23" t="n">
+        <v>258.3893783020887</v>
+      </c>
+      <c r="AH23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ23" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK23" t="n">
+        <v>26</v>
+      </c>
+      <c r="AL23" t="n">
+        <v>100</v>
+      </c>
+      <c r="AM23" t="n">
+        <v>303</v>
+      </c>
+      <c r="AN23" t="n">
+        <v>100</v>
+      </c>
+      <c r="AO23" t="n">
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
full testing of rapid_drawdown completed
</commit_message>
<xml_diff>
--- a/slices.xlsx
+++ b/slices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BC33"/>
+  <dimension ref="A1:BC35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -775,7 +775,7 @@
         <v>4680</v>
       </c>
       <c r="V2" t="n">
-        <v>48939.95174402206</v>
+        <v>15008.25186816677</v>
       </c>
       <c r="W2" t="n">
         <v>-26.14313661539639</v>
@@ -814,13 +814,13 @@
         <v>0</v>
       </c>
       <c r="AI2" t="n">
-        <v>4543.620153217147</v>
+        <v>4809.641312765598</v>
       </c>
       <c r="AJ2" t="n">
         <v>0</v>
       </c>
       <c r="AK2" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL2" t="n">
         <v>302</v>
@@ -832,7 +832,7 @@
         <v>77.49393656635976</v>
       </c>
       <c r="AO2" t="n">
-        <v>4835.62164174085</v>
+        <v>1590.821641740849</v>
       </c>
       <c r="AP2" t="n">
         <v>25.49393656635976</v>
@@ -874,7 +874,7 @@
         <v>226.9606994594122</v>
       </c>
       <c r="BC2" t="n">
-        <v>224.9299715619468</v>
+        <v>225.4311810455798</v>
       </c>
     </row>
     <row r="3">
@@ -942,7 +942,7 @@
         <v>4680</v>
       </c>
       <c r="V3" t="n">
-        <v>48939.95174402204</v>
+        <v>15008.25186816676</v>
       </c>
       <c r="W3" t="n">
         <v>-15.68588196923784</v>
@@ -981,13 +981,13 @@
         <v>0</v>
       </c>
       <c r="AI3" t="n">
-        <v>7956.193020083265</v>
+        <v>8977.607177841677</v>
       </c>
       <c r="AJ3" t="n">
-        <v>26095.85575850611</v>
+        <v>11513.51457947194</v>
       </c>
       <c r="AK3" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL3" t="n">
         <v>302</v>
@@ -999,7 +999,7 @@
         <v>82.04602606178787</v>
       </c>
       <c r="AO3" t="n">
-        <v>5119.672026255563</v>
+        <v>1874.872026255563</v>
       </c>
       <c r="AP3" t="n">
         <v>30.04602606178787</v>
@@ -1011,10 +1011,10 @@
         <v>3</v>
       </c>
       <c r="AS3" t="n">
-        <v>0</v>
+        <v>329.3132493637388</v>
       </c>
       <c r="AT3" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU3" t="n">
         <v>0</v>
@@ -1038,10 +1038,10 @@
         <v>500</v>
       </c>
       <c r="BB3" t="n">
-        <v>224.9299715619468</v>
+        <v>225.4311810455798</v>
       </c>
       <c r="BC3" t="n">
-        <v>223.0338552390597</v>
+        <v>223.6813207226634</v>
       </c>
     </row>
     <row r="4">
@@ -1109,7 +1109,7 @@
         <v>4680</v>
       </c>
       <c r="V4" t="n">
-        <v>48939.95174402204</v>
+        <v>15008.25186816676</v>
       </c>
       <c r="W4" t="n">
         <v>-5.228627323079278</v>
@@ -1148,13 +1148,13 @@
         <v>0</v>
       </c>
       <c r="AI4" t="n">
-        <v>10790.25519150946</v>
+        <v>12212.24722423189</v>
       </c>
       <c r="AJ4" t="n">
-        <v>53055.94313664488</v>
+        <v>26305.22147201417</v>
       </c>
       <c r="AK4" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL4" t="n">
         <v>302</v>
@@ -1166,7 +1166,7 @@
         <v>86.14069752800373</v>
       </c>
       <c r="AO4" t="n">
-        <v>5375.179525747432</v>
+        <v>2130.379525747433</v>
       </c>
       <c r="AP4" t="n">
         <v>34.14069752800373</v>
@@ -1178,10 +1178,10 @@
         <v>3</v>
       </c>
       <c r="AS4" t="n">
-        <v>0</v>
+        <v>432.0937997478318</v>
       </c>
       <c r="AT4" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU4" t="n">
         <v>0</v>
@@ -1205,10 +1205,10 @@
         <v>500</v>
       </c>
       <c r="BB4" t="n">
-        <v>223.0338552390597</v>
+        <v>223.6813207226634</v>
       </c>
       <c r="BC4" t="n">
-        <v>221.3179507928353</v>
+        <v>222.1305294053409</v>
       </c>
     </row>
     <row r="5">
@@ -1276,13 +1276,13 @@
         <v>4440.8</v>
       </c>
       <c r="V5" t="n">
-        <v>55281.46232548887</v>
+        <v>15947.7878772505</v>
       </c>
       <c r="W5" t="n">
-        <v>5.699733941467123</v>
+        <v>5.575757575757575</v>
       </c>
       <c r="X5" t="n">
-        <v>228.8999113138224</v>
+        <v>228.8585858585859</v>
       </c>
       <c r="Y5" t="n">
         <v>1435.2</v>
@@ -1315,13 +1315,13 @@
         <v>0</v>
       </c>
       <c r="AI5" t="n">
-        <v>17905.26608221402</v>
+        <v>19557.29789469548</v>
       </c>
       <c r="AJ5" t="n">
-        <v>80072.3560251849</v>
+        <v>43039.77570948644</v>
       </c>
       <c r="AK5" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL5" t="n">
         <v>302</v>
@@ -1333,7 +1333,7 @@
         <v>89.96863978565443</v>
       </c>
       <c r="AO5" t="n">
-        <v>5614.043122624837</v>
+        <v>2369.243122624836</v>
       </c>
       <c r="AP5" t="n">
         <v>37.96863978565443</v>
@@ -1345,10 +1345,10 @@
         <v>3</v>
       </c>
       <c r="AS5" t="n">
-        <v>0</v>
+        <v>631.1259180437812</v>
       </c>
       <c r="AT5" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU5" t="n">
         <v>0</v>
@@ -1372,10 +1372,10 @@
         <v>500</v>
       </c>
       <c r="BB5" t="n">
-        <v>221.3179507928353</v>
+        <v>222.1305294053409</v>
       </c>
       <c r="BC5" t="n">
-        <v>220.8639018031953</v>
+        <v>221.0882853388693</v>
       </c>
     </row>
     <row r="6">
@@ -1443,13 +1443,13 @@
         <v>4201.6</v>
       </c>
       <c r="V6" t="n">
-        <v>52381.86452962512</v>
+        <v>13048.19008138676</v>
       </c>
       <c r="W6" t="n">
-        <v>17.19695146409948</v>
+        <v>17.03703703703704</v>
       </c>
       <c r="X6" t="n">
-        <v>232.7323171546998</v>
+        <v>232.679012345679</v>
       </c>
       <c r="Y6" t="n">
         <v>1196</v>
@@ -1482,13 +1482,13 @@
         <v>0</v>
       </c>
       <c r="AI6" t="n">
-        <v>23205.58773066313</v>
+        <v>25210.97285106122</v>
       </c>
       <c r="AJ6" t="n">
-        <v>128387.6862987642</v>
+        <v>69898.86340028018</v>
       </c>
       <c r="AK6" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL6" t="n">
         <v>302</v>
@@ -1500,7 +1500,7 @@
         <v>93.48145309779147</v>
       </c>
       <c r="AO6" t="n">
-        <v>5833.242673302188</v>
+        <v>2588.442673302188</v>
       </c>
       <c r="AP6" t="n">
         <v>41.48145309779147</v>
@@ -1512,10 +1512,10 @@
         <v>3</v>
       </c>
       <c r="AS6" t="n">
-        <v>0</v>
+        <v>810.4805783812471</v>
       </c>
       <c r="AT6" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU6" t="n">
         <v>0</v>
@@ -1539,10 +1539,10 @@
         <v>500</v>
       </c>
       <c r="BB6" t="n">
-        <v>220.8639018031953</v>
+        <v>221.0882853388693</v>
       </c>
       <c r="BC6" t="n">
-        <v>220.621351866741</v>
+        <v>220.231045410163</v>
       </c>
     </row>
     <row r="7">
@@ -1610,13 +1610,13 @@
         <v>3962.4</v>
       </c>
       <c r="V7" t="n">
-        <v>49482.26673376142</v>
+        <v>10148.59228552304</v>
       </c>
       <c r="W7" t="n">
-        <v>28.69384288747346</v>
+        <v>28.47619047619047</v>
       </c>
       <c r="X7" t="n">
-        <v>236.5646142958245</v>
+        <v>236.4920634920635</v>
       </c>
       <c r="Y7" t="n">
         <v>956.8000000000001</v>
@@ -1649,13 +1649,13 @@
         <v>0</v>
       </c>
       <c r="AI7" t="n">
-        <v>27868.85533783479</v>
+        <v>30041.34656013166</v>
       </c>
       <c r="AJ7" t="n">
-        <v>175704.329248657</v>
+        <v>98015.17649231029</v>
       </c>
       <c r="AK7" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL7" t="n">
         <v>302</v>
@@ -1667,7 +1667,7 @@
         <v>96.5037138984838</v>
       </c>
       <c r="AO7" t="n">
-        <v>6021.831747265389</v>
+        <v>2777.031747265389</v>
       </c>
       <c r="AP7" t="n">
         <v>44.5037138984838</v>
@@ -1679,10 +1679,10 @@
         <v>3</v>
       </c>
       <c r="AS7" t="n">
-        <v>0</v>
+        <v>971.5025980843435</v>
       </c>
       <c r="AT7" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU7" t="n">
         <v>0</v>
@@ -1706,10 +1706,10 @@
         <v>500</v>
       </c>
       <c r="BB7" t="n">
-        <v>220.621351866741</v>
+        <v>220.231045410163</v>
       </c>
       <c r="BC7" t="n">
-        <v>220.5441645937615</v>
+        <v>219.5161370911698</v>
       </c>
     </row>
     <row r="8">
@@ -1777,13 +1777,13 @@
         <v>3723.2</v>
       </c>
       <c r="V8" t="n">
-        <v>46582.6689378977</v>
+        <v>7248.994489659317</v>
       </c>
       <c r="W8" t="n">
-        <v>40.19034731619305</v>
+        <v>39.86666666666667</v>
       </c>
       <c r="X8" t="n">
-        <v>240.396782438731</v>
+        <v>240.2888888888889</v>
       </c>
       <c r="Y8" t="n">
         <v>717.6</v>
@@ -1816,13 +1816,13 @@
         <v>0</v>
       </c>
       <c r="AI8" t="n">
-        <v>31979.15451072062</v>
+        <v>34169.76263950856</v>
       </c>
       <c r="AJ8" t="n">
-        <v>221136.5001688582</v>
+        <v>126305.7716277646</v>
       </c>
       <c r="AK8" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL8" t="n">
         <v>302</v>
@@ -1834,7 +1834,7 @@
         <v>99.05039555604031</v>
       </c>
       <c r="AO8" t="n">
-        <v>6180.744682696915</v>
+        <v>2935.944682696916</v>
       </c>
       <c r="AP8" t="n">
         <v>47.05039555604031</v>
@@ -1846,10 +1846,10 @@
         <v>3</v>
       </c>
       <c r="AS8" t="n">
-        <v>0</v>
+        <v>1115.621328190638</v>
       </c>
       <c r="AT8" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU8" t="n">
         <v>0</v>
@@ -1873,10 +1873,10 @@
         <v>500</v>
       </c>
       <c r="BB8" t="n">
-        <v>220.5441645937615</v>
+        <v>219.5161370911698</v>
       </c>
       <c r="BC8" t="n">
-        <v>220.6347069338855</v>
+        <v>218.948445605419</v>
       </c>
     </row>
     <row r="9">
@@ -1944,13 +1944,13 @@
         <v>3484</v>
       </c>
       <c r="V9" t="n">
-        <v>43683.07114203394</v>
+        <v>4349.396693795587</v>
       </c>
       <c r="W9" t="n">
-        <v>51.68638768638769</v>
+        <v>51.11111111111111</v>
       </c>
       <c r="X9" t="n">
-        <v>244.2287958954626</v>
+        <v>244.037037037037</v>
       </c>
       <c r="Y9" t="n">
         <v>478.4</v>
@@ -1983,13 +1983,13 @@
         <v>0</v>
       </c>
       <c r="AI9" t="n">
-        <v>35604.22122262369</v>
+        <v>37693.04201635743</v>
       </c>
       <c r="AJ9" t="n">
-        <v>263935.0684396337</v>
+        <v>153869.6421162079</v>
       </c>
       <c r="AK9" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL9" t="n">
         <v>302</v>
@@ -2001,7 +2001,7 @@
         <v>101.1336448813473</v>
       </c>
       <c r="AO9" t="n">
-        <v>6310.739440596073</v>
+        <v>3065.939440596073</v>
       </c>
       <c r="AP9" t="n">
         <v>49.13364488134732</v>
@@ -2013,10 +2013,10 @@
         <v>3</v>
       </c>
       <c r="AS9" t="n">
-        <v>0</v>
+        <v>1244.019462749877</v>
       </c>
       <c r="AT9" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU9" t="n">
         <v>0</v>
@@ -2040,10 +2040,10 @@
         <v>500</v>
       </c>
       <c r="BB9" t="n">
-        <v>220.6347069338855</v>
+        <v>218.948445605419</v>
       </c>
       <c r="BC9" t="n">
-        <v>220.9028375006855</v>
+        <v>218.5346448429478</v>
       </c>
     </row>
     <row r="10">
@@ -2111,13 +2111,13 @@
         <v>3244.8</v>
       </c>
       <c r="V10" t="n">
-        <v>40783.47334617023</v>
+        <v>1449.798897931863</v>
       </c>
       <c r="W10" t="n">
-        <v>63.18186501803194</v>
+        <v>61.33333333333334</v>
       </c>
       <c r="X10" t="n">
-        <v>248.0606216726773</v>
+        <v>247.4444444444444</v>
       </c>
       <c r="Y10" t="n">
         <v>239.2</v>
@@ -2150,13 +2150,13 @@
         <v>0</v>
       </c>
       <c r="AI10" t="n">
-        <v>38799.01260469509</v>
+        <v>40689.16999579535</v>
       </c>
       <c r="AJ10" t="n">
-        <v>303466.0388375637</v>
+        <v>179956.8941547487</v>
       </c>
       <c r="AK10" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL10" t="n">
         <v>302</v>
@@ -2168,7 +2168,7 @@
         <v>102.7630919843723</v>
       </c>
       <c r="AO10" t="n">
-        <v>6412.416939824831</v>
+        <v>3167.616939824831</v>
       </c>
       <c r="AP10" t="n">
         <v>50.76309198437229</v>
@@ -2180,10 +2180,10 @@
         <v>3</v>
       </c>
       <c r="AS10" t="n">
-        <v>0</v>
+        <v>1357.68173501815</v>
       </c>
       <c r="AT10" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU10" t="n">
         <v>0</v>
@@ -2207,10 +2207,10 @@
         <v>500</v>
       </c>
       <c r="BB10" t="n">
-        <v>220.9028375006855</v>
+        <v>218.5346448429478</v>
       </c>
       <c r="BC10" t="n">
-        <v>221.3586513121523</v>
+        <v>218.2768135330926</v>
       </c>
     </row>
     <row r="11">
@@ -2278,13 +2278,13 @@
         <v>2995.2</v>
       </c>
       <c r="V11" t="n">
-        <v>39465.22519890137</v>
+        <v>0</v>
       </c>
       <c r="W11" t="n">
-        <v>74.92</v>
+        <v>75</v>
       </c>
       <c r="X11" t="n">
-        <v>251.9733333333333</v>
+        <v>252</v>
       </c>
       <c r="Y11" t="n">
         <v>0</v>
@@ -2317,13 +2317,13 @@
         <v>0</v>
       </c>
       <c r="AI11" t="n">
-        <v>43476.95841281787</v>
+        <v>46768.14544980528</v>
       </c>
       <c r="AJ11" t="n">
-        <v>339193.9725566463</v>
+        <v>203945.1990320346</v>
       </c>
       <c r="AK11" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL11" t="n">
         <v>302</v>
@@ -2335,7 +2335,7 @@
         <v>103.9668856017163</v>
       </c>
       <c r="AO11" t="n">
-        <v>6487.533661547096</v>
+        <v>3242.733661547096</v>
       </c>
       <c r="AP11" t="n">
         <v>51.96688560171629</v>
@@ -2347,10 +2347,10 @@
         <v>3</v>
       </c>
       <c r="AS11" t="n">
-        <v>0</v>
+        <v>1459.450899384659</v>
       </c>
       <c r="AT11" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU11" t="n">
         <v>0</v>
@@ -2374,10 +2374,10 @@
         <v>500</v>
       </c>
       <c r="BB11" t="n">
-        <v>221.3586513121523</v>
+        <v>218.2768135330926</v>
       </c>
       <c r="BC11" t="n">
-        <v>222.0430850950196</v>
+        <v>218.2506154287172</v>
       </c>
     </row>
     <row r="12">
@@ -2445,13 +2445,13 @@
         <v>2745.6</v>
       </c>
       <c r="V12" t="n">
-        <v>36308.00718298926</v>
+        <v>0</v>
       </c>
       <c r="W12" t="n">
-        <v>86.91304347826087</v>
+        <v>87</v>
       </c>
       <c r="X12" t="n">
-        <v>255.9710144927536</v>
+        <v>256</v>
       </c>
       <c r="Y12" t="n">
         <v>0</v>
@@ -2484,13 +2484,13 @@
         <v>0</v>
       </c>
       <c r="AI12" t="n">
-        <v>46140.44889262198</v>
+        <v>52242.04521738145</v>
       </c>
       <c r="AJ12" t="n">
-        <v>371936.5790305276</v>
+        <v>226828.9570850847</v>
       </c>
       <c r="AK12" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL12" t="n">
         <v>302</v>
@@ -2502,7 +2502,7 @@
         <v>104.7209936558745</v>
       </c>
       <c r="AO12" t="n">
-        <v>6534.59000412657</v>
+        <v>3289.790004126569</v>
       </c>
       <c r="AP12" t="n">
         <v>52.72099365587451</v>
@@ -2514,10 +2514,10 @@
         <v>3</v>
       </c>
       <c r="AS12" t="n">
-        <v>0</v>
+        <v>1549.157092777992</v>
       </c>
       <c r="AT12" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU12" t="n">
         <v>0</v>
@@ -2541,10 +2541,10 @@
         <v>500</v>
       </c>
       <c r="BB12" t="n">
-        <v>222.0430850950196</v>
+        <v>218.2506154287172</v>
       </c>
       <c r="BC12" t="n">
-        <v>222.9507077700802</v>
+        <v>218.5348502718074</v>
       </c>
     </row>
     <row r="13">
@@ -2612,13 +2612,13 @@
         <v>2496</v>
       </c>
       <c r="V13" t="n">
-        <v>33150.78916707716</v>
+        <v>0</v>
       </c>
       <c r="W13" t="n">
-        <v>98.9047619047619</v>
+        <v>99</v>
       </c>
       <c r="X13" t="n">
-        <v>259.968253968254</v>
+        <v>260</v>
       </c>
       <c r="Y13" t="n">
         <v>0</v>
@@ -2651,13 +2651,13 @@
         <v>0</v>
       </c>
       <c r="AI13" t="n">
-        <v>48443.53473649127</v>
+        <v>57250.72194976862</v>
       </c>
       <c r="AJ13" t="n">
-        <v>399625.8299652084</v>
+        <v>247484.8473477278</v>
       </c>
       <c r="AK13" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL13" t="n">
         <v>302</v>
@@ -2669,7 +2669,7 @@
         <v>104.99834983049</v>
       </c>
       <c r="AO13" t="n">
-        <v>6551.897029422575</v>
+        <v>3307.097029422575</v>
       </c>
       <c r="AP13" t="n">
         <v>52.99834983048999</v>
@@ -2681,10 +2681,10 @@
         <v>3</v>
       </c>
       <c r="AS13" t="n">
-        <v>0</v>
+        <v>1625.131978456381</v>
       </c>
       <c r="AT13" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU13" t="n">
         <v>0</v>
@@ -2708,10 +2708,10 @@
         <v>500</v>
       </c>
       <c r="BB13" t="n">
-        <v>222.9507077700802</v>
+        <v>218.5348502718074</v>
       </c>
       <c r="BC13" t="n">
-        <v>224.0893058491556</v>
+        <v>219.1420000489811</v>
       </c>
     </row>
     <row r="14">
@@ -2779,13 +2779,13 @@
         <v>2246.4</v>
       </c>
       <c r="V14" t="n">
-        <v>29993.57115116504</v>
+        <v>0</v>
       </c>
       <c r="W14" t="n">
-        <v>110.8947368421053</v>
+        <v>111</v>
       </c>
       <c r="X14" t="n">
-        <v>263.9649122807018</v>
+        <v>264</v>
       </c>
       <c r="Y14" t="n">
         <v>0</v>
@@ -2818,13 +2818,13 @@
         <v>0</v>
       </c>
       <c r="AI14" t="n">
-        <v>50414.5541482565</v>
+        <v>61850.68423909927</v>
       </c>
       <c r="AJ14" t="n">
-        <v>421919.2717764943</v>
+        <v>265284.7150103289</v>
       </c>
       <c r="AK14" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL14" t="n">
         <v>302</v>
@@ -2836,7 +2836,7 @@
         <v>104.8002642006774</v>
       </c>
       <c r="AO14" t="n">
-        <v>6539.536486122267</v>
+        <v>3294.736486122267</v>
       </c>
       <c r="AP14" t="n">
         <v>52.80026420067736</v>
@@ -2848,10 +2848,10 @@
         <v>3</v>
       </c>
       <c r="AS14" t="n">
-        <v>0</v>
+        <v>1687.915593292729</v>
       </c>
       <c r="AT14" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU14" t="n">
         <v>0</v>
@@ -2875,10 +2875,10 @@
         <v>500</v>
       </c>
       <c r="BB14" t="n">
-        <v>224.0893058491556</v>
+        <v>219.1420000489811</v>
       </c>
       <c r="BC14" t="n">
-        <v>225.466016413486</v>
+        <v>220.0799332532034</v>
       </c>
     </row>
     <row r="15">
@@ -2946,13 +2946,13 @@
         <v>1996.8</v>
       </c>
       <c r="V15" t="n">
-        <v>26836.35313525294</v>
+        <v>0</v>
       </c>
       <c r="W15" t="n">
-        <v>122.8823529411765</v>
+        <v>123</v>
       </c>
       <c r="X15" t="n">
-        <v>267.9607843137255</v>
+        <v>268</v>
       </c>
       <c r="Y15" t="n">
         <v>0</v>
@@ -2985,13 +2985,13 @@
         <v>0</v>
       </c>
       <c r="AI15" t="n">
-        <v>52076.06808737793</v>
+        <v>66090.25786249049</v>
       </c>
       <c r="AJ15" t="n">
-        <v>438548.2020312129</v>
+        <v>279695.936161857</v>
       </c>
       <c r="AK15" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL15" t="n">
         <v>302</v>
@@ -3003,7 +3003,7 @@
         <v>104.1258016125071</v>
       </c>
       <c r="AO15" t="n">
-        <v>6497.450020620441</v>
+        <v>3252.650020620441</v>
       </c>
       <c r="AP15" t="n">
         <v>52.12580161250708</v>
@@ -3015,10 +3015,10 @@
         <v>3</v>
       </c>
       <c r="AS15" t="n">
-        <v>0</v>
+        <v>1737.951845292605</v>
       </c>
       <c r="AT15" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU15" t="n">
         <v>0</v>
@@ -3042,10 +3042,10 @@
         <v>500</v>
       </c>
       <c r="BB15" t="n">
-        <v>225.466016413486</v>
+        <v>220.0799332532034</v>
       </c>
       <c r="BC15" t="n">
-        <v>227.0876262175159</v>
+        <v>221.3553969960361</v>
       </c>
     </row>
     <row r="16">
@@ -3113,13 +3113,13 @@
         <v>1747.2</v>
       </c>
       <c r="V16" t="n">
-        <v>23679.13511934083</v>
+        <v>0</v>
       </c>
       <c r="W16" t="n">
-        <v>134.8666666666667</v>
+        <v>135</v>
       </c>
       <c r="X16" t="n">
-        <v>271.9555555555556</v>
+        <v>272</v>
       </c>
       <c r="Y16" t="n">
         <v>0</v>
@@ -3152,13 +3152,13 @@
         <v>0</v>
       </c>
       <c r="AI16" t="n">
-        <v>53445.64482812858</v>
+        <v>70011.25998380958</v>
       </c>
       <c r="AJ16" t="n">
-        <v>449312.854881048</v>
+        <v>290271.85390487</v>
       </c>
       <c r="AK16" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL16" t="n">
         <v>302</v>
@@ -3170,7 +3170,7 @@
         <v>102.9717594725458</v>
       </c>
       <c r="AO16" t="n">
-        <v>6425.437791086861</v>
+        <v>3180.63779108686</v>
       </c>
       <c r="AP16" t="n">
         <v>50.97175947254584</v>
@@ -3182,10 +3182,10 @@
         <v>3</v>
       </c>
       <c r="AS16" t="n">
-        <v>0</v>
+        <v>1775.60069041958</v>
       </c>
       <c r="AT16" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU16" t="n">
         <v>0</v>
@@ -3209,10 +3209,10 @@
         <v>500</v>
       </c>
       <c r="BB16" t="n">
-        <v>227.0876262175159</v>
+        <v>221.3553969960361</v>
       </c>
       <c r="BC16" t="n">
-        <v>228.9608064194144</v>
+        <v>222.9761367009934</v>
       </c>
     </row>
     <row r="17">
@@ -3280,13 +3280,13 @@
         <v>1497.6</v>
       </c>
       <c r="V17" t="n">
-        <v>20521.91710342871</v>
+        <v>0</v>
       </c>
       <c r="W17" t="n">
-        <v>146.8461538461538</v>
+        <v>147</v>
       </c>
       <c r="X17" t="n">
-        <v>275.948717948718</v>
+        <v>276</v>
       </c>
       <c r="Y17" t="n">
         <v>0</v>
@@ -3319,13 +3319,13 @@
         <v>0</v>
       </c>
       <c r="AI17" t="n">
-        <v>54536.42256796331</v>
+        <v>73650.35945072916</v>
       </c>
       <c r="AJ17" t="n">
-        <v>454079.3943563246</v>
+        <v>296644.6417244546</v>
       </c>
       <c r="AK17" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL17" t="n">
         <v>302</v>
@@ -3337,7 +3337,7 @@
         <v>101.3325909419153</v>
       </c>
       <c r="AO17" t="n">
-        <v>6323.153674775516</v>
+        <v>3078.353674775517</v>
       </c>
       <c r="AP17" t="n">
         <v>49.33259094191533</v>
@@ -3349,10 +3349,10 @@
         <v>3</v>
       </c>
       <c r="AS17" t="n">
-        <v>0</v>
+        <v>1801.147510863156</v>
       </c>
       <c r="AT17" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU17" t="n">
         <v>0</v>
@@ -3376,10 +3376,10 @@
         <v>500</v>
       </c>
       <c r="BB17" t="n">
-        <v>228.9608064194144</v>
+        <v>222.9761367009934</v>
       </c>
       <c r="BC17" t="n">
-        <v>231.0922813925373</v>
+        <v>224.9524983173323</v>
       </c>
     </row>
     <row r="18">
@@ -3447,13 +3447,13 @@
         <v>1248</v>
       </c>
       <c r="V18" t="n">
-        <v>17364.6990875166</v>
+        <v>0</v>
       </c>
       <c r="W18" t="n">
-        <v>158.8181818181818</v>
+        <v>159</v>
       </c>
       <c r="X18" t="n">
-        <v>279.9393939393939</v>
+        <v>280</v>
       </c>
       <c r="Y18" t="n">
         <v>0</v>
@@ -3486,13 +3486,13 @@
         <v>0</v>
       </c>
       <c r="AI18" t="n">
-        <v>55357.48781382537</v>
+        <v>77040.21663236298</v>
       </c>
       <c r="AJ18" t="n">
-        <v>452778.5768840038</v>
+        <v>298520.2530645037</v>
       </c>
       <c r="AK18" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL18" t="n">
         <v>302</v>
@@ -3504,7 +3504,7 @@
         <v>99.20026917888214</v>
       </c>
       <c r="AO18" t="n">
-        <v>6190.096796762246</v>
+        <v>2945.296796762245</v>
       </c>
       <c r="AP18" t="n">
         <v>47.20026917888214</v>
@@ -3516,10 +3516,10 @@
         <v>3</v>
       </c>
       <c r="AS18" t="n">
-        <v>0</v>
+        <v>1814.810261438687</v>
       </c>
       <c r="AT18" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU18" t="n">
         <v>0</v>
@@ -3543,10 +3543,10 @@
         <v>500</v>
       </c>
       <c r="BB18" t="n">
-        <v>231.0922813925373</v>
+        <v>224.9524983173323</v>
       </c>
       <c r="BC18" t="n">
-        <v>233.4889280682864</v>
+        <v>227.2990667177201</v>
       </c>
     </row>
     <row r="19">
@@ -3614,13 +3614,13 @@
         <v>998.3999999999999</v>
       </c>
       <c r="V19" t="n">
-        <v>14207.48107160449</v>
+        <v>0</v>
       </c>
       <c r="W19" t="n">
-        <v>170.7777777777778</v>
+        <v>171</v>
       </c>
       <c r="X19" t="n">
-        <v>283.9259259259259</v>
+        <v>284</v>
       </c>
       <c r="Y19" t="n">
         <v>0</v>
@@ -3653,13 +3653,13 @@
         <v>0</v>
       </c>
       <c r="AI19" t="n">
-        <v>55914.09232218968</v>
+        <v>80210.47826520583</v>
       </c>
       <c r="AJ19" t="n">
-        <v>445406.0435246101</v>
+        <v>295675.2440302533</v>
       </c>
       <c r="AK19" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL19" t="n">
         <v>302</v>
@@ -3671,7 +3671,7 @@
         <v>96.56408470823459</v>
       </c>
       <c r="AO19" t="n">
-        <v>6025.598885793838</v>
+        <v>2780.798885793838</v>
       </c>
       <c r="AP19" t="n">
         <v>44.56408470823459</v>
@@ -3683,10 +3683,10 @@
         <v>3</v>
       </c>
       <c r="AS19" t="n">
-        <v>0</v>
+        <v>1816.744798511666</v>
       </c>
       <c r="AT19" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU19" t="n">
         <v>0</v>
@@ -3710,10 +3710,10 @@
         <v>500</v>
       </c>
       <c r="BB19" t="n">
-        <v>233.4889280682864</v>
+        <v>227.2990667177201</v>
       </c>
       <c r="BC19" t="n">
-        <v>236.1577902653766</v>
+        <v>230.0368609207815</v>
       </c>
     </row>
     <row r="20">
@@ -3781,13 +3781,13 @@
         <v>748.7999999999998</v>
       </c>
       <c r="V20" t="n">
-        <v>11050.26305569239</v>
+        <v>0</v>
       </c>
       <c r="W20" t="n">
-        <v>182.7142857142857</v>
+        <v>183</v>
       </c>
       <c r="X20" t="n">
-        <v>287.9047619047619</v>
+        <v>288</v>
       </c>
       <c r="Y20" t="n">
         <v>0</v>
@@ -3820,13 +3820,13 @@
         <v>0</v>
       </c>
       <c r="AI20" t="n">
-        <v>56207.71877635512</v>
+        <v>83188.69353686424</v>
       </c>
       <c r="AJ20" t="n">
-        <v>432024.2998567366</v>
+        <v>287955.3667448947</v>
       </c>
       <c r="AK20" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL20" t="n">
         <v>302</v>
@@ -3838,7 +3838,7 @@
         <v>93.41036357686392</v>
       </c>
       <c r="AO20" t="n">
-        <v>5828.806687196308</v>
+        <v>2584.006687196308</v>
       </c>
       <c r="AP20" t="n">
         <v>41.41036357686392</v>
@@ -3850,10 +3850,10 @@
         <v>3</v>
       </c>
       <c r="AS20" t="n">
-        <v>0</v>
+        <v>1807.048696794647</v>
       </c>
       <c r="AT20" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU20" t="n">
         <v>0</v>
@@ -3877,10 +3877,10 @@
         <v>500</v>
       </c>
       <c r="BB20" t="n">
-        <v>236.1577902653766</v>
+        <v>230.0368609207815</v>
       </c>
       <c r="BC20" t="n">
-        <v>239.1059690477155</v>
+        <v>233.1968334687808</v>
       </c>
     </row>
     <row r="21">
@@ -3948,13 +3948,13 @@
         <v>499.1999999999999</v>
       </c>
       <c r="V21" t="n">
-        <v>7893.045039780274</v>
+        <v>0</v>
       </c>
       <c r="W21" t="n">
-        <v>194.6</v>
+        <v>195</v>
       </c>
       <c r="X21" t="n">
-        <v>291.8666666666667</v>
+        <v>292</v>
       </c>
       <c r="Y21" t="n">
         <v>0</v>
@@ -3987,13 +3987,13 @@
         <v>0</v>
       </c>
       <c r="AI21" t="n">
-        <v>56235.99352496694</v>
+        <v>86001.21636129919</v>
       </c>
       <c r="AJ21" t="n">
-        <v>412766.5478714991</v>
+        <v>275275.935957937</v>
       </c>
       <c r="AK21" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL21" t="n">
         <v>302</v>
@@ -4005,7 +4005,7 @@
         <v>89.72208813367109</v>
       </c>
       <c r="AO21" t="n">
-        <v>5598.658299541076</v>
+        <v>2353.858299541076</v>
       </c>
       <c r="AP21" t="n">
         <v>37.72208813367109</v>
@@ -4017,10 +4017,10 @@
         <v>3</v>
       </c>
       <c r="AS21" t="n">
-        <v>0</v>
+        <v>1785.763782645116</v>
       </c>
       <c r="AT21" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU21" t="n">
         <v>0</v>
@@ -4044,10 +4044,10 @@
         <v>500</v>
       </c>
       <c r="BB21" t="n">
-        <v>239.1059690477155</v>
+        <v>233.1968334687808</v>
       </c>
       <c r="BC21" t="n">
-        <v>242.3403050646783</v>
+        <v>236.8260899717558</v>
       </c>
     </row>
     <row r="22">
@@ -4115,13 +4115,13 @@
         <v>249.5999999999999</v>
       </c>
       <c r="V22" t="n">
-        <v>4735.827023868163</v>
+        <v>0</v>
       </c>
       <c r="W22" t="n">
-        <v>206.3333333333333</v>
+        <v>207</v>
       </c>
       <c r="X22" t="n">
-        <v>295.7777777777778</v>
+        <v>296</v>
       </c>
       <c r="Y22" t="n">
         <v>0</v>
@@ -4154,13 +4154,13 @@
         <v>0</v>
       </c>
       <c r="AI22" t="n">
-        <v>55992.43200270776</v>
+        <v>88674.16625156651</v>
       </c>
       <c r="AJ22" t="n">
-        <v>387842.6623253361</v>
+        <v>257624.0825957633</v>
       </c>
       <c r="AK22" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL22" t="n">
         <v>302</v>
@@ -4172,7 +4172,7 @@
         <v>85.4783942384322</v>
       </c>
       <c r="AO22" t="n">
-        <v>5333.851800478169</v>
+        <v>2089.051800478169</v>
       </c>
       <c r="AP22" t="n">
         <v>33.4783942384322</v>
@@ -4184,10 +4184,10 @@
         <v>3</v>
       </c>
       <c r="AS22" t="n">
-        <v>0</v>
+        <v>1752.877562568534</v>
       </c>
       <c r="AT22" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU22" t="n">
         <v>0</v>
@@ -4211,10 +4211,10 @@
         <v>500</v>
       </c>
       <c r="BB22" t="n">
-        <v>242.3403050646783</v>
+        <v>236.8260899717558</v>
       </c>
       <c r="BC22" t="n">
-        <v>245.8666755818656</v>
+        <v>240.9999668932002</v>
       </c>
     </row>
     <row r="23">
@@ -4282,13 +4282,13 @@
         <v>0</v>
       </c>
       <c r="V23" t="n">
-        <v>1578.609007956054</v>
+        <v>0</v>
       </c>
       <c r="W23" t="n">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="X23" t="n">
-        <v>299.3333333333333</v>
+        <v>300</v>
       </c>
       <c r="Y23" t="n">
         <v>0</v>
@@ -4321,13 +4321,13 @@
         <v>0</v>
       </c>
       <c r="AI23" t="n">
-        <v>55465.98706720017</v>
+        <v>91234.53911566269</v>
       </c>
       <c r="AJ23" t="n">
-        <v>357547.7707914739</v>
+        <v>235063.1384211905</v>
       </c>
       <c r="AK23" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL23" t="n">
         <v>302</v>
@@ -4339,7 +4339,7 @@
         <v>80.65390720390053</v>
       </c>
       <c r="AO23" t="n">
-        <v>5032.803809523393</v>
+        <v>1788.003809523393</v>
       </c>
       <c r="AP23" t="n">
         <v>28.65390720390053</v>
@@ -4351,10 +4351,10 @@
         <v>3</v>
       </c>
       <c r="AS23" t="n">
-        <v>0</v>
+        <v>1708.323702110393</v>
       </c>
       <c r="AT23" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU23" t="n">
         <v>0</v>
@@ -4378,10 +4378,10 @@
         <v>500</v>
       </c>
       <c r="BB23" t="n">
-        <v>245.8666755818656</v>
+        <v>240.9999668932002</v>
       </c>
       <c r="BC23" t="n">
-        <v>249.6885194253123</v>
+        <v>245.8478302358911</v>
       </c>
     </row>
     <row r="24">
@@ -4488,13 +4488,13 @@
         <v>0</v>
       </c>
       <c r="AI24" t="n">
-        <v>29554.86840171283</v>
+        <v>49414.67696447067</v>
       </c>
       <c r="AJ24" t="n">
-        <v>322274.1273427026</v>
+        <v>207739.5636526302</v>
       </c>
       <c r="AK24" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL24" t="n">
         <v>302</v>
@@ -4506,7 +4506,7 @@
         <v>76.54941206232553</v>
       </c>
       <c r="AO24" t="n">
-        <v>4776.683312689113</v>
+        <v>1531.883312689113</v>
       </c>
       <c r="AP24" t="n">
         <v>24.54941206232553</v>
@@ -4518,10 +4518,10 @@
         <v>3</v>
       </c>
       <c r="AS24" t="n">
-        <v>0</v>
+        <v>1689.712676798973</v>
       </c>
       <c r="AT24" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU24" t="n">
         <v>0</v>
@@ -4545,10 +4545,10 @@
         <v>500</v>
       </c>
       <c r="BB24" t="n">
-        <v>249.6885194253123</v>
+        <v>245.8478302358911</v>
       </c>
       <c r="BC24" t="n">
-        <v>251.8712734632473</v>
+        <v>248.7492613416833</v>
       </c>
     </row>
     <row r="25">
@@ -4655,13 +4655,13 @@
         <v>0</v>
       </c>
       <c r="AI25" t="n">
-        <v>52536.81108489564</v>
+        <v>82043.59821428305</v>
       </c>
       <c r="AJ25" t="n">
-        <v>301749.9172158669</v>
+        <v>191529.2451701057</v>
       </c>
       <c r="AK25" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL25" t="n">
         <v>302</v>
@@ -4673,7 +4673,7 @@
         <v>72.18722134676915</v>
       </c>
       <c r="AO25" t="n">
-        <v>4504.482612038395</v>
+        <v>1259.682612038395</v>
       </c>
       <c r="AP25" t="n">
         <v>20.18722134676915</v>
@@ -4712,10 +4712,10 @@
         <v>500</v>
       </c>
       <c r="BB25" t="n">
-        <v>251.8712734632473</v>
+        <v>248.7492613416833</v>
       </c>
       <c r="BC25" t="n">
-        <v>255.6382276421844</v>
+        <v>250.8943198892712</v>
       </c>
     </row>
     <row r="26">
@@ -4732,40 +4732,40 @@
         <v>307.9705928522</v>
       </c>
       <c r="E26" t="n">
-        <v>256.4558892783</v>
+        <v>255.5039257395192</v>
       </c>
       <c r="F26" t="n">
-        <v>240.5186813850825</v>
+        <v>239.9470648510229</v>
       </c>
       <c r="G26" t="n">
-        <v>312.4852964261</v>
+        <v>312.1679752465064</v>
       </c>
       <c r="H26" t="n">
-        <v>249.68383391745</v>
+        <v>249.2078521480596</v>
       </c>
       <c r="I26" t="n">
-        <v>236.5540855056332</v>
+        <v>236.2842119679544</v>
       </c>
       <c r="J26" t="n">
-        <v>310.22794463915</v>
+        <v>310.0692840493532</v>
       </c>
       <c r="K26" t="n">
-        <v>273.4934190443298</v>
+        <v>273.273050812584</v>
       </c>
       <c r="L26" t="n">
-        <v>13.54411072169998</v>
+        <v>12.59214718291921</v>
       </c>
       <c r="M26" t="n">
-        <v>29.6042296756933</v>
+        <v>29.50076336153666</v>
       </c>
       <c r="N26" t="n">
-        <v>15.57763975012023</v>
+        <v>14.46792634516044</v>
       </c>
       <c r="O26" t="n">
-        <v>63.86027680425002</v>
+        <v>64.653579753234</v>
       </c>
       <c r="P26" t="n">
-        <v>9.813582329266808</v>
+        <v>9.131492328164768</v>
       </c>
       <c r="Q26" t="n">
         <v>0</v>
@@ -4774,7 +4774,7 @@
         <v>0</v>
       </c>
       <c r="S26" t="n">
-        <v>124332.1144379776</v>
+        <v>115794.1056577217</v>
       </c>
       <c r="T26" t="n">
         <v>0</v>
@@ -4786,10 +4786,10 @@
         <v>0</v>
       </c>
       <c r="W26" t="n">
-        <v>249.68383391745</v>
+        <v>249.2078521480596</v>
       </c>
       <c r="X26" t="n">
-        <v>310.22794463915</v>
+        <v>310.0692840493532</v>
       </c>
       <c r="Y26" t="n">
         <v>0</v>
@@ -4801,10 +4801,10 @@
         <v>0</v>
       </c>
       <c r="AB26" t="n">
-        <v>249.68383391745</v>
+        <v>249.2078521480596</v>
       </c>
       <c r="AC26" t="n">
-        <v>310.22794463915</v>
+        <v>310.0692840493532</v>
       </c>
       <c r="AD26" t="n">
         <v>18.4349488229219</v>
@@ -4822,13 +4822,13 @@
         <v>0</v>
       </c>
       <c r="AI26" t="n">
-        <v>64963.18025992646</v>
+        <v>99734.7600861197</v>
       </c>
       <c r="AJ26" t="n">
-        <v>268057.489121651</v>
+        <v>190543.4911443599</v>
       </c>
       <c r="AK26" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL26" t="n">
         <v>302</v>
@@ -4837,25 +4837,25 @@
         <v>250</v>
       </c>
       <c r="AN26" t="n">
-        <v>65.44591449436683</v>
+        <v>65.71578803204557</v>
       </c>
       <c r="AO26" t="n">
-        <v>4083.82506444849</v>
+        <v>855.8651731996433</v>
       </c>
       <c r="AP26" t="n">
-        <v>13.44591449436683</v>
+        <v>13.71578803204557</v>
       </c>
       <c r="AQ26" t="n">
-        <v>839.0250644484903</v>
+        <v>855.8651731996433</v>
       </c>
       <c r="AR26" t="n">
         <v>2</v>
       </c>
       <c r="AS26" t="n">
-        <v>100</v>
+        <v>1954.42982969774</v>
       </c>
       <c r="AT26" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="AU26" t="n">
         <v>100</v>
@@ -4879,10 +4879,10 @@
         <v>500</v>
       </c>
       <c r="BB26" t="n">
-        <v>255.6382276421844</v>
+        <v>250.8943198892712</v>
       </c>
       <c r="BC26" t="n">
-        <v>261.0744509168618</v>
+        <v>256.5392840337933</v>
       </c>
     </row>
     <row r="27">
@@ -4890,49 +4890,49 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>256.4558892783</v>
+        <v>255.5039257395192</v>
       </c>
       <c r="C27" t="n">
-        <v>240.5186813850825</v>
+        <v>239.9470648510229</v>
       </c>
       <c r="D27" t="n">
-        <v>312.4852964261</v>
+        <v>312.1679752465064</v>
       </c>
       <c r="E27" t="n">
-        <v>270</v>
+        <v>268.0960729224384</v>
       </c>
       <c r="F27" t="n">
-        <v>249.18333388708</v>
+        <v>247.9033711688031</v>
       </c>
       <c r="G27" t="n">
-        <v>317</v>
+        <v>316.3653576408128</v>
       </c>
       <c r="H27" t="n">
-        <v>263.22794463915</v>
+        <v>261.7999993309788</v>
       </c>
       <c r="I27" t="n">
-        <v>244.7243879864773</v>
+        <v>243.8169400282383</v>
       </c>
       <c r="J27" t="n">
-        <v>314.74264821305</v>
+        <v>314.2666664436596</v>
       </c>
       <c r="K27" t="n">
-        <v>279.9388409451448</v>
+        <v>279.2428480674242</v>
       </c>
       <c r="L27" t="n">
-        <v>13.54411072170001</v>
+        <v>12.59214718291918</v>
       </c>
       <c r="M27" t="n">
-        <v>32.59560004170945</v>
+        <v>32.27567183802313</v>
       </c>
       <c r="N27" t="n">
-        <v>16.07621471394894</v>
+        <v>14.89333681160057</v>
       </c>
       <c r="O27" t="n">
-        <v>41.28675893475003</v>
+        <v>43.66666778170196</v>
       </c>
       <c r="P27" t="n">
-        <v>28.7315012918227</v>
+        <v>26.78305863371935</v>
       </c>
       <c r="Q27" t="n">
         <v>0</v>
@@ -4941,7 +4941,7 @@
         <v>0</v>
       </c>
       <c r="S27" t="n">
-        <v>117374.4557270968</v>
+        <v>109877.3968534481</v>
       </c>
       <c r="T27" t="n">
         <v>0</v>
@@ -4953,10 +4953,10 @@
         <v>0</v>
       </c>
       <c r="W27" t="n">
-        <v>263.22794463915</v>
+        <v>261.7999993309788</v>
       </c>
       <c r="X27" t="n">
-        <v>314.74264821305</v>
+        <v>314.2666664436596</v>
       </c>
       <c r="Y27" t="n">
         <v>0</v>
@@ -4968,13 +4968,13 @@
         <v>0</v>
       </c>
       <c r="AB27" t="n">
-        <v>263.22794463915</v>
+        <v>261.7999993309788</v>
       </c>
       <c r="AC27" t="n">
-        <v>314.74264821305</v>
+        <v>314.2666664436596</v>
       </c>
       <c r="AD27" t="n">
-        <v>18.43494882292208</v>
+        <v>18.43494882292217</v>
       </c>
       <c r="AE27" t="n">
         <v>0</v>
@@ -4989,40 +4989,40 @@
         <v>0</v>
       </c>
       <c r="AI27" t="n">
-        <v>65630.88028562661</v>
+        <v>102027.0208185539</v>
       </c>
       <c r="AJ27" t="n">
-        <v>219546.5527265481</v>
+        <v>156528.377667738</v>
       </c>
       <c r="AK27" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL27" t="n">
         <v>302</v>
       </c>
       <c r="AM27" t="n">
-        <v>248.5224636675087</v>
+        <v>248.7023622890106</v>
       </c>
       <c r="AN27" t="n">
-        <v>57.2756120135227</v>
+        <v>58.18305997176168</v>
       </c>
       <c r="AO27" t="n">
-        <v>3573.998189643817</v>
+        <v>304.8503490721872</v>
       </c>
       <c r="AP27" t="n">
-        <v>3.798075681031378</v>
+        <v>4.885422260772231</v>
       </c>
       <c r="AQ27" t="n">
-        <v>236.999922496358</v>
+        <v>304.8503490721872</v>
       </c>
       <c r="AR27" t="n">
         <v>2</v>
       </c>
       <c r="AS27" t="n">
-        <v>100</v>
+        <v>1921.656952333146</v>
       </c>
       <c r="AT27" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="AU27" t="n">
         <v>100</v>
@@ -5046,10 +5046,10 @@
         <v>500</v>
       </c>
       <c r="BB27" t="n">
-        <v>261.0744509168618</v>
+        <v>256.5392840337933</v>
       </c>
       <c r="BC27" t="n">
-        <v>267.3664935992609</v>
+        <v>262.9159103501156</v>
       </c>
     </row>
     <row r="28">
@@ -5057,49 +5057,49 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
+        <v>268.0960729224384</v>
+      </c>
+      <c r="C28" t="n">
+        <v>247.9033711688031</v>
+      </c>
+      <c r="D28" t="n">
+        <v>316.3653576408128</v>
+      </c>
+      <c r="E28" t="n">
         <v>270</v>
       </c>
-      <c r="C28" t="n">
+      <c r="F28" t="n">
         <v>249.18333388708</v>
-      </c>
-      <c r="D28" t="n">
-        <v>317</v>
-      </c>
-      <c r="E28" t="n">
-        <v>280</v>
-      </c>
-      <c r="F28" t="n">
-        <v>256.2603848366048</v>
       </c>
       <c r="G28" t="n">
         <v>317</v>
       </c>
       <c r="H28" t="n">
-        <v>275</v>
+        <v>269.0480364612192</v>
       </c>
       <c r="I28" t="n">
-        <v>252.6460026601551</v>
+        <v>248.5407361646696</v>
       </c>
       <c r="J28" t="n">
-        <v>317</v>
+        <v>316.6826788204064</v>
       </c>
       <c r="K28" t="n">
-        <v>284.9911960405029</v>
+        <v>282.8176985366475</v>
       </c>
       <c r="L28" t="n">
-        <v>10</v>
+        <v>1.903927077561605</v>
       </c>
       <c r="M28" t="n">
-        <v>35.27895092088615</v>
+        <v>33.91168090449393</v>
       </c>
       <c r="N28" t="n">
-        <v>12.24965043551492</v>
+        <v>2.294168430736113</v>
       </c>
       <c r="O28" t="n">
-        <v>20</v>
+        <v>31.58660589796796</v>
       </c>
       <c r="P28" t="n">
-        <v>44.35399733984491</v>
+        <v>36.55533675776883</v>
       </c>
       <c r="Q28" t="n">
         <v>0</v>
@@ -5108,7 +5108,7 @@
         <v>0</v>
       </c>
       <c r="S28" t="n">
-        <v>79111.87675461078</v>
+        <v>16008.36513104093</v>
       </c>
       <c r="T28" t="n">
         <v>0</v>
@@ -5120,10 +5120,10 @@
         <v>0</v>
       </c>
       <c r="W28" t="n">
-        <v>275</v>
+        <v>269.0480364612192</v>
       </c>
       <c r="X28" t="n">
-        <v>317</v>
+        <v>316.6826788204064</v>
       </c>
       <c r="Y28" t="n">
         <v>0</v>
@@ -5135,13 +5135,13 @@
         <v>0</v>
       </c>
       <c r="AB28" t="n">
-        <v>275</v>
+        <v>269.0480364612192</v>
       </c>
       <c r="AC28" t="n">
-        <v>317</v>
+        <v>316.6826788204064</v>
       </c>
       <c r="AD28" t="n">
-        <v>0</v>
+        <v>18.4349488229215</v>
       </c>
       <c r="AE28" t="n">
         <v>0</v>
@@ -5156,25 +5156,25 @@
         <v>0</v>
       </c>
       <c r="AI28" t="n">
-        <v>46496.23521070655</v>
+        <v>15540.93158954682</v>
       </c>
       <c r="AJ28" t="n">
-        <v>167932.3339164592</v>
+        <v>120421.4454335728</v>
       </c>
       <c r="AK28" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL28" t="n">
         <v>302</v>
       </c>
       <c r="AM28" t="n">
-        <v>247.0393700787401</v>
+        <v>247.7892237529173</v>
       </c>
       <c r="AN28" t="n">
-        <v>49.35399733984491</v>
+        <v>53.45926383533038</v>
       </c>
       <c r="AO28" t="n">
-        <v>3079.689434006322</v>
+        <v>0</v>
       </c>
       <c r="AP28" t="n">
         <v>0</v>
@@ -5186,10 +5186,10 @@
         <v>2</v>
       </c>
       <c r="AS28" t="n">
-        <v>100</v>
+        <v>1894.92903761589</v>
       </c>
       <c r="AT28" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="AU28" t="n">
         <v>100</v>
@@ -5213,10 +5213,10 @@
         <v>500</v>
       </c>
       <c r="BB28" t="n">
-        <v>267.3664935992609</v>
+        <v>262.9159103501156</v>
       </c>
       <c r="BC28" t="n">
-        <v>272.6809092517566</v>
+        <v>263.958410652745</v>
       </c>
     </row>
     <row r="29">
@@ -5224,49 +5224,49 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C29" t="n">
-        <v>256.2603848366048</v>
+        <v>249.18333388708</v>
       </c>
       <c r="D29" t="n">
         <v>317</v>
       </c>
       <c r="E29" t="n">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="F29" t="n">
-        <v>268.0862229189478</v>
+        <v>256.2603848366048</v>
       </c>
       <c r="G29" t="n">
         <v>317</v>
       </c>
       <c r="H29" t="n">
-        <v>287.5</v>
+        <v>275</v>
       </c>
       <c r="I29" t="n">
-        <v>261.9816183569009</v>
+        <v>252.6460026601551</v>
       </c>
       <c r="J29" t="n">
         <v>317</v>
       </c>
       <c r="K29" t="n">
-        <v>289.5909651308048</v>
+        <v>284.9911960405029</v>
       </c>
       <c r="L29" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="M29" t="n">
-        <v>38.22942360091947</v>
+        <v>35.27895092088615</v>
       </c>
       <c r="N29" t="n">
-        <v>19.09516387395373</v>
+        <v>12.24965043551492</v>
       </c>
       <c r="O29" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="P29" t="n">
-        <v>45.01838164309913</v>
+        <v>44.35399733984491</v>
       </c>
       <c r="Q29" t="n">
         <v>0</v>
@@ -5275,7 +5275,7 @@
         <v>0</v>
       </c>
       <c r="S29" t="n">
-        <v>101133.6384068714</v>
+        <v>79111.87675461078</v>
       </c>
       <c r="T29" t="n">
         <v>0</v>
@@ -5287,7 +5287,7 @@
         <v>0</v>
       </c>
       <c r="W29" t="n">
-        <v>287.5</v>
+        <v>275</v>
       </c>
       <c r="X29" t="n">
         <v>317</v>
@@ -5302,7 +5302,7 @@
         <v>0</v>
       </c>
       <c r="AB29" t="n">
-        <v>287.5</v>
+        <v>275</v>
       </c>
       <c r="AC29" t="n">
         <v>317</v>
@@ -5323,25 +5323,25 @@
         <v>0</v>
       </c>
       <c r="AI29" t="n">
-        <v>69440.0549974773</v>
+        <v>76968.48623203085</v>
       </c>
       <c r="AJ29" t="n">
-        <v>129403.0452330912</v>
+        <v>114849.1496236757</v>
       </c>
       <c r="AK29" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL29" t="n">
-        <v>294.8</v>
+        <v>302</v>
       </c>
       <c r="AM29" t="n">
-        <v>245.4645669291339</v>
+        <v>247.0393700787401</v>
       </c>
       <c r="AN29" t="n">
-        <v>32.81838164309914</v>
+        <v>49.35399733984491</v>
       </c>
       <c r="AO29" t="n">
-        <v>2047.867014529387</v>
+        <v>0</v>
       </c>
       <c r="AP29" t="n">
         <v>0</v>
@@ -5353,10 +5353,10 @@
         <v>2</v>
       </c>
       <c r="AS29" t="n">
-        <v>100</v>
+        <v>1797.149434863024</v>
       </c>
       <c r="AT29" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="AU29" t="n">
         <v>100</v>
@@ -5380,10 +5380,10 @@
         <v>500</v>
       </c>
       <c r="BB29" t="n">
-        <v>272.6809092517566</v>
+        <v>263.958410652745</v>
       </c>
       <c r="BC29" t="n">
-        <v>281.6392408841587</v>
+        <v>269.8556013324605</v>
       </c>
     </row>
     <row r="30">
@@ -5391,49 +5391,49 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="C30" t="n">
-        <v>268.0862229189478</v>
+        <v>256.2603848366048</v>
       </c>
       <c r="D30" t="n">
         <v>317</v>
       </c>
       <c r="E30" t="n">
-        <v>310</v>
+        <v>294.0961416450144</v>
       </c>
       <c r="F30" t="n">
-        <v>281.5761002087912</v>
+        <v>267.32922874044</v>
       </c>
       <c r="G30" t="n">
         <v>317</v>
       </c>
       <c r="H30" t="n">
-        <v>302.5</v>
+        <v>287.0480708225072</v>
       </c>
       <c r="I30" t="n">
-        <v>274.6053461148646</v>
+        <v>261.6263034611866</v>
       </c>
       <c r="J30" t="n">
         <v>317</v>
       </c>
       <c r="K30" t="n">
-        <v>295.8960805939707</v>
+        <v>289.4134533034873</v>
       </c>
       <c r="L30" t="n">
-        <v>15</v>
+        <v>14.09614164501443</v>
       </c>
       <c r="M30" t="n">
-        <v>41.93728966273724</v>
+        <v>38.12071639108666</v>
       </c>
       <c r="N30" t="n">
-        <v>20.16463090523105</v>
+        <v>17.9177945501973</v>
       </c>
       <c r="O30" t="n">
         <v>10</v>
       </c>
       <c r="P30" t="n">
-        <v>32.39465388513543</v>
+        <v>45.37369653881342</v>
       </c>
       <c r="Q30" t="n">
         <v>0</v>
@@ -5442,7 +5442,7 @@
         <v>0</v>
       </c>
       <c r="S30" t="n">
-        <v>78032.21660979783</v>
+        <v>95650.65156728784</v>
       </c>
       <c r="T30" t="n">
         <v>0</v>
@@ -5454,7 +5454,7 @@
         <v>0</v>
       </c>
       <c r="W30" t="n">
-        <v>302.5</v>
+        <v>287.0480708225072</v>
       </c>
       <c r="X30" t="n">
         <v>317</v>
@@ -5469,7 +5469,7 @@
         <v>0</v>
       </c>
       <c r="AB30" t="n">
-        <v>302.5</v>
+        <v>287.0480708225072</v>
       </c>
       <c r="AC30" t="n">
         <v>317</v>
@@ -5490,25 +5490,25 @@
         <v>0</v>
       </c>
       <c r="AI30" t="n">
-        <v>71256.11320178556</v>
+        <v>92150.79199698831</v>
       </c>
       <c r="AJ30" t="n">
-        <v>76810.44197673268</v>
+        <v>85808.84068009281</v>
       </c>
       <c r="AK30" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL30" t="n">
-        <v>284</v>
+        <v>295.1253890077948</v>
       </c>
       <c r="AM30" t="n">
-        <v>243.5748031496063</v>
+        <v>245.521502888503</v>
       </c>
       <c r="AN30" t="n">
-        <v>9.394653885135426</v>
+        <v>33.49908554660823</v>
       </c>
       <c r="AO30" t="n">
-        <v>586.2264024324505</v>
+        <v>0</v>
       </c>
       <c r="AP30" t="n">
         <v>0</v>
@@ -5520,10 +5520,10 @@
         <v>2</v>
       </c>
       <c r="AS30" t="n">
-        <v>100</v>
+        <v>1731.573846220569</v>
       </c>
       <c r="AT30" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="AU30" t="n">
         <v>100</v>
@@ -5547,10 +5547,10 @@
         <v>500</v>
       </c>
       <c r="BB30" t="n">
-        <v>281.6392408841587</v>
+        <v>269.8556013324605</v>
       </c>
       <c r="BC30" t="n">
-        <v>291.7449440256041</v>
+        <v>279.1655088703386</v>
       </c>
     </row>
     <row r="31">
@@ -5558,49 +5558,49 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>310</v>
+        <v>294.0961416450144</v>
       </c>
       <c r="C31" t="n">
-        <v>281.5761002087912</v>
+        <v>267.32922874044</v>
       </c>
       <c r="D31" t="n">
         <v>317</v>
       </c>
       <c r="E31" t="n">
-        <v>318.4661842062161</v>
+        <v>308.1922832900289</v>
       </c>
       <c r="F31" t="n">
-        <v>290.0439894683278</v>
+        <v>279.8523832096191</v>
       </c>
       <c r="G31" t="n">
         <v>317</v>
       </c>
       <c r="H31" t="n">
-        <v>314.233092103108</v>
+        <v>301.1442124675216</v>
       </c>
       <c r="I31" t="n">
-        <v>285.7263846201749</v>
+        <v>273.3946033501838</v>
       </c>
       <c r="J31" t="n">
         <v>317</v>
       </c>
       <c r="K31" t="n">
-        <v>301.454842212406</v>
+        <v>295.2915249073496</v>
       </c>
       <c r="L31" t="n">
-        <v>8.466184206216099</v>
+        <v>14.09614164501443</v>
       </c>
       <c r="M31" t="n">
-        <v>44.9945816810336</v>
+        <v>41.59356991882218</v>
       </c>
       <c r="N31" t="n">
-        <v>11.9718604305319</v>
+        <v>18.84831952309793</v>
       </c>
       <c r="O31" t="n">
-        <v>18.4661842062161</v>
+        <v>10</v>
       </c>
       <c r="P31" t="n">
-        <v>12.80743117360902</v>
+        <v>33.60539664981616</v>
       </c>
       <c r="Q31" t="n">
         <v>0</v>
@@ -5609,7 +5609,7 @@
         <v>0</v>
       </c>
       <c r="S31" t="n">
-        <v>32770.73336042141</v>
+        <v>75412.36166421766</v>
       </c>
       <c r="T31" t="n">
         <v>0</v>
@@ -5621,7 +5621,7 @@
         <v>0</v>
       </c>
       <c r="W31" t="n">
-        <v>314.233092103108</v>
+        <v>301.1442124675216</v>
       </c>
       <c r="X31" t="n">
         <v>317</v>
@@ -5636,7 +5636,7 @@
         <v>0</v>
       </c>
       <c r="AB31" t="n">
-        <v>314.233092103108</v>
+        <v>301.1442124675216</v>
       </c>
       <c r="AC31" t="n">
         <v>317</v>
@@ -5657,22 +5657,22 @@
         <v>0</v>
       </c>
       <c r="AI31" t="n">
-        <v>34769.2807506508</v>
+        <v>69855.93973925312</v>
       </c>
       <c r="AJ31" t="n">
-        <v>35506.78413051547</v>
+        <v>49910.6907874201</v>
       </c>
       <c r="AK31" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL31" t="n">
-        <v>275.5521736857622</v>
+        <v>284.9761670233844</v>
       </c>
       <c r="AM31" t="n">
-        <v>242.0966183177187</v>
+        <v>243.7456110277138</v>
       </c>
       <c r="AN31" t="n">
-        <v>0</v>
+        <v>11.58156367320055</v>
       </c>
       <c r="AO31" t="n">
         <v>0</v>
@@ -5687,10 +5687,10 @@
         <v>2</v>
       </c>
       <c r="AS31" t="n">
-        <v>100</v>
+        <v>1692.795292190144</v>
       </c>
       <c r="AT31" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="AU31" t="n">
         <v>100</v>
@@ -5714,10 +5714,10 @@
         <v>500</v>
       </c>
       <c r="BB31" t="n">
-        <v>291.7449440256041</v>
+        <v>279.1655088703386</v>
       </c>
       <c r="BC31" t="n">
-        <v>298.9023848024814</v>
+        <v>289.1160755631824</v>
       </c>
     </row>
     <row r="32">
@@ -5725,49 +5725,49 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>318.4661842062161</v>
+        <v>308.1922832900289</v>
       </c>
       <c r="C32" t="n">
-        <v>290.0439894683278</v>
+        <v>279.8523832096191</v>
       </c>
       <c r="D32" t="n">
         <v>317</v>
       </c>
       <c r="E32" t="n">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="F32" t="n">
-        <v>291.6517338685056</v>
+        <v>281.5761002087912</v>
       </c>
       <c r="G32" t="n">
         <v>317</v>
       </c>
       <c r="H32" t="n">
-        <v>319.233092103108</v>
+        <v>309.0961416450144</v>
       </c>
       <c r="I32" t="n">
-        <v>290.8449108271325</v>
+        <v>280.7106852827342</v>
       </c>
       <c r="J32" t="n">
         <v>317</v>
       </c>
       <c r="K32" t="n">
-        <v>303.9224554135662</v>
+        <v>298.9438132490557</v>
       </c>
       <c r="L32" t="n">
-        <v>1.533815793783901</v>
+        <v>1.807716709971146</v>
       </c>
       <c r="M32" t="n">
-        <v>46.34765756676472</v>
+        <v>43.63693880970561</v>
       </c>
       <c r="N32" t="n">
-        <v>2.222017106722985</v>
+        <v>2.49778774832297</v>
       </c>
       <c r="O32" t="n">
-        <v>26.15508917286746</v>
+        <v>10</v>
       </c>
       <c r="P32" t="n">
-        <v>0</v>
+        <v>26.28931471726582</v>
       </c>
       <c r="Q32" t="n">
         <v>0</v>
@@ -5776,7 +5776,7 @@
         <v>0</v>
       </c>
       <c r="S32" t="n">
-        <v>5014.636107646304</v>
+        <v>8057.529175451133</v>
       </c>
       <c r="T32" t="n">
         <v>0</v>
@@ -5788,7 +5788,7 @@
         <v>0</v>
       </c>
       <c r="W32" t="n">
-        <v>319.233092103108</v>
+        <v>309.0961416450144</v>
       </c>
       <c r="X32" t="n">
         <v>317</v>
@@ -5803,7 +5803,7 @@
         <v>0</v>
       </c>
       <c r="AB32" t="n">
-        <v>319.233092103108</v>
+        <v>309.0961416450144</v>
       </c>
       <c r="AC32" t="n">
         <v>317</v>
@@ -5824,19 +5824,19 @@
         <v>0</v>
       </c>
       <c r="AI32" t="n">
-        <v>5089.816654582743</v>
+        <v>7293.940399052739</v>
       </c>
       <c r="AJ32" t="n">
-        <v>17602.1899851712</v>
+        <v>24199.24456073595</v>
       </c>
       <c r="AK32" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL32" t="n">
-        <v>269.8014658382884</v>
+        <v>279.2507780155896</v>
       </c>
       <c r="AM32" t="n">
-        <v>240.8094428460008</v>
+        <v>242.7437931785809</v>
       </c>
       <c r="AN32" t="n">
         <v>0</v>
@@ -5851,25 +5851,25 @@
         <v>0</v>
       </c>
       <c r="AR32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AS32" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AT32" t="n">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="AU32" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AV32" t="n">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="AW32" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="AX32" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AY32" t="n">
         <v>303</v>
@@ -5881,10 +5881,10 @@
         <v>500</v>
       </c>
       <c r="BB32" t="n">
-        <v>298.9023848024814</v>
+        <v>289.1160755631824</v>
       </c>
       <c r="BC32" t="n">
-        <v>300.3378441159492</v>
+        <v>290.4859069447912</v>
       </c>
     </row>
     <row r="33">
@@ -5892,49 +5892,49 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="C33" t="n">
-        <v>291.6517338685056</v>
+        <v>281.5761002087912</v>
       </c>
       <c r="D33" t="n">
         <v>317</v>
       </c>
       <c r="E33" t="n">
-        <v>337.051583908027</v>
+        <v>318.4661842062161</v>
       </c>
       <c r="F33" t="n">
-        <v>311.2791835363793</v>
+        <v>290.0439894683278</v>
       </c>
       <c r="G33" t="n">
-        <v>311.3161386973243</v>
+        <v>317</v>
       </c>
       <c r="H33" t="n">
-        <v>328.5257919540135</v>
+        <v>314.233092103108</v>
       </c>
       <c r="I33" t="n">
-        <v>301.040299528294</v>
+        <v>285.7263846201749</v>
       </c>
       <c r="J33" t="n">
-        <v>314.1580693486622</v>
+        <v>317</v>
       </c>
       <c r="K33" t="n">
-        <v>307.5991844384781</v>
+        <v>301.454842212406</v>
       </c>
       <c r="L33" t="n">
-        <v>17.051583908027</v>
+        <v>8.466184206216099</v>
       </c>
       <c r="M33" t="n">
-        <v>48.95643583704144</v>
+        <v>44.9945816810336</v>
       </c>
       <c r="N33" t="n">
-        <v>25.96822331605339</v>
+        <v>11.9718604305319</v>
       </c>
       <c r="O33" t="n">
-        <v>13.11776982036815</v>
+        <v>18.4661842062161</v>
       </c>
       <c r="P33" t="n">
-        <v>0</v>
+        <v>12.80743117360902</v>
       </c>
       <c r="Q33" t="n">
         <v>0</v>
@@ -5943,7 +5943,7 @@
         <v>0</v>
       </c>
       <c r="S33" t="n">
-        <v>27959.84409727398</v>
+        <v>32770.73336042141</v>
       </c>
       <c r="T33" t="n">
         <v>0</v>
@@ -5955,10 +5955,10 @@
         <v>0</v>
       </c>
       <c r="W33" t="n">
-        <v>328.5257919540135</v>
+        <v>314.233092103108</v>
       </c>
       <c r="X33" t="n">
-        <v>314.1580693486621</v>
+        <v>317</v>
       </c>
       <c r="Y33" t="n">
         <v>0</v>
@@ -5970,13 +5970,13 @@
         <v>0</v>
       </c>
       <c r="AB33" t="n">
-        <v>328.5257919540135</v>
+        <v>314.233092103108</v>
       </c>
       <c r="AC33" t="n">
-        <v>314.1580693486621</v>
+        <v>317</v>
       </c>
       <c r="AD33" t="n">
-        <v>-18.43494882292201</v>
+        <v>0</v>
       </c>
       <c r="AE33" t="n">
         <v>0</v>
@@ -5991,19 +5991,19 @@
         <v>0</v>
       </c>
       <c r="AI33" t="n">
-        <v>28947.28402691607</v>
+        <v>29699.61440625088</v>
       </c>
       <c r="AJ33" t="n">
-        <v>15155.05469438251</v>
+        <v>21556.69796185395</v>
       </c>
       <c r="AK33" t="n">
-        <v>4.635086452349682</v>
+        <v>10.0336813442187</v>
       </c>
       <c r="AL33" t="n">
-        <v>258.3893783020887</v>
+        <v>275.5521736857622</v>
       </c>
       <c r="AM33" t="n">
-        <v>238.1958710129337</v>
+        <v>242.0966183177187</v>
       </c>
       <c r="AN33" t="n">
         <v>0</v>
@@ -6018,25 +6018,25 @@
         <v>0</v>
       </c>
       <c r="AR33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AS33" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AT33" t="n">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="AU33" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AV33" t="n">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="AW33" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="AX33" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AY33" t="n">
         <v>303</v>
@@ -6048,9 +6048,343 @@
         <v>500</v>
       </c>
       <c r="BB33" t="n">
-        <v>300.3378441159492</v>
+        <v>290.4859069447912</v>
       </c>
       <c r="BC33" t="n">
+        <v>298.1518487255724</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="n">
+        <v>318.4661842062161</v>
+      </c>
+      <c r="C34" t="n">
+        <v>290.0439894683278</v>
+      </c>
+      <c r="D34" t="n">
+        <v>317</v>
+      </c>
+      <c r="E34" t="n">
+        <v>320</v>
+      </c>
+      <c r="F34" t="n">
+        <v>291.6517338685056</v>
+      </c>
+      <c r="G34" t="n">
+        <v>317</v>
+      </c>
+      <c r="H34" t="n">
+        <v>319.233092103108</v>
+      </c>
+      <c r="I34" t="n">
+        <v>290.8449108271325</v>
+      </c>
+      <c r="J34" t="n">
+        <v>317</v>
+      </c>
+      <c r="K34" t="n">
+        <v>303.9224554135662</v>
+      </c>
+      <c r="L34" t="n">
+        <v>1.533815793783901</v>
+      </c>
+      <c r="M34" t="n">
+        <v>46.34765756676472</v>
+      </c>
+      <c r="N34" t="n">
+        <v>2.222017106722985</v>
+      </c>
+      <c r="O34" t="n">
+        <v>26.15508917286746</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0</v>
+      </c>
+      <c r="R34" t="n">
+        <v>0</v>
+      </c>
+      <c r="S34" t="n">
+        <v>5014.636107646304</v>
+      </c>
+      <c r="T34" t="n">
+        <v>0</v>
+      </c>
+      <c r="U34" t="n">
+        <v>0</v>
+      </c>
+      <c r="V34" t="n">
+        <v>0</v>
+      </c>
+      <c r="W34" t="n">
+        <v>319.233092103108</v>
+      </c>
+      <c r="X34" t="n">
+        <v>317</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB34" t="n">
+        <v>319.233092103108</v>
+      </c>
+      <c r="AC34" t="n">
+        <v>317</v>
+      </c>
+      <c r="AD34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI34" t="n">
+        <v>4263.280232645016</v>
+      </c>
+      <c r="AJ34" t="n">
+        <v>10169.58036087929</v>
+      </c>
+      <c r="AK34" t="n">
+        <v>10.0336813442187</v>
+      </c>
+      <c r="AL34" t="n">
+        <v>269.8014658382884</v>
+      </c>
+      <c r="AM34" t="n">
+        <v>240.8094428460008</v>
+      </c>
+      <c r="AN34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR34" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT34" t="n">
+        <v>34</v>
+      </c>
+      <c r="AU34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV34" t="n">
+        <v>34</v>
+      </c>
+      <c r="AW34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY34" t="n">
+        <v>303</v>
+      </c>
+      <c r="AZ34" t="n">
+        <v>100</v>
+      </c>
+      <c r="BA34" t="n">
+        <v>500</v>
+      </c>
+      <c r="BB34" t="n">
+        <v>298.1518487255724</v>
+      </c>
+      <c r="BC34" t="n">
+        <v>299.5662279724844</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="n">
+        <v>320</v>
+      </c>
+      <c r="C35" t="n">
+        <v>291.6517338685056</v>
+      </c>
+      <c r="D35" t="n">
+        <v>317</v>
+      </c>
+      <c r="E35" t="n">
+        <v>337.051583908027</v>
+      </c>
+      <c r="F35" t="n">
+        <v>311.2791835363793</v>
+      </c>
+      <c r="G35" t="n">
+        <v>311.3161386973243</v>
+      </c>
+      <c r="H35" t="n">
+        <v>328.5257919540135</v>
+      </c>
+      <c r="I35" t="n">
+        <v>301.040299528294</v>
+      </c>
+      <c r="J35" t="n">
+        <v>314.1580693486622</v>
+      </c>
+      <c r="K35" t="n">
+        <v>307.5991844384781</v>
+      </c>
+      <c r="L35" t="n">
+        <v>17.051583908027</v>
+      </c>
+      <c r="M35" t="n">
+        <v>48.95643583704144</v>
+      </c>
+      <c r="N35" t="n">
+        <v>25.96822331605339</v>
+      </c>
+      <c r="O35" t="n">
+        <v>13.11776982036815</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0</v>
+      </c>
+      <c r="R35" t="n">
+        <v>0</v>
+      </c>
+      <c r="S35" t="n">
+        <v>27959.84409727398</v>
+      </c>
+      <c r="T35" t="n">
+        <v>0</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0</v>
+      </c>
+      <c r="V35" t="n">
+        <v>0</v>
+      </c>
+      <c r="W35" t="n">
+        <v>328.5257919540135</v>
+      </c>
+      <c r="X35" t="n">
+        <v>314.1580693486621</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB35" t="n">
+        <v>328.5257919540135</v>
+      </c>
+      <c r="AC35" t="n">
+        <v>314.1580693486621</v>
+      </c>
+      <c r="AD35" t="n">
+        <v>-18.43494882292201</v>
+      </c>
+      <c r="AE35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI35" t="n">
+        <v>23901.10876768024</v>
+      </c>
+      <c r="AJ35" t="n">
+        <v>8815.713596802616</v>
+      </c>
+      <c r="AK35" t="n">
+        <v>10.0336813442187</v>
+      </c>
+      <c r="AL35" t="n">
+        <v>258.3893783020887</v>
+      </c>
+      <c r="AM35" t="n">
+        <v>238.1958710129337</v>
+      </c>
+      <c r="AN35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT35" t="n">
+        <v>34</v>
+      </c>
+      <c r="AU35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV35" t="n">
+        <v>34</v>
+      </c>
+      <c r="AW35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY35" t="n">
+        <v>303</v>
+      </c>
+      <c r="AZ35" t="n">
+        <v>100</v>
+      </c>
+      <c r="BA35" t="n">
+        <v>500</v>
+      </c>
+      <c r="BB35" t="n">
+        <v>299.5662279724844</v>
+      </c>
+      <c r="BC35" t="n">
         <v>311.2791835363793</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tweaked iteration output for spencer function
</commit_message>
<xml_diff>
--- a/slices.xlsx
+++ b/slices.xlsx
@@ -806,13 +806,13 @@
         <v>0</v>
       </c>
       <c r="AH2" t="n">
-        <v>11317.62602429964</v>
+        <v>11317.62602429963</v>
       </c>
       <c r="AI2" t="n">
         <v>0</v>
       </c>
       <c r="AJ2" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK2" t="n">
         <v>40</v>
@@ -974,7 +974,7 @@
         <v>13477.29448018663</v>
       </c>
       <c r="AJ3" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK3" t="n">
         <v>40</v>
@@ -1133,10 +1133,10 @@
         <v>17751.85753509717</v>
       </c>
       <c r="AI4" t="n">
-        <v>32499.2110722354</v>
+        <v>32499.21107223539</v>
       </c>
       <c r="AJ4" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK4" t="n">
         <v>40</v>
@@ -1295,10 +1295,10 @@
         <v>18820.66143346557</v>
       </c>
       <c r="AI5" t="n">
-        <v>53804.60629613389</v>
+        <v>53804.60629613388</v>
       </c>
       <c r="AJ5" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK5" t="n">
         <v>40</v>
@@ -1457,10 +1457,10 @@
         <v>19349.98648437063</v>
       </c>
       <c r="AI6" t="n">
-        <v>75771.3080637363</v>
+        <v>75771.30806373629</v>
       </c>
       <c r="AJ6" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK6" t="n">
         <v>40</v>
@@ -1619,10 +1619,10 @@
         <v>19559.03471502128</v>
       </c>
       <c r="AI7" t="n">
-        <v>97467.44547917457</v>
+        <v>97467.44547917454</v>
       </c>
       <c r="AJ7" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK7" t="n">
         <v>40</v>
@@ -1778,13 +1778,13 @@
         <v>0</v>
       </c>
       <c r="AH8" t="n">
-        <v>19561.36761118835</v>
+        <v>19561.36761118836</v>
       </c>
       <c r="AI8" t="n">
         <v>118309.4394021396</v>
       </c>
       <c r="AJ8" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK8" t="n">
         <v>40</v>
@@ -1946,7 +1946,7 @@
         <v>137911.9766290364</v>
       </c>
       <c r="AJ9" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK9" t="n">
         <v>40</v>
@@ -1998,7 +1998,7 @@
         <v>23.61950805794151</v>
       </c>
       <c r="BB9" t="n">
-        <v>22.57007461923094</v>
+        <v>22.57007461923093</v>
       </c>
     </row>
     <row r="10">
@@ -2108,7 +2108,7 @@
         <v>156012.939114407</v>
       </c>
       <c r="AJ10" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK10" t="n">
         <v>40</v>
@@ -2157,7 +2157,7 @@
         <v>100</v>
       </c>
       <c r="BA10" t="n">
-        <v>22.57007461923094</v>
+        <v>22.57007461923093</v>
       </c>
       <c r="BB10" t="n">
         <v>21.76708375754968</v>
@@ -2270,7 +2270,7 @@
         <v>172432.2112434889</v>
       </c>
       <c r="AJ11" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK11" t="n">
         <v>42.40000000000001</v>
@@ -2432,7 +2432,7 @@
         <v>188537.3130599339</v>
       </c>
       <c r="AJ12" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK12" t="n">
         <v>47.19999999999999</v>
@@ -2594,7 +2594,7 @@
         <v>203716.974361009</v>
       </c>
       <c r="AJ13" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK13" t="n">
         <v>52</v>
@@ -2646,7 +2646,7 @@
         <v>20.57760578902214</v>
       </c>
       <c r="BB13" t="n">
-        <v>20.24833926794443</v>
+        <v>20.24833926794444</v>
       </c>
     </row>
     <row r="14">
@@ -2753,10 +2753,10 @@
         <v>25442.23319545473</v>
       </c>
       <c r="AI14" t="n">
-        <v>217402.6642131996</v>
+        <v>217402.6642131995</v>
       </c>
       <c r="AJ14" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK14" t="n">
         <v>54.7323076923077</v>
@@ -2805,10 +2805,10 @@
         <v>100</v>
       </c>
       <c r="BA14" t="n">
-        <v>20.24833926794443</v>
+        <v>20.24833926794444</v>
       </c>
       <c r="BB14" t="n">
-        <v>20.11906034835862</v>
+        <v>20.11906034835863</v>
       </c>
     </row>
     <row r="15">
@@ -2918,7 +2918,7 @@
         <v>229330.2004507779</v>
       </c>
       <c r="AJ15" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK15" t="n">
         <v>57.46461538461539</v>
@@ -2967,7 +2967,7 @@
         <v>100</v>
       </c>
       <c r="BA15" t="n">
-        <v>20.11906034835862</v>
+        <v>20.11906034835863</v>
       </c>
       <c r="BB15" t="n">
         <v>20.21147899762014</v>
@@ -3077,10 +3077,10 @@
         <v>30011.36661046745</v>
       </c>
       <c r="AI16" t="n">
-        <v>239061.0622172657</v>
+        <v>239061.0622172656</v>
       </c>
       <c r="AJ16" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK16" t="n">
         <v>60.25576923076924</v>
@@ -3132,7 +3132,7 @@
         <v>20.21147899762014</v>
       </c>
       <c r="BB16" t="n">
-        <v>20.55823523216588</v>
+        <v>20.55823523216587</v>
       </c>
     </row>
     <row r="17">
@@ -3239,10 +3239,10 @@
         <v>32072.95743680699</v>
       </c>
       <c r="AI17" t="n">
-        <v>246490.5974818672</v>
+        <v>246490.5974818671</v>
       </c>
       <c r="AJ17" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK17" t="n">
         <v>62.36875</v>
@@ -3291,7 +3291,7 @@
         <v>100</v>
       </c>
       <c r="BA17" t="n">
-        <v>20.55823523216588</v>
+        <v>20.55823523216587</v>
       </c>
       <c r="BB17" t="n">
         <v>21.17062982863898</v>
@@ -3404,7 +3404,7 @@
         <v>250833.9473181817</v>
       </c>
       <c r="AJ18" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK18" t="n">
         <v>64.22125</v>
@@ -3566,7 +3566,7 @@
         <v>251718.8815973146</v>
       </c>
       <c r="AJ19" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK19" t="n">
         <v>66.07375</v>
@@ -3725,10 +3725,10 @@
         <v>35510.75656883991</v>
       </c>
       <c r="AI20" t="n">
-        <v>248776.1359866335</v>
+        <v>248776.1359866334</v>
       </c>
       <c r="AJ20" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK20" t="n">
         <v>67.91661969216291</v>
@@ -3890,7 +3890,7 @@
         <v>241809.9190239766</v>
       </c>
       <c r="AJ21" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK21" t="n">
         <v>69.74985907648876</v>
@@ -3942,7 +3942,7 @@
         <v>24.80192387432286</v>
       </c>
       <c r="BB21" t="n">
-        <v>26.66898176015048</v>
+        <v>26.66898176015047</v>
       </c>
     </row>
     <row r="22">
@@ -4049,10 +4049,10 @@
         <v>31553.45525720306</v>
       </c>
       <c r="AI22" t="n">
-        <v>230921.6507813646</v>
+        <v>230921.6507813645</v>
       </c>
       <c r="AJ22" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK22" t="n">
         <v>71.13078461486758</v>
@@ -4101,10 +4101,10 @@
         <v>100</v>
       </c>
       <c r="BA22" t="n">
-        <v>26.66898176015048</v>
+        <v>26.66898176015047</v>
       </c>
       <c r="BB22" t="n">
-        <v>28.88484828798597</v>
+        <v>28.88484828798596</v>
       </c>
     </row>
     <row r="23">
@@ -4211,10 +4211,10 @@
         <v>29602.92656515625</v>
       </c>
       <c r="AI23" t="n">
-        <v>216360.0285344744</v>
+        <v>216360.0285344743</v>
       </c>
       <c r="AJ23" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK23" t="n">
         <v>72.44024131795746</v>
@@ -4263,7 +4263,7 @@
         <v>100</v>
       </c>
       <c r="BA23" t="n">
-        <v>28.88484828798597</v>
+        <v>28.88484828798596</v>
       </c>
       <c r="BB23" t="n">
         <v>31.47232262250964</v>
@@ -4376,7 +4376,7 @@
         <v>198365.2050125867</v>
       </c>
       <c r="AJ24" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK24" t="n">
         <v>73.74969802104734</v>
@@ -4535,10 +4535,10 @@
         <v>25346.71586438311</v>
       </c>
       <c r="AI25" t="n">
-        <v>177213.6937657181</v>
+        <v>177213.693765718</v>
       </c>
       <c r="AJ25" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK25" t="n">
         <v>75.05915472413723</v>
@@ -4700,7 +4700,7 @@
         <v>153247.0240096841</v>
       </c>
       <c r="AJ26" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK26" t="n">
         <v>76.13947459408594</v>
@@ -4862,7 +4862,7 @@
         <v>126937.1294059171</v>
       </c>
       <c r="AJ27" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK27" t="n">
         <v>76.63494469795778</v>
@@ -5021,10 +5021,10 @@
         <v>17862.80904852692</v>
       </c>
       <c r="AI28" t="n">
-        <v>98981.19624938579</v>
+        <v>98981.19624938577</v>
       </c>
       <c r="AJ28" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK28" t="n">
         <v>77.13041480182963</v>
@@ -5183,10 +5183,10 @@
         <v>16579.8442975558</v>
       </c>
       <c r="AI29" t="n">
-        <v>70309.02047071593</v>
+        <v>70309.02047071591</v>
       </c>
       <c r="AJ29" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK29" t="n">
         <v>77.64764520950705</v>
@@ -5238,7 +5238,7 @@
         <v>51.94529155823766</v>
       </c>
       <c r="BB29" t="n">
-        <v>59.28645644434174</v>
+        <v>59.28645644434175</v>
       </c>
     </row>
     <row r="30">
@@ -5345,10 +5345,10 @@
         <v>12717.22034841454</v>
       </c>
       <c r="AI30" t="n">
-        <v>38815.57235723775</v>
+        <v>38815.57235723773</v>
       </c>
       <c r="AJ30" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK30" t="n">
         <v>78.18663592099003</v>
@@ -5397,10 +5397,10 @@
         <v>100</v>
       </c>
       <c r="BA30" t="n">
-        <v>59.28645644434174</v>
+        <v>59.28645644434175</v>
       </c>
       <c r="BB30" t="n">
-        <v>69.67837750865294</v>
+        <v>69.67837750865299</v>
       </c>
     </row>
     <row r="31">
@@ -5507,10 +5507,10 @@
         <v>4335.435134915772</v>
       </c>
       <c r="AI31" t="n">
-        <v>10489.17808583611</v>
+        <v>10489.17808583609</v>
       </c>
       <c r="AJ31" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK31" t="n">
         <v>78.63592483281701</v>
@@ -5559,10 +5559,10 @@
         <v>100</v>
       </c>
       <c r="BA31" t="n">
-        <v>69.67837750865294</v>
+        <v>69.67837750865299</v>
       </c>
       <c r="BB31" t="n">
-        <v>81.1313647094801</v>
+        <v>81.13136470947836</v>
       </c>
     </row>
     <row r="32">
@@ -5666,13 +5666,13 @@
         <v>0</v>
       </c>
       <c r="AH32" t="n">
-        <v>-259.6222692424315</v>
+        <v>-259.6222692424313</v>
       </c>
       <c r="AI32" t="n">
-        <v>-347.0443053239087</v>
+        <v>-347.0443053239233</v>
       </c>
       <c r="AJ32" t="n">
-        <v>8.916729211007276</v>
+        <v>8.916729211007279</v>
       </c>
       <c r="AK32" t="n">
         <v>78.85555568812021</v>
@@ -5721,7 +5721,7 @@
         <v>100</v>
       </c>
       <c r="BA32" t="n">
-        <v>81.1313647094801</v>
+        <v>81.13136470947836</v>
       </c>
       <c r="BB32" t="n">
         <v>83.98856233604299</v>

</xml_diff>

<commit_message>
corrected bishop method in both documentation and bishop function. horizontal component of dload was subtracted in denominator when it should have been added to the numerator.
</commit_message>
<xml_diff>
--- a/slices.xlsx
+++ b/slices.xlsx
@@ -804,7 +804,7 @@
         <v>0</v>
       </c>
       <c r="AI2" t="n">
-        <v>-8251.841415697163</v>
+        <v>1970.676132921329</v>
       </c>
       <c r="AJ2" t="n">
         <v>0</v>
@@ -965,7 +965,7 @@
         <v>0</v>
       </c>
       <c r="AI3" t="n">
-        <v>-4341.313547344951</v>
+        <v>5451.591659061644</v>
       </c>
       <c r="AJ3" t="n">
         <v>0</v>
@@ -1126,7 +1126,7 @@
         <v>0</v>
       </c>
       <c r="AI4" t="n">
-        <v>-614.6760451651353</v>
+        <v>8398.79062580929</v>
       </c>
       <c r="AJ4" t="n">
         <v>0</v>
@@ -1287,7 +1287,7 @@
         <v>0</v>
       </c>
       <c r="AI5" t="n">
-        <v>-493.2453263126663</v>
+        <v>15120.55495915894</v>
       </c>
       <c r="AJ5" t="n">
         <v>0</v>
@@ -1448,7 +1448,7 @@
         <v>0</v>
       </c>
       <c r="AI6" t="n">
-        <v>8246.121445242607</v>
+        <v>21592.12108922844</v>
       </c>
       <c r="AJ6" t="n">
         <v>0</v>
@@ -1609,7 +1609,7 @@
         <v>0</v>
       </c>
       <c r="AI7" t="n">
-        <v>16427.12684309075</v>
+        <v>27304.98484780873</v>
       </c>
       <c r="AJ7" t="n">
         <v>0</v>
@@ -1770,7 +1770,7 @@
         <v>0</v>
       </c>
       <c r="AI8" t="n">
-        <v>23978.1114189677</v>
+        <v>32360.63244316275</v>
       </c>
       <c r="AJ8" t="n">
         <v>0</v>
@@ -1931,7 +1931,7 @@
         <v>0</v>
       </c>
       <c r="AI9" t="n">
-        <v>30839.94056658806</v>
+        <v>36839.96172348834</v>
       </c>
       <c r="AJ9" t="n">
         <v>0</v>
@@ -2092,7 +2092,7 @@
         <v>0</v>
       </c>
       <c r="AI10" t="n">
-        <v>36964.06202181718</v>
+        <v>40807.87515397542</v>
       </c>
       <c r="AJ10" t="n">
         <v>0</v>
@@ -2253,7 +2253,7 @@
         <v>0</v>
       </c>
       <c r="AI11" t="n">
-        <v>42311.09037905956</v>
+        <v>44316.61197830974</v>
       </c>
       <c r="AJ11" t="n">
         <v>0</v>
@@ -2414,7 +2414,7 @@
         <v>0</v>
       </c>
       <c r="AI12" t="n">
-        <v>46849.79911299139</v>
+        <v>47408.19017166216</v>
       </c>
       <c r="AJ12" t="n">
         <v>0</v>
@@ -2575,7 +2575,7 @@
         <v>0</v>
       </c>
       <c r="AI13" t="n">
-        <v>50556.44178377492</v>
+        <v>50116.20432672538</v>
       </c>
       <c r="AJ13" t="n">
         <v>0</v>
@@ -2736,7 +2736,7 @@
         <v>0</v>
       </c>
       <c r="AI14" t="n">
-        <v>53414.35391270815</v>
+        <v>52467.14487454593</v>
       </c>
       <c r="AJ14" t="n">
         <v>0</v>
@@ -2897,7 +2897,7 @@
         <v>0</v>
       </c>
       <c r="AI15" t="n">
-        <v>55413.81026403054</v>
+        <v>54481.35000948822</v>
       </c>
       <c r="AJ15" t="n">
         <v>0</v>
@@ -3058,7 +3058,7 @@
         <v>0</v>
       </c>
       <c r="AI16" t="n">
-        <v>56552.13235495334</v>
+        <v>56173.6641139854</v>
       </c>
       <c r="AJ16" t="n">
         <v>0</v>
@@ -3219,7 +3219,7 @@
         <v>0</v>
       </c>
       <c r="AI17" t="n">
-        <v>56834.06069484398</v>
+        <v>57553.84892010906</v>
       </c>
       <c r="AJ17" t="n">
         <v>0</v>
@@ -3380,7 +3380,7 @@
         <v>0</v>
       </c>
       <c r="AI18" t="n">
-        <v>56272.42822503048</v>
+        <v>58626.77178063371</v>
       </c>
       <c r="AJ18" t="n">
         <v>0</v>
@@ -3541,7 +3541,7 @@
         <v>0</v>
       </c>
       <c r="AI19" t="n">
-        <v>54889.19891146557</v>
+        <v>59392.37602664282</v>
       </c>
       <c r="AJ19" t="n">
         <v>0</v>
@@ -3702,7 +3702,7 @@
         <v>0</v>
       </c>
       <c r="AI20" t="n">
-        <v>52716.97291215158</v>
+        <v>59845.41860986569</v>
       </c>
       <c r="AJ20" t="n">
         <v>0</v>
@@ -3863,7 +3863,7 @@
         <v>0</v>
       </c>
       <c r="AI21" t="n">
-        <v>49801.11409398797</v>
+        <v>59974.93694152016</v>
       </c>
       <c r="AJ21" t="n">
         <v>0</v>
@@ -4024,7 +4024,7 @@
         <v>0</v>
       </c>
       <c r="AI22" t="n">
-        <v>46202.73822777813</v>
+        <v>59763.37586622223</v>
       </c>
       <c r="AJ22" t="n">
         <v>0</v>
@@ -4185,7 +4185,7 @@
         <v>0</v>
       </c>
       <c r="AI23" t="n">
-        <v>22667.4012155776</v>
+        <v>31040.20166374412</v>
       </c>
       <c r="AJ23" t="n">
         <v>0</v>
@@ -4346,7 +4346,7 @@
         <v>0</v>
       </c>
       <c r="AI24" t="n">
-        <v>39515.37990749106</v>
+        <v>53355.25426620171</v>
       </c>
       <c r="AJ24" t="n">
         <v>0</v>
@@ -4507,7 +4507,7 @@
         <v>0</v>
       </c>
       <c r="AI25" t="n">
-        <v>44477.31101720523</v>
+        <v>67308.01980792976</v>
       </c>
       <c r="AJ25" t="n">
         <v>0</v>
@@ -4668,7 +4668,7 @@
         <v>0</v>
       </c>
       <c r="AI26" t="n">
-        <v>41423.8905918161</v>
+        <v>68100.93149641833</v>
       </c>
       <c r="AJ26" t="n">
         <v>0</v>
@@ -4829,7 +4829,7 @@
         <v>0</v>
       </c>
       <c r="AI27" t="n">
-        <v>3441.259899017444</v>
+        <v>5932.181724629349</v>
       </c>
       <c r="AJ27" t="n">
         <v>0</v>
@@ -4990,7 +4990,7 @@
         <v>0</v>
       </c>
       <c r="AI28" t="n">
-        <v>23420.07600054663</v>
+        <v>42411.46612653913</v>
       </c>
       <c r="AJ28" t="n">
         <v>0</v>
@@ -5151,7 +5151,7 @@
         <v>0</v>
       </c>
       <c r="AI29" t="n">
-        <v>37825.64585000658</v>
+        <v>67399.13600942053</v>
       </c>
       <c r="AJ29" t="n">
         <v>0</v>
@@ -5312,7 +5312,7 @@
         <v>0</v>
       </c>
       <c r="AI30" t="n">
-        <v>42818.05969967307</v>
+        <v>68056.72395030156</v>
       </c>
       <c r="AJ30" t="n">
         <v>0</v>
@@ -5473,7 +5473,7 @@
         <v>0</v>
       </c>
       <c r="AI31" t="n">
-        <v>5759.475066946553</v>
+        <v>8430.712381303023</v>
       </c>
       <c r="AJ31" t="n">
         <v>0</v>
@@ -5634,7 +5634,7 @@
         <v>0</v>
       </c>
       <c r="AI32" t="n">
-        <v>23182.30146913127</v>
+        <v>35061.06583760159</v>
       </c>
       <c r="AJ32" t="n">
         <v>0</v>
@@ -5795,7 +5795,7 @@
         <v>0</v>
       </c>
       <c r="AI33" t="n">
-        <v>3453.808841955788</v>
+        <v>5045.932645310533</v>
       </c>
       <c r="AJ33" t="n">
         <v>0</v>
@@ -5956,7 +5956,7 @@
         <v>0</v>
       </c>
       <c r="AI34" t="n">
-        <v>18359.14837864525</v>
+        <v>28804.4628332987</v>
       </c>
       <c r="AJ34" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
partial debug of left vs right spencer method
</commit_message>
<xml_diff>
--- a/slices.xlsx
+++ b/slices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BB32"/>
+  <dimension ref="A1:BH22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -696,10 +696,40 @@
       </c>
       <c r="BA1" s="1" t="inlineStr">
         <is>
+          <t>ma</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>Q</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>y_q</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>Fh</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>Fv</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>Mo</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
           <t>yt_l</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>yt_r</t>
         </is>
@@ -806,13 +836,13 @@
         <v>0</v>
       </c>
       <c r="AH2" t="n">
-        <v>-1241.865167945649</v>
+        <v>-263.4870953536603</v>
       </c>
       <c r="AI2" t="n">
         <v>0</v>
       </c>
       <c r="AJ2" t="n">
-        <v>-12.59201158446214</v>
+        <v>8.895522366703</v>
       </c>
       <c r="AK2" t="n">
         <v>78.855630874209</v>
@@ -861,10 +891,28 @@
         <v>100</v>
       </c>
       <c r="BA2" t="n">
+        <v>1.678125644678302</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>-351.0899306809409</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>81.21329877556784</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>-356.6588438338362</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG2" t="n">
         <v>84.00000000000006</v>
       </c>
-      <c r="BB2" t="n">
-        <v>81.10333903249868</v>
+      <c r="BH2" t="n">
+        <v>81.29034428031295</v>
       </c>
     </row>
     <row r="3">
@@ -968,13 +1016,13 @@
         <v>0</v>
       </c>
       <c r="AH3" t="n">
-        <v>9231.680999382566</v>
+        <v>4332.228964849945</v>
       </c>
       <c r="AI3" t="n">
-        <v>1309.489942778073</v>
+        <v>351.0899306809409</v>
       </c>
       <c r="AJ3" t="n">
-        <v>-12.59201158446214</v>
+        <v>8.895522366703</v>
       </c>
       <c r="AK3" t="n">
         <v>78.63592483281701</v>
@@ -1023,10 +1071,28 @@
         <v>100</v>
       </c>
       <c r="BA3" t="n">
-        <v>81.10333903249868</v>
+        <v>1.455854622958788</v>
       </c>
       <c r="BB3" t="n">
-        <v>68.8721918279556</v>
+        <v>10830.68295521836</v>
+      </c>
+      <c r="BC3" t="n">
+        <v>70.37079750256237</v>
+      </c>
+      <c r="BD3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>-7857.753192819717</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>81.29034428031295</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>70.34040709215394</v>
       </c>
     </row>
     <row r="4">
@@ -1043,46 +1109,46 @@
         <v>84</v>
       </c>
       <c r="E4" t="n">
-        <v>88.35526636193472</v>
+        <v>95.00281847022481</v>
       </c>
       <c r="F4" t="n">
-        <v>50.07315218453382</v>
+        <v>39.9962422235724</v>
       </c>
       <c r="G4" t="n">
         <v>84</v>
       </c>
       <c r="H4" t="n">
-        <v>85.03149030778968</v>
+        <v>88.35526636193472</v>
       </c>
       <c r="I4" t="n">
-        <v>56.34605099463901</v>
+        <v>50.07315218453382</v>
       </c>
       <c r="J4" t="n">
         <v>84</v>
       </c>
       <c r="K4" t="n">
-        <v>70.39056154462311</v>
+        <v>67.36263848542323</v>
       </c>
       <c r="L4" t="n">
-        <v>6.647552108290071</v>
+        <v>13.29510421658016</v>
       </c>
       <c r="M4" t="n">
-        <v>64.11670545590695</v>
+        <v>60.04838530603909</v>
       </c>
       <c r="N4" t="n">
-        <v>15.22783679312429</v>
+        <v>26.62916806949235</v>
       </c>
       <c r="O4" t="n">
         <v>20</v>
       </c>
       <c r="P4" t="n">
-        <v>7.653949005360992</v>
+        <v>13.92684781546618</v>
       </c>
       <c r="Q4" t="n">
         <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>23389.23846323404</v>
+        <v>56786.33813691734</v>
       </c>
       <c r="S4" t="n">
         <v>0</v>
@@ -1094,7 +1160,7 @@
         <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>85.03149030778968</v>
+        <v>88.35526636193472</v>
       </c>
       <c r="W4" t="n">
         <v>84</v>
@@ -1109,7 +1175,7 @@
         <v>0</v>
       </c>
       <c r="AA4" t="n">
-        <v>85.03149030778968</v>
+        <v>88.35526636193472</v>
       </c>
       <c r="AB4" t="n">
         <v>84</v>
@@ -1130,23 +1196,23 @@
         <v>0</v>
       </c>
       <c r="AH4" t="n">
-        <v>23560.21640914562</v>
+        <v>29608.86634539621</v>
       </c>
       <c r="AI4" t="n">
-        <v>-13361.81753735482</v>
+        <v>-10479.59302453742</v>
       </c>
       <c r="AJ4" t="n">
-        <v>-12.59201158446214</v>
+        <v>8.895522366703</v>
       </c>
       <c r="AK4" t="n">
-        <v>78.18663592099003</v>
+        <v>77.91714056524853</v>
       </c>
       <c r="AL4" t="inlineStr"/>
       <c r="AM4" t="n">
-        <v>21.84058492635102</v>
+        <v>27.84398838071471</v>
       </c>
       <c r="AN4" t="n">
-        <v>1362.852499404304</v>
+        <v>1737.464874956598</v>
       </c>
       <c r="AO4" t="n">
         <v>0</v>
@@ -1185,10 +1251,28 @@
         <v>100</v>
       </c>
       <c r="BA4" t="n">
-        <v>68.8721918279556</v>
+        <v>1.138292633052306</v>
       </c>
       <c r="BB4" t="n">
-        <v>58.85646752225637</v>
+        <v>61020.96489264639</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>50.07315218453382</v>
+      </c>
+      <c r="BD4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE4" t="n">
+        <v>-56786.33813691734</v>
+      </c>
+      <c r="BF4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG4" t="n">
+        <v>70.34040709215394</v>
+      </c>
+      <c r="BH4" t="n">
+        <v>54.23659600662612</v>
       </c>
     </row>
     <row r="5">
@@ -1196,55 +1280,55 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>88.35526636193472</v>
+        <v>95.00281847022481</v>
       </c>
       <c r="C5" t="n">
-        <v>50.07315218453382</v>
+        <v>39.9962422235724</v>
       </c>
       <c r="D5" t="n">
         <v>84</v>
       </c>
       <c r="E5" t="n">
-        <v>95.00281847022481</v>
+        <v>104.169015391854</v>
       </c>
       <c r="F5" t="n">
-        <v>39.9962422235724</v>
+        <v>29.40983340832391</v>
       </c>
       <c r="G5" t="n">
         <v>84</v>
       </c>
       <c r="H5" t="n">
-        <v>91.67904241607977</v>
+        <v>99.58591693103941</v>
       </c>
       <c r="I5" t="n">
-        <v>44.70426754894582</v>
+        <v>34.32872717186068</v>
       </c>
       <c r="J5" t="n">
         <v>84</v>
       </c>
       <c r="K5" t="n">
-        <v>64.74468346367284</v>
+        <v>59.40035712622747</v>
       </c>
       <c r="L5" t="n">
-        <v>6.647552108290085</v>
+        <v>9.166196921629194</v>
       </c>
       <c r="M5" t="n">
-        <v>56.42986469458384</v>
+        <v>48.95035398098552</v>
       </c>
       <c r="N5" t="n">
-        <v>12.02181762249784</v>
+        <v>13.95769645826263</v>
       </c>
       <c r="O5" t="n">
         <v>20</v>
       </c>
       <c r="P5" t="n">
-        <v>19.29573245105418</v>
+        <v>24</v>
       </c>
       <c r="Q5" t="n">
-        <v>0</v>
+        <v>5.671272828139323</v>
       </c>
       <c r="R5" t="n">
-        <v>32675.96191387502</v>
+        <v>57092.64759767729</v>
       </c>
       <c r="S5" t="n">
         <v>0</v>
@@ -1256,7 +1340,7 @@
         <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>91.67904241607977</v>
+        <v>99.58591693103941</v>
       </c>
       <c r="W5" t="n">
         <v>84</v>
@@ -1271,7 +1355,7 @@
         <v>0</v>
       </c>
       <c r="AA5" t="n">
-        <v>91.67904241607977</v>
+        <v>99.58591693103941</v>
       </c>
       <c r="AB5" t="n">
         <v>84</v>
@@ -1292,23 +1376,23 @@
         <v>0</v>
       </c>
       <c r="AH5" t="n">
-        <v>26860.66182373601</v>
+        <v>27922.23588484879</v>
       </c>
       <c r="AI5" t="n">
-        <v>-48403.63821004717</v>
+        <v>-71500.5579171838</v>
       </c>
       <c r="AJ5" t="n">
-        <v>-12.59201158446214</v>
+        <v>8.895522366703</v>
       </c>
       <c r="AK5" t="n">
-        <v>77.64764520950705</v>
+        <v>77.00654727586166</v>
       </c>
       <c r="AL5" t="inlineStr"/>
       <c r="AM5" t="n">
-        <v>32.94337766056123</v>
+        <v>42.67782010400099</v>
       </c>
       <c r="AN5" t="n">
-        <v>2055.666766019021</v>
+        <v>2663.095974489661</v>
       </c>
       <c r="AO5" t="n">
         <v>0</v>
@@ -1317,19 +1401,19 @@
         <v>0</v>
       </c>
       <c r="AQ5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AR5" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="AS5" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="AT5" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="AU5" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="AV5" t="n">
         <v>0</v>
@@ -1347,10 +1431,28 @@
         <v>100</v>
       </c>
       <c r="BA5" t="n">
-        <v>58.85646752225637</v>
+        <v>1.069840496192237</v>
       </c>
       <c r="BB5" t="n">
-        <v>51.66261464278417</v>
+        <v>42888.23194393673</v>
+      </c>
+      <c r="BC5" t="n">
+        <v>34.32872717186068</v>
+      </c>
+      <c r="BD5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE5" t="n">
+        <v>-57092.64759767729</v>
+      </c>
+      <c r="BF5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG5" t="n">
+        <v>54.23659600662612</v>
+      </c>
+      <c r="BH5" t="n">
+        <v>47.93816565962794</v>
       </c>
     </row>
     <row r="6">
@@ -1358,43 +1460,43 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>95.00281847022481</v>
+        <v>104.169015391854</v>
       </c>
       <c r="C6" t="n">
-        <v>39.9962422235724</v>
+        <v>29.40983340832391</v>
       </c>
       <c r="D6" t="n">
         <v>84</v>
       </c>
       <c r="E6" t="n">
-        <v>101.1136164179776</v>
+        <v>113.3352123134832</v>
       </c>
       <c r="F6" t="n">
-        <v>32.61452440495614</v>
+        <v>21.27609029286714</v>
       </c>
       <c r="G6" t="n">
         <v>84</v>
       </c>
       <c r="H6" t="n">
-        <v>98.05821744410122</v>
+        <v>108.7521138526686</v>
       </c>
       <c r="I6" t="n">
-        <v>36.12541900629962</v>
+        <v>25.09193914530816</v>
       </c>
       <c r="J6" t="n">
         <v>84</v>
       </c>
       <c r="K6" t="n">
-        <v>60.35722423340079</v>
+        <v>54.53993804737763</v>
       </c>
       <c r="L6" t="n">
-        <v>6.1107979477528</v>
+        <v>9.166196921629208</v>
       </c>
       <c r="M6" t="n">
-        <v>50.30163884472133</v>
+        <v>41.48919998896996</v>
       </c>
       <c r="N6" t="n">
-        <v>9.566869719827167</v>
+        <v>12.23659619144324</v>
       </c>
       <c r="O6" t="n">
         <v>20</v>
@@ -1403,10 +1505,10 @@
         <v>24</v>
       </c>
       <c r="Q6" t="n">
-        <v>3.874580993700377</v>
+        <v>14.90806085469184</v>
       </c>
       <c r="R6" t="n">
-        <v>36612.50792286657</v>
+        <v>68268.58837034137</v>
       </c>
       <c r="S6" t="n">
         <v>0</v>
@@ -1418,7 +1520,7 @@
         <v>0</v>
       </c>
       <c r="V6" t="n">
-        <v>98.05821744410122</v>
+        <v>108.7521138526686</v>
       </c>
       <c r="W6" t="n">
         <v>84</v>
@@ -1433,7 +1535,7 @@
         <v>0</v>
       </c>
       <c r="AA6" t="n">
-        <v>98.05821744410122</v>
+        <v>108.7521138526686</v>
       </c>
       <c r="AB6" t="n">
         <v>84</v>
@@ -1454,23 +1556,23 @@
         <v>0</v>
       </c>
       <c r="AH6" t="n">
-        <v>26709.84170154852</v>
+        <v>33698.74511679153</v>
       </c>
       <c r="AI6" t="n">
-        <v>-84287.2020252737</v>
+        <v>-114388.7898611205</v>
       </c>
       <c r="AJ6" t="n">
-        <v>-12.59201158446214</v>
+        <v>8.895522366703</v>
       </c>
       <c r="AK6" t="n">
-        <v>77.13041480182963</v>
+        <v>76.26334212005389</v>
       </c>
       <c r="AL6" t="inlineStr"/>
       <c r="AM6" t="n">
-        <v>41.00499579553001</v>
+        <v>51.17140297474573</v>
       </c>
       <c r="AN6" t="n">
-        <v>2558.711737641072</v>
+        <v>3193.095545624134</v>
       </c>
       <c r="AO6" t="n">
         <v>0</v>
@@ -1509,10 +1611,28 @@
         <v>100</v>
       </c>
       <c r="BA6" t="n">
-        <v>51.66261464278417</v>
+        <v>1.016032064889689</v>
       </c>
       <c r="BB6" t="n">
-        <v>46.28133066795252</v>
+        <v>40158.86560829845</v>
+      </c>
+      <c r="BC6" t="n">
+        <v>25.09193914530816</v>
+      </c>
+      <c r="BD6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE6" t="n">
+        <v>-68268.58837034137</v>
+      </c>
+      <c r="BF6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG6" t="n">
+        <v>47.93816565962794</v>
+      </c>
+      <c r="BH6" t="n">
+        <v>43.24988273506372</v>
       </c>
     </row>
     <row r="7">
@@ -1520,43 +1640,43 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>101.1136164179776</v>
+        <v>113.3352123134832</v>
       </c>
       <c r="C7" t="n">
-        <v>32.61452440495614</v>
+        <v>21.27609029286714</v>
       </c>
       <c r="D7" t="n">
         <v>84</v>
       </c>
       <c r="E7" t="n">
-        <v>107.2244143657304</v>
+        <v>122.5014092351124</v>
       </c>
       <c r="F7" t="n">
-        <v>26.47129817593819</v>
+        <v>14.88890808066871</v>
       </c>
       <c r="G7" t="n">
         <v>84</v>
       </c>
       <c r="H7" t="n">
-        <v>104.169015391854</v>
+        <v>117.9183107742978</v>
       </c>
       <c r="I7" t="n">
-        <v>29.40983340832391</v>
+        <v>17.8922612956589</v>
       </c>
       <c r="J7" t="n">
         <v>84</v>
       </c>
       <c r="K7" t="n">
-        <v>56.80134330051643</v>
+        <v>50.80018675408928</v>
       </c>
       <c r="L7" t="n">
-        <v>6.1107979477528</v>
+        <v>9.166196921629194</v>
       </c>
       <c r="M7" t="n">
-        <v>45.09756562240492</v>
+        <v>34.80720979910493</v>
       </c>
       <c r="N7" t="n">
-        <v>8.656726910846217</v>
+        <v>11.16362119609144</v>
       </c>
       <c r="O7" t="n">
         <v>20</v>
@@ -1565,10 +1685,10 @@
         <v>24</v>
       </c>
       <c r="Q7" t="n">
-        <v>10.59016659167609</v>
+        <v>22.1077387043411</v>
       </c>
       <c r="R7" t="n">
-        <v>42029.46936595559</v>
+        <v>76979.75214270862</v>
       </c>
       <c r="S7" t="n">
         <v>0</v>
@@ -1580,7 +1700,7 @@
         <v>0</v>
       </c>
       <c r="V7" t="n">
-        <v>104.169015391854</v>
+        <v>117.9183107742978</v>
       </c>
       <c r="W7" t="n">
         <v>84</v>
@@ -1595,7 +1715,7 @@
         <v>0</v>
       </c>
       <c r="AA7" t="n">
-        <v>104.169015391854</v>
+        <v>117.9183107742978</v>
       </c>
       <c r="AB7" t="n">
         <v>84</v>
@@ -1616,23 +1736,23 @@
         <v>0</v>
       </c>
       <c r="AH7" t="n">
-        <v>28498.50615663057</v>
+        <v>38871.17335038891</v>
       </c>
       <c r="AI7" t="n">
-        <v>-115520.4019070571</v>
+        <v>-154547.655469419</v>
       </c>
       <c r="AJ7" t="n">
-        <v>-12.59201158446214</v>
+        <v>8.895522366703</v>
       </c>
       <c r="AK7" t="n">
-        <v>76.63494469795778</v>
+        <v>74.73179054836476</v>
       </c>
       <c r="AL7" t="inlineStr"/>
       <c r="AM7" t="n">
-        <v>47.22511128963387</v>
+        <v>56.83952925270586</v>
       </c>
       <c r="AN7" t="n">
-        <v>2946.846944473154</v>
+        <v>3546.786625368845</v>
       </c>
       <c r="AO7" t="n">
         <v>0</v>
@@ -1671,10 +1791,28 @@
         <v>100</v>
       </c>
       <c r="BA7" t="n">
-        <v>46.28133066795252</v>
+        <v>0.9857795027894882</v>
       </c>
       <c r="BB7" t="n">
-        <v>41.68578293242115</v>
+        <v>34920.67772916342</v>
+      </c>
+      <c r="BC7" t="n">
+        <v>17.8922612956589</v>
+      </c>
+      <c r="BD7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE7" t="n">
+        <v>-76979.75214270862</v>
+      </c>
+      <c r="BF7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG7" t="n">
+        <v>43.24988273506372</v>
+      </c>
+      <c r="BH7" t="n">
+        <v>39.87869496594512</v>
       </c>
     </row>
     <row r="8">
@@ -1682,43 +1820,43 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>107.2244143657304</v>
+        <v>122.5014092351124</v>
       </c>
       <c r="C8" t="n">
-        <v>26.47129817593819</v>
+        <v>14.88890808066871</v>
       </c>
       <c r="D8" t="n">
         <v>84</v>
       </c>
       <c r="E8" t="n">
-        <v>113.3352123134832</v>
+        <v>131.6676061567416</v>
       </c>
       <c r="F8" t="n">
-        <v>21.27609029286715</v>
+        <v>9.876176047546991</v>
       </c>
       <c r="G8" t="n">
         <v>84</v>
       </c>
       <c r="H8" t="n">
-        <v>110.2798133396068</v>
+        <v>127.084507695927</v>
       </c>
       <c r="I8" t="n">
-        <v>23.76813370614713</v>
+        <v>12.22696543209685</v>
       </c>
       <c r="J8" t="n">
         <v>84</v>
       </c>
       <c r="K8" t="n">
-        <v>53.84969198703253</v>
+        <v>47.87788594012094</v>
       </c>
       <c r="L8" t="n">
-        <v>6.110797947752786</v>
+        <v>9.166196921629208</v>
       </c>
       <c r="M8" t="n">
-        <v>40.33096531417925</v>
+        <v>28.63022324310317</v>
       </c>
       <c r="N8" t="n">
-        <v>8.016067616916711</v>
+        <v>10.44306712961831</v>
       </c>
       <c r="O8" t="n">
         <v>20</v>
@@ -1727,10 +1865,10 @@
         <v>24</v>
       </c>
       <c r="Q8" t="n">
-        <v>16.23186629385287</v>
+        <v>27.77303456790315</v>
       </c>
       <c r="R8" t="n">
-        <v>46580.20724492621</v>
+        <v>83834.4088533293</v>
       </c>
       <c r="S8" t="n">
         <v>0</v>
@@ -1742,7 +1880,7 @@
         <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>110.2798133396068</v>
+        <v>127.084507695927</v>
       </c>
       <c r="W8" t="n">
         <v>84</v>
@@ -1757,7 +1895,7 @@
         <v>0</v>
       </c>
       <c r="AA8" t="n">
-        <v>110.2798133396068</v>
+        <v>127.084507695927</v>
       </c>
       <c r="AB8" t="n">
         <v>84</v>
@@ -1778,23 +1916,23 @@
         <v>0</v>
       </c>
       <c r="AH8" t="n">
-        <v>29768.47732398442</v>
+        <v>43650.1036060939</v>
       </c>
       <c r="AI8" t="n">
-        <v>-144319.386807589</v>
+        <v>-189468.3331985824</v>
       </c>
       <c r="AJ8" t="n">
-        <v>-12.59201158446214</v>
+        <v>8.895522366703</v>
       </c>
       <c r="AK8" t="n">
-        <v>76.13947459408594</v>
+        <v>72.76760549372993</v>
       </c>
       <c r="AL8" t="inlineStr"/>
       <c r="AM8" t="n">
-        <v>52.37134088793881</v>
+        <v>60.54064006163308</v>
       </c>
       <c r="AN8" t="n">
-        <v>3267.971671407382</v>
+        <v>3777.735939845904</v>
       </c>
       <c r="AO8" t="n">
         <v>0</v>
@@ -1833,10 +1971,28 @@
         <v>100</v>
       </c>
       <c r="BA8" t="n">
-        <v>41.68578293242115</v>
+        <v>0.9707839877130248</v>
       </c>
       <c r="BB8" t="n">
-        <v>37.72071648040119</v>
+        <v>28185.44380533544</v>
+      </c>
+      <c r="BC8" t="n">
+        <v>12.22696543209685</v>
+      </c>
+      <c r="BD8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE8" t="n">
+        <v>-83834.4088533293</v>
+      </c>
+      <c r="BF8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG8" t="n">
+        <v>39.87869496594512</v>
+      </c>
+      <c r="BH8" t="n">
+        <v>37.63965025753598</v>
       </c>
     </row>
     <row r="9">
@@ -1844,43 +2000,43 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>113.3352123134832</v>
+        <v>131.6676061567416</v>
       </c>
       <c r="C9" t="n">
-        <v>21.27609029286715</v>
+        <v>9.876176047546991</v>
       </c>
       <c r="D9" t="n">
         <v>84</v>
       </c>
       <c r="E9" t="n">
-        <v>119.446010261236</v>
+        <v>140.8338030783708</v>
       </c>
       <c r="F9" t="n">
-        <v>16.85101188766453</v>
+        <v>6.017709179269019</v>
       </c>
       <c r="G9" t="n">
         <v>84</v>
       </c>
       <c r="H9" t="n">
-        <v>116.3906112873596</v>
+        <v>136.2507046175562</v>
       </c>
       <c r="I9" t="n">
-        <v>18.97568541030031</v>
+        <v>7.812733485778423</v>
       </c>
       <c r="J9" t="n">
         <v>84</v>
       </c>
       <c r="K9" t="n">
-        <v>51.36089406872483</v>
+        <v>45.61046841803196</v>
       </c>
       <c r="L9" t="n">
-        <v>6.110797947752815</v>
+        <v>9.166196921629194</v>
       </c>
       <c r="M9" t="n">
-        <v>35.88030576684071</v>
+        <v>22.79859334072413</v>
       </c>
       <c r="N9" t="n">
-        <v>7.541931059457129</v>
+        <v>9.943018453871977</v>
       </c>
       <c r="O9" t="n">
         <v>20</v>
@@ -1889,10 +2045,10 @@
         <v>24</v>
       </c>
       <c r="Q9" t="n">
-        <v>21.02431458969969</v>
+        <v>32.18726651422158</v>
       </c>
       <c r="R9" t="n">
-        <v>50445.91742877474</v>
+        <v>89175.35579798571</v>
       </c>
       <c r="S9" t="n">
         <v>0</v>
@@ -1904,7 +2060,7 @@
         <v>0</v>
       </c>
       <c r="V9" t="n">
-        <v>116.3906112873596</v>
+        <v>136.2507046175562</v>
       </c>
       <c r="W9" t="n">
         <v>84</v>
@@ -1919,7 +2075,7 @@
         <v>0</v>
       </c>
       <c r="AA9" t="n">
-        <v>116.3906112873596</v>
+        <v>136.2507046175562</v>
       </c>
       <c r="AB9" t="n">
         <v>84</v>
@@ -1940,23 +2096,23 @@
         <v>0</v>
       </c>
       <c r="AH9" t="n">
-        <v>30920.1226636353</v>
+        <v>48042.79535698028</v>
       </c>
       <c r="AI9" t="n">
-        <v>-169958.8168828885</v>
+        <v>-217653.7770039178</v>
       </c>
       <c r="AJ9" t="n">
-        <v>-12.59201158446214</v>
+        <v>8.895522366703</v>
       </c>
       <c r="AK9" t="n">
-        <v>75.05915472413723</v>
+        <v>70.80342043909509</v>
       </c>
       <c r="AL9" t="inlineStr"/>
       <c r="AM9" t="n">
-        <v>56.08346931383691</v>
+        <v>62.99068695331667</v>
       </c>
       <c r="AN9" t="n">
-        <v>3499.608485183423</v>
+        <v>3930.61886588696</v>
       </c>
       <c r="AO9" t="n">
         <v>0</v>
@@ -1995,10 +2151,28 @@
         <v>100</v>
       </c>
       <c r="BA9" t="n">
-        <v>37.72071648040119</v>
+        <v>0.9671987351467956</v>
       </c>
       <c r="BB9" t="n">
-        <v>34.28886333997961</v>
+        <v>20462.32272574432</v>
+      </c>
+      <c r="BC9" t="n">
+        <v>7.812733485778423</v>
+      </c>
+      <c r="BD9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE9" t="n">
+        <v>-89175.35579798571</v>
+      </c>
+      <c r="BF9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG9" t="n">
+        <v>37.63965025753598</v>
+      </c>
+      <c r="BH9" t="n">
+        <v>36.44950854230976</v>
       </c>
     </row>
     <row r="10">
@@ -2006,43 +2180,43 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>119.446010261236</v>
+        <v>140.8338030783708</v>
       </c>
       <c r="C10" t="n">
-        <v>16.85101188766453</v>
+        <v>6.017709179269019</v>
       </c>
       <c r="D10" t="n">
         <v>84</v>
       </c>
       <c r="E10" t="n">
-        <v>125.5568082089888</v>
+        <v>150</v>
       </c>
       <c r="F10" t="n">
-        <v>13.07836411159025</v>
+        <v>3.175416344814579</v>
       </c>
       <c r="G10" t="n">
         <v>84</v>
       </c>
       <c r="H10" t="n">
-        <v>122.5014092351124</v>
+        <v>145.4169015391854</v>
       </c>
       <c r="I10" t="n">
-        <v>14.88890808066871</v>
+        <v>4.475970115066076</v>
       </c>
       <c r="J10" t="n">
         <v>84</v>
       </c>
       <c r="K10" t="n">
-        <v>49.24908341006158</v>
+        <v>43.90109028185986</v>
       </c>
       <c r="L10" t="n">
-        <v>6.110797947752786</v>
+        <v>9.166196921629194</v>
       </c>
       <c r="M10" t="n">
-        <v>31.66729456830227</v>
+        <v>17.2073735282605</v>
       </c>
       <c r="N10" t="n">
-        <v>7.179790330436168</v>
+        <v>9.595697472845927</v>
       </c>
       <c r="O10" t="n">
         <v>20</v>
@@ -2051,10 +2225,10 @@
         <v>24</v>
       </c>
       <c r="Q10" t="n">
-        <v>25.11109191933129</v>
+        <v>35.52402988493392</v>
       </c>
       <c r="R10" t="n">
-        <v>53742.41553726079</v>
+        <v>93212.63257604709</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
@@ -2066,7 +2240,7 @@
         <v>0</v>
       </c>
       <c r="V10" t="n">
-        <v>122.5014092351124</v>
+        <v>145.4169015391854</v>
       </c>
       <c r="W10" t="n">
         <v>84</v>
@@ -2081,7 +2255,7 @@
         <v>0</v>
       </c>
       <c r="AA10" t="n">
-        <v>122.5014092351124</v>
+        <v>145.4169015391854</v>
       </c>
       <c r="AB10" t="n">
         <v>84</v>
@@ -2102,23 +2276,23 @@
         <v>0</v>
       </c>
       <c r="AH10" t="n">
-        <v>31945.95796741925</v>
+        <v>52500.90525190541</v>
       </c>
       <c r="AI10" t="n">
-        <v>-191919.3972456553</v>
+        <v>-238116.0997296621</v>
       </c>
       <c r="AJ10" t="n">
-        <v>-12.59201158446214</v>
+        <v>8.895522366703</v>
       </c>
       <c r="AK10" t="n">
-        <v>73.74969802104734</v>
+        <v>68.37492953824437</v>
       </c>
       <c r="AL10" t="inlineStr"/>
       <c r="AM10" t="n">
-        <v>58.86078994037862</v>
+        <v>63.8989594231783</v>
       </c>
       <c r="AN10" t="n">
-        <v>3672.913292279626</v>
+        <v>3987.295068006326</v>
       </c>
       <c r="AO10" t="n">
         <v>0</v>
@@ -2157,10 +2331,28 @@
         <v>100</v>
       </c>
       <c r="BA10" t="n">
-        <v>34.28886333997961</v>
+        <v>0.973212052632304</v>
       </c>
       <c r="BB10" t="n">
-        <v>31.31727320420182</v>
+        <v>11907.22927254531</v>
+      </c>
+      <c r="BC10" t="n">
+        <v>4.475970115066076</v>
+      </c>
+      <c r="BD10" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE10" t="n">
+        <v>-93212.63257604709</v>
+      </c>
+      <c r="BF10" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG10" t="n">
+        <v>36.44950854230976</v>
+      </c>
+      <c r="BH10" t="n">
+        <v>36.32727754193699</v>
       </c>
     </row>
     <row r="11">
@@ -2168,55 +2360,55 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>125.5568082089888</v>
+        <v>150</v>
       </c>
       <c r="C11" t="n">
-        <v>13.07836411159025</v>
+        <v>3.175416344814579</v>
       </c>
       <c r="D11" t="n">
         <v>84</v>
       </c>
       <c r="E11" t="n">
-        <v>131.6676061567416</v>
+        <v>158.2333333333333</v>
       </c>
       <c r="F11" t="n">
-        <v>9.876176047546991</v>
+        <v>1.415625533815515</v>
       </c>
       <c r="G11" t="n">
-        <v>84</v>
+        <v>77.33333333333334</v>
       </c>
       <c r="H11" t="n">
-        <v>128.6122071828652</v>
+        <v>154.1166666666667</v>
       </c>
       <c r="I11" t="n">
-        <v>11.41008704398351</v>
+        <v>2.20487543395177</v>
       </c>
       <c r="J11" t="n">
-        <v>84</v>
+        <v>80.66666666666666</v>
       </c>
       <c r="K11" t="n">
-        <v>47.45771498882042</v>
+        <v>41.02997495415351</v>
       </c>
       <c r="L11" t="n">
-        <v>6.110797947752815</v>
+        <v>8.23333333333332</v>
       </c>
       <c r="M11" t="n">
-        <v>27.63762763254577</v>
+        <v>12.05399136403763</v>
       </c>
       <c r="N11" t="n">
-        <v>6.897848461355562</v>
+        <v>8.418960934778243</v>
       </c>
       <c r="O11" t="n">
-        <v>20</v>
+        <v>16.66666666666666</v>
       </c>
       <c r="P11" t="n">
         <v>24</v>
       </c>
       <c r="Q11" t="n">
-        <v>28.58991295601649</v>
+        <v>37.79512456604823</v>
       </c>
       <c r="R11" t="n">
-        <v>56548.52070086898</v>
+        <v>82626.63026726997</v>
       </c>
       <c r="S11" t="n">
         <v>0</v>
@@ -2228,10 +2420,10 @@
         <v>0</v>
       </c>
       <c r="V11" t="n">
-        <v>128.6122071828652</v>
+        <v>154.1166666666667</v>
       </c>
       <c r="W11" t="n">
-        <v>84</v>
+        <v>80.66666666666667</v>
       </c>
       <c r="X11" t="n">
         <v>0</v>
@@ -2243,13 +2435,13 @@
         <v>0</v>
       </c>
       <c r="AA11" t="n">
-        <v>128.6122071828652</v>
+        <v>154.1166666666667</v>
       </c>
       <c r="AB11" t="n">
-        <v>84</v>
+        <v>80.66666666666667</v>
       </c>
       <c r="AC11" t="n">
-        <v>-0</v>
+        <v>38.99766642858375</v>
       </c>
       <c r="AD11" t="n">
         <v>0</v>
@@ -2264,23 +2456,23 @@
         <v>0</v>
       </c>
       <c r="AH11" t="n">
-        <v>32836.91553143966</v>
+        <v>47579.47600472617</v>
       </c>
       <c r="AI11" t="n">
-        <v>-209938.9217988499</v>
+        <v>-250023.3290022075</v>
       </c>
       <c r="AJ11" t="n">
-        <v>-12.59201158446214</v>
+        <v>8.895522366703</v>
       </c>
       <c r="AK11" t="n">
-        <v>72.44024131795746</v>
+        <v>65.765</v>
       </c>
       <c r="AL11" t="inlineStr"/>
       <c r="AM11" t="n">
-        <v>61.03015427397395</v>
+        <v>63.56012456604823</v>
       </c>
       <c r="AN11" t="n">
-        <v>3808.281626695974</v>
+        <v>3966.15177292141</v>
       </c>
       <c r="AO11" t="n">
         <v>0</v>
@@ -2319,10 +2511,28 @@
         <v>100</v>
       </c>
       <c r="BA11" t="n">
-        <v>31.31727320420182</v>
+        <v>0.9871907645947534</v>
       </c>
       <c r="BB11" t="n">
-        <v>28.75440603700956</v>
+        <v>3004.42021786584</v>
+      </c>
+      <c r="BC11" t="n">
+        <v>2.20487543395177</v>
+      </c>
+      <c r="BD11" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE11" t="n">
+        <v>-82626.63026726997</v>
+      </c>
+      <c r="BF11" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG11" t="n">
+        <v>36.32727754193699</v>
+      </c>
+      <c r="BH11" t="n">
+        <v>37.20310813535692</v>
       </c>
     </row>
     <row r="12">
@@ -2330,55 +2540,55 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>131.6676061567416</v>
+        <v>158.2333333333333</v>
       </c>
       <c r="C12" t="n">
-        <v>9.876176047546991</v>
+        <v>1.415625533815515</v>
       </c>
       <c r="D12" t="n">
-        <v>84</v>
+        <v>77.33333333333334</v>
       </c>
       <c r="E12" t="n">
-        <v>137.7784041044944</v>
+        <v>166.4666666666667</v>
       </c>
       <c r="F12" t="n">
-        <v>7.185384777010029</v>
+        <v>0.3647541167172079</v>
       </c>
       <c r="G12" t="n">
-        <v>84</v>
+        <v>70.66666666666666</v>
       </c>
       <c r="H12" t="n">
-        <v>134.723005130618</v>
+        <v>162.35</v>
       </c>
       <c r="I12" t="n">
-        <v>8.469875536565695</v>
+        <v>0.8033392699129251</v>
       </c>
       <c r="J12" t="n">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="K12" t="n">
-        <v>45.94755473718361</v>
+        <v>36.88463875631324</v>
       </c>
       <c r="L12" t="n">
-        <v>6.110797947752786</v>
+        <v>8.233333333333348</v>
       </c>
       <c r="M12" t="n">
-        <v>23.75145594212175</v>
+        <v>7.267387142297566</v>
       </c>
       <c r="N12" t="n">
-        <v>6.676269680146683</v>
+        <v>8.300010577711028</v>
       </c>
       <c r="O12" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="P12" t="n">
         <v>24</v>
       </c>
       <c r="Q12" t="n">
-        <v>31.5301244634343</v>
+        <v>39.19666073008707</v>
       </c>
       <c r="R12" t="n">
-        <v>58920.16977567312</v>
+        <v>77014.26421479211</v>
       </c>
       <c r="S12" t="n">
         <v>0</v>
@@ -2390,10 +2600,10 @@
         <v>0</v>
       </c>
       <c r="V12" t="n">
-        <v>134.723005130618</v>
+        <v>162.35</v>
       </c>
       <c r="W12" t="n">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="X12" t="n">
         <v>0</v>
@@ -2405,13 +2615,13 @@
         <v>0</v>
       </c>
       <c r="AA12" t="n">
-        <v>134.723005130618</v>
+        <v>162.35</v>
       </c>
       <c r="AB12" t="n">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="AC12" t="n">
-        <v>-0</v>
+        <v>38.99766642858377</v>
       </c>
       <c r="AD12" t="n">
         <v>0</v>
@@ -2426,23 +2636,23 @@
         <v>0</v>
       </c>
       <c r="AH12" t="n">
-        <v>33634.52020851032</v>
+        <v>44131.6554115867</v>
       </c>
       <c r="AI12" t="n">
-        <v>-223888.8203151459</v>
+        <v>-253027.7492200733</v>
       </c>
       <c r="AJ12" t="n">
-        <v>-12.59201158446214</v>
+        <v>8.895522366703</v>
       </c>
       <c r="AK12" t="n">
-        <v>71.13078461486758</v>
+        <v>63.295</v>
       </c>
       <c r="AL12" t="inlineStr"/>
       <c r="AM12" t="n">
-        <v>62.66090907830188</v>
+        <v>62.49166073008708</v>
       </c>
       <c r="AN12" t="n">
-        <v>3910.040726486037</v>
+        <v>3899.479629557433</v>
       </c>
       <c r="AO12" t="n">
         <v>0</v>
@@ -2481,10 +2691,28 @@
         <v>100</v>
       </c>
       <c r="BA12" t="n">
-        <v>28.75440603700956</v>
+        <v>1.007940701782509</v>
       </c>
       <c r="BB12" t="n">
-        <v>26.56712855357358</v>
+        <v>-3582.902287020448</v>
+      </c>
+      <c r="BC12" t="n">
+        <v>0.8033392699129251</v>
+      </c>
+      <c r="BD12" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE12" t="n">
+        <v>-77014.26421479211</v>
+      </c>
+      <c r="BF12" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG12" t="n">
+        <v>37.20310813535692</v>
+      </c>
+      <c r="BH12" t="n">
+        <v>39.02383752628205</v>
       </c>
     </row>
     <row r="13">
@@ -2492,55 +2720,55 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>137.7784041044944</v>
+        <v>166.4666666666667</v>
       </c>
       <c r="C13" t="n">
-        <v>7.185384777010029</v>
+        <v>0.3647541167172079</v>
       </c>
       <c r="D13" t="n">
-        <v>84</v>
+        <v>70.66666666666666</v>
       </c>
       <c r="E13" t="n">
-        <v>143.8892020522472</v>
+        <v>174.7</v>
       </c>
       <c r="F13" t="n">
-        <v>4.962542905157136</v>
+        <v>0.0004500010125099152</v>
       </c>
       <c r="G13" t="n">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="H13" t="n">
-        <v>140.8338030783708</v>
+        <v>170.5833333333333</v>
       </c>
       <c r="I13" t="n">
-        <v>6.017709179269019</v>
+        <v>0.09758233378155978</v>
       </c>
       <c r="J13" t="n">
-        <v>84</v>
+        <v>67.33333333333334</v>
       </c>
       <c r="K13" t="n">
-        <v>44.69045170069924</v>
+        <v>33.07691852283967</v>
       </c>
       <c r="L13" t="n">
-        <v>6.110797947752786</v>
+        <v>8.23333333333332</v>
       </c>
       <c r="M13" t="n">
-        <v>19.9781626017629</v>
+        <v>2.531387044257777</v>
       </c>
       <c r="N13" t="n">
-        <v>6.502073842197558</v>
+        <v>8.241375459842734</v>
       </c>
       <c r="O13" t="n">
-        <v>20</v>
+        <v>3.333333333333343</v>
       </c>
       <c r="P13" t="n">
         <v>24</v>
       </c>
       <c r="Q13" t="n">
-        <v>33.98229082073098</v>
+        <v>39.90241766621844</v>
       </c>
       <c r="R13" t="n">
-        <v>60898.14927064375</v>
+        <v>70645.72529742388</v>
       </c>
       <c r="S13" t="n">
         <v>0</v>
@@ -2552,10 +2780,10 @@
         <v>0</v>
       </c>
       <c r="V13" t="n">
-        <v>140.8338030783708</v>
+        <v>170.5833333333333</v>
       </c>
       <c r="W13" t="n">
-        <v>84</v>
+        <v>67.33333333333333</v>
       </c>
       <c r="X13" t="n">
         <v>0</v>
@@ -2567,13 +2795,13 @@
         <v>0</v>
       </c>
       <c r="AA13" t="n">
-        <v>140.8338030783708</v>
+        <v>170.5833333333333</v>
       </c>
       <c r="AB13" t="n">
-        <v>84</v>
+        <v>67.33333333333333</v>
       </c>
       <c r="AC13" t="n">
-        <v>-0</v>
+        <v>38.99766642858375</v>
       </c>
       <c r="AD13" t="n">
         <v>0</v>
@@ -2588,23 +2816,23 @@
         <v>0</v>
       </c>
       <c r="AH13" t="n">
-        <v>34390.01015456274</v>
+        <v>40423.34472842945</v>
       </c>
       <c r="AI13" t="n">
-        <v>-233691.4905462345</v>
+        <v>-249444.8469330529</v>
       </c>
       <c r="AJ13" t="n">
-        <v>-12.59201158446214</v>
+        <v>8.895522366703</v>
       </c>
       <c r="AK13" t="n">
-        <v>69.74985907648876</v>
+        <v>60.73076923076924</v>
       </c>
       <c r="AL13" t="inlineStr"/>
       <c r="AM13" t="n">
-        <v>63.73214989721974</v>
+        <v>60.63318689698768</v>
       </c>
       <c r="AN13" t="n">
-        <v>3976.886153586512</v>
+        <v>3783.510862372031</v>
       </c>
       <c r="AO13" t="n">
         <v>0</v>
@@ -2643,10 +2871,28 @@
         <v>100</v>
       </c>
       <c r="BA13" t="n">
-        <v>26.56712855357358</v>
+        <v>1.036616181329966</v>
       </c>
       <c r="BB13" t="n">
-        <v>24.73718209590243</v>
+        <v>-9273.070980026772</v>
+      </c>
+      <c r="BC13" t="n">
+        <v>0.09758233378155978</v>
+      </c>
+      <c r="BD13" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE13" t="n">
+        <v>-70645.72529742388</v>
+      </c>
+      <c r="BF13" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG13" t="n">
+        <v>39.02383752628205</v>
+      </c>
+      <c r="BH13" t="n">
+        <v>41.84031032800412</v>
       </c>
     </row>
     <row r="14">
@@ -2654,55 +2900,55 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>143.8892020522472</v>
+        <v>174.7</v>
       </c>
       <c r="C14" t="n">
-        <v>4.962542905157136</v>
+        <v>0.0004500010125099152</v>
       </c>
       <c r="D14" t="n">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E14" t="n">
-        <v>150</v>
+        <v>184.5666666666667</v>
       </c>
       <c r="F14" t="n">
-        <v>3.175416344814579</v>
+        <v>0.4586573885559346</v>
       </c>
       <c r="G14" t="n">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="H14" t="n">
-        <v>146.9446010261236</v>
+        <v>179.6333333333333</v>
       </c>
       <c r="I14" t="n">
-        <v>4.016175381387228</v>
+        <v>0.107396558993301</v>
       </c>
       <c r="J14" t="n">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="K14" t="n">
-        <v>43.665820486883</v>
+        <v>29.42922364652098</v>
       </c>
       <c r="L14" t="n">
-        <v>6.110797947752815</v>
+        <v>9.866666666666674</v>
       </c>
       <c r="M14" t="n">
-        <v>16.29327132015469</v>
+        <v>-2.655655212963555</v>
       </c>
       <c r="N14" t="n">
-        <v>6.366487240984389</v>
+        <v>9.877274519623073</v>
       </c>
       <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="n">
         <v>20</v>
       </c>
-      <c r="P14" t="n">
-        <v>24</v>
-      </c>
       <c r="Q14" t="n">
-        <v>35.98382461861277</v>
+        <v>39.8926034410067</v>
       </c>
       <c r="R14" t="n">
-        <v>62512.63712907195</v>
+        <v>75636.12672156718</v>
       </c>
       <c r="S14" t="n">
         <v>0</v>
@@ -2714,10 +2960,10 @@
         <v>0</v>
       </c>
       <c r="V14" t="n">
-        <v>146.9446010261236</v>
+        <v>179.6333333333333</v>
       </c>
       <c r="W14" t="n">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="X14" t="n">
         <v>0</v>
@@ -2729,13 +2975,13 @@
         <v>0</v>
       </c>
       <c r="AA14" t="n">
-        <v>146.9446010261236</v>
+        <v>179.6333333333333</v>
       </c>
       <c r="AB14" t="n">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="AC14" t="n">
-        <v>-0</v>
+        <v>39.03551289874686</v>
       </c>
       <c r="AD14" t="n">
         <v>0</v>
@@ -2750,23 +2996,23 @@
         <v>0</v>
       </c>
       <c r="AH14" t="n">
-        <v>35247.85495846123</v>
+        <v>44278.44925609089</v>
       </c>
       <c r="AI14" t="n">
-        <v>-239291.2708023732</v>
+        <v>-240171.7759530261</v>
       </c>
       <c r="AJ14" t="n">
-        <v>-12.59201158446214</v>
+        <v>8.895522366703</v>
       </c>
       <c r="AK14" t="n">
-        <v>67.91661969216293</v>
+        <v>56.55384615384616</v>
       </c>
       <c r="AL14" t="inlineStr"/>
       <c r="AM14" t="n">
-        <v>63.9004443107757</v>
+        <v>56.44644959485286</v>
       </c>
       <c r="AN14" t="n">
-        <v>3987.387724992403</v>
+        <v>3522.258454718818</v>
       </c>
       <c r="AO14" t="n">
         <v>0</v>
@@ -2805,10 +3051,28 @@
         <v>100</v>
       </c>
       <c r="BA14" t="n">
-        <v>24.73718209590243</v>
+        <v>1.078668815540194</v>
       </c>
       <c r="BB14" t="n">
-        <v>23.26327390709199</v>
+        <v>-17548.00094839134</v>
+      </c>
+      <c r="BC14" t="n">
+        <v>0.107396558993301</v>
+      </c>
+      <c r="BD14" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE14" t="n">
+        <v>-75636.12672156718</v>
+      </c>
+      <c r="BF14" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG14" t="n">
+        <v>41.84031032800412</v>
+      </c>
+      <c r="BH14" t="n">
+        <v>46.73499959460959</v>
       </c>
     </row>
     <row r="15">
@@ -2816,55 +3080,55 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>150</v>
+        <v>184.5666666666667</v>
       </c>
       <c r="C15" t="n">
-        <v>3.175416344814579</v>
+        <v>0.4586573885559346</v>
       </c>
       <c r="D15" t="n">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="E15" t="n">
-        <v>156.175</v>
+        <v>194.4333333333333</v>
       </c>
       <c r="F15" t="n">
-        <v>1.787885803226899</v>
+        <v>1.906444882675629</v>
       </c>
       <c r="G15" t="n">
-        <v>78.99999999999999</v>
+        <v>48</v>
       </c>
       <c r="H15" t="n">
-        <v>153.0875</v>
+        <v>189.5</v>
       </c>
       <c r="I15" t="n">
-        <v>2.430320571655045</v>
+        <v>1.056834495757116</v>
       </c>
       <c r="J15" t="n">
-        <v>81.5</v>
+        <v>52</v>
       </c>
       <c r="K15" t="n">
-        <v>41.57288960342415</v>
+        <v>26.10232366321593</v>
       </c>
       <c r="L15" t="n">
-        <v>6.175000000000011</v>
+        <v>9.866666666666674</v>
       </c>
       <c r="M15" t="n">
-        <v>12.65764524391063</v>
+        <v>-8.33727918890569</v>
       </c>
       <c r="N15" t="n">
-        <v>6.328810380621291</v>
+        <v>9.972054781533719</v>
       </c>
       <c r="O15" t="n">
-        <v>17.5</v>
+        <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="Q15" t="n">
-        <v>37.56967942834495</v>
+        <v>38.94316550424288</v>
       </c>
       <c r="R15" t="n">
-        <v>62455.17070204408</v>
+        <v>64927.57875272598</v>
       </c>
       <c r="S15" t="n">
         <v>0</v>
@@ -2876,10 +3140,10 @@
         <v>0</v>
       </c>
       <c r="V15" t="n">
-        <v>153.0875</v>
+        <v>189.5</v>
       </c>
       <c r="W15" t="n">
-        <v>81.5</v>
+        <v>52</v>
       </c>
       <c r="X15" t="n">
         <v>0</v>
@@ -2891,13 +3155,13 @@
         <v>0</v>
       </c>
       <c r="AA15" t="n">
-        <v>153.0875</v>
+        <v>189.5</v>
       </c>
       <c r="AB15" t="n">
-        <v>81.5</v>
+        <v>52</v>
       </c>
       <c r="AC15" t="n">
-        <v>38.99766642858377</v>
+        <v>39.03551289874686</v>
       </c>
       <c r="AD15" t="n">
         <v>0</v>
@@ -2912,23 +3176,23 @@
         <v>0</v>
       </c>
       <c r="AH15" t="n">
-        <v>34647.27039230418</v>
+        <v>39308.15327048204</v>
       </c>
       <c r="AI15" t="n">
-        <v>-240598.5438619145</v>
+        <v>-222623.7750046348</v>
       </c>
       <c r="AJ15" t="n">
-        <v>-12.59201158446214</v>
+        <v>8.895522366703</v>
       </c>
       <c r="AK15" t="n">
-        <v>66.07375</v>
+        <v>52</v>
       </c>
       <c r="AL15" t="inlineStr"/>
       <c r="AM15" t="n">
-        <v>63.64342942834496</v>
+        <v>50.94316550424288</v>
       </c>
       <c r="AN15" t="n">
-        <v>3971.349996328725</v>
+        <v>3178.853527464756</v>
       </c>
       <c r="AO15" t="n">
         <v>0</v>
@@ -2967,10 +3231,28 @@
         <v>100</v>
       </c>
       <c r="BA15" t="n">
-        <v>23.26327390709199</v>
+        <v>1.14002513776078</v>
       </c>
       <c r="BB15" t="n">
-        <v>22.11339813559103</v>
+        <v>-22839.97067289398</v>
+      </c>
+      <c r="BC15" t="n">
+        <v>1.056834495757116</v>
+      </c>
+      <c r="BD15" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE15" t="n">
+        <v>-64927.57875272598</v>
+      </c>
+      <c r="BF15" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG15" t="n">
+        <v>46.73499959460959</v>
+      </c>
+      <c r="BH15" t="n">
+        <v>53.58964730465238</v>
       </c>
     </row>
     <row r="16">
@@ -2978,55 +3260,55 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>156.175</v>
+        <v>194.4333333333333</v>
       </c>
       <c r="C16" t="n">
-        <v>1.787885803226899</v>
+        <v>1.906444882675629</v>
       </c>
       <c r="D16" t="n">
-        <v>78.99999999999999</v>
+        <v>48</v>
       </c>
       <c r="E16" t="n">
-        <v>162.35</v>
+        <v>204.3</v>
       </c>
       <c r="F16" t="n">
-        <v>0.8033392699129251</v>
+        <v>4.388755891370195</v>
       </c>
       <c r="G16" t="n">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="H16" t="n">
-        <v>159.2625</v>
+        <v>199.3666666666667</v>
       </c>
       <c r="I16" t="n">
-        <v>1.246108462754748</v>
+        <v>3.0140960986827</v>
       </c>
       <c r="J16" t="n">
-        <v>76.5</v>
+        <v>44</v>
       </c>
       <c r="K16" t="n">
-        <v>38.39854900472974</v>
+        <v>23.34150559669511</v>
       </c>
       <c r="L16" t="n">
-        <v>6.174999999999983</v>
+        <v>9.866666666666674</v>
       </c>
       <c r="M16" t="n">
-        <v>9.054564536251398</v>
+        <v>-14.10305156392162</v>
       </c>
       <c r="N16" t="n">
-        <v>6.252918142138295</v>
+        <v>10.17329969590835</v>
       </c>
       <c r="O16" t="n">
-        <v>12.5</v>
+        <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="Q16" t="n">
-        <v>38.75389153724525</v>
+        <v>36.9859039013173</v>
       </c>
       <c r="R16" t="n">
-        <v>59406.67199200844</v>
+        <v>52906.44124107569</v>
       </c>
       <c r="S16" t="n">
         <v>0</v>
@@ -3038,10 +3320,10 @@
         <v>0</v>
       </c>
       <c r="V16" t="n">
-        <v>159.2625</v>
+        <v>199.3666666666667</v>
       </c>
       <c r="W16" t="n">
-        <v>76.5</v>
+        <v>44</v>
       </c>
       <c r="X16" t="n">
         <v>0</v>
@@ -3053,13 +3335,13 @@
         <v>0</v>
       </c>
       <c r="AA16" t="n">
-        <v>159.2625</v>
+        <v>199.3666666666667</v>
       </c>
       <c r="AB16" t="n">
-        <v>76.5</v>
+        <v>44</v>
       </c>
       <c r="AC16" t="n">
-        <v>38.99766642858373</v>
+        <v>39.03551289874686</v>
       </c>
       <c r="AD16" t="n">
         <v>0</v>
@@ -3074,23 +3356,23 @@
         <v>0</v>
       </c>
       <c r="AH16" t="n">
-        <v>31860.86985474124</v>
+        <v>35635.91984382608</v>
       </c>
       <c r="AI16" t="n">
-        <v>-237888.2349704002</v>
+        <v>-199783.8043317408</v>
       </c>
       <c r="AJ16" t="n">
-        <v>-12.59201158446214</v>
+        <v>8.895522366703</v>
       </c>
       <c r="AK16" t="n">
-        <v>64.22125</v>
+        <v>44</v>
       </c>
       <c r="AL16" t="inlineStr"/>
       <c r="AM16" t="n">
-        <v>62.97514153724525</v>
+        <v>40.9859039013173</v>
       </c>
       <c r="AN16" t="n">
-        <v>3929.648831924103</v>
+        <v>2557.520403442199</v>
       </c>
       <c r="AO16" t="n">
         <v>0</v>
@@ -3129,10 +3411,28 @@
         <v>100</v>
       </c>
       <c r="BA16" t="n">
-        <v>22.11339813559103</v>
+        <v>1.222895098458222</v>
       </c>
       <c r="BB16" t="n">
-        <v>21.26106846593072</v>
+        <v>-26471.29153442189</v>
+      </c>
+      <c r="BC16" t="n">
+        <v>3.0140960986827</v>
+      </c>
+      <c r="BD16" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE16" t="n">
+        <v>-52906.44124107569</v>
+      </c>
+      <c r="BF16" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG16" t="n">
+        <v>53.58964730465238</v>
+      </c>
+      <c r="BH16" t="n">
+        <v>62.9766463448568</v>
       </c>
     </row>
     <row r="17">
@@ -3140,55 +3440,55 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>162.35</v>
+        <v>204.3</v>
       </c>
       <c r="C17" t="n">
-        <v>0.8033392699129251</v>
+        <v>4.388755891370195</v>
       </c>
       <c r="D17" t="n">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="E17" t="n">
-        <v>168.525</v>
+        <v>212.7495302549625</v>
       </c>
       <c r="F17" t="n">
-        <v>0.2098483065588255</v>
+        <v>7.398850085273409</v>
       </c>
       <c r="G17" t="n">
-        <v>69.00000000000001</v>
+        <v>40</v>
       </c>
       <c r="H17" t="n">
-        <v>165.4375</v>
+        <v>208.5247651274813</v>
       </c>
       <c r="I17" t="n">
-        <v>0.4582570287720955</v>
+        <v>5.786995997647878</v>
       </c>
       <c r="J17" t="n">
-        <v>71.5</v>
+        <v>40</v>
       </c>
       <c r="K17" t="n">
-        <v>35.41815342926989</v>
+        <v>22.89349799882394</v>
       </c>
       <c r="L17" t="n">
-        <v>6.174999999999983</v>
+        <v>8.449530254962525</v>
       </c>
       <c r="M17" t="n">
-        <v>5.487293448773431</v>
+        <v>-19.58759818966366</v>
       </c>
       <c r="N17" t="n">
-        <v>6.203427643199737</v>
+        <v>8.96853926316963</v>
       </c>
       <c r="O17" t="n">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="P17" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>39.5417429712279</v>
+        <v>34.21300400235212</v>
       </c>
       <c r="R17" t="n">
-        <v>56035.09969584771</v>
+        <v>38159.06324089572</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
@@ -3200,10 +3500,10 @@
         <v>0</v>
       </c>
       <c r="V17" t="n">
-        <v>165.4375</v>
+        <v>208.5247651274813</v>
       </c>
       <c r="W17" t="n">
-        <v>71.5</v>
+        <v>40</v>
       </c>
       <c r="X17" t="n">
         <v>0</v>
@@ -3215,13 +3515,13 @@
         <v>0</v>
       </c>
       <c r="AA17" t="n">
-        <v>165.4375</v>
+        <v>208.5247651274813</v>
       </c>
       <c r="AB17" t="n">
-        <v>71.5</v>
+        <v>40</v>
       </c>
       <c r="AC17" t="n">
-        <v>38.99766642858373</v>
+        <v>-0</v>
       </c>
       <c r="AD17" t="n">
         <v>0</v>
@@ -3236,23 +3536,23 @@
         <v>0</v>
       </c>
       <c r="AH17" t="n">
-        <v>29051.6597596172</v>
+        <v>28870.73921816798</v>
       </c>
       <c r="AI17" t="n">
-        <v>-231832.7248642761</v>
+        <v>-173312.5127973189</v>
       </c>
       <c r="AJ17" t="n">
-        <v>-12.59201158446214</v>
+        <v>8.895522366703</v>
       </c>
       <c r="AK17" t="n">
-        <v>62.36875</v>
+        <v>40</v>
       </c>
       <c r="AL17" t="inlineStr"/>
       <c r="AM17" t="n">
-        <v>61.9104929712279</v>
+        <v>34.21300400235212</v>
       </c>
       <c r="AN17" t="n">
-        <v>3863.214761404621</v>
+        <v>2134.891449746772</v>
       </c>
       <c r="AO17" t="n">
         <v>0</v>
@@ -3291,10 +3591,28 @@
         <v>100</v>
       </c>
       <c r="BA17" t="n">
-        <v>21.26106846593072</v>
+        <v>1.327139287109632</v>
       </c>
       <c r="BB17" t="n">
-        <v>20.68451386084556</v>
+        <v>-25302.58192169503</v>
+      </c>
+      <c r="BC17" t="n">
+        <v>5.786995997647878</v>
+      </c>
+      <c r="BD17" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE17" t="n">
+        <v>-38159.06324089572</v>
+      </c>
+      <c r="BF17" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG17" t="n">
+        <v>62.9766463448568</v>
+      </c>
+      <c r="BH17" t="n">
+        <v>74.18885215816957</v>
       </c>
     </row>
     <row r="18">
@@ -3302,55 +3620,55 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>168.525</v>
+        <v>212.7495302549625</v>
       </c>
       <c r="C18" t="n">
-        <v>0.2098483065588255</v>
+        <v>7.398850085273409</v>
       </c>
       <c r="D18" t="n">
-        <v>69.00000000000001</v>
+        <v>40</v>
       </c>
       <c r="E18" t="n">
-        <v>174.7</v>
+        <v>221.1990605099251</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0004500010125099152</v>
+        <v>11.31151817738515</v>
       </c>
       <c r="G18" t="n">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="H18" t="n">
-        <v>171.6125</v>
+        <v>216.9742953824438</v>
       </c>
       <c r="I18" t="n">
-        <v>0.05739225060214892</v>
+        <v>9.235697947114929</v>
       </c>
       <c r="J18" t="n">
-        <v>66.5</v>
+        <v>40</v>
       </c>
       <c r="K18" t="n">
-        <v>32.62382833889529</v>
+        <v>24.61784897355746</v>
       </c>
       <c r="L18" t="n">
-        <v>6.175000000000011</v>
+        <v>8.449530254962525</v>
       </c>
       <c r="M18" t="n">
-        <v>1.941265923951766</v>
+        <v>-24.8183601564723</v>
       </c>
       <c r="N18" t="n">
-        <v>6.178546006607693</v>
+        <v>9.309310008288602</v>
       </c>
       <c r="O18" t="n">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="P18" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="Q18" t="n">
-        <v>39.94260774939785</v>
+        <v>30.76430205288507</v>
       </c>
       <c r="R18" t="n">
-        <v>52348.09457653428</v>
+        <v>34312.59492786288</v>
       </c>
       <c r="S18" t="n">
         <v>0</v>
@@ -3362,10 +3680,10 @@
         <v>0</v>
       </c>
       <c r="V18" t="n">
-        <v>171.6125</v>
+        <v>216.9742953824438</v>
       </c>
       <c r="W18" t="n">
-        <v>66.5</v>
+        <v>40</v>
       </c>
       <c r="X18" t="n">
         <v>0</v>
@@ -3377,13 +3695,13 @@
         <v>0</v>
       </c>
       <c r="AA18" t="n">
-        <v>171.6125</v>
+        <v>216.9742953824438</v>
       </c>
       <c r="AB18" t="n">
-        <v>66.5</v>
+        <v>40</v>
       </c>
       <c r="AC18" t="n">
-        <v>38.99766642858377</v>
+        <v>-0</v>
       </c>
       <c r="AD18" t="n">
         <v>0</v>
@@ -3398,23 +3716,23 @@
         <v>0</v>
       </c>
       <c r="AH18" t="n">
-        <v>26281.38612822751</v>
+        <v>29310.87146346142</v>
       </c>
       <c r="AI18" t="n">
-        <v>-222934.2798657535</v>
+        <v>-148009.9308756239</v>
       </c>
       <c r="AJ18" t="n">
-        <v>-12.59201158446214</v>
+        <v>8.895522366703</v>
       </c>
       <c r="AK18" t="n">
-        <v>60.25576923076924</v>
+        <v>40</v>
       </c>
       <c r="AL18" t="inlineStr"/>
       <c r="AM18" t="n">
-        <v>60.19837698016709</v>
+        <v>30.76430205288507</v>
       </c>
       <c r="AN18" t="n">
-        <v>3756.378723562426</v>
+        <v>1919.692448100029</v>
       </c>
       <c r="AO18" t="n">
         <v>0</v>
@@ -3453,10 +3771,28 @@
         <v>100</v>
       </c>
       <c r="BA18" t="n">
-        <v>20.68451386084556</v>
+        <v>1.458141175153545</v>
       </c>
       <c r="BB18" t="n">
-        <v>20.36654100848288</v>
+        <v>-28895.43671521074</v>
+      </c>
+      <c r="BC18" t="n">
+        <v>9.235697947114929</v>
+      </c>
+      <c r="BD18" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE18" t="n">
+        <v>-34312.59492786288</v>
+      </c>
+      <c r="BF18" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG18" t="n">
+        <v>74.18885215816957</v>
+      </c>
+      <c r="BH18" t="n">
+        <v>91.42843112700038</v>
       </c>
     </row>
     <row r="19">
@@ -3464,55 +3800,55 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>174.7</v>
+        <v>221.1990605099251</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0004500010125099152</v>
+        <v>11.31151817738515</v>
       </c>
       <c r="D19" t="n">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="E19" t="n">
-        <v>180.62</v>
+        <v>229.6485907648876</v>
       </c>
       <c r="F19" t="n">
-        <v>0.158046894103677</v>
+        <v>16.25317004559611</v>
       </c>
       <c r="G19" t="n">
-        <v>59.19999999999999</v>
+        <v>40</v>
       </c>
       <c r="H19" t="n">
-        <v>177.66</v>
+        <v>225.4238256374063</v>
       </c>
       <c r="I19" t="n">
-        <v>0.03538426022936392</v>
+        <v>13.64354217495692</v>
       </c>
       <c r="J19" t="n">
-        <v>61.59999999999999</v>
+        <v>40</v>
       </c>
       <c r="K19" t="n">
-        <v>30.15934747246974</v>
+        <v>26.82177108747846</v>
       </c>
       <c r="L19" t="n">
-        <v>5.920000000000016</v>
+        <v>8.449530254962553</v>
       </c>
       <c r="M19" t="n">
-        <v>-1.524247520525697</v>
+        <v>-30.28079917114116</v>
       </c>
       <c r="N19" t="n">
-        <v>5.922095489679116</v>
+        <v>9.784479896200905</v>
       </c>
       <c r="O19" t="n">
         <v>0</v>
       </c>
       <c r="P19" t="n">
-        <v>21.59999999999999</v>
+        <v>0</v>
       </c>
       <c r="Q19" t="n">
-        <v>39.96461573977064</v>
+        <v>26.35645782504308</v>
       </c>
       <c r="R19" t="n">
-        <v>46574.58932368648</v>
+        <v>29396.35879043768</v>
       </c>
       <c r="S19" t="n">
         <v>0</v>
@@ -3524,10 +3860,10 @@
         <v>0</v>
       </c>
       <c r="V19" t="n">
-        <v>177.66</v>
+        <v>225.4238256374063</v>
       </c>
       <c r="W19" t="n">
-        <v>61.59999999999999</v>
+        <v>40</v>
       </c>
       <c r="X19" t="n">
         <v>0</v>
@@ -3539,13 +3875,13 @@
         <v>0</v>
       </c>
       <c r="AA19" t="n">
-        <v>177.66</v>
+        <v>225.4238256374063</v>
       </c>
       <c r="AB19" t="n">
-        <v>61.59999999999999</v>
+        <v>40</v>
       </c>
       <c r="AC19" t="n">
-        <v>39.03551289874687</v>
+        <v>-0</v>
       </c>
       <c r="AD19" t="n">
         <v>0</v>
@@ -3560,23 +3896,23 @@
         <v>0</v>
       </c>
       <c r="AH19" t="n">
-        <v>22898.50835564055</v>
+        <v>29300.49886779593</v>
       </c>
       <c r="AI19" t="n">
-        <v>-211665.927168838</v>
+        <v>-119114.4941604131</v>
       </c>
       <c r="AJ19" t="n">
-        <v>-12.59201158446214</v>
+        <v>8.895522366703</v>
       </c>
       <c r="AK19" t="n">
-        <v>57.46461538461539</v>
+        <v>40</v>
       </c>
       <c r="AL19" t="inlineStr"/>
       <c r="AM19" t="n">
-        <v>57.42923112438602</v>
+        <v>26.35645782504308</v>
       </c>
       <c r="AN19" t="n">
-        <v>3583.584022161688</v>
+        <v>1644.642968282688</v>
       </c>
       <c r="AO19" t="n">
         <v>0</v>
@@ -3615,10 +3951,28 @@
         <v>100</v>
       </c>
       <c r="BA19" t="n">
-        <v>20.36654100848288</v>
+        <v>1.641974102634091</v>
       </c>
       <c r="BB19" t="n">
-        <v>20.29925737948861</v>
+        <v>-31670.94512690204</v>
+      </c>
+      <c r="BC19" t="n">
+        <v>13.64354217495692</v>
+      </c>
+      <c r="BD19" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE19" t="n">
+        <v>-29396.35879043768</v>
+      </c>
+      <c r="BF19" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG19" t="n">
+        <v>91.42843112700038</v>
+      </c>
+      <c r="BH19" t="n">
+        <v>121.1631101942303</v>
       </c>
     </row>
     <row r="20">
@@ -3626,55 +3980,55 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>180.62</v>
+        <v>229.6485907648876</v>
       </c>
       <c r="C20" t="n">
-        <v>0.158046894103677</v>
+        <v>16.25317004559611</v>
       </c>
       <c r="D20" t="n">
-        <v>59.19999999999999</v>
+        <v>40</v>
       </c>
       <c r="E20" t="n">
-        <v>186.54</v>
+        <v>238.0981210198501</v>
       </c>
       <c r="F20" t="n">
-        <v>0.6680897193656108</v>
+        <v>22.4201886843984</v>
       </c>
       <c r="G20" t="n">
-        <v>54.40000000000001</v>
+        <v>40</v>
       </c>
       <c r="H20" t="n">
-        <v>183.58</v>
+        <v>233.8733558923689</v>
       </c>
       <c r="I20" t="n">
-        <v>0.3687619267932547</v>
+        <v>19.16728406164694</v>
       </c>
       <c r="J20" t="n">
-        <v>56.80000000000001</v>
+        <v>40</v>
       </c>
       <c r="K20" t="n">
-        <v>28.03316659594709</v>
+        <v>29.58364203082347</v>
       </c>
       <c r="L20" t="n">
-        <v>5.919999999999987</v>
+        <v>8.449530254962525</v>
       </c>
       <c r="M20" t="n">
-        <v>-4.922029561265584</v>
+        <v>-36.0671891153162</v>
       </c>
       <c r="N20" t="n">
-        <v>5.94191150736289</v>
+        <v>10.4531069590765</v>
       </c>
       <c r="O20" t="n">
         <v>0</v>
       </c>
       <c r="P20" t="n">
-        <v>16.80000000000001</v>
+        <v>0</v>
       </c>
       <c r="Q20" t="n">
-        <v>39.63123807320675</v>
+        <v>20.83271593835306</v>
       </c>
       <c r="R20" t="n">
-        <v>42904.15467992659</v>
+        <v>23235.51959706836</v>
       </c>
       <c r="S20" t="n">
         <v>0</v>
@@ -3686,10 +4040,10 @@
         <v>0</v>
       </c>
       <c r="V20" t="n">
-        <v>183.58</v>
+        <v>233.8733558923689</v>
       </c>
       <c r="W20" t="n">
-        <v>56.8</v>
+        <v>40</v>
       </c>
       <c r="X20" t="n">
         <v>0</v>
@@ -3701,13 +4055,13 @@
         <v>0</v>
       </c>
       <c r="AA20" t="n">
-        <v>183.58</v>
+        <v>233.8733558923689</v>
       </c>
       <c r="AB20" t="n">
-        <v>56.8</v>
+        <v>40</v>
       </c>
       <c r="AC20" t="n">
-        <v>39.03551289874684</v>
+        <v>-0</v>
       </c>
       <c r="AD20" t="n">
         <v>0</v>
@@ -3722,23 +4076,23 @@
         <v>0</v>
       </c>
       <c r="AH20" t="n">
-        <v>20702.00269810001</v>
+        <v>28498.1906706416</v>
       </c>
       <c r="AI20" t="n">
-        <v>-198969.7966492592</v>
+        <v>-87443.54903351111</v>
       </c>
       <c r="AJ20" t="n">
-        <v>-12.59201158446214</v>
+        <v>8.895522366703</v>
       </c>
       <c r="AK20" t="n">
-        <v>54.7323076923077</v>
+        <v>40</v>
       </c>
       <c r="AL20" t="inlineStr"/>
       <c r="AM20" t="n">
-        <v>54.36354576551444</v>
+        <v>20.83271593835306</v>
       </c>
       <c r="AN20" t="n">
-        <v>3392.285255768101</v>
+        <v>1299.961474553231</v>
       </c>
       <c r="AO20" t="n">
         <v>0</v>
@@ -3777,10 +4131,28 @@
         <v>100</v>
       </c>
       <c r="BA20" t="n">
-        <v>20.29925737948861</v>
+        <v>1.916918684164843</v>
       </c>
       <c r="BB20" t="n">
-        <v>20.45104921027798</v>
+        <v>-32979.61200600352</v>
+      </c>
+      <c r="BC20" t="n">
+        <v>19.16728406164694</v>
+      </c>
+      <c r="BD20" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE20" t="n">
+        <v>-23235.51959706836</v>
+      </c>
+      <c r="BF20" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG20" t="n">
+        <v>121.1631101942303</v>
+      </c>
+      <c r="BH20" t="n">
+        <v>184.6476505058534</v>
       </c>
     </row>
     <row r="21">
@@ -3788,55 +4160,55 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>186.54</v>
+        <v>238.0981210198501</v>
       </c>
       <c r="C21" t="n">
-        <v>0.6680897193656108</v>
+        <v>22.4201886843984</v>
       </c>
       <c r="D21" t="n">
-        <v>54.40000000000001</v>
+        <v>40</v>
       </c>
       <c r="E21" t="n">
-        <v>192.46</v>
+        <v>246.5476512748127</v>
       </c>
       <c r="F21" t="n">
-        <v>1.536055329882302</v>
+        <v>30.13632133176927</v>
       </c>
       <c r="G21" t="n">
-        <v>49.59999999999999</v>
+        <v>40</v>
       </c>
       <c r="H21" t="n">
-        <v>189.5</v>
+        <v>242.3228861473314</v>
       </c>
       <c r="I21" t="n">
-        <v>1.056834495757116</v>
+        <v>26.05658243769463</v>
       </c>
       <c r="J21" t="n">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="K21" t="n">
-        <v>26.10232366321593</v>
+        <v>33.02829121884731</v>
       </c>
       <c r="L21" t="n">
-        <v>5.920000000000016</v>
+        <v>8.449530254962525</v>
       </c>
       <c r="M21" t="n">
-        <v>-8.33727918890569</v>
+        <v>-42.31676170129219</v>
       </c>
       <c r="N21" t="n">
-        <v>5.983232868920243</v>
+        <v>11.42702154365921</v>
       </c>
       <c r="O21" t="n">
         <v>0</v>
       </c>
       <c r="P21" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="Q21" t="n">
-        <v>38.94316550424288</v>
+        <v>13.94341756230537</v>
       </c>
       <c r="R21" t="n">
-        <v>38956.54725163566</v>
+        <v>15551.62336863631</v>
       </c>
       <c r="S21" t="n">
         <v>0</v>
@@ -3848,10 +4220,10 @@
         <v>0</v>
       </c>
       <c r="V21" t="n">
-        <v>189.5</v>
+        <v>242.3228861473314</v>
       </c>
       <c r="W21" t="n">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="X21" t="n">
         <v>0</v>
@@ -3863,13 +4235,13 @@
         <v>0</v>
       </c>
       <c r="AA21" t="n">
-        <v>189.5</v>
+        <v>242.3228861473314</v>
       </c>
       <c r="AB21" t="n">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="AC21" t="n">
-        <v>39.03551289874687</v>
+        <v>-0</v>
       </c>
       <c r="AD21" t="n">
         <v>0</v>
@@ -3884,23 +4256,23 @@
         <v>0</v>
       </c>
       <c r="AH21" t="n">
-        <v>18404.70181422855</v>
+        <v>26047.20868866945</v>
       </c>
       <c r="AI21" t="n">
-        <v>-184829.3776668262</v>
+        <v>-54463.93702750759</v>
       </c>
       <c r="AJ21" t="n">
-        <v>-12.59201158446214</v>
+        <v>8.895522366703</v>
       </c>
       <c r="AK21" t="n">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="AL21" t="inlineStr"/>
       <c r="AM21" t="n">
-        <v>50.94316550424288</v>
+        <v>13.94341756230537</v>
       </c>
       <c r="AN21" t="n">
-        <v>3178.853527464756</v>
+        <v>870.0692558878551</v>
       </c>
       <c r="AO21" t="n">
         <v>0</v>
@@ -3939,10 +4311,28 @@
         <v>100</v>
       </c>
       <c r="BA21" t="n">
-        <v>20.45104921027798</v>
+        <v>2.373142190457793</v>
       </c>
       <c r="BB21" t="n">
-        <v>20.79528295231001</v>
+        <v>-31418.82957509765</v>
+      </c>
+      <c r="BC21" t="n">
+        <v>26.05658243769463</v>
+      </c>
+      <c r="BD21" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE21" t="n">
+        <v>-15551.62336863631</v>
+      </c>
+      <c r="BF21" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG21" t="n">
+        <v>184.6476505058534</v>
+      </c>
+      <c r="BH21" t="n">
+        <v>403.0887235040509</v>
       </c>
     </row>
     <row r="22">
@@ -3950,55 +4340,55 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>192.46</v>
+        <v>246.5476512748127</v>
       </c>
       <c r="C22" t="n">
-        <v>1.536055329882302</v>
+        <v>30.13632133176927</v>
       </c>
       <c r="D22" t="n">
-        <v>49.59999999999999</v>
+        <v>40</v>
       </c>
       <c r="E22" t="n">
-        <v>198.38</v>
+        <v>254.9971815297752</v>
       </c>
       <c r="F22" t="n">
-        <v>2.771528861140681</v>
+        <v>39.9962422235724</v>
       </c>
       <c r="G22" t="n">
-        <v>44.80000000000001</v>
+        <v>40</v>
       </c>
       <c r="H22" t="n">
-        <v>195.42</v>
+        <v>250.7724164022939</v>
       </c>
       <c r="I22" t="n">
-        <v>2.107080950663246</v>
+        <v>34.74250301645503</v>
       </c>
       <c r="J22" t="n">
-        <v>47.19999999999999</v>
+        <v>40</v>
       </c>
       <c r="K22" t="n">
-        <v>24.37447267967641</v>
+        <v>37.37125150822752</v>
       </c>
       <c r="L22" t="n">
-        <v>5.919999999999987</v>
+        <v>8.449530254962525</v>
       </c>
       <c r="M22" t="n">
-        <v>-11.78267182494637</v>
+        <v>-49.263973919933</v>
       </c>
       <c r="N22" t="n">
-        <v>6.047424121673585</v>
+        <v>12.94798397966922</v>
       </c>
       <c r="O22" t="n">
         <v>0</v>
       </c>
       <c r="P22" t="n">
-        <v>7.199999999999989</v>
+        <v>0</v>
       </c>
       <c r="Q22" t="n">
-        <v>37.89291904933675</v>
+        <v>5.257496983544968</v>
       </c>
       <c r="R22" t="n">
-        <v>34725.92266191363</v>
+        <v>5863.88613727454</v>
       </c>
       <c r="S22" t="n">
         <v>0</v>
@@ -4010,10 +4400,10 @@
         <v>0</v>
       </c>
       <c r="V22" t="n">
-        <v>195.42</v>
+        <v>250.7724164022939</v>
       </c>
       <c r="W22" t="n">
-        <v>47.2</v>
+        <v>40</v>
       </c>
       <c r="X22" t="n">
         <v>0</v>
@@ -4025,13 +4415,13 @@
         <v>0</v>
       </c>
       <c r="AA22" t="n">
-        <v>195.42</v>
+        <v>250.7724164022939</v>
       </c>
       <c r="AB22" t="n">
-        <v>47.2</v>
+        <v>40</v>
       </c>
       <c r="AC22" t="n">
-        <v>39.03551289874684</v>
+        <v>-0</v>
       </c>
       <c r="AD22" t="n">
         <v>0</v>
@@ -4046,23 +4436,23 @@
         <v>0</v>
       </c>
       <c r="AH22" t="n">
-        <v>16754.09093738034</v>
+        <v>19153.27415695275</v>
       </c>
       <c r="AI22" t="n">
-        <v>-169728.8879802307</v>
+        <v>-23045.10745240993</v>
       </c>
       <c r="AJ22" t="n">
-        <v>-12.59201158446214</v>
+        <v>8.895522366703</v>
       </c>
       <c r="AK22" t="n">
-        <v>47.19999999999999</v>
+        <v>40</v>
       </c>
       <c r="AL22" t="inlineStr"/>
       <c r="AM22" t="n">
-        <v>45.09291904933674</v>
+        <v>5.257496983544968</v>
       </c>
       <c r="AN22" t="n">
-        <v>2813.798148678613</v>
+        <v>328.067811773206</v>
       </c>
       <c r="AO22" t="n">
         <v>0</v>
@@ -4101,1629 +4491,27 @@
         <v>100</v>
       </c>
       <c r="BA22" t="n">
-        <v>20.79528295231001</v>
+        <v>3.288665664667144</v>
       </c>
       <c r="BB22" t="n">
-        <v>21.32983365182106</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>22</v>
-      </c>
-      <c r="B23" t="n">
-        <v>198.38</v>
-      </c>
-      <c r="C23" t="n">
-        <v>2.771528861140681</v>
-      </c>
-      <c r="D23" t="n">
-        <v>44.80000000000001</v>
-      </c>
-      <c r="E23" t="n">
-        <v>204.3</v>
-      </c>
-      <c r="F23" t="n">
-        <v>4.388755891370195</v>
-      </c>
-      <c r="G23" t="n">
-        <v>40</v>
-      </c>
-      <c r="H23" t="n">
-        <v>201.34</v>
-      </c>
-      <c r="I23" t="n">
-        <v>3.531329437998366</v>
-      </c>
-      <c r="J23" t="n">
-        <v>42.40000000000001</v>
-      </c>
-      <c r="K23" t="n">
-        <v>22.86273198634178</v>
-      </c>
-      <c r="L23" t="n">
-        <v>5.920000000000016</v>
-      </c>
-      <c r="M23" t="n">
-        <v>-15.27190219150265</v>
-      </c>
-      <c r="N23" t="n">
-        <v>6.136707353290577</v>
-      </c>
-      <c r="O23" t="n">
-        <v>0</v>
-      </c>
-      <c r="P23" t="n">
-        <v>2.400000000000006</v>
-      </c>
-      <c r="Q23" t="n">
-        <v>36.46867056200163</v>
-      </c>
-      <c r="R23" t="n">
-        <v>30203.03792397064</v>
-      </c>
-      <c r="S23" t="n">
-        <v>0</v>
-      </c>
-      <c r="T23" t="n">
-        <v>0</v>
-      </c>
-      <c r="U23" t="n">
-        <v>0</v>
-      </c>
-      <c r="V23" t="n">
-        <v>201.34</v>
-      </c>
-      <c r="W23" t="n">
-        <v>42.40000000000001</v>
-      </c>
-      <c r="X23" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y23" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA23" t="n">
-        <v>201.34</v>
-      </c>
-      <c r="AB23" t="n">
-        <v>42.40000000000001</v>
-      </c>
-      <c r="AC23" t="n">
-        <v>39.03551289874687</v>
-      </c>
-      <c r="AD23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH23" t="n">
-        <v>15002.73811382946</v>
-      </c>
-      <c r="AI23" t="n">
-        <v>-153877.9237214754</v>
-      </c>
-      <c r="AJ23" t="n">
-        <v>-12.59201158446214</v>
-      </c>
-      <c r="AK23" t="n">
-        <v>42.40000000000001</v>
-      </c>
-      <c r="AL23" t="inlineStr"/>
-      <c r="AM23" t="n">
-        <v>38.86867056200164</v>
-      </c>
-      <c r="AN23" t="n">
-        <v>2425.405043068902</v>
-      </c>
-      <c r="AO23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ23" t="n">
-        <v>3</v>
-      </c>
-      <c r="AR23" t="n">
-        <v>400</v>
-      </c>
-      <c r="AS23" t="n">
-        <v>27</v>
-      </c>
-      <c r="AT23" t="n">
-        <v>400</v>
-      </c>
-      <c r="AU23" t="n">
-        <v>27</v>
-      </c>
-      <c r="AV23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX23" t="n">
-        <v>100</v>
-      </c>
-      <c r="AY23" t="n">
-        <v>175</v>
-      </c>
-      <c r="AZ23" t="n">
-        <v>100</v>
-      </c>
-      <c r="BA23" t="n">
-        <v>21.32983365182106</v>
-      </c>
-      <c r="BB23" t="n">
-        <v>22.00257430671242</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>23</v>
-      </c>
-      <c r="B24" t="n">
-        <v>204.3</v>
-      </c>
-      <c r="C24" t="n">
-        <v>4.388755891370195</v>
-      </c>
-      <c r="D24" t="n">
-        <v>40</v>
-      </c>
-      <c r="E24" t="n">
-        <v>209.933020169975</v>
-      </c>
-      <c r="F24" t="n">
-        <v>6.300031473836029</v>
-      </c>
-      <c r="G24" t="n">
-        <v>40</v>
-      </c>
-      <c r="H24" t="n">
-        <v>207.1165100849875</v>
-      </c>
-      <c r="I24" t="n">
-        <v>5.29767806457491</v>
-      </c>
-      <c r="J24" t="n">
-        <v>40</v>
-      </c>
-      <c r="K24" t="n">
-        <v>22.64883903228746</v>
-      </c>
-      <c r="L24" t="n">
-        <v>5.633020169975026</v>
-      </c>
-      <c r="M24" t="n">
-        <v>-18.73339988139484</v>
-      </c>
-      <c r="N24" t="n">
-        <v>5.948133113162767</v>
-      </c>
-      <c r="O24" t="n">
-        <v>0</v>
-      </c>
-      <c r="P24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q24" t="n">
-        <v>34.70232193542509</v>
-      </c>
-      <c r="R24" t="n">
-        <v>25803.21208175255</v>
-      </c>
-      <c r="S24" t="n">
-        <v>0</v>
-      </c>
-      <c r="T24" t="n">
-        <v>0</v>
-      </c>
-      <c r="U24" t="n">
-        <v>0</v>
-      </c>
-      <c r="V24" t="n">
-        <v>207.1165100849875</v>
-      </c>
-      <c r="W24" t="n">
-        <v>40</v>
-      </c>
-      <c r="X24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA24" t="n">
-        <v>207.1165100849875</v>
-      </c>
-      <c r="AB24" t="n">
-        <v>40</v>
-      </c>
-      <c r="AC24" t="n">
-        <v>-0</v>
-      </c>
-      <c r="AD24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH24" t="n">
-        <v>13232.31940262001</v>
-      </c>
-      <c r="AI24" t="n">
-        <v>-137831.3814387678</v>
-      </c>
-      <c r="AJ24" t="n">
-        <v>-12.59201158446214</v>
-      </c>
-      <c r="AK24" t="n">
-        <v>40</v>
-      </c>
-      <c r="AL24" t="inlineStr"/>
-      <c r="AM24" t="n">
-        <v>34.70232193542509</v>
-      </c>
-      <c r="AN24" t="n">
-        <v>2165.424888770526</v>
-      </c>
-      <c r="AO24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ24" t="n">
-        <v>3</v>
-      </c>
-      <c r="AR24" t="n">
-        <v>400</v>
-      </c>
-      <c r="AS24" t="n">
-        <v>27</v>
-      </c>
-      <c r="AT24" t="n">
-        <v>400</v>
-      </c>
-      <c r="AU24" t="n">
-        <v>27</v>
-      </c>
-      <c r="AV24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX24" t="n">
-        <v>100</v>
-      </c>
-      <c r="AY24" t="n">
-        <v>175</v>
-      </c>
-      <c r="AZ24" t="n">
-        <v>100</v>
-      </c>
-      <c r="BA24" t="n">
-        <v>22.00257430671242</v>
-      </c>
-      <c r="BB24" t="n">
-        <v>22.80621535499205</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>24</v>
-      </c>
-      <c r="B25" t="n">
-        <v>209.933020169975</v>
-      </c>
-      <c r="C25" t="n">
-        <v>6.300031473836029</v>
-      </c>
-      <c r="D25" t="n">
-        <v>40</v>
-      </c>
-      <c r="E25" t="n">
-        <v>215.5660403399501</v>
-      </c>
-      <c r="F25" t="n">
-        <v>8.59761288052951</v>
-      </c>
-      <c r="G25" t="n">
-        <v>40</v>
-      </c>
-      <c r="H25" t="n">
-        <v>212.7495302549626</v>
-      </c>
-      <c r="I25" t="n">
-        <v>7.398850085273423</v>
-      </c>
-      <c r="J25" t="n">
-        <v>40</v>
-      </c>
-      <c r="K25" t="n">
-        <v>23.69942504263671</v>
-      </c>
-      <c r="L25" t="n">
-        <v>5.633020169975026</v>
-      </c>
-      <c r="M25" t="n">
-        <v>-22.17862197551927</v>
-      </c>
-      <c r="N25" t="n">
-        <v>6.083099589111251</v>
-      </c>
-      <c r="O25" t="n">
-        <v>0</v>
-      </c>
-      <c r="P25" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q25" t="n">
-        <v>32.60114991472658</v>
-      </c>
-      <c r="R25" t="n">
-        <v>24240.86742449254</v>
-      </c>
-      <c r="S25" t="n">
-        <v>0</v>
-      </c>
-      <c r="T25" t="n">
-        <v>0</v>
-      </c>
-      <c r="U25" t="n">
-        <v>0</v>
-      </c>
-      <c r="V25" t="n">
-        <v>212.7495302549626</v>
-      </c>
-      <c r="W25" t="n">
-        <v>40</v>
-      </c>
-      <c r="X25" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y25" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA25" t="n">
-        <v>212.7495302549626</v>
-      </c>
-      <c r="AB25" t="n">
-        <v>40</v>
-      </c>
-      <c r="AC25" t="n">
-        <v>-0</v>
-      </c>
-      <c r="AD25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH25" t="n">
-        <v>12829.10108922903</v>
-      </c>
-      <c r="AI25" t="n">
-        <v>-122162.3065673442</v>
-      </c>
-      <c r="AJ25" t="n">
-        <v>-12.59201158446214</v>
-      </c>
-      <c r="AK25" t="n">
-        <v>40</v>
-      </c>
-      <c r="AL25" t="inlineStr"/>
-      <c r="AM25" t="n">
-        <v>32.60114991472658</v>
-      </c>
-      <c r="AN25" t="n">
-        <v>2034.311754678938</v>
-      </c>
-      <c r="AO25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ25" t="n">
-        <v>3</v>
-      </c>
-      <c r="AR25" t="n">
-        <v>400</v>
-      </c>
-      <c r="AS25" t="n">
-        <v>27</v>
-      </c>
-      <c r="AT25" t="n">
-        <v>400</v>
-      </c>
-      <c r="AU25" t="n">
-        <v>27</v>
-      </c>
-      <c r="AV25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX25" t="n">
-        <v>100</v>
-      </c>
-      <c r="AY25" t="n">
-        <v>175</v>
-      </c>
-      <c r="AZ25" t="n">
-        <v>100</v>
-      </c>
-      <c r="BA25" t="n">
-        <v>22.80621535499205</v>
-      </c>
-      <c r="BB25" t="n">
-        <v>23.86421100248573</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>25</v>
-      </c>
-      <c r="B26" t="n">
-        <v>215.5660403399501</v>
-      </c>
-      <c r="C26" t="n">
-        <v>8.59761288052951</v>
-      </c>
-      <c r="D26" t="n">
-        <v>40</v>
-      </c>
-      <c r="E26" t="n">
-        <v>221.1990605099251</v>
-      </c>
-      <c r="F26" t="n">
-        <v>11.31151817738515</v>
-      </c>
-      <c r="G26" t="n">
-        <v>40</v>
-      </c>
-      <c r="H26" t="n">
-        <v>218.3825504249376</v>
-      </c>
-      <c r="I26" t="n">
-        <v>9.900308998156106</v>
-      </c>
-      <c r="J26" t="n">
-        <v>40</v>
-      </c>
-      <c r="K26" t="n">
-        <v>24.95015449907805</v>
-      </c>
-      <c r="L26" t="n">
-        <v>5.633020169974998</v>
-      </c>
-      <c r="M26" t="n">
-        <v>-25.71058241180675</v>
-      </c>
-      <c r="N26" t="n">
-        <v>6.251986113758945</v>
-      </c>
-      <c r="O26" t="n">
-        <v>0</v>
-      </c>
-      <c r="P26" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q26" t="n">
-        <v>30.09969100184389</v>
-      </c>
-      <c r="R26" t="n">
-        <v>22380.88598108901</v>
-      </c>
-      <c r="S26" t="n">
-        <v>0</v>
-      </c>
-      <c r="T26" t="n">
-        <v>0</v>
-      </c>
-      <c r="U26" t="n">
-        <v>0</v>
-      </c>
-      <c r="V26" t="n">
-        <v>218.3825504249376</v>
-      </c>
-      <c r="W26" t="n">
-        <v>40</v>
-      </c>
-      <c r="X26" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y26" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA26" t="n">
-        <v>218.3825504249376</v>
-      </c>
-      <c r="AB26" t="n">
-        <v>40</v>
-      </c>
-      <c r="AC26" t="n">
-        <v>-0</v>
-      </c>
-      <c r="AD26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH26" t="n">
-        <v>12320.78466993414</v>
-      </c>
-      <c r="AI26" t="n">
-        <v>-105609.3590517556</v>
-      </c>
-      <c r="AJ26" t="n">
-        <v>-12.59201158446214</v>
-      </c>
-      <c r="AK26" t="n">
-        <v>40</v>
-      </c>
-      <c r="AL26" t="inlineStr"/>
-      <c r="AM26" t="n">
-        <v>30.09969100184389</v>
-      </c>
-      <c r="AN26" t="n">
-        <v>1878.220718515059</v>
-      </c>
-      <c r="AO26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ26" t="n">
-        <v>3</v>
-      </c>
-      <c r="AR26" t="n">
-        <v>400</v>
-      </c>
-      <c r="AS26" t="n">
-        <v>27</v>
-      </c>
-      <c r="AT26" t="n">
-        <v>400</v>
-      </c>
-      <c r="AU26" t="n">
-        <v>27</v>
-      </c>
-      <c r="AV26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX26" t="n">
-        <v>100</v>
-      </c>
-      <c r="AY26" t="n">
-        <v>175</v>
-      </c>
-      <c r="AZ26" t="n">
-        <v>100</v>
-      </c>
-      <c r="BA26" t="n">
-        <v>23.86421100248573</v>
-      </c>
-      <c r="BB26" t="n">
-        <v>25.19577389045321</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>26</v>
-      </c>
-      <c r="B27" t="n">
-        <v>221.1990605099251</v>
-      </c>
-      <c r="C27" t="n">
-        <v>11.31151817738515</v>
-      </c>
-      <c r="D27" t="n">
-        <v>40</v>
-      </c>
-      <c r="E27" t="n">
-        <v>226.8320806799001</v>
-      </c>
-      <c r="F27" t="n">
-        <v>14.48137388619759</v>
-      </c>
-      <c r="G27" t="n">
-        <v>40</v>
-      </c>
-      <c r="H27" t="n">
-        <v>224.0155705949126</v>
-      </c>
-      <c r="I27" t="n">
-        <v>12.83651085887428</v>
-      </c>
-      <c r="J27" t="n">
-        <v>40</v>
-      </c>
-      <c r="K27" t="n">
-        <v>26.41825542943714</v>
-      </c>
-      <c r="L27" t="n">
-        <v>5.633020169975026</v>
-      </c>
-      <c r="M27" t="n">
-        <v>-29.35081618795352</v>
-      </c>
-      <c r="N27" t="n">
-        <v>6.462591419274929</v>
-      </c>
-      <c r="O27" t="n">
-        <v>0</v>
-      </c>
-      <c r="P27" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q27" t="n">
-        <v>27.16348914112572</v>
-      </c>
-      <c r="R27" t="n">
-        <v>20197.64765288936</v>
-      </c>
-      <c r="S27" t="n">
-        <v>0</v>
-      </c>
-      <c r="T27" t="n">
-        <v>0</v>
-      </c>
-      <c r="U27" t="n">
-        <v>0</v>
-      </c>
-      <c r="V27" t="n">
-        <v>224.0155705949126</v>
-      </c>
-      <c r="W27" t="n">
-        <v>40</v>
-      </c>
-      <c r="X27" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y27" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA27" t="n">
-        <v>224.0155705949126</v>
-      </c>
-      <c r="AB27" t="n">
-        <v>40</v>
-      </c>
-      <c r="AC27" t="n">
-        <v>-0</v>
-      </c>
-      <c r="AD27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH27" t="n">
-        <v>11688.09364112812</v>
-      </c>
-      <c r="AI27" t="n">
-        <v>-88433.79737836694</v>
-      </c>
-      <c r="AJ27" t="n">
-        <v>-12.59201158446214</v>
-      </c>
-      <c r="AK27" t="n">
-        <v>40</v>
-      </c>
-      <c r="AL27" t="inlineStr"/>
-      <c r="AM27" t="n">
-        <v>27.16348914112572</v>
-      </c>
-      <c r="AN27" t="n">
-        <v>1695.001722406245</v>
-      </c>
-      <c r="AO27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ27" t="n">
-        <v>3</v>
-      </c>
-      <c r="AR27" t="n">
-        <v>400</v>
-      </c>
-      <c r="AS27" t="n">
-        <v>27</v>
-      </c>
-      <c r="AT27" t="n">
-        <v>400</v>
-      </c>
-      <c r="AU27" t="n">
-        <v>27</v>
-      </c>
-      <c r="AV27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX27" t="n">
-        <v>100</v>
-      </c>
-      <c r="AY27" t="n">
-        <v>175</v>
-      </c>
-      <c r="AZ27" t="n">
-        <v>100</v>
-      </c>
-      <c r="BA27" t="n">
-        <v>25.19577389045321</v>
-      </c>
-      <c r="BB27" t="n">
-        <v>26.82511222770668</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>27</v>
-      </c>
-      <c r="B28" t="n">
-        <v>226.8320806799001</v>
-      </c>
-      <c r="C28" t="n">
-        <v>14.48137388619759</v>
-      </c>
-      <c r="D28" t="n">
-        <v>40</v>
-      </c>
-      <c r="E28" t="n">
-        <v>232.4651008498751</v>
-      </c>
-      <c r="F28" t="n">
-        <v>18.16014305783715</v>
-      </c>
-      <c r="G28" t="n">
-        <v>40</v>
-      </c>
-      <c r="H28" t="n">
-        <v>229.6485907648876</v>
-      </c>
-      <c r="I28" t="n">
-        <v>16.25317004559611</v>
-      </c>
-      <c r="J28" t="n">
-        <v>40</v>
-      </c>
-      <c r="K28" t="n">
-        <v>28.12658502279805</v>
-      </c>
-      <c r="L28" t="n">
-        <v>5.633020169975026</v>
-      </c>
-      <c r="M28" t="n">
-        <v>-33.12626395872771</v>
-      </c>
-      <c r="N28" t="n">
-        <v>6.726248830005786</v>
-      </c>
-      <c r="O28" t="n">
-        <v>0</v>
-      </c>
-      <c r="P28" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q28" t="n">
-        <v>23.74682995440389</v>
-      </c>
-      <c r="R28" t="n">
-        <v>17657.1611180084</v>
-      </c>
-      <c r="S28" t="n">
-        <v>0</v>
-      </c>
-      <c r="T28" t="n">
-        <v>0</v>
-      </c>
-      <c r="U28" t="n">
-        <v>0</v>
-      </c>
-      <c r="V28" t="n">
-        <v>229.6485907648876</v>
-      </c>
-      <c r="W28" t="n">
-        <v>40</v>
-      </c>
-      <c r="X28" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y28" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA28" t="n">
-        <v>229.6485907648876</v>
-      </c>
-      <c r="AB28" t="n">
-        <v>40</v>
-      </c>
-      <c r="AC28" t="n">
-        <v>-0</v>
-      </c>
-      <c r="AD28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH28" t="n">
-        <v>10903.99530870849</v>
-      </c>
-      <c r="AI28" t="n">
-        <v>-70964.27123867802</v>
-      </c>
-      <c r="AJ28" t="n">
-        <v>-12.59201158446214</v>
-      </c>
-      <c r="AK28" t="n">
-        <v>40</v>
-      </c>
-      <c r="AL28" t="inlineStr"/>
-      <c r="AM28" t="n">
-        <v>23.74682995440389</v>
-      </c>
-      <c r="AN28" t="n">
-        <v>1481.802189154803</v>
-      </c>
-      <c r="AO28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ28" t="n">
-        <v>3</v>
-      </c>
-      <c r="AR28" t="n">
-        <v>400</v>
-      </c>
-      <c r="AS28" t="n">
-        <v>27</v>
-      </c>
-      <c r="AT28" t="n">
-        <v>400</v>
-      </c>
-      <c r="AU28" t="n">
-        <v>27</v>
-      </c>
-      <c r="AV28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX28" t="n">
-        <v>100</v>
-      </c>
-      <c r="AY28" t="n">
-        <v>175</v>
-      </c>
-      <c r="AZ28" t="n">
-        <v>100</v>
-      </c>
-      <c r="BA28" t="n">
-        <v>26.82511222770668</v>
-      </c>
-      <c r="BB28" t="n">
-        <v>28.78286171498854</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>28</v>
-      </c>
-      <c r="B29" t="n">
-        <v>232.4651008498751</v>
-      </c>
-      <c r="C29" t="n">
-        <v>18.16014305783715</v>
-      </c>
-      <c r="D29" t="n">
-        <v>40</v>
-      </c>
-      <c r="E29" t="n">
-        <v>238.0981210198501</v>
-      </c>
-      <c r="F29" t="n">
-        <v>22.4201886843984</v>
-      </c>
-      <c r="G29" t="n">
-        <v>40</v>
-      </c>
-      <c r="H29" t="n">
-        <v>235.2816109348626</v>
-      </c>
-      <c r="I29" t="n">
-        <v>20.21198471513499</v>
-      </c>
-      <c r="J29" t="n">
-        <v>40</v>
-      </c>
-      <c r="K29" t="n">
-        <v>30.10599235756749</v>
-      </c>
-      <c r="L29" t="n">
-        <v>5.633020169975026</v>
-      </c>
-      <c r="M29" t="n">
-        <v>-37.07185398528599</v>
-      </c>
-      <c r="N29" t="n">
-        <v>7.059982818050563</v>
-      </c>
-      <c r="O29" t="n">
-        <v>0</v>
-      </c>
-      <c r="P29" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q29" t="n">
-        <v>19.78801528486501</v>
-      </c>
-      <c r="R29" t="n">
-        <v>14713.55017749127</v>
-      </c>
-      <c r="S29" t="n">
-        <v>0</v>
-      </c>
-      <c r="T29" t="n">
-        <v>0</v>
-      </c>
-      <c r="U29" t="n">
-        <v>0</v>
-      </c>
-      <c r="V29" t="n">
-        <v>235.2816109348626</v>
-      </c>
-      <c r="W29" t="n">
-        <v>40</v>
-      </c>
-      <c r="X29" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y29" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA29" t="n">
-        <v>235.2816109348626</v>
-      </c>
-      <c r="AB29" t="n">
-        <v>40</v>
-      </c>
-      <c r="AC29" t="n">
-        <v>-0</v>
-      </c>
-      <c r="AD29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH29" t="n">
-        <v>9930.024339107735</v>
-      </c>
-      <c r="AI29" t="n">
-        <v>-53620.42746064258</v>
-      </c>
-      <c r="AJ29" t="n">
-        <v>-12.59201158446214</v>
-      </c>
-      <c r="AK29" t="n">
-        <v>40</v>
-      </c>
-      <c r="AL29" t="inlineStr"/>
-      <c r="AM29" t="n">
-        <v>19.78801528486501</v>
-      </c>
-      <c r="AN29" t="n">
-        <v>1234.772153775577</v>
-      </c>
-      <c r="AO29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ29" t="n">
-        <v>3</v>
-      </c>
-      <c r="AR29" t="n">
-        <v>400</v>
-      </c>
-      <c r="AS29" t="n">
-        <v>27</v>
-      </c>
-      <c r="AT29" t="n">
-        <v>400</v>
-      </c>
-      <c r="AU29" t="n">
-        <v>27</v>
-      </c>
-      <c r="AV29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX29" t="n">
-        <v>100</v>
-      </c>
-      <c r="AY29" t="n">
-        <v>175</v>
-      </c>
-      <c r="AZ29" t="n">
-        <v>100</v>
-      </c>
-      <c r="BA29" t="n">
-        <v>28.78286171498854</v>
-      </c>
-      <c r="BB29" t="n">
-        <v>31.10761129392932</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>29</v>
-      </c>
-      <c r="B30" t="n">
-        <v>238.0981210198501</v>
-      </c>
-      <c r="C30" t="n">
-        <v>22.4201886843984</v>
-      </c>
-      <c r="D30" t="n">
-        <v>40</v>
-      </c>
-      <c r="E30" t="n">
-        <v>243.7311411898252</v>
-      </c>
-      <c r="F30" t="n">
-        <v>27.36371271365587</v>
-      </c>
-      <c r="G30" t="n">
-        <v>40</v>
-      </c>
-      <c r="H30" t="n">
-        <v>240.9146311048377</v>
-      </c>
-      <c r="I30" t="n">
-        <v>24.79852789796487</v>
-      </c>
-      <c r="J30" t="n">
-        <v>40</v>
-      </c>
-      <c r="K30" t="n">
-        <v>32.39926394898244</v>
-      </c>
-      <c r="L30" t="n">
-        <v>5.633020169975026</v>
-      </c>
-      <c r="M30" t="n">
-        <v>-41.23479807737511</v>
-      </c>
-      <c r="N30" t="n">
-        <v>7.490571677017189</v>
-      </c>
-      <c r="O30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P30" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q30" t="n">
-        <v>15.20147210203513</v>
-      </c>
-      <c r="R30" t="n">
-        <v>11303.1862632581</v>
-      </c>
-      <c r="S30" t="n">
-        <v>0</v>
-      </c>
-      <c r="T30" t="n">
-        <v>0</v>
-      </c>
-      <c r="U30" t="n">
-        <v>0</v>
-      </c>
-      <c r="V30" t="n">
-        <v>240.9146311048377</v>
-      </c>
-      <c r="W30" t="n">
-        <v>40</v>
-      </c>
-      <c r="X30" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y30" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA30" t="n">
-        <v>240.9146311048377</v>
-      </c>
-      <c r="AB30" t="n">
-        <v>40</v>
-      </c>
-      <c r="AC30" t="n">
-        <v>-0</v>
-      </c>
-      <c r="AD30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH30" t="n">
-        <v>8710.32241126048</v>
-      </c>
-      <c r="AI30" t="n">
-        <v>-36949.83461256242</v>
-      </c>
-      <c r="AJ30" t="n">
-        <v>-12.59201158446214</v>
-      </c>
-      <c r="AK30" t="n">
-        <v>40</v>
-      </c>
-      <c r="AL30" t="inlineStr"/>
-      <c r="AM30" t="n">
-        <v>15.20147210203513</v>
-      </c>
-      <c r="AN30" t="n">
-        <v>948.5718591669919</v>
-      </c>
-      <c r="AO30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ30" t="n">
-        <v>3</v>
-      </c>
-      <c r="AR30" t="n">
-        <v>400</v>
-      </c>
-      <c r="AS30" t="n">
-        <v>27</v>
-      </c>
-      <c r="AT30" t="n">
-        <v>400</v>
-      </c>
-      <c r="AU30" t="n">
-        <v>27</v>
-      </c>
-      <c r="AV30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX30" t="n">
-        <v>100</v>
-      </c>
-      <c r="AY30" t="n">
-        <v>175</v>
-      </c>
-      <c r="AZ30" t="n">
-        <v>100</v>
-      </c>
-      <c r="BA30" t="n">
-        <v>31.10761129392932</v>
-      </c>
-      <c r="BB30" t="n">
-        <v>33.84607134908812</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>30</v>
-      </c>
-      <c r="B31" t="n">
-        <v>243.7311411898252</v>
-      </c>
-      <c r="C31" t="n">
-        <v>27.36371271365587</v>
-      </c>
-      <c r="D31" t="n">
-        <v>40</v>
-      </c>
-      <c r="E31" t="n">
-        <v>249.3641613598002</v>
-      </c>
-      <c r="F31" t="n">
-        <v>33.14215449736955</v>
-      </c>
-      <c r="G31" t="n">
-        <v>40</v>
-      </c>
-      <c r="H31" t="n">
-        <v>246.5476512748127</v>
-      </c>
-      <c r="I31" t="n">
-        <v>30.13632133176927</v>
-      </c>
-      <c r="J31" t="n">
-        <v>40</v>
-      </c>
-      <c r="K31" t="n">
-        <v>35.06816066588463</v>
-      </c>
-      <c r="L31" t="n">
-        <v>5.633020169974998</v>
-      </c>
-      <c r="M31" t="n">
-        <v>-45.68226472964457</v>
-      </c>
-      <c r="N31" t="n">
-        <v>8.062873695393474</v>
-      </c>
-      <c r="O31" t="n">
-        <v>0</v>
-      </c>
-      <c r="P31" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q31" t="n">
-        <v>9.863678668230733</v>
-      </c>
-      <c r="R31" t="n">
-        <v>7334.22371725505</v>
-      </c>
-      <c r="S31" t="n">
-        <v>0</v>
-      </c>
-      <c r="T31" t="n">
-        <v>0</v>
-      </c>
-      <c r="U31" t="n">
-        <v>0</v>
-      </c>
-      <c r="V31" t="n">
-        <v>246.5476512748127</v>
-      </c>
-      <c r="W31" t="n">
-        <v>40</v>
-      </c>
-      <c r="X31" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y31" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA31" t="n">
-        <v>246.5476512748127</v>
-      </c>
-      <c r="AB31" t="n">
-        <v>40</v>
-      </c>
-      <c r="AC31" t="n">
-        <v>-0</v>
-      </c>
-      <c r="AD31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH31" t="n">
-        <v>7162.074069035806</v>
-      </c>
-      <c r="AI31" t="n">
-        <v>-21688.44822887022</v>
-      </c>
-      <c r="AJ31" t="n">
-        <v>-12.59201158446214</v>
-      </c>
-      <c r="AK31" t="n">
-        <v>40</v>
-      </c>
-      <c r="AL31" t="inlineStr"/>
-      <c r="AM31" t="n">
-        <v>9.863678668230733</v>
-      </c>
-      <c r="AN31" t="n">
-        <v>615.4935488975977</v>
-      </c>
-      <c r="AO31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ31" t="n">
-        <v>3</v>
-      </c>
-      <c r="AR31" t="n">
-        <v>400</v>
-      </c>
-      <c r="AS31" t="n">
-        <v>27</v>
-      </c>
-      <c r="AT31" t="n">
-        <v>400</v>
-      </c>
-      <c r="AU31" t="n">
-        <v>27</v>
-      </c>
-      <c r="AV31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX31" t="n">
-        <v>100</v>
-      </c>
-      <c r="AY31" t="n">
-        <v>175</v>
-      </c>
-      <c r="AZ31" t="n">
-        <v>100</v>
-      </c>
-      <c r="BA31" t="n">
-        <v>33.84607134908812</v>
-      </c>
-      <c r="BB31" t="n">
-        <v>37.04343097984174</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>31</v>
-      </c>
-      <c r="B32" t="n">
-        <v>249.3641613598002</v>
-      </c>
-      <c r="C32" t="n">
-        <v>33.14215449736955</v>
-      </c>
-      <c r="D32" t="n">
-        <v>40</v>
-      </c>
-      <c r="E32" t="n">
-        <v>254.9971815297752</v>
-      </c>
-      <c r="F32" t="n">
-        <v>39.9962422235724</v>
-      </c>
-      <c r="G32" t="n">
-        <v>40</v>
-      </c>
-      <c r="H32" t="n">
-        <v>252.1806714447877</v>
-      </c>
-      <c r="I32" t="n">
-        <v>36.41427868356184</v>
-      </c>
-      <c r="J32" t="n">
-        <v>40</v>
-      </c>
-      <c r="K32" t="n">
-        <v>38.20713934178092</v>
-      </c>
-      <c r="L32" t="n">
-        <v>5.633020169975026</v>
-      </c>
-      <c r="M32" t="n">
-        <v>-50.51640860175686</v>
-      </c>
-      <c r="N32" t="n">
-        <v>8.858938851919227</v>
-      </c>
-      <c r="O32" t="n">
-        <v>0</v>
-      </c>
-      <c r="P32" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q32" t="n">
-        <v>3.58572131643816</v>
-      </c>
-      <c r="R32" t="n">
-        <v>2666.194145921534</v>
-      </c>
-      <c r="S32" t="n">
-        <v>0</v>
-      </c>
-      <c r="T32" t="n">
-        <v>0</v>
-      </c>
-      <c r="U32" t="n">
-        <v>0</v>
-      </c>
-      <c r="V32" t="n">
-        <v>252.1806714447877</v>
-      </c>
-      <c r="W32" t="n">
-        <v>40</v>
-      </c>
-      <c r="X32" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y32" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA32" t="n">
-        <v>252.1806714447877</v>
-      </c>
-      <c r="AB32" t="n">
-        <v>40</v>
-      </c>
-      <c r="AC32" t="n">
-        <v>-0</v>
-      </c>
-      <c r="AD32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH32" t="n">
-        <v>5162.117053507664</v>
-      </c>
-      <c r="AI32" t="n">
-        <v>-8865.586769683929</v>
-      </c>
-      <c r="AJ32" t="n">
-        <v>-12.59201158446214</v>
-      </c>
-      <c r="AK32" t="n">
-        <v>40</v>
-      </c>
-      <c r="AL32" t="inlineStr"/>
-      <c r="AM32" t="n">
-        <v>3.58572131643816</v>
-      </c>
-      <c r="AN32" t="n">
-        <v>223.7490101457412</v>
-      </c>
-      <c r="AO32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ32" t="n">
-        <v>3</v>
-      </c>
-      <c r="AR32" t="n">
-        <v>400</v>
-      </c>
-      <c r="AS32" t="n">
-        <v>27</v>
-      </c>
-      <c r="AT32" t="n">
-        <v>400</v>
-      </c>
-      <c r="AU32" t="n">
-        <v>27</v>
-      </c>
-      <c r="AV32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX32" t="n">
-        <v>100</v>
-      </c>
-      <c r="AY32" t="n">
-        <v>175</v>
-      </c>
-      <c r="AZ32" t="n">
-        <v>100</v>
-      </c>
-      <c r="BA32" t="n">
-        <v>37.04343097984174</v>
-      </c>
-      <c r="BB32" t="n">
+        <v>-23041.79589910862</v>
+      </c>
+      <c r="BC22" t="n">
+        <v>34.74250301645503</v>
+      </c>
+      <c r="BD22" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE22" t="n">
+        <v>-5863.88613727454</v>
+      </c>
+      <c r="BF22" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG22" t="n">
+        <v>403.0887235040509</v>
+      </c>
+      <c r="BH22" t="n">
         <v>39.9962422235724</v>
       </c>
     </row>

</xml_diff>

<commit_message>
continuing debugging of spencer for right-facing slopes. no solution yet.
</commit_message>
<xml_diff>
--- a/slices.xlsx
+++ b/slices.xlsx
@@ -836,13 +836,13 @@
         <v>0</v>
       </c>
       <c r="AH2" t="n">
-        <v>-263.4870953536603</v>
+        <v>-1238.89293509685</v>
       </c>
       <c r="AI2" t="n">
         <v>0</v>
       </c>
       <c r="AJ2" t="n">
-        <v>8.895522366703</v>
+        <v>-12.52138795235413</v>
       </c>
       <c r="AK2" t="n">
         <v>78.855630874209</v>
@@ -891,10 +891,10 @@
         <v>100</v>
       </c>
       <c r="BA2" t="n">
-        <v>1.678125644678302</v>
+        <v>2.525643448558156</v>
       </c>
       <c r="BB2" t="n">
-        <v>-351.0899306809409</v>
+        <v>-1306.467707567553</v>
       </c>
       <c r="BC2" t="n">
         <v>81.21329877556784</v>
@@ -912,7 +912,7 @@
         <v>84.00000000000006</v>
       </c>
       <c r="BH2" t="n">
-        <v>81.29034428031295</v>
+        <v>81.10397589356462</v>
       </c>
     </row>
     <row r="3">
@@ -1016,13 +1016,13 @@
         <v>0</v>
       </c>
       <c r="AH3" t="n">
-        <v>4332.228964849945</v>
+        <v>9178.426058408142</v>
       </c>
       <c r="AI3" t="n">
-        <v>351.0899306809409</v>
+        <v>1306.467707567553</v>
       </c>
       <c r="AJ3" t="n">
-        <v>8.895522366703</v>
+        <v>-12.52138795235413</v>
       </c>
       <c r="AK3" t="n">
         <v>78.63592483281701</v>
@@ -1071,10 +1071,10 @@
         <v>100</v>
       </c>
       <c r="BA3" t="n">
-        <v>1.455854622958788</v>
+        <v>1.97470111438668</v>
       </c>
       <c r="BB3" t="n">
-        <v>10830.68295521836</v>
+        <v>14619.35178207635</v>
       </c>
       <c r="BC3" t="n">
         <v>70.37079750256237</v>
@@ -1089,10 +1089,10 @@
         <v>0</v>
       </c>
       <c r="BG3" t="n">
-        <v>81.29034428031295</v>
+        <v>81.10397589356462</v>
       </c>
       <c r="BH3" t="n">
-        <v>70.34040709215394</v>
+        <v>68.87335299518907</v>
       </c>
     </row>
     <row r="4">
@@ -1196,13 +1196,13 @@
         <v>0</v>
       </c>
       <c r="AH4" t="n">
-        <v>29608.86634539621</v>
+        <v>50902.93712701974</v>
       </c>
       <c r="AI4" t="n">
-        <v>-10479.59302453742</v>
+        <v>-13312.8840745088</v>
       </c>
       <c r="AJ4" t="n">
-        <v>8.895522366703</v>
+        <v>-12.52138795235413</v>
       </c>
       <c r="AK4" t="n">
         <v>77.91714056524853</v>
@@ -1251,10 +1251,10 @@
         <v>100</v>
       </c>
       <c r="BA4" t="n">
-        <v>1.138292633052306</v>
+        <v>1.287292231038373</v>
       </c>
       <c r="BB4" t="n">
-        <v>61020.96489264639</v>
+        <v>72130.61487837438</v>
       </c>
       <c r="BC4" t="n">
         <v>50.07315218453382</v>
@@ -1269,10 +1269,10 @@
         <v>0</v>
       </c>
       <c r="BG4" t="n">
-        <v>70.34040709215394</v>
+        <v>68.87335299518907</v>
       </c>
       <c r="BH4" t="n">
-        <v>54.23659600662612</v>
+        <v>51.29604027399181</v>
       </c>
     </row>
     <row r="5">
@@ -1376,13 +1376,13 @@
         <v>0</v>
       </c>
       <c r="AH5" t="n">
-        <v>27922.23588484879</v>
+        <v>40737.30859266572</v>
       </c>
       <c r="AI5" t="n">
-        <v>-71500.5579171838</v>
+        <v>-85443.49895288318</v>
       </c>
       <c r="AJ5" t="n">
-        <v>8.895522366703</v>
+        <v>-12.52138795235413</v>
       </c>
       <c r="AK5" t="n">
         <v>77.00654727586166</v>
@@ -1431,10 +1431,10 @@
         <v>100</v>
       </c>
       <c r="BA5" t="n">
-        <v>1.069840496192237</v>
+        <v>1.19620909154821</v>
       </c>
       <c r="BB5" t="n">
-        <v>42888.23194393673</v>
+        <v>45999.73653439412</v>
       </c>
       <c r="BC5" t="n">
         <v>34.32872717186068</v>
@@ -1449,10 +1449,10 @@
         <v>0</v>
       </c>
       <c r="BG5" t="n">
-        <v>54.23659600662612</v>
+        <v>51.29604027399181</v>
       </c>
       <c r="BH5" t="n">
-        <v>47.93816565962794</v>
+        <v>43.67869361320182</v>
       </c>
     </row>
     <row r="6">
@@ -1556,13 +1556,13 @@
         <v>0</v>
       </c>
       <c r="AH6" t="n">
-        <v>33698.74511679153</v>
+        <v>44147.78855750636</v>
       </c>
       <c r="AI6" t="n">
-        <v>-114388.7898611205</v>
+        <v>-131443.2354872773</v>
       </c>
       <c r="AJ6" t="n">
-        <v>8.895522366703</v>
+        <v>-12.52138795235413</v>
       </c>
       <c r="AK6" t="n">
         <v>76.26334212005389</v>
@@ -1611,10 +1611,10 @@
         <v>100</v>
       </c>
       <c r="BA6" t="n">
-        <v>1.016032064889689</v>
+        <v>1.08969729518768</v>
       </c>
       <c r="BB6" t="n">
-        <v>40158.86560829845</v>
+        <v>39649.88084506032</v>
       </c>
       <c r="BC6" t="n">
         <v>25.09193914530816</v>
@@ -1629,10 +1629,10 @@
         <v>0</v>
       </c>
       <c r="BG6" t="n">
-        <v>47.93816565962794</v>
+        <v>43.67869361320182</v>
       </c>
       <c r="BH6" t="n">
-        <v>43.24988273506372</v>
+        <v>37.57150888578319</v>
       </c>
     </row>
     <row r="7">
@@ -1736,13 +1736,13 @@
         <v>0</v>
       </c>
       <c r="AH7" t="n">
-        <v>38871.17335038891</v>
+        <v>46724.66041240805</v>
       </c>
       <c r="AI7" t="n">
-        <v>-154547.655469419</v>
+        <v>-171093.1163323376</v>
       </c>
       <c r="AJ7" t="n">
-        <v>8.895522366703</v>
+        <v>-12.52138795235413</v>
       </c>
       <c r="AK7" t="n">
         <v>74.73179054836476</v>
@@ -1791,10 +1791,10 @@
         <v>100</v>
       </c>
       <c r="BA7" t="n">
-        <v>0.9857795027894882</v>
+        <v>1.022798475221807</v>
       </c>
       <c r="BB7" t="n">
-        <v>34920.67772916342</v>
+        <v>31435.85858423841</v>
       </c>
       <c r="BC7" t="n">
         <v>17.8922612956589</v>
@@ -1809,10 +1809,10 @@
         <v>0</v>
       </c>
       <c r="BG7" t="n">
-        <v>43.24988273506372</v>
+        <v>37.57150888578319</v>
       </c>
       <c r="BH7" t="n">
-        <v>39.87869496594512</v>
+        <v>32.63926217169369</v>
       </c>
     </row>
     <row r="8">
@@ -1916,13 +1916,13 @@
         <v>0</v>
       </c>
       <c r="AH8" t="n">
-        <v>43650.1036060939</v>
+        <v>48888.13030562105</v>
       </c>
       <c r="AI8" t="n">
-        <v>-189468.3331985824</v>
+        <v>-202528.974916576</v>
       </c>
       <c r="AJ8" t="n">
-        <v>8.895522366703</v>
+        <v>-12.52138795235413</v>
       </c>
       <c r="AK8" t="n">
         <v>72.76760549372993</v>
@@ -1971,10 +1971,10 @@
         <v>100</v>
       </c>
       <c r="BA8" t="n">
-        <v>0.9707839877130248</v>
+        <v>0.9790507117737064</v>
       </c>
       <c r="BB8" t="n">
-        <v>28185.44380533544</v>
+        <v>22422.59851412284</v>
       </c>
       <c r="BC8" t="n">
         <v>12.22696543209685</v>
@@ -1989,10 +1989,10 @@
         <v>0</v>
       </c>
       <c r="BG8" t="n">
-        <v>39.87869496594512</v>
+        <v>32.63926217169369</v>
       </c>
       <c r="BH8" t="n">
-        <v>37.63965025753598</v>
+        <v>28.67038553945456</v>
       </c>
     </row>
     <row r="9">
@@ -2096,13 +2096,13 @@
         <v>0</v>
       </c>
       <c r="AH9" t="n">
-        <v>48042.79535698028</v>
+        <v>50700.3740035157</v>
       </c>
       <c r="AI9" t="n">
-        <v>-217653.7770039178</v>
+        <v>-224951.5734306988</v>
       </c>
       <c r="AJ9" t="n">
-        <v>8.895522366703</v>
+        <v>-12.52138795235413</v>
       </c>
       <c r="AK9" t="n">
         <v>70.80342043909509</v>
@@ -2151,10 +2151,10 @@
         <v>100</v>
       </c>
       <c r="BA9" t="n">
-        <v>0.9671987351467956</v>
+        <v>0.9507818989724603</v>
       </c>
       <c r="BB9" t="n">
-        <v>20462.32272574432</v>
+        <v>13101.04485691148</v>
       </c>
       <c r="BC9" t="n">
         <v>7.812733485778423</v>
@@ -2169,10 +2169,10 @@
         <v>0</v>
       </c>
       <c r="BG9" t="n">
-        <v>37.63965025753598</v>
+        <v>28.67038553945456</v>
       </c>
       <c r="BH9" t="n">
-        <v>36.44950854230976</v>
+        <v>25.5428297092451</v>
       </c>
     </row>
     <row r="10">
@@ -2276,13 +2276,13 @@
         <v>0</v>
       </c>
       <c r="AH10" t="n">
-        <v>52500.90525190541</v>
+        <v>52534.46950646966</v>
       </c>
       <c r="AI10" t="n">
-        <v>-238116.0997296621</v>
+        <v>-238052.6182876103</v>
       </c>
       <c r="AJ10" t="n">
-        <v>8.895522366703</v>
+        <v>-12.52138795235413</v>
       </c>
       <c r="AK10" t="n">
         <v>68.37492953824437</v>
@@ -2331,10 +2331,10 @@
         <v>100</v>
       </c>
       <c r="BA10" t="n">
-        <v>0.973212052632304</v>
+        <v>0.9340007043994232</v>
       </c>
       <c r="BB10" t="n">
-        <v>11907.22927254531</v>
+        <v>3538.823694418776</v>
       </c>
       <c r="BC10" t="n">
         <v>4.475970115066076</v>
@@ -2349,10 +2349,10 @@
         <v>0</v>
       </c>
       <c r="BG10" t="n">
-        <v>36.44950854230976</v>
+        <v>25.5428297092451</v>
       </c>
       <c r="BH10" t="n">
-        <v>36.32727754193699</v>
+        <v>23.21346531281761</v>
       </c>
     </row>
     <row r="11">
@@ -2456,13 +2456,13 @@
         <v>0</v>
       </c>
       <c r="AH11" t="n">
-        <v>47579.47600472617</v>
+        <v>45571.09884572247</v>
       </c>
       <c r="AI11" t="n">
-        <v>-250023.3290022075</v>
+        <v>-241591.4419820291</v>
       </c>
       <c r="AJ11" t="n">
-        <v>8.895522366703</v>
+        <v>-12.52138795235413</v>
       </c>
       <c r="AK11" t="n">
         <v>65.765</v>
@@ -2511,10 +2511,10 @@
         <v>100</v>
       </c>
       <c r="BA11" t="n">
-        <v>0.9871907645947534</v>
+        <v>0.9267320521775275</v>
       </c>
       <c r="BB11" t="n">
-        <v>3004.42021786584</v>
+        <v>-4431.075802492084</v>
       </c>
       <c r="BC11" t="n">
         <v>2.20487543395177</v>
@@ -2529,10 +2529,10 @@
         <v>0</v>
       </c>
       <c r="BG11" t="n">
-        <v>36.32727754193699</v>
+        <v>23.21346531281761</v>
       </c>
       <c r="BH11" t="n">
-        <v>37.20310813535692</v>
+        <v>21.76039464570018</v>
       </c>
     </row>
     <row r="12">
@@ -2636,13 +2636,13 @@
         <v>0</v>
       </c>
       <c r="AH12" t="n">
-        <v>44131.6554115867</v>
+        <v>40617.54697997558</v>
       </c>
       <c r="AI12" t="n">
-        <v>-253027.7492200733</v>
+        <v>-237160.366179537</v>
       </c>
       <c r="AJ12" t="n">
-        <v>8.895522366703</v>
+        <v>-12.52138795235413</v>
       </c>
       <c r="AK12" t="n">
         <v>63.295</v>
@@ -2691,10 +2691,10 @@
         <v>100</v>
       </c>
       <c r="BA12" t="n">
-        <v>1.007940701782509</v>
+        <v>0.9267441586507567</v>
       </c>
       <c r="BB12" t="n">
-        <v>-3582.902287020448</v>
+        <v>-10079.08169338501</v>
       </c>
       <c r="BC12" t="n">
         <v>0.8033392699129251</v>
@@ -2709,10 +2709,10 @@
         <v>0</v>
       </c>
       <c r="BG12" t="n">
-        <v>37.20310813535692</v>
+        <v>21.76039464570018</v>
       </c>
       <c r="BH12" t="n">
-        <v>39.02383752628205</v>
+        <v>20.82149048541144</v>
       </c>
     </row>
     <row r="13">
@@ -2816,13 +2816,13 @@
         <v>0</v>
       </c>
       <c r="AH13" t="n">
-        <v>40423.34472842945</v>
+        <v>35617.52180241271</v>
       </c>
       <c r="AI13" t="n">
-        <v>-249444.8469330529</v>
+        <v>-227081.284486152</v>
       </c>
       <c r="AJ13" t="n">
-        <v>8.895522366703</v>
+        <v>-12.52138795235413</v>
       </c>
       <c r="AK13" t="n">
         <v>60.73076923076924</v>
@@ -2871,10 +2871,10 @@
         <v>100</v>
       </c>
       <c r="BA13" t="n">
-        <v>1.036616181329966</v>
+        <v>0.9331624845914369</v>
       </c>
       <c r="BB13" t="n">
-        <v>-9273.070980026772</v>
+        <v>-14546.80934947369</v>
       </c>
       <c r="BC13" t="n">
         <v>0.09758233378155978</v>
@@ -2889,10 +2889,10 @@
         <v>0</v>
       </c>
       <c r="BG13" t="n">
-        <v>39.02383752628205</v>
+        <v>20.82149048541144</v>
       </c>
       <c r="BH13" t="n">
-        <v>41.84031032800412</v>
+        <v>20.34884085465865</v>
       </c>
     </row>
     <row r="14">
@@ -2996,13 +2996,13 @@
         <v>0</v>
       </c>
       <c r="AH14" t="n">
-        <v>44278.44925609089</v>
+        <v>36981.55298073561</v>
       </c>
       <c r="AI14" t="n">
-        <v>-240171.7759530261</v>
+        <v>-212534.4751366783</v>
       </c>
       <c r="AJ14" t="n">
-        <v>8.895522366703</v>
+        <v>-12.52138795235413</v>
       </c>
       <c r="AK14" t="n">
         <v>56.55384615384616</v>
@@ -3051,10 +3051,10 @@
         <v>100</v>
       </c>
       <c r="BA14" t="n">
-        <v>1.078668815540194</v>
+        <v>0.9477745788647102</v>
       </c>
       <c r="BB14" t="n">
-        <v>-17548.00094839134</v>
+        <v>-22079.09239733252</v>
       </c>
       <c r="BC14" t="n">
         <v>0.107396558993301</v>
@@ -3069,10 +3069,10 @@
         <v>0</v>
       </c>
       <c r="BG14" t="n">
-        <v>41.84031032800412</v>
+        <v>20.34884085465865</v>
       </c>
       <c r="BH14" t="n">
-        <v>46.73499959460959</v>
+        <v>20.37712354942133</v>
       </c>
     </row>
     <row r="15">
@@ -3176,13 +3176,13 @@
         <v>0</v>
       </c>
       <c r="AH15" t="n">
-        <v>39308.15327048204</v>
+        <v>30703.13424109436</v>
       </c>
       <c r="AI15" t="n">
-        <v>-222623.7750046348</v>
+        <v>-190455.3827393458</v>
       </c>
       <c r="AJ15" t="n">
-        <v>8.895522366703</v>
+        <v>-12.52138795235413</v>
       </c>
       <c r="AK15" t="n">
         <v>52</v>
@@ -3231,10 +3231,10 @@
         <v>100</v>
       </c>
       <c r="BA15" t="n">
-        <v>1.14002513776078</v>
+        <v>0.9736183493953846</v>
       </c>
       <c r="BB15" t="n">
-        <v>-22839.97067289398</v>
+        <v>-25199.09552290288</v>
       </c>
       <c r="BC15" t="n">
         <v>1.056834495757116</v>
@@ -3249,10 +3249,10 @@
         <v>0</v>
       </c>
       <c r="BG15" t="n">
-        <v>46.73499959460959</v>
+        <v>20.37712354942133</v>
       </c>
       <c r="BH15" t="n">
-        <v>53.58964730465238</v>
+        <v>20.96485846113388</v>
       </c>
     </row>
     <row r="16">
@@ -3356,13 +3356,13 @@
         <v>0</v>
       </c>
       <c r="AH16" t="n">
-        <v>35635.91984382608</v>
+        <v>26032.49947366162</v>
       </c>
       <c r="AI16" t="n">
-        <v>-199783.8043317408</v>
+        <v>-165256.2872164429</v>
       </c>
       <c r="AJ16" t="n">
-        <v>8.895522366703</v>
+        <v>-12.52138795235413</v>
       </c>
       <c r="AK16" t="n">
         <v>44</v>
@@ -3411,10 +3411,10 @@
         <v>100</v>
       </c>
       <c r="BA16" t="n">
-        <v>1.222895098458222</v>
+        <v>1.011777104389915</v>
       </c>
       <c r="BB16" t="n">
-        <v>-26471.29153442189</v>
+        <v>-26778.41970269778</v>
       </c>
       <c r="BC16" t="n">
         <v>3.0140960986827</v>
@@ -3429,10 +3429,10 @@
         <v>0</v>
       </c>
       <c r="BG16" t="n">
-        <v>53.58964730465238</v>
+        <v>20.96485846113388</v>
       </c>
       <c r="BH16" t="n">
-        <v>62.9766463448568</v>
+        <v>22.03300056412582</v>
       </c>
     </row>
     <row r="17">
@@ -3536,13 +3536,13 @@
         <v>0</v>
       </c>
       <c r="AH17" t="n">
-        <v>28870.73921816798</v>
+        <v>19744.03263057223</v>
       </c>
       <c r="AI17" t="n">
-        <v>-173312.5127973189</v>
+        <v>-138477.8675137452</v>
       </c>
       <c r="AJ17" t="n">
-        <v>8.895522366703</v>
+        <v>-12.52138795235413</v>
       </c>
       <c r="AK17" t="n">
         <v>40</v>
@@ -3591,10 +3591,10 @@
         <v>100</v>
       </c>
       <c r="BA17" t="n">
-        <v>1.327139287109632</v>
+        <v>1.061317485883823</v>
       </c>
       <c r="BB17" t="n">
-        <v>-25302.58192169503</v>
+        <v>-23900.02137026326</v>
       </c>
       <c r="BC17" t="n">
         <v>5.786995997647878</v>
@@ -3609,10 +3609,10 @@
         <v>0</v>
       </c>
       <c r="BG17" t="n">
-        <v>62.9766463448568</v>
+        <v>22.03300056412582</v>
       </c>
       <c r="BH17" t="n">
-        <v>74.18885215816957</v>
+        <v>23.34954780239644</v>
       </c>
     </row>
     <row r="18">
@@ -3716,13 +3716,13 @@
         <v>0</v>
       </c>
       <c r="AH18" t="n">
-        <v>29310.87146346142</v>
+        <v>18726.97334774573</v>
       </c>
       <c r="AI18" t="n">
-        <v>-148009.9308756239</v>
+        <v>-114577.8461434819</v>
       </c>
       <c r="AJ18" t="n">
-        <v>8.895522366703</v>
+        <v>-12.52138795235413</v>
       </c>
       <c r="AK18" t="n">
         <v>40</v>
@@ -3771,10 +3771,10 @@
         <v>100</v>
       </c>
       <c r="BA18" t="n">
-        <v>1.458141175153545</v>
+        <v>1.12336742583117</v>
       </c>
       <c r="BB18" t="n">
-        <v>-28895.43671521074</v>
+        <v>-25610.0576362883</v>
       </c>
       <c r="BC18" t="n">
         <v>9.235697947114929</v>
@@ -3789,10 +3789,10 @@
         <v>0</v>
       </c>
       <c r="BG18" t="n">
-        <v>74.18885215816957</v>
+        <v>23.34954780239644</v>
       </c>
       <c r="BH18" t="n">
-        <v>91.42843112700038</v>
+        <v>25.26571607735314</v>
       </c>
     </row>
     <row r="19">
@@ -3896,13 +3896,13 @@
         <v>0</v>
       </c>
       <c r="AH19" t="n">
-        <v>29300.49886779593</v>
+        <v>17305.62432390504</v>
       </c>
       <c r="AI19" t="n">
-        <v>-119114.4941604131</v>
+        <v>-88967.78850719359</v>
       </c>
       <c r="AJ19" t="n">
-        <v>8.895522366703</v>
+        <v>-12.52138795235413</v>
       </c>
       <c r="AK19" t="n">
         <v>40</v>
@@ -3951,10 +3951,10 @@
         <v>100</v>
       </c>
       <c r="BA19" t="n">
-        <v>1.641974102634091</v>
+        <v>1.207839240417992</v>
       </c>
       <c r="BB19" t="n">
-        <v>-31670.94512690204</v>
+        <v>-26266.89058348348</v>
       </c>
       <c r="BC19" t="n">
         <v>13.64354217495692</v>
@@ -3969,10 +3969,10 @@
         <v>0</v>
       </c>
       <c r="BG19" t="n">
-        <v>91.42843112700038</v>
+        <v>25.26571607735314</v>
       </c>
       <c r="BH19" t="n">
-        <v>121.1631101942303</v>
+        <v>27.86493428664652</v>
       </c>
     </row>
     <row r="20">
@@ -4076,13 +4076,13 @@
         <v>0</v>
       </c>
       <c r="AH20" t="n">
-        <v>28498.1906706416</v>
+        <v>15339.6100186595</v>
       </c>
       <c r="AI20" t="n">
-        <v>-87443.54903351111</v>
+        <v>-62700.8979237101</v>
       </c>
       <c r="AJ20" t="n">
-        <v>8.895522366703</v>
+        <v>-12.52138795235413</v>
       </c>
       <c r="AK20" t="n">
         <v>40</v>
@@ -4131,10 +4131,10 @@
         <v>100</v>
       </c>
       <c r="BA20" t="n">
-        <v>1.916918684164843</v>
+        <v>1.326632289745931</v>
       </c>
       <c r="BB20" t="n">
-        <v>-32979.61200600352</v>
+        <v>-25398.75199663377</v>
       </c>
       <c r="BC20" t="n">
         <v>19.16728406164694</v>
@@ -4149,10 +4149,10 @@
         <v>0</v>
       </c>
       <c r="BG20" t="n">
-        <v>121.1631101942303</v>
+        <v>27.86493428664652</v>
       </c>
       <c r="BH20" t="n">
-        <v>184.6476505058534</v>
+        <v>31.2717180758355</v>
       </c>
     </row>
     <row r="21">
@@ -4256,13 +4256,13 @@
         <v>0</v>
       </c>
       <c r="AH21" t="n">
-        <v>26047.20868866945</v>
+        <v>12587.38274117362</v>
       </c>
       <c r="AI21" t="n">
-        <v>-54463.93702750759</v>
+        <v>-37302.14592707633</v>
       </c>
       <c r="AJ21" t="n">
-        <v>8.895522366703</v>
+        <v>-12.52138795235413</v>
       </c>
       <c r="AK21" t="n">
         <v>40</v>
@@ -4311,10 +4311,10 @@
         <v>100</v>
       </c>
       <c r="BA21" t="n">
-        <v>2.373142190457793</v>
+        <v>1.50350259473588</v>
       </c>
       <c r="BB21" t="n">
-        <v>-31418.82957509765</v>
+        <v>-22198.0169999653</v>
       </c>
       <c r="BC21" t="n">
         <v>26.05658243769463</v>
@@ -4329,10 +4329,10 @@
         <v>0</v>
       </c>
       <c r="BG21" t="n">
-        <v>184.6476505058534</v>
+        <v>31.2717180758355</v>
       </c>
       <c r="BH21" t="n">
-        <v>403.0887235040509</v>
+        <v>35.68076560686083</v>
       </c>
     </row>
     <row r="22">
@@ -4436,13 +4436,13 @@
         <v>0</v>
       </c>
       <c r="AH22" t="n">
-        <v>19153.27415695275</v>
+        <v>8614.414358475264</v>
       </c>
       <c r="AI22" t="n">
-        <v>-23045.10745240993</v>
+        <v>-15104.12892711103</v>
       </c>
       <c r="AJ22" t="n">
-        <v>8.895522366703</v>
+        <v>-12.52138795235413</v>
       </c>
       <c r="AK22" t="n">
         <v>40</v>
@@ -4491,10 +4491,10 @@
         <v>100</v>
       </c>
       <c r="BA22" t="n">
-        <v>3.288665664667144</v>
+        <v>1.794330196609224</v>
       </c>
       <c r="BB22" t="n">
-        <v>-23041.79589910862</v>
+        <v>-15104.12892711105</v>
       </c>
       <c r="BC22" t="n">
         <v>34.74250301645503</v>
@@ -4509,7 +4509,7 @@
         <v>0</v>
       </c>
       <c r="BG22" t="n">
-        <v>403.0887235040509</v>
+        <v>35.68076560686083</v>
       </c>
       <c r="BH22" t="n">
         <v>39.9962422235724</v>

</xml_diff>

<commit_message>
Fixed bug for Spencer's Method for right-facing slopes
</commit_message>
<xml_diff>
--- a/slices.xlsx
+++ b/slices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BH22"/>
+  <dimension ref="A1:BB22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -696,40 +696,10 @@
       </c>
       <c r="BA1" s="1" t="inlineStr">
         <is>
-          <t>ma</t>
+          <t>yt_l</t>
         </is>
       </c>
       <c r="BB1" s="1" t="inlineStr">
-        <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="BC1" s="1" t="inlineStr">
-        <is>
-          <t>y_q</t>
-        </is>
-      </c>
-      <c r="BD1" s="1" t="inlineStr">
-        <is>
-          <t>Fh</t>
-        </is>
-      </c>
-      <c r="BE1" s="1" t="inlineStr">
-        <is>
-          <t>Fv</t>
-        </is>
-      </c>
-      <c r="BF1" s="1" t="inlineStr">
-        <is>
-          <t>Mo</t>
-        </is>
-      </c>
-      <c r="BG1" s="1" t="inlineStr">
-        <is>
-          <t>yt_l</t>
-        </is>
-      </c>
-      <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>yt_r</t>
         </is>
@@ -836,13 +806,13 @@
         <v>0</v>
       </c>
       <c r="AH2" t="n">
-        <v>-1238.89293509685</v>
+        <v>-263.490129717897</v>
       </c>
       <c r="AI2" t="n">
         <v>0</v>
       </c>
       <c r="AJ2" t="n">
-        <v>-12.52138795235413</v>
+        <v>-8.895705300300689</v>
       </c>
       <c r="AK2" t="n">
         <v>78.855630874209</v>
@@ -891,28 +861,10 @@
         <v>100</v>
       </c>
       <c r="BA2" t="n">
-        <v>2.525643448558156</v>
+        <v>84.00000000000006</v>
       </c>
       <c r="BB2" t="n">
-        <v>-1306.467707567553</v>
-      </c>
-      <c r="BC2" t="n">
-        <v>81.21329877556784</v>
-      </c>
-      <c r="BD2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE2" t="n">
-        <v>-356.6588438338362</v>
-      </c>
-      <c r="BF2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG2" t="n">
-        <v>84.00000000000006</v>
-      </c>
-      <c r="BH2" t="n">
-        <v>81.10397589356462</v>
+        <v>81.13625166065518</v>
       </c>
     </row>
     <row r="3">
@@ -1016,13 +968,13 @@
         <v>0</v>
       </c>
       <c r="AH3" t="n">
-        <v>9178.426058408142</v>
+        <v>4332.154894227278</v>
       </c>
       <c r="AI3" t="n">
-        <v>1306.467707567553</v>
+        <v>-351.0935560601921</v>
       </c>
       <c r="AJ3" t="n">
-        <v>-12.52138795235413</v>
+        <v>-8.895705300300689</v>
       </c>
       <c r="AK3" t="n">
         <v>78.63592483281701</v>
@@ -1071,28 +1023,10 @@
         <v>100</v>
       </c>
       <c r="BA3" t="n">
-        <v>1.97470111438668</v>
+        <v>81.13625166065518</v>
       </c>
       <c r="BB3" t="n">
-        <v>14619.35178207635</v>
-      </c>
-      <c r="BC3" t="n">
-        <v>70.37079750256237</v>
-      </c>
-      <c r="BD3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE3" t="n">
-        <v>-7857.753192819717</v>
-      </c>
-      <c r="BF3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG3" t="n">
-        <v>81.10397589356462</v>
-      </c>
-      <c r="BH3" t="n">
-        <v>68.87335299518907</v>
+        <v>69.67467870263968</v>
       </c>
     </row>
     <row r="4">
@@ -1196,13 +1130,13 @@
         <v>0</v>
       </c>
       <c r="AH4" t="n">
-        <v>50902.93712701974</v>
+        <v>29608.58027461288</v>
       </c>
       <c r="AI4" t="n">
-        <v>-13312.8840745088</v>
+        <v>10479.5238595941</v>
       </c>
       <c r="AJ4" t="n">
-        <v>-12.52138795235413</v>
+        <v>-8.895705300300689</v>
       </c>
       <c r="AK4" t="n">
         <v>77.91714056524853</v>
@@ -1251,28 +1185,10 @@
         <v>100</v>
       </c>
       <c r="BA4" t="n">
-        <v>1.287292231038373</v>
+        <v>69.67467870263968</v>
       </c>
       <c r="BB4" t="n">
-        <v>72130.61487837438</v>
-      </c>
-      <c r="BC4" t="n">
-        <v>50.07315218453382</v>
-      </c>
-      <c r="BD4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE4" t="n">
-        <v>-56786.33813691734</v>
-      </c>
-      <c r="BF4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG4" t="n">
-        <v>68.87335299518907</v>
-      </c>
-      <c r="BH4" t="n">
-        <v>51.29604027399181</v>
+        <v>51.7531074920696</v>
       </c>
     </row>
     <row r="5">
@@ -1376,13 +1292,13 @@
         <v>0</v>
       </c>
       <c r="AH5" t="n">
-        <v>40737.30859266572</v>
+        <v>27922.04264876728</v>
       </c>
       <c r="AI5" t="n">
-        <v>-85443.49895288318</v>
+        <v>71500.27834923461</v>
       </c>
       <c r="AJ5" t="n">
-        <v>-12.52138795235413</v>
+        <v>-8.895705300300689</v>
       </c>
       <c r="AK5" t="n">
         <v>77.00654727586166</v>
@@ -1431,28 +1347,10 @@
         <v>100</v>
       </c>
       <c r="BA5" t="n">
-        <v>1.19620909154821</v>
+        <v>51.7531074920696</v>
       </c>
       <c r="BB5" t="n">
-        <v>45999.73653439412</v>
-      </c>
-      <c r="BC5" t="n">
-        <v>34.32872717186068</v>
-      </c>
-      <c r="BD5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE5" t="n">
-        <v>-57092.64759767729</v>
-      </c>
-      <c r="BF5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG5" t="n">
-        <v>51.29604027399181</v>
-      </c>
-      <c r="BH5" t="n">
-        <v>43.67869361320182</v>
+        <v>44.05438597026956</v>
       </c>
     </row>
     <row r="6">
@@ -1556,13 +1454,13 @@
         <v>0</v>
       </c>
       <c r="AH6" t="n">
-        <v>44147.78855750636</v>
+        <v>33698.57345613423</v>
       </c>
       <c r="AI6" t="n">
-        <v>-131443.2354872773</v>
+        <v>114388.3728871403</v>
       </c>
       <c r="AJ6" t="n">
-        <v>-12.52138795235413</v>
+        <v>-8.895705300300689</v>
       </c>
       <c r="AK6" t="n">
         <v>76.26334212005389</v>
@@ -1611,28 +1509,10 @@
         <v>100</v>
       </c>
       <c r="BA6" t="n">
-        <v>1.08969729518768</v>
+        <v>44.05438597026956</v>
       </c>
       <c r="BB6" t="n">
-        <v>39649.88084506032</v>
-      </c>
-      <c r="BC6" t="n">
-        <v>25.09193914530816</v>
-      </c>
-      <c r="BD6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE6" t="n">
-        <v>-68268.58837034137</v>
-      </c>
-      <c r="BF6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG6" t="n">
-        <v>43.67869361320182</v>
-      </c>
-      <c r="BH6" t="n">
-        <v>37.57150888578319</v>
+        <v>37.87874927014892</v>
       </c>
     </row>
     <row r="7">
@@ -1736,13 +1616,13 @@
         <v>0</v>
       </c>
       <c r="AH7" t="n">
-        <v>46724.66041240805</v>
+        <v>38871.0276108088</v>
       </c>
       <c r="AI7" t="n">
-        <v>-171093.1163323376</v>
+        <v>154547.120363853</v>
       </c>
       <c r="AJ7" t="n">
-        <v>-12.52138795235413</v>
+        <v>-8.895705300300689</v>
       </c>
       <c r="AK7" t="n">
         <v>74.73179054836476</v>
@@ -1791,28 +1671,10 @@
         <v>100</v>
       </c>
       <c r="BA7" t="n">
-        <v>1.022798475221807</v>
+        <v>37.87874927014892</v>
       </c>
       <c r="BB7" t="n">
-        <v>31435.85858423841</v>
-      </c>
-      <c r="BC7" t="n">
-        <v>17.8922612956589</v>
-      </c>
-      <c r="BD7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE7" t="n">
-        <v>-76979.75214270862</v>
-      </c>
-      <c r="BF7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG7" t="n">
-        <v>37.57150888578319</v>
-      </c>
-      <c r="BH7" t="n">
-        <v>32.63926217169369</v>
+        <v>32.8925908389824</v>
       </c>
     </row>
     <row r="8">
@@ -1916,13 +1778,13 @@
         <v>0</v>
       </c>
       <c r="AH8" t="n">
-        <v>48888.13030562105</v>
+        <v>43649.98656765717</v>
       </c>
       <c r="AI8" t="n">
-        <v>-202528.974916576</v>
+        <v>189467.6940758316</v>
       </c>
       <c r="AJ8" t="n">
-        <v>-12.52138795235413</v>
+        <v>-8.895705300300689</v>
       </c>
       <c r="AK8" t="n">
         <v>72.76760549372993</v>
@@ -1971,28 +1833,10 @@
         <v>100</v>
       </c>
       <c r="BA8" t="n">
-        <v>0.9790507117737064</v>
+        <v>32.8925908389824</v>
       </c>
       <c r="BB8" t="n">
-        <v>22422.59851412284</v>
-      </c>
-      <c r="BC8" t="n">
-        <v>12.22696543209685</v>
-      </c>
-      <c r="BD8" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE8" t="n">
-        <v>-83834.4088533293</v>
-      </c>
-      <c r="BF8" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG8" t="n">
-        <v>32.63926217169369</v>
-      </c>
-      <c r="BH8" t="n">
-        <v>28.67038553945456</v>
+        <v>28.87466999988604</v>
       </c>
     </row>
     <row r="9">
@@ -2096,13 +1940,13 @@
         <v>0</v>
       </c>
       <c r="AH9" t="n">
-        <v>50700.3740035157</v>
+        <v>48042.70950462885</v>
       </c>
       <c r="AI9" t="n">
-        <v>-224951.5734306988</v>
+        <v>217653.0421241137</v>
       </c>
       <c r="AJ9" t="n">
-        <v>-12.52138795235413</v>
+        <v>-8.895705300300689</v>
       </c>
       <c r="AK9" t="n">
         <v>70.80342043909509</v>
@@ -2151,28 +1995,10 @@
         <v>100</v>
       </c>
       <c r="BA9" t="n">
-        <v>0.9507818989724603</v>
+        <v>28.87466999988604</v>
       </c>
       <c r="BB9" t="n">
-        <v>13101.04485691148</v>
-      </c>
-      <c r="BC9" t="n">
-        <v>7.812733485778423</v>
-      </c>
-      <c r="BD9" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE9" t="n">
-        <v>-89175.35579798571</v>
-      </c>
-      <c r="BF9" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG9" t="n">
-        <v>28.67038553945456</v>
-      </c>
-      <c r="BH9" t="n">
-        <v>25.5428297092451</v>
+        <v>25.69169069832504</v>
       </c>
     </row>
     <row r="10">
@@ -2276,13 +2102,13 @@
         <v>0</v>
       </c>
       <c r="AH10" t="n">
-        <v>52534.46950646966</v>
+        <v>52500.85350505389</v>
       </c>
       <c r="AI10" t="n">
-        <v>-238052.6182876103</v>
+        <v>238115.2714811733</v>
       </c>
       <c r="AJ10" t="n">
-        <v>-12.52138795235413</v>
+        <v>-8.895705300300689</v>
       </c>
       <c r="AK10" t="n">
         <v>68.37492953824437</v>
@@ -2331,28 +2157,10 @@
         <v>100</v>
       </c>
       <c r="BA10" t="n">
-        <v>0.9340007043994232</v>
+        <v>25.69169069832504</v>
       </c>
       <c r="BB10" t="n">
-        <v>3538.823694418776</v>
-      </c>
-      <c r="BC10" t="n">
-        <v>4.475970115066076</v>
-      </c>
-      <c r="BD10" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE10" t="n">
-        <v>-93212.63257604709</v>
-      </c>
-      <c r="BF10" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG10" t="n">
-        <v>25.5428297092451</v>
-      </c>
-      <c r="BH10" t="n">
-        <v>23.21346531281761</v>
+        <v>23.28078639983498</v>
       </c>
     </row>
     <row r="11">
@@ -2456,13 +2264,13 @@
         <v>0</v>
       </c>
       <c r="AH11" t="n">
-        <v>45571.09884572247</v>
+        <v>47579.46138868868</v>
       </c>
       <c r="AI11" t="n">
-        <v>-241591.4419820291</v>
+        <v>250022.4030152136</v>
       </c>
       <c r="AJ11" t="n">
-        <v>-12.52138795235413</v>
+        <v>-8.895705300300689</v>
       </c>
       <c r="AK11" t="n">
         <v>65.765</v>
@@ -2511,28 +2319,10 @@
         <v>100</v>
       </c>
       <c r="BA11" t="n">
-        <v>0.9267320521775275</v>
+        <v>23.28078639983498</v>
       </c>
       <c r="BB11" t="n">
-        <v>-4431.075802492084</v>
-      </c>
-      <c r="BC11" t="n">
-        <v>2.20487543395177</v>
-      </c>
-      <c r="BD11" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE11" t="n">
-        <v>-82626.63026726997</v>
-      </c>
-      <c r="BF11" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG11" t="n">
-        <v>23.21346531281761</v>
-      </c>
-      <c r="BH11" t="n">
-        <v>21.76039464570018</v>
+        <v>21.74951749706717</v>
       </c>
     </row>
     <row r="12">
@@ -2636,13 +2426,13 @@
         <v>0</v>
       </c>
       <c r="AH12" t="n">
-        <v>40617.54697997558</v>
+        <v>44131.66947491431</v>
       </c>
       <c r="AI12" t="n">
-        <v>-237160.366179537</v>
+        <v>253026.7317882518</v>
       </c>
       <c r="AJ12" t="n">
-        <v>-12.52138795235413</v>
+        <v>-8.895705300300689</v>
       </c>
       <c r="AK12" t="n">
         <v>63.295</v>
@@ -2691,28 +2481,10 @@
         <v>100</v>
       </c>
       <c r="BA12" t="n">
-        <v>0.9267441586507567</v>
+        <v>21.74951749706717</v>
       </c>
       <c r="BB12" t="n">
-        <v>-10079.08169338501</v>
-      </c>
-      <c r="BC12" t="n">
-        <v>0.8033392699129251</v>
-      </c>
-      <c r="BD12" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE12" t="n">
-        <v>-77014.26421479211</v>
-      </c>
-      <c r="BF12" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG12" t="n">
-        <v>21.76039464570018</v>
-      </c>
-      <c r="BH12" t="n">
-        <v>20.82149048541144</v>
+        <v>20.75245860086207</v>
       </c>
     </row>
     <row r="13">
@@ -2816,13 +2588,13 @@
         <v>0</v>
       </c>
       <c r="AH13" t="n">
-        <v>35617.52180241271</v>
+        <v>40423.3848287001</v>
       </c>
       <c r="AI13" t="n">
-        <v>-227081.284486152</v>
+        <v>249443.7370002513</v>
       </c>
       <c r="AJ13" t="n">
-        <v>-12.52138795235413</v>
+        <v>-8.895705300300689</v>
       </c>
       <c r="AK13" t="n">
         <v>60.73076923076924</v>
@@ -2871,28 +2643,10 @@
         <v>100</v>
       </c>
       <c r="BA13" t="n">
-        <v>0.9331624845914369</v>
+        <v>20.75245860086207</v>
       </c>
       <c r="BB13" t="n">
-        <v>-14546.80934947369</v>
-      </c>
-      <c r="BC13" t="n">
-        <v>0.09758233378155978</v>
-      </c>
-      <c r="BD13" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE13" t="n">
-        <v>-70645.72529742388</v>
-      </c>
-      <c r="BF13" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG13" t="n">
-        <v>20.82149048541144</v>
-      </c>
-      <c r="BH13" t="n">
-        <v>20.34884085465865</v>
+        <v>20.23640734131954</v>
       </c>
     </row>
     <row r="14">
@@ -2996,13 +2750,13 @@
         <v>0</v>
       </c>
       <c r="AH14" t="n">
-        <v>36981.55298073561</v>
+        <v>44278.52931612825</v>
       </c>
       <c r="AI14" t="n">
-        <v>-212534.4751366783</v>
+        <v>240170.5697123781</v>
       </c>
       <c r="AJ14" t="n">
-        <v>-12.52138795235413</v>
+        <v>-8.895705300300689</v>
       </c>
       <c r="AK14" t="n">
         <v>56.55384615384616</v>
@@ -3051,28 +2805,10 @@
         <v>100</v>
       </c>
       <c r="BA14" t="n">
-        <v>0.9477745788647102</v>
+        <v>20.23640734131954</v>
       </c>
       <c r="BB14" t="n">
-        <v>-22079.09239733252</v>
-      </c>
-      <c r="BC14" t="n">
-        <v>0.107396558993301</v>
-      </c>
-      <c r="BD14" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE14" t="n">
-        <v>-75636.12672156718</v>
-      </c>
-      <c r="BF14" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG14" t="n">
-        <v>20.34884085465865</v>
-      </c>
-      <c r="BH14" t="n">
-        <v>20.37712354942133</v>
+        <v>20.217882391099</v>
       </c>
     </row>
     <row r="15">
@@ -3176,13 +2912,13 @@
         <v>0</v>
       </c>
       <c r="AH15" t="n">
-        <v>30703.13424109436</v>
+        <v>39308.26420413349</v>
       </c>
       <c r="AI15" t="n">
-        <v>-190455.3827393458</v>
+        <v>222622.4430803917</v>
       </c>
       <c r="AJ15" t="n">
-        <v>-12.52138795235413</v>
+        <v>-8.895705300300689</v>
       </c>
       <c r="AK15" t="n">
         <v>52</v>
@@ -3231,28 +2967,10 @@
         <v>100</v>
       </c>
       <c r="BA15" t="n">
-        <v>0.9736183493953846</v>
+        <v>20.217882391099</v>
       </c>
       <c r="BB15" t="n">
-        <v>-25199.09552290288</v>
-      </c>
-      <c r="BC15" t="n">
-        <v>1.056834495757116</v>
-      </c>
-      <c r="BD15" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE15" t="n">
-        <v>-64927.57875272598</v>
-      </c>
-      <c r="BF15" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG15" t="n">
-        <v>20.37712354942133</v>
-      </c>
-      <c r="BH15" t="n">
-        <v>20.96485846113388</v>
+        <v>20.77587039197478</v>
       </c>
     </row>
     <row r="16">
@@ -3356,13 +3074,13 @@
         <v>0</v>
       </c>
       <c r="AH16" t="n">
-        <v>26032.49947366162</v>
+        <v>35636.05959501668</v>
       </c>
       <c r="AI16" t="n">
-        <v>-165256.2872164429</v>
+        <v>199782.3330560254</v>
       </c>
       <c r="AJ16" t="n">
-        <v>-12.52138795235413</v>
+        <v>-8.895705300300689</v>
       </c>
       <c r="AK16" t="n">
         <v>44</v>
@@ -3411,28 +3129,10 @@
         <v>100</v>
       </c>
       <c r="BA16" t="n">
-        <v>1.011777104389915</v>
+        <v>20.77587039197478</v>
       </c>
       <c r="BB16" t="n">
-        <v>-26778.41970269778</v>
-      </c>
-      <c r="BC16" t="n">
-        <v>3.0140960986827</v>
-      </c>
-      <c r="BD16" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE16" t="n">
-        <v>-52906.44124107569</v>
-      </c>
-      <c r="BF16" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG16" t="n">
-        <v>20.96485846113388</v>
-      </c>
-      <c r="BH16" t="n">
-        <v>22.03300056412582</v>
+        <v>21.82653761969504</v>
       </c>
     </row>
     <row r="17">
@@ -3536,13 +3236,13 @@
         <v>0</v>
       </c>
       <c r="AH17" t="n">
-        <v>19744.03263057223</v>
+        <v>28870.8861214081</v>
       </c>
       <c r="AI17" t="n">
-        <v>-138477.8675137452</v>
+        <v>173310.8829600393</v>
       </c>
       <c r="AJ17" t="n">
-        <v>-12.52138795235413</v>
+        <v>-8.895705300300689</v>
       </c>
       <c r="AK17" t="n">
         <v>40</v>
@@ -3591,28 +3291,10 @@
         <v>100</v>
       </c>
       <c r="BA17" t="n">
-        <v>1.061317485883823</v>
+        <v>21.82653761969504</v>
       </c>
       <c r="BB17" t="n">
-        <v>-23900.02137026326</v>
-      </c>
-      <c r="BC17" t="n">
-        <v>5.786995997647878</v>
-      </c>
-      <c r="BD17" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE17" t="n">
-        <v>-38159.06324089572</v>
-      </c>
-      <c r="BF17" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG17" t="n">
-        <v>22.03300056412582</v>
-      </c>
-      <c r="BH17" t="n">
-        <v>23.34954780239644</v>
+        <v>23.13302111351473</v>
       </c>
     </row>
     <row r="18">
@@ -3716,13 +3398,13 @@
         <v>0</v>
       </c>
       <c r="AH18" t="n">
-        <v>18726.97334774573</v>
+        <v>29311.05773992906</v>
       </c>
       <c r="AI18" t="n">
-        <v>-114577.8461434819</v>
+        <v>148008.1418949654</v>
       </c>
       <c r="AJ18" t="n">
-        <v>-12.52138795235413</v>
+        <v>-8.895705300300689</v>
       </c>
       <c r="AK18" t="n">
         <v>40</v>
@@ -3771,28 +3453,10 @@
         <v>100</v>
       </c>
       <c r="BA18" t="n">
-        <v>1.12336742583117</v>
+        <v>23.13302111351473</v>
       </c>
       <c r="BB18" t="n">
-        <v>-25610.0576362883</v>
-      </c>
-      <c r="BC18" t="n">
-        <v>9.235697947114929</v>
-      </c>
-      <c r="BD18" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE18" t="n">
-        <v>-34312.59492786288</v>
-      </c>
-      <c r="BF18" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG18" t="n">
-        <v>23.34954780239644</v>
-      </c>
-      <c r="BH18" t="n">
-        <v>25.26571607735314</v>
+        <v>25.02146089394151</v>
       </c>
     </row>
     <row r="19">
@@ -3896,13 +3560,13 @@
         <v>0</v>
       </c>
       <c r="AH19" t="n">
-        <v>17305.62432390504</v>
+        <v>29300.73188562266</v>
       </c>
       <c r="AI19" t="n">
-        <v>-88967.78850719359</v>
+        <v>119112.5078362852</v>
       </c>
       <c r="AJ19" t="n">
-        <v>-12.52138795235413</v>
+        <v>-8.895705300300689</v>
       </c>
       <c r="AK19" t="n">
         <v>40</v>
@@ -3951,28 +3615,10 @@
         <v>100</v>
       </c>
       <c r="BA19" t="n">
-        <v>1.207839240417992</v>
+        <v>25.02146089394151</v>
       </c>
       <c r="BB19" t="n">
-        <v>-26266.89058348348</v>
-      </c>
-      <c r="BC19" t="n">
-        <v>13.64354217495692</v>
-      </c>
-      <c r="BD19" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE19" t="n">
-        <v>-29396.35879043768</v>
-      </c>
-      <c r="BF19" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG19" t="n">
-        <v>25.26571607735314</v>
-      </c>
-      <c r="BH19" t="n">
-        <v>27.86493428664652</v>
+        <v>27.58051703355543</v>
       </c>
     </row>
     <row r="20">
@@ -4076,13 +3722,13 @@
         <v>0</v>
       </c>
       <c r="AH20" t="n">
-        <v>15339.6100186595</v>
+        <v>28498.47933690739</v>
       </c>
       <c r="AI20" t="n">
-        <v>-62700.8979237101</v>
+        <v>87441.31792979216</v>
       </c>
       <c r="AJ20" t="n">
-        <v>-12.52138795235413</v>
+        <v>-8.895705300300689</v>
       </c>
       <c r="AK20" t="n">
         <v>40</v>
@@ -4131,28 +3777,10 @@
         <v>100</v>
       </c>
       <c r="BA20" t="n">
-        <v>1.326632289745931</v>
+        <v>27.58051703355543</v>
       </c>
       <c r="BB20" t="n">
-        <v>-25398.75199663377</v>
-      </c>
-      <c r="BC20" t="n">
-        <v>19.16728406164694</v>
-      </c>
-      <c r="BD20" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE20" t="n">
-        <v>-23235.51959706836</v>
-      </c>
-      <c r="BF20" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG20" t="n">
-        <v>27.86493428664652</v>
-      </c>
-      <c r="BH20" t="n">
-        <v>31.2717180758355</v>
+        <v>30.95233001688217</v>
       </c>
     </row>
     <row r="21">
@@ -4256,13 +3884,13 @@
         <v>0</v>
       </c>
       <c r="AH21" t="n">
-        <v>12587.38274117362</v>
+        <v>26047.55986138142</v>
       </c>
       <c r="AI21" t="n">
-        <v>-37302.14592707633</v>
+        <v>54461.40285713836</v>
       </c>
       <c r="AJ21" t="n">
-        <v>-12.52138795235413</v>
+        <v>-8.895705300300689</v>
       </c>
       <c r="AK21" t="n">
         <v>40</v>
@@ -4311,28 +3939,10 @@
         <v>100</v>
       </c>
       <c r="BA21" t="n">
-        <v>1.50350259473588</v>
+        <v>30.95233001688217</v>
       </c>
       <c r="BB21" t="n">
-        <v>-22198.0169999653</v>
-      </c>
-      <c r="BC21" t="n">
-        <v>26.05658243769463</v>
-      </c>
-      <c r="BD21" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE21" t="n">
-        <v>-15551.62336863631</v>
-      </c>
-      <c r="BF21" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG21" t="n">
-        <v>31.2717180758355</v>
-      </c>
-      <c r="BH21" t="n">
-        <v>35.68076560686083</v>
+        <v>35.40375914414403</v>
       </c>
     </row>
     <row r="22">
@@ -4436,13 +4046,13 @@
         <v>0</v>
       </c>
       <c r="AH22" t="n">
-        <v>8614.414358475264</v>
+        <v>19153.65912806178</v>
       </c>
       <c r="AI22" t="n">
-        <v>-15104.12892711103</v>
+        <v>23042.20337559174</v>
       </c>
       <c r="AJ22" t="n">
-        <v>-12.52138795235413</v>
+        <v>-8.895705300300689</v>
       </c>
       <c r="AK22" t="n">
         <v>40</v>
@@ -4491,27 +4101,9 @@
         <v>100</v>
       </c>
       <c r="BA22" t="n">
-        <v>1.794330196609224</v>
+        <v>35.40375914414403</v>
       </c>
       <c r="BB22" t="n">
-        <v>-15104.12892711105</v>
-      </c>
-      <c r="BC22" t="n">
-        <v>34.74250301645503</v>
-      </c>
-      <c r="BD22" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE22" t="n">
-        <v>-5863.88613727454</v>
-      </c>
-      <c r="BF22" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG22" t="n">
-        <v>35.68076560686083</v>
-      </c>
-      <c r="BH22" t="n">
         <v>39.9962422235724</v>
       </c>
     </row>

</xml_diff>